<commit_message>
Fixed the Kosovo-Trinidad confusion, see https://github.com/IndEcol/IE_data_commons/issues/25.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20445" windowHeight="9683" tabRatio="603" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20445" windowHeight="9683" tabRatio="603"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="13" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7562" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7598" uniqueCount="1384">
   <si>
     <t>Description</t>
   </si>
@@ -4118,6 +4118,63 @@
   </si>
   <si>
     <t>YSTAFDB, MFA, metal cycle, material, resource, stocks, minor elements, minor metals</t>
+  </si>
+  <si>
+    <t>RECC-Global_v2_4</t>
+  </si>
+  <si>
+    <t>RECC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resource efficiency; dynamic MFA; </t>
+  </si>
+  <si>
+    <t>https://cie.research.yale.edu/research/resource-efficiency-climate-change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECC = Resource Efficiency and Climate Change mitigation </t>
+  </si>
+  <si>
+    <t>The Group of Seven (G7) member countries requested that the International Resource Panel conduct an assessment of the potential contribution of Resource Efficiency to Climate Change mitigation (RECC). The RECC model and database was developed for that purpose, and the main quantitative results are archived here.</t>
+  </si>
+  <si>
+    <t>stocks, flows</t>
+  </si>
+  <si>
+    <t>whole economy, with focus on material production, use phase, and waste management</t>
+  </si>
+  <si>
+    <t>processes relevant for materials, economy-wide</t>
+  </si>
+  <si>
+    <t>residential buildings, non-residential buildings, passenger vehicles, other vehicles, infrastructure, industry assets, appliances</t>
+  </si>
+  <si>
+    <t>13 residential building, 24 non-residential building, and 6 passenger vehicle types</t>
+  </si>
+  <si>
+    <t>13 material groups: construction grade steel, automotive steel, stainless steel, cast iron, wrought Al, cast Al, copper electric grade, plastics, cement, wood and wood products, zinc, concrete, concrete aggregates</t>
+  </si>
+  <si>
+    <t>materials and material groups whose production is relevant for GHG emissions</t>
+  </si>
+  <si>
+    <t>20 countries and world regions</t>
+  </si>
+  <si>
+    <t>2016-2060</t>
+  </si>
+  <si>
+    <t>Future material cycle data and energy and GHG extensions for end-use sectors under different socioeconomic, climate policy, and resource efficiency scenarios</t>
+  </si>
+  <si>
+    <t>resource efficiency; dynamic MFA; steel; aluminium; cement;</t>
+  </si>
+  <si>
+    <t>ODYM_RECC_SysDef_v2_4.png</t>
+  </si>
+  <si>
+    <t>DOI XXX (Nat Comms)</t>
   </si>
 </sst>
 </file>
@@ -4240,7 +4297,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4292,6 +4349,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4478,7 +4541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -4798,6 +4861,8 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -5087,8 +5152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5120,7 +5185,9 @@
       <c r="F3" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="39" t="s">
+        <v>1366</v>
+      </c>
       <c r="H3" s="36"/>
       <c r="I3" s="36"/>
     </row>
@@ -5140,6 +5207,9 @@
       <c r="F4" s="57">
         <v>2</v>
       </c>
+      <c r="G4" s="57">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="154"/>
@@ -5155,6 +5225,9 @@
       <c r="F5" s="119" t="s">
         <v>1132</v>
       </c>
+      <c r="G5" s="119" t="s">
+        <v>1366</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="155" t="s">
@@ -5166,6 +5239,7 @@
       <c r="D6" s="26"/>
       <c r="E6" s="52"/>
       <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="155"/>
@@ -5175,6 +5249,7 @@
       <c r="D7" s="26"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="155"/>
@@ -5184,6 +5259,7 @@
       <c r="D8" s="26"/>
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="155"/>
@@ -5193,6 +5269,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="155"/>
@@ -5202,6 +5279,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="52"/>
       <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="155"/>
@@ -5211,6 +5289,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="52"/>
       <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="155"/>
@@ -5220,6 +5299,7 @@
       <c r="D12" s="24"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="155"/>
@@ -5229,6 +5309,7 @@
       <c r="D13" s="24"/>
       <c r="E13" s="52"/>
       <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="155"/>
@@ -5238,6 +5319,7 @@
       <c r="D14" s="24"/>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="155"/>
@@ -5247,6 +5329,7 @@
       <c r="D15" s="24"/>
       <c r="E15" s="52"/>
       <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="155"/>
@@ -5256,8 +5339,9 @@
       <c r="D16" s="25"/>
       <c r="E16" s="52"/>
       <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" s="155"/>
       <c r="C17" s="27" t="s">
         <v>434</v>
@@ -5265,8 +5349,9 @@
       <c r="D17" s="25"/>
       <c r="E17" s="52"/>
       <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="155"/>
       <c r="C18" s="27" t="s">
         <v>435</v>
@@ -5274,8 +5359,9 @@
       <c r="D18" s="25"/>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="156" t="s">
         <v>0</v>
       </c>
@@ -5287,8 +5373,11 @@
       <c r="F19" s="119" t="s">
         <v>1006</v>
       </c>
+      <c r="G19" s="119" t="s">
+        <v>1370</v>
+      </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="156"/>
       <c r="C20" s="27" t="s">
         <v>437</v>
@@ -5302,8 +5391,11 @@
       <c r="F20" s="119" t="s">
         <v>1007</v>
       </c>
+      <c r="G20" s="119" t="s">
+        <v>1367</v>
+      </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="156"/>
       <c r="C21" s="27" t="s">
         <v>438</v>
@@ -5313,8 +5405,11 @@
       <c r="F21" s="119" t="s">
         <v>1008</v>
       </c>
+      <c r="G21" s="119" t="s">
+        <v>1369</v>
+      </c>
     </row>
-    <row r="22" spans="2:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="157" t="s">
         <v>8</v>
       </c>
@@ -5328,8 +5423,11 @@
       <c r="F22" s="52" t="s">
         <v>860</v>
       </c>
+      <c r="G22" s="52" t="s">
+        <v>860</v>
+      </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="157"/>
       <c r="C23" s="26" t="s">
         <v>440</v>
@@ -5337,8 +5435,9 @@
       <c r="D23" s="25"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="157"/>
       <c r="C24" s="25" t="s">
         <v>441</v>
@@ -5346,8 +5445,9 @@
       <c r="D24" s="24"/>
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="157"/>
       <c r="C25" s="25" t="s">
         <v>443</v>
@@ -5357,8 +5457,11 @@
       <c r="F25" s="52" t="s">
         <v>1005</v>
       </c>
+      <c r="G25" s="90" t="s">
+        <v>1368</v>
+      </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="157"/>
       <c r="C26" s="25" t="s">
         <v>444</v>
@@ -5368,8 +5471,9 @@
         <v>208</v>
       </c>
       <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" s="157"/>
       <c r="C27" s="25" t="s">
         <v>445</v>
@@ -5377,8 +5481,9 @@
       <c r="D27" s="24"/>
       <c r="E27" s="52"/>
       <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
     </row>
-    <row r="28" spans="2:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="158" t="s">
         <v>9</v>
       </c>
@@ -5394,8 +5499,11 @@
       <c r="F28" s="123">
         <v>43347</v>
       </c>
+      <c r="G28" s="123">
+        <v>44404</v>
+      </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="158"/>
       <c r="C29" s="25" t="s">
         <v>447</v>
@@ -5409,8 +5517,11 @@
       <c r="F29" s="124" t="s">
         <v>30</v>
       </c>
+      <c r="G29" s="124" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" s="151" t="s">
         <v>185</v>
       </c>
@@ -5420,8 +5531,9 @@
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" s="152"/>
       <c r="C31" s="108" t="s">
         <v>449</v>
@@ -5429,8 +5541,9 @@
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="153"/>
       <c r="C32" s="109" t="s">
         <v>450</v>
@@ -5438,6 +5551,7 @@
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5454,13 +5568,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O39"/>
+  <dimension ref="B2:P39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5475,16 +5589,17 @@
     <col min="11" max="13" width="10.6640625" style="105"/>
     <col min="14" max="14" width="64.53125" customWidth="1"/>
     <col min="15" max="15" width="55.53125" customWidth="1"/>
+    <col min="16" max="16" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="32"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -5525,8 +5640,11 @@
       <c r="O3" s="39" t="s">
         <v>1269</v>
       </c>
+      <c r="P3" s="173" t="s">
+        <v>1365</v>
+      </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="159" t="s">
         <v>2</v>
       </c>
@@ -5569,8 +5687,11 @@
       <c r="O4" s="141">
         <v>11</v>
       </c>
+      <c r="P4" s="141">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="160"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
@@ -5611,8 +5732,11 @@
       <c r="O5" s="118" t="s">
         <v>1273</v>
       </c>
+      <c r="P5" t="s">
+        <v>1365</v>
+      </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="33"/>
       <c r="C6" s="54" t="s">
         <v>453</v>
@@ -5651,8 +5775,11 @@
       <c r="O6" s="135" t="s">
         <v>1151</v>
       </c>
+      <c r="P6" t="s">
+        <v>1151</v>
+      </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
@@ -5693,8 +5820,11 @@
       <c r="O7" s="121" t="s">
         <v>11</v>
       </c>
+      <c r="P7" t="s">
+        <v>1366</v>
+      </c>
     </row>
-    <row r="8" spans="2:15" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="155" t="s">
         <v>6</v>
       </c>
@@ -5735,8 +5865,11 @@
       <c r="O8" s="121" t="s">
         <v>1274</v>
       </c>
+      <c r="P8" t="s">
+        <v>1371</v>
+      </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="155"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
@@ -5775,8 +5908,11 @@
       <c r="O9" s="121" t="s">
         <v>1274</v>
       </c>
+      <c r="P9" s="105" t="s">
+        <v>1371</v>
+      </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="155"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
@@ -5815,8 +5951,11 @@
       <c r="O10" s="121" t="s">
         <v>1013</v>
       </c>
+      <c r="P10" t="s">
+        <v>1013</v>
+      </c>
     </row>
-    <row r="11" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B11" s="155"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
@@ -5855,8 +5994,11 @@
       <c r="O11" s="121" t="s">
         <v>779</v>
       </c>
+      <c r="P11" t="s">
+        <v>1372</v>
+      </c>
     </row>
-    <row r="12" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B12" s="155"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
@@ -5895,8 +6037,11 @@
       <c r="O12" s="121" t="s">
         <v>1275</v>
       </c>
+      <c r="P12" t="s">
+        <v>1373</v>
+      </c>
     </row>
-    <row r="13" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B13" s="155"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
@@ -5935,8 +6080,11 @@
       <c r="O13" s="20" t="s">
         <v>1276</v>
       </c>
+      <c r="P13" t="s">
+        <v>1374</v>
+      </c>
     </row>
-    <row r="14" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B14" s="155"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
@@ -5975,8 +6123,11 @@
       <c r="O14" s="20" t="s">
         <v>1276</v>
       </c>
+      <c r="P14" t="s">
+        <v>1375</v>
+      </c>
     </row>
-    <row r="15" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B15" s="155"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
@@ -6015,8 +6166,11 @@
       <c r="O15" s="20" t="s">
         <v>565</v>
       </c>
+      <c r="P15" t="s">
+        <v>1377</v>
+      </c>
     </row>
-    <row r="16" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B16" s="155"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
@@ -6055,8 +6209,11 @@
       <c r="O16" s="20" t="s">
         <v>1277</v>
       </c>
+      <c r="P16" s="105" t="s">
+        <v>1376</v>
+      </c>
     </row>
-    <row r="17" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B17" s="155"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
@@ -6095,8 +6252,11 @@
       <c r="O17" s="20" t="s">
         <v>188</v>
       </c>
+      <c r="P17" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B18" s="155"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
@@ -6135,8 +6295,11 @@
       <c r="O18" s="20" t="s">
         <v>568</v>
       </c>
+      <c r="P18" t="s">
+        <v>1378</v>
+      </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="155"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
@@ -6175,8 +6338,11 @@
       <c r="O19" s="20" t="s">
         <v>1278</v>
       </c>
+      <c r="P19" t="s">
+        <v>1379</v>
+      </c>
     </row>
-    <row r="20" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B20" s="155"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
@@ -6215,8 +6381,11 @@
       <c r="O20" s="20" t="s">
         <v>1279</v>
       </c>
+      <c r="P20" t="s">
+        <v>1279</v>
+      </c>
     </row>
-    <row r="21" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B21" s="156" t="s">
         <v>0</v>
       </c>
@@ -6257,8 +6426,11 @@
       <c r="O21" s="20" t="s">
         <v>1280</v>
       </c>
+      <c r="P21" t="s">
+        <v>1380</v>
+      </c>
     </row>
-    <row r="22" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B22" s="156"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
@@ -6299,8 +6471,11 @@
       <c r="O22" s="20" t="s">
         <v>1281</v>
       </c>
+      <c r="P22" t="s">
+        <v>1381</v>
+      </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B23" s="156"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
@@ -6339,8 +6514,11 @@
       <c r="O23" s="118" t="s">
         <v>1272</v>
       </c>
+      <c r="P23" t="s">
+        <v>1382</v>
+      </c>
     </row>
-    <row r="24" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B24" s="156"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
@@ -6379,8 +6557,11 @@
       <c r="O24" s="140" t="s">
         <v>11</v>
       </c>
+      <c r="P24" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" spans="2:15" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="157" t="s">
         <v>8</v>
       </c>
@@ -6421,8 +6602,11 @@
       <c r="O25" s="19" t="s">
         <v>860</v>
       </c>
+      <c r="P25" t="s">
+        <v>860</v>
+      </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B26" s="157"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
@@ -6461,8 +6645,11 @@
       <c r="O26" s="20" t="s">
         <v>857</v>
       </c>
+      <c r="P26" t="s">
+        <v>857</v>
+      </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B27" s="157"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
@@ -6501,8 +6688,11 @@
       <c r="O27" s="118" t="s">
         <v>1271</v>
       </c>
+      <c r="P27" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B28" s="157"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
@@ -6541,8 +6731,11 @@
       <c r="O28" s="20" t="s">
         <v>1270</v>
       </c>
+      <c r="P28" s="174" t="s">
+        <v>1383</v>
+      </c>
     </row>
-    <row r="29" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B29" s="157"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
@@ -6581,8 +6774,11 @@
       <c r="O29" s="20" t="s">
         <v>1270</v>
       </c>
+      <c r="P29" s="174" t="s">
+        <v>1383</v>
+      </c>
     </row>
-    <row r="30" spans="2:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B30" s="157"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
@@ -6621,8 +6817,11 @@
       <c r="O30" s="20" t="s">
         <v>1270</v>
       </c>
+      <c r="P30" s="174" t="s">
+        <v>1383</v>
+      </c>
     </row>
-    <row r="31" spans="2:15" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:16" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="158" t="s">
         <v>9</v>
       </c>
@@ -6665,8 +6864,11 @@
       <c r="O31" s="142">
         <v>43779</v>
       </c>
+      <c r="P31" s="142">
+        <v>44404</v>
+      </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B32" s="161"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
@@ -6705,6 +6907,9 @@
         <v>30</v>
       </c>
       <c r="O32" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="P32" t="s">
         <v>30</v>
       </c>
     </row>
@@ -31553,7 +31758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
Added parser for Eurostat CE datasets.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8058" uniqueCount="1504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8130" uniqueCount="1543">
   <si>
     <t>Description</t>
   </si>
@@ -4327,9 +4327,6 @@
     <t>upload complete</t>
   </si>
   <si>
-    <t>tbd.</t>
-  </si>
-  <si>
     <t>2_IUS_ResidentlBldngs_RECCv2.4</t>
   </si>
   <si>
@@ -4535,6 +4532,126 @@
   </si>
   <si>
     <t>RECC_SysDef_Model_v2_5.png</t>
+  </si>
+  <si>
+    <t>Our World in Data</t>
+  </si>
+  <si>
+    <t>Our World in Data (OWID) is a scientific online publication that focuses on large global problems such as poverty, disease, hunger, climate change, war, existential risks, and inequality.</t>
+  </si>
+  <si>
+    <t>OWID</t>
+  </si>
+  <si>
+    <t>https://ourworldindata.org/</t>
+  </si>
+  <si>
+    <t>OWID = Our World in Data</t>
+  </si>
+  <si>
+    <t>energy; economics; poverty; disease; hunger; climate change; war; existential risks; inequality;</t>
+  </si>
+  <si>
+    <t>OWID_Energy</t>
+  </si>
+  <si>
+    <t>EUROSTAT_CE_Indicators</t>
+  </si>
+  <si>
+    <t>EUROSTAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ec.europa.eu/eurostat/web/main/data/database </t>
+  </si>
+  <si>
+    <t>Eurostat ('European Statistical Office'; DG ESTAT) is the main provider of statistical information to the institutions of the European Union (EU).</t>
+  </si>
+  <si>
+    <t>EU; statistics;</t>
+  </si>
+  <si>
+    <t>Eurostat = 'European Statistical Office'</t>
+  </si>
+  <si>
+    <t>one aggregate process/supply chain</t>
+  </si>
+  <si>
+    <t>225 countries</t>
+  </si>
+  <si>
+    <t>2000-2022</t>
+  </si>
+  <si>
+    <t>flows, stocks, shares, env. indicators</t>
+  </si>
+  <si>
+    <t>energy, mass, capacity, shares</t>
+  </si>
+  <si>
+    <t>energy flows, capacity stocks, market shares, env. indicators</t>
+  </si>
+  <si>
+    <t>Energy system</t>
+  </si>
+  <si>
+    <t>Electricity, primary energy</t>
+  </si>
+  <si>
+    <t>different resolution levels, from aggregate to specific technology</t>
+  </si>
+  <si>
+    <t>OWID energy statistics</t>
+  </si>
+  <si>
+    <t>energy; electricity; renewables; capacity;</t>
+  </si>
+  <si>
+    <t>Hannah Ritchie, Max Roser and Pablo Rosado</t>
+  </si>
+  <si>
+    <t>Hannah Ritchie, Max Roser and Pablo Rosado (2022) - "Energy". Published online at OurWorldInData.org. Retrieved from: 'https://ourworldindata.org/energy' [Online Resource]</t>
+  </si>
+  <si>
+    <t>https://ourworldindata.org/energy</t>
+  </si>
+  <si>
+    <t>all EU member states, EFTA, UK, and membership candidates</t>
+  </si>
+  <si>
+    <t>EU, Europe</t>
+  </si>
+  <si>
+    <t>per capita flows, trade flows, recycling rates and shares</t>
+  </si>
+  <si>
+    <t>flows, shares, general ratios</t>
+  </si>
+  <si>
+    <t>aggregate economy, municipal sources of waste, households</t>
+  </si>
+  <si>
+    <t>waste, total, packaging, plastic packaging</t>
+  </si>
+  <si>
+    <t>waste materials</t>
+  </si>
+  <si>
+    <t>EUROSTAT key circular economy indicators (selected)</t>
+  </si>
+  <si>
+    <t>waste; circular economy; EUROSTAT; packaging waste; municipal waste; plastic waste;</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/web/circular-economy/database</t>
+  </si>
+  <si>
+    <t>Eurostat Circular Economy Database</t>
+  </si>
+  <si>
+    <t>© European Union</t>
+  </si>
+  <si>
+    <t>entire industry, waste management</t>
   </si>
 </sst>
 </file>
@@ -4657,7 +4774,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4715,12 +4832,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4913,7 +5024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -5171,8 +5282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5184,6 +5294,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5540,7 +5656,7 @@
   <dimension ref="B2:I32"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5549,6 +5665,7 @@
     <col min="4" max="4" width="33" style="51" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="13.15" x14ac:dyDescent="0.4">
@@ -5575,11 +5692,15 @@
       <c r="G3" s="39" t="s">
         <v>1365</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="H3" s="161" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I3" s="161" t="s">
+        <v>1511</v>
+      </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="165" t="s">
+      <c r="B4" s="170" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -5597,9 +5718,15 @@
       <c r="G4" s="57">
         <v>3</v>
       </c>
+      <c r="H4" s="57">
+        <v>4</v>
+      </c>
+      <c r="I4" s="57">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="165"/>
+      <c r="B5" s="170"/>
       <c r="C5" s="26" t="s">
         <v>422</v>
       </c>
@@ -5615,9 +5742,15 @@
       <c r="G5" s="119" t="s">
         <v>1365</v>
       </c>
+      <c r="H5" s="119" t="s">
+        <v>1505</v>
+      </c>
+      <c r="I5" s="119" t="s">
+        <v>1511</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="166" t="s">
+      <c r="B6" s="171" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -5627,9 +5760,11 @@
       <c r="E6" s="52"/>
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="166"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="26" t="s">
         <v>424</v>
       </c>
@@ -5637,9 +5772,11 @@
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="166"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="26" t="s">
         <v>425</v>
       </c>
@@ -5647,9 +5784,11 @@
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
       <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="166"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="28" t="s">
         <v>426</v>
       </c>
@@ -5657,9 +5796,11 @@
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="166"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="27" t="s">
         <v>427</v>
       </c>
@@ -5667,9 +5808,11 @@
       <c r="E10" s="52"/>
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="166"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="27" t="s">
         <v>428</v>
       </c>
@@ -5677,9 +5820,11 @@
       <c r="E11" s="52"/>
       <c r="F11" s="52"/>
       <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="166"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="27" t="s">
         <v>429</v>
       </c>
@@ -5687,9 +5832,11 @@
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
       <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="166"/>
+      <c r="B13" s="171"/>
       <c r="C13" s="27" t="s">
         <v>430</v>
       </c>
@@ -5697,9 +5844,11 @@
       <c r="E13" s="52"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="166"/>
+      <c r="B14" s="171"/>
       <c r="C14" s="27" t="s">
         <v>431</v>
       </c>
@@ -5707,9 +5856,11 @@
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="166"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="27" t="s">
         <v>432</v>
       </c>
@@ -5717,9 +5868,11 @@
       <c r="E15" s="52"/>
       <c r="F15" s="52"/>
       <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="166"/>
+      <c r="B16" s="171"/>
       <c r="C16" s="27" t="s">
         <v>433</v>
       </c>
@@ -5727,9 +5880,11 @@
       <c r="E16" s="52"/>
       <c r="F16" s="52"/>
       <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="166"/>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="171"/>
       <c r="C17" s="27" t="s">
         <v>434</v>
       </c>
@@ -5737,9 +5892,11 @@
       <c r="E17" s="52"/>
       <c r="F17" s="52"/>
       <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="166"/>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="171"/>
       <c r="C18" s="27" t="s">
         <v>435</v>
       </c>
@@ -5747,9 +5904,11 @@
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
       <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="167" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="172" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -5763,9 +5922,15 @@
       <c r="G19" s="119" t="s">
         <v>1369</v>
       </c>
+      <c r="H19" s="119" t="s">
+        <v>1504</v>
+      </c>
+      <c r="I19" s="119" t="s">
+        <v>1513</v>
+      </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="167"/>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="172"/>
       <c r="C20" s="27" t="s">
         <v>437</v>
       </c>
@@ -5781,9 +5946,15 @@
       <c r="G20" s="119" t="s">
         <v>1366</v>
       </c>
+      <c r="H20" s="119" t="s">
+        <v>1508</v>
+      </c>
+      <c r="I20" s="119" t="s">
+        <v>1514</v>
+      </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="167"/>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="172"/>
       <c r="C21" s="27" t="s">
         <v>438</v>
       </c>
@@ -5795,9 +5966,15 @@
       <c r="G21" s="119" t="s">
         <v>1368</v>
       </c>
+      <c r="H21" s="119" t="s">
+        <v>1507</v>
+      </c>
+      <c r="I21" s="119" t="s">
+        <v>1515</v>
+      </c>
     </row>
-    <row r="22" spans="2:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="168" t="s">
+    <row r="22" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="173" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -5813,9 +5990,15 @@
       <c r="G22" s="52" t="s">
         <v>860</v>
       </c>
+      <c r="H22" s="119" t="s">
+        <v>861</v>
+      </c>
+      <c r="I22" s="119" t="s">
+        <v>861</v>
+      </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="168"/>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B23" s="173"/>
       <c r="C23" s="26" t="s">
         <v>440</v>
       </c>
@@ -5823,9 +6006,11 @@
       <c r="E23" s="52"/>
       <c r="F23" s="52"/>
       <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="168"/>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24" s="173"/>
       <c r="C24" s="25" t="s">
         <v>441</v>
       </c>
@@ -5833,9 +6018,11 @@
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
       <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="168"/>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25" s="173"/>
       <c r="C25" s="25" t="s">
         <v>443</v>
       </c>
@@ -5847,9 +6034,15 @@
       <c r="G25" s="90" t="s">
         <v>1367</v>
       </c>
+      <c r="H25" s="90" t="s">
+        <v>1506</v>
+      </c>
+      <c r="I25" s="90" t="s">
+        <v>1512</v>
+      </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="168"/>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B26" s="173"/>
       <c r="C26" s="25" t="s">
         <v>444</v>
       </c>
@@ -5859,9 +6052,11 @@
       </c>
       <c r="F26" s="52"/>
       <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="168"/>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B27" s="173"/>
       <c r="C27" s="25" t="s">
         <v>445</v>
       </c>
@@ -5869,9 +6064,11 @@
       <c r="E27" s="52"/>
       <c r="F27" s="52"/>
       <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
     </row>
-    <row r="28" spans="2:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="169" t="s">
+    <row r="28" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="174" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -5889,9 +6086,15 @@
       <c r="G28" s="123">
         <v>44404</v>
       </c>
+      <c r="H28" s="123">
+        <v>45144</v>
+      </c>
+      <c r="I28" s="123">
+        <v>45144</v>
+      </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="169"/>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="174"/>
       <c r="C29" s="25" t="s">
         <v>447</v>
       </c>
@@ -5907,9 +6110,15 @@
       <c r="G29" s="124" t="s">
         <v>30</v>
       </c>
+      <c r="H29" s="124" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="124" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="162" t="s">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B30" s="167" t="s">
         <v>185</v>
       </c>
       <c r="C30" s="107" t="s">
@@ -5919,9 +6128,11 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="163"/>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B31" s="168"/>
       <c r="C31" s="108" t="s">
         <v>449</v>
       </c>
@@ -5929,9 +6140,11 @@
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="164"/>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B32" s="169"/>
       <c r="C32" s="109" t="s">
         <v>450</v>
       </c>
@@ -5939,6 +6152,8 @@
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5955,13 +6170,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R39"/>
+  <dimension ref="B2:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q23" sqref="Q23"/>
+      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5979,16 +6194,18 @@
     <col min="16" max="16" width="38.6640625" customWidth="1"/>
     <col min="17" max="17" width="37.19921875" customWidth="1"/>
     <col min="18" max="18" width="39.265625" customWidth="1"/>
+    <col min="19" max="19" width="37.3984375" customWidth="1"/>
+    <col min="20" max="20" width="34.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:20" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:20" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="32"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -6038,9 +6255,15 @@
       <c r="R3" s="82" t="s">
         <v>1384</v>
       </c>
+      <c r="S3" s="163" t="s">
+        <v>1509</v>
+      </c>
+      <c r="T3" s="163" t="s">
+        <v>1510</v>
+      </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B4" s="170" t="s">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B4" s="175" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -6091,9 +6314,15 @@
       <c r="R4" s="141">
         <v>14</v>
       </c>
+      <c r="S4" s="141">
+        <v>15</v>
+      </c>
+      <c r="T4" s="141">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="171"/>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B5" s="176"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
       </c>
@@ -6142,8 +6371,14 @@
       <c r="R5" s="29" t="s">
         <v>1384</v>
       </c>
+      <c r="S5" s="164" t="s">
+        <v>1509</v>
+      </c>
+      <c r="T5" s="164" t="s">
+        <v>1510</v>
+      </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="33"/>
       <c r="C6" s="54" t="s">
         <v>453</v>
@@ -6191,8 +6426,14 @@
       <c r="R6" s="29" t="s">
         <v>1150</v>
       </c>
+      <c r="S6" s="164" t="s">
+        <v>1150</v>
+      </c>
+      <c r="T6" s="164" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
@@ -6242,9 +6483,15 @@
       <c r="R7" s="29" t="s">
         <v>1365</v>
       </c>
+      <c r="S7" s="40" t="s">
+        <v>1505</v>
+      </c>
+      <c r="T7" s="40" t="s">
+        <v>1511</v>
+      </c>
     </row>
-    <row r="8" spans="2:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="166" t="s">
+    <row r="8" spans="2:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="171" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="54" t="s">
@@ -6293,9 +6540,15 @@
       <c r="R8" s="29" t="s">
         <v>1370</v>
       </c>
+      <c r="S8" s="40" t="s">
+        <v>1519</v>
+      </c>
+      <c r="T8" s="164" t="s">
+        <v>1533</v>
+      </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="166"/>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B9" s="171"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
       </c>
@@ -6342,9 +6595,15 @@
       <c r="R9" s="29" t="s">
         <v>1370</v>
       </c>
+      <c r="S9" s="40" t="s">
+        <v>1521</v>
+      </c>
+      <c r="T9" s="164" t="s">
+        <v>1532</v>
+      </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B10" s="166"/>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B10" s="171"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
       </c>
@@ -6391,9 +6650,15 @@
       <c r="R10" s="29" t="s">
         <v>1013</v>
       </c>
+      <c r="S10" s="40" t="s">
+        <v>1520</v>
+      </c>
+      <c r="T10" s="164" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="11" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="166"/>
+    <row r="11" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="171"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
       </c>
@@ -6440,9 +6705,15 @@
       <c r="R11" s="29" t="s">
         <v>1371</v>
       </c>
+      <c r="S11" s="40" t="s">
+        <v>1522</v>
+      </c>
+      <c r="T11" s="164" t="s">
+        <v>1542</v>
+      </c>
     </row>
-    <row r="12" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="166"/>
+    <row r="12" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="171"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -6489,9 +6760,15 @@
       <c r="R12" s="29" t="s">
         <v>1372</v>
       </c>
+      <c r="S12" s="164" t="s">
+        <v>1516</v>
+      </c>
+      <c r="T12" s="164" t="s">
+        <v>1534</v>
+      </c>
     </row>
-    <row r="13" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="166"/>
+    <row r="13" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="171"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -6538,9 +6815,15 @@
       <c r="R13" s="29" t="s">
         <v>1383</v>
       </c>
+      <c r="S13" s="40" t="s">
+        <v>1523</v>
+      </c>
+      <c r="T13" s="164" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="14" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="166"/>
+    <row r="14" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="171"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -6587,9 +6870,15 @@
       <c r="R14" s="29" t="s">
         <v>1374</v>
       </c>
+      <c r="S14" s="40" t="s">
+        <v>1524</v>
+      </c>
+      <c r="T14" s="164" t="s">
+        <v>1535</v>
+      </c>
     </row>
-    <row r="15" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="166"/>
+    <row r="15" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="171"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -6636,9 +6925,15 @@
       <c r="R15" s="29" t="s">
         <v>1376</v>
       </c>
+      <c r="S15" s="164" t="s">
+        <v>11</v>
+      </c>
+      <c r="T15" s="164" t="s">
+        <v>1536</v>
+      </c>
     </row>
-    <row r="16" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="166"/>
+    <row r="16" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="171"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -6685,9 +6980,15 @@
       <c r="R16" s="29" t="s">
         <v>1375</v>
       </c>
+      <c r="S16" s="164" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="164" t="s">
+        <v>1535</v>
+      </c>
     </row>
-    <row r="17" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="166"/>
+    <row r="17" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="171"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -6734,9 +7035,15 @@
       <c r="R17" s="29" t="s">
         <v>19</v>
       </c>
+      <c r="S17" s="164" t="s">
+        <v>819</v>
+      </c>
+      <c r="T17" s="164" t="s">
+        <v>1531</v>
+      </c>
     </row>
-    <row r="18" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="166"/>
+    <row r="18" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="171"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -6783,9 +7090,15 @@
       <c r="R18" s="29" t="s">
         <v>1385</v>
       </c>
+      <c r="S18" s="164" t="s">
+        <v>1517</v>
+      </c>
+      <c r="T18" s="164" t="s">
+        <v>1530</v>
+      </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B19" s="166"/>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B19" s="171"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -6832,9 +7145,15 @@
       <c r="R19" s="29" t="s">
         <v>1378</v>
       </c>
+      <c r="S19" s="164" t="s">
+        <v>1518</v>
+      </c>
+      <c r="T19" s="164" t="s">
+        <v>1518</v>
+      </c>
     </row>
-    <row r="20" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="166"/>
+    <row r="20" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="171"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -6881,9 +7200,15 @@
       <c r="R20" s="29" t="s">
         <v>1278</v>
       </c>
+      <c r="S20" s="29" t="s">
+        <v>1278</v>
+      </c>
+      <c r="T20" s="164" t="s">
+        <v>1278</v>
+      </c>
     </row>
-    <row r="21" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="167" t="s">
+    <row r="21" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="172" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -6932,9 +7257,15 @@
       <c r="R21" s="29" t="s">
         <v>1379</v>
       </c>
+      <c r="S21" s="40" t="s">
+        <v>1525</v>
+      </c>
+      <c r="T21" s="164" t="s">
+        <v>1537</v>
+      </c>
     </row>
-    <row r="22" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="167"/>
+    <row r="22" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="172"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -6983,9 +7314,15 @@
       <c r="R22" s="29" t="s">
         <v>1380</v>
       </c>
+      <c r="S22" s="40" t="s">
+        <v>1526</v>
+      </c>
+      <c r="T22" s="164" t="s">
+        <v>1538</v>
+      </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B23" s="167"/>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B23" s="172"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
       </c>
@@ -7024,17 +7361,23 @@
         <v>1271</v>
       </c>
       <c r="P23" s="146" t="s">
+        <v>1501</v>
+      </c>
+      <c r="Q23" s="162" t="s">
         <v>1502</v>
-      </c>
-      <c r="Q23" s="24" t="s">
-        <v>1503</v>
       </c>
       <c r="R23" s="154" t="s">
         <v>1388</v>
       </c>
+      <c r="S23" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="T23" s="164" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="24" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B24" s="167"/>
+    <row r="24" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="172"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
       </c>
@@ -7081,9 +7424,15 @@
       <c r="R24" s="29" t="s">
         <v>11</v>
       </c>
+      <c r="S24" s="164" t="s">
+        <v>11</v>
+      </c>
+      <c r="T24" s="164" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" spans="2:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="168" t="s">
+    <row r="25" spans="2:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="173" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -7132,9 +7481,15 @@
       <c r="R25" s="29" t="s">
         <v>860</v>
       </c>
+      <c r="S25" s="40" t="s">
+        <v>861</v>
+      </c>
+      <c r="T25" s="40" t="s">
+        <v>861</v>
+      </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B26" s="168"/>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B26" s="173"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
       </c>
@@ -7181,9 +7536,15 @@
       <c r="R26" s="29" t="s">
         <v>857</v>
       </c>
+      <c r="S26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="T26" s="164" t="s">
+        <v>1541</v>
+      </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B27" s="168"/>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B27" s="173"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
       </c>
@@ -7230,9 +7591,15 @@
       <c r="R27" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="S27" s="40" t="s">
+        <v>1527</v>
+      </c>
+      <c r="T27" s="164" t="s">
+        <v>1511</v>
+      </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B28" s="168"/>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B28" s="173"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
       </c>
@@ -7279,9 +7646,15 @@
       <c r="R28" s="154" t="s">
         <v>1388</v>
       </c>
+      <c r="S28" s="90" t="s">
+        <v>1529</v>
+      </c>
+      <c r="T28" s="90" t="s">
+        <v>1539</v>
+      </c>
     </row>
-    <row r="29" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="168"/>
+    <row r="29" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="173"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
       </c>
@@ -7328,9 +7701,15 @@
       <c r="R29" s="154" t="s">
         <v>1388</v>
       </c>
+      <c r="S29" s="90" t="s">
+        <v>1529</v>
+      </c>
+      <c r="T29" s="62" t="s">
+        <v>1539</v>
+      </c>
     </row>
-    <row r="30" spans="2:18" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="168"/>
+    <row r="30" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="173"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
       </c>
@@ -7377,9 +7756,15 @@
       <c r="R30" s="154" t="s">
         <v>1388</v>
       </c>
+      <c r="S30" s="62" t="s">
+        <v>1528</v>
+      </c>
+      <c r="T30" s="62" t="s">
+        <v>1540</v>
+      </c>
     </row>
-    <row r="31" spans="2:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="169" t="s">
+    <row r="31" spans="2:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="174" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -7430,9 +7815,15 @@
       <c r="R31" s="142">
         <v>44871</v>
       </c>
+      <c r="S31" s="165">
+        <v>45144</v>
+      </c>
+      <c r="T31" s="165">
+        <v>45164</v>
+      </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B32" s="172"/>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B32" s="177"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
       </c>
@@ -7481,9 +7872,15 @@
       <c r="R32" s="29" t="s">
         <v>30</v>
       </c>
+      <c r="S32" s="164" t="s">
+        <v>30</v>
+      </c>
+      <c r="T32" s="164" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B33" s="162" t="s">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B33" s="167" t="s">
         <v>185</v>
       </c>
       <c r="C33" s="83" t="s">
@@ -7504,9 +7901,11 @@
       <c r="P33" s="146"/>
       <c r="Q33" s="24"/>
       <c r="R33" s="29"/>
+      <c r="S33" s="164"/>
+      <c r="T33" s="164"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B34" s="163"/>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B34" s="168"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
       </c>
@@ -7525,9 +7924,11 @@
       <c r="P34" s="146"/>
       <c r="Q34" s="24"/>
       <c r="R34" s="29"/>
+      <c r="S34" s="164"/>
+      <c r="T34" s="164"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B35" s="164"/>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B35" s="169"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
       </c>
@@ -7546,8 +7947,10 @@
       <c r="P35" s="151"/>
       <c r="Q35" s="152"/>
       <c r="R35" s="30"/>
+      <c r="S35" s="166"/>
+      <c r="T35" s="166"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.35">
       <c r="I39" s="12"/>
     </row>
   </sheetData>
@@ -7571,10 +7974,10 @@
   <dimension ref="A1:DA74"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="BK6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="BM6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BR7" sqref="BR7"/>
+      <selection pane="bottomRight" activeCell="CB5" sqref="CB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7834,32 +8237,32 @@
       <c r="BQ1" s="12" t="s">
         <v>693</v>
       </c>
-      <c r="BR1" s="156" t="s">
+      <c r="BR1" s="155" t="s">
         <v>1433</v>
       </c>
-      <c r="BS1" s="156" t="s">
+      <c r="BS1" s="155" t="s">
         <v>1433</v>
       </c>
-      <c r="BT1" s="156" t="s">
+      <c r="BT1" s="155" t="s">
         <v>1433</v>
       </c>
-      <c r="BU1" s="156" t="s">
+      <c r="BU1" s="155" t="s">
         <v>1433</v>
       </c>
-      <c r="BV1" s="156" t="s">
+      <c r="BV1" s="155" t="s">
         <v>1433</v>
       </c>
-      <c r="BW1" s="156" t="s">
+      <c r="BW1" s="155" t="s">
         <v>1433</v>
       </c>
       <c r="BX1" s="155" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="BY1" s="155" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="BZ1" s="155" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="2" spans="1:78" ht="13.9" x14ac:dyDescent="0.4">
@@ -8148,7 +8551,7 @@
       <c r="A4" s="41">
         <v>1</v>
       </c>
-      <c r="B4" s="175" t="s">
+      <c r="B4" s="180" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -8384,7 +8787,7 @@
       <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="176"/>
+      <c r="B5" s="181"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -8596,22 +8999,22 @@
         <v>1420</v>
       </c>
       <c r="BU5" s="115" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="BV5" s="115" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="BW5" s="115" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="BX5" s="115" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="BY5" s="115" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="BZ5" s="115" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="6" spans="1:78" ht="13.9" x14ac:dyDescent="0.4">
@@ -8828,29 +9231,29 @@
         <v>1421</v>
       </c>
       <c r="BU6" s="115" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="BV6" s="115" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="BW6" s="105" t="s">
         <v>1405</v>
       </c>
       <c r="BX6" s="115" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="BY6" s="115" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="BZ6" s="115" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="7" spans="1:78" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A7" s="92">
         <v>4</v>
       </c>
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="182" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -9084,7 +9487,7 @@
       <c r="A8" s="92">
         <v>5</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="182"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -9318,7 +9721,7 @@
       <c r="A9" s="92">
         <v>6</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -9552,7 +9955,7 @@
       <c r="A10" s="92">
         <v>7</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -9764,7 +10167,7 @@
         <v>4</v>
       </c>
       <c r="BU10" s="115" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="BV10" s="115" t="s">
         <v>412</v>
@@ -9786,7 +10189,7 @@
       <c r="A11" s="92">
         <v>8</v>
       </c>
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="183" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -10001,26 +10404,26 @@
         <v>782</v>
       </c>
       <c r="BV11" s="115" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="BW11" s="115" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="BX11" s="115" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="BY11" s="115" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="BZ11" s="115" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="12" spans="1:78" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="92">
         <v>9</v>
       </c>
-      <c r="B12" s="179"/>
+      <c r="B12" s="184"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -10230,29 +10633,29 @@
         <v>11</v>
       </c>
       <c r="BU12" s="115" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="BV12" s="115" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="BW12" s="115" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="BX12" s="115" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="BY12" s="115" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="BZ12" s="115" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="13" spans="1:78" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="92">
         <v>10</v>
       </c>
-      <c r="B13" s="179"/>
+      <c r="B13" s="184"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -10474,7 +10877,7 @@
         <v>11</v>
       </c>
       <c r="BY13" s="115" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="BZ13" s="115" t="s">
         <v>11</v>
@@ -10484,7 +10887,7 @@
       <c r="A14" s="92">
         <v>11</v>
       </c>
-      <c r="B14" s="179"/>
+      <c r="B14" s="184"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -10697,7 +11100,7 @@
         <v>11</v>
       </c>
       <c r="BV14" s="115" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="BW14" s="115" t="s">
         <v>11</v>
@@ -10706,7 +11109,7 @@
         <v>11</v>
       </c>
       <c r="BY14" s="115" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="BZ14" s="115" t="s">
         <v>11</v>
@@ -10716,7 +11119,7 @@
       <c r="A15" s="92">
         <v>12</v>
       </c>
-      <c r="B15" s="179"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -10935,20 +11338,20 @@
         <v>11</v>
       </c>
       <c r="BX15" s="115" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="BY15" s="115" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="BZ15" s="115" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="16" spans="1:78" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="92">
         <v>13</v>
       </c>
-      <c r="B16" s="179"/>
+      <c r="B16" s="184"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -11167,20 +11570,20 @@
         <v>11</v>
       </c>
       <c r="BX16" s="115" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="BY16" s="115" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="BZ16" s="115" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="17" spans="1:78" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="92">
         <v>14</v>
       </c>
-      <c r="B17" s="179"/>
+      <c r="B17" s="184"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -11412,7 +11815,7 @@
       <c r="A18" s="92">
         <v>15</v>
       </c>
-      <c r="B18" s="179"/>
+      <c r="B18" s="184"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -11625,10 +12028,10 @@
         <v>129</v>
       </c>
       <c r="BV18" s="115" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="BW18" s="115" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="BX18" s="115" t="s">
         <v>129</v>
@@ -11644,7 +12047,7 @@
       <c r="A19" s="92">
         <v>16</v>
       </c>
-      <c r="B19" s="179"/>
+      <c r="B19" s="184"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -11860,7 +12263,7 @@
         <v>130</v>
       </c>
       <c r="BW19" s="115" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="BX19" s="115" t="s">
         <v>1378</v>
@@ -11876,7 +12279,7 @@
       <c r="A20" s="92">
         <v>17</v>
       </c>
-      <c r="B20" s="179"/>
+      <c r="B20" s="184"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -12108,7 +12511,7 @@
       <c r="A21" s="92">
         <v>18</v>
       </c>
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="185" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -12314,29 +12717,29 @@
         <v>1425</v>
       </c>
       <c r="BU21" s="115" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="BV21" s="115" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="BW21" s="115" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="BX21" s="115" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="BY21" s="115" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="BZ21" s="115" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="22" spans="1:78" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="92">
         <v>19</v>
       </c>
-      <c r="B22" s="180"/>
+      <c r="B22" s="185"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -12548,29 +12951,29 @@
         <v>1426</v>
       </c>
       <c r="BU22" s="115" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="BV22" s="115" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="BW22" s="115" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="BX22" s="115" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="BY22" s="115" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="BZ22" s="115" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="23" spans="1:78" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A23" s="92">
         <v>20</v>
       </c>
-      <c r="B23" s="180"/>
+      <c r="B23" s="185"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -12804,7 +13207,7 @@
       <c r="A24" s="92">
         <v>21</v>
       </c>
-      <c r="B24" s="180"/>
+      <c r="B24" s="185"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -13015,7 +13418,7 @@
       <c r="BT24" s="105">
         <v>1242</v>
       </c>
-      <c r="BU24" s="157">
+      <c r="BU24" s="156">
         <v>0</v>
       </c>
       <c r="BV24" s="69">
@@ -13024,13 +13427,13 @@
       <c r="BW24" s="69">
         <v>0</v>
       </c>
-      <c r="BX24" s="157">
+      <c r="BX24" s="156">
         <v>0</v>
       </c>
-      <c r="BY24" s="157">
+      <c r="BY24" s="156">
         <v>0</v>
       </c>
-      <c r="BZ24" s="157">
+      <c r="BZ24" s="156">
         <v>0</v>
       </c>
     </row>
@@ -13038,7 +13441,7 @@
       <c r="A25" s="92">
         <v>22</v>
       </c>
-      <c r="B25" s="180"/>
+      <c r="B25" s="185"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -13251,13 +13654,13 @@
         <v>11</v>
       </c>
       <c r="BV25" s="115" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="BW25" s="115" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="BX25" s="115" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="BY25" s="115" t="s">
         <v>11</v>
@@ -13270,7 +13673,7 @@
       <c r="A26" s="92">
         <v>23</v>
       </c>
-      <c r="B26" s="181" t="s">
+      <c r="B26" s="186" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="64" t="s">
@@ -13486,10 +13889,10 @@
       <c r="BU26" s="115" t="s">
         <v>698</v>
       </c>
-      <c r="BV26" s="161" t="s">
+      <c r="BV26" s="160" t="s">
         <v>853</v>
       </c>
-      <c r="BW26" s="161" t="s">
+      <c r="BW26" s="160" t="s">
         <v>702</v>
       </c>
       <c r="BX26" s="115" t="s">
@@ -13506,7 +13909,7 @@
       <c r="A27" s="92">
         <v>24</v>
       </c>
-      <c r="B27" s="181"/>
+      <c r="B27" s="186"/>
       <c r="C27" s="64" t="s">
         <v>464</v>
       </c>
@@ -13720,10 +14123,10 @@
       <c r="BU27" s="115">
         <v>77</v>
       </c>
-      <c r="BV27" s="161">
+      <c r="BV27" s="160">
         <v>12</v>
       </c>
-      <c r="BW27" s="161">
+      <c r="BW27" s="160">
         <v>3</v>
       </c>
       <c r="BX27" s="115">
@@ -13740,7 +14143,7 @@
       <c r="A28" s="92">
         <v>25</v>
       </c>
-      <c r="B28" s="181"/>
+      <c r="B28" s="186"/>
       <c r="C28" s="64" t="s">
         <v>465</v>
       </c>
@@ -13950,19 +14353,19 @@
         <v>698</v>
       </c>
       <c r="BU28" s="115" t="s">
-        <v>1441</v>
-      </c>
-      <c r="BV28" s="161" t="s">
-        <v>1441</v>
-      </c>
-      <c r="BW28" s="161" t="s">
-        <v>1468</v>
+        <v>1440</v>
+      </c>
+      <c r="BV28" s="160" t="s">
+        <v>1440</v>
+      </c>
+      <c r="BW28" s="160" t="s">
+        <v>1467</v>
       </c>
       <c r="BX28" s="115" t="s">
         <v>849</v>
       </c>
       <c r="BY28" s="115" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="BZ28" s="115" t="s">
         <v>849</v>
@@ -13972,7 +14375,7 @@
       <c r="A29" s="92">
         <v>26</v>
       </c>
-      <c r="B29" s="181"/>
+      <c r="B29" s="186"/>
       <c r="C29" s="64" t="s">
         <v>466</v>
       </c>
@@ -14184,10 +14587,10 @@
       <c r="BU29" s="115">
         <v>7</v>
       </c>
-      <c r="BV29" s="161">
+      <c r="BV29" s="160">
         <v>7</v>
       </c>
-      <c r="BW29" s="161">
+      <c r="BW29" s="160">
         <v>79</v>
       </c>
       <c r="BX29" s="115">
@@ -14204,7 +14607,7 @@
       <c r="A30" s="92">
         <v>27</v>
       </c>
-      <c r="B30" s="181"/>
+      <c r="B30" s="186"/>
       <c r="C30" s="64" t="s">
         <v>467</v>
       </c>
@@ -14416,17 +14819,17 @@
       <c r="BU30" s="115" t="s">
         <v>697</v>
       </c>
-      <c r="BV30" s="161" t="s">
+      <c r="BV30" s="160" t="s">
         <v>698</v>
       </c>
-      <c r="BW30" s="161" t="s">
+      <c r="BW30" s="160" t="s">
         <v>699</v>
       </c>
       <c r="BX30" s="115" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="BY30" s="115" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="BZ30" s="115" t="s">
         <v>696</v>
@@ -14436,7 +14839,7 @@
       <c r="A31" s="92">
         <v>28</v>
       </c>
-      <c r="B31" s="181"/>
+      <c r="B31" s="186"/>
       <c r="C31" s="64" t="s">
         <v>468</v>
       </c>
@@ -14648,10 +15051,10 @@
       <c r="BU31" s="115">
         <v>6</v>
       </c>
-      <c r="BV31" s="161">
+      <c r="BV31" s="160">
         <v>77</v>
       </c>
-      <c r="BW31" s="161">
+      <c r="BW31" s="160">
         <v>6</v>
       </c>
       <c r="BX31" s="115">
@@ -14668,7 +15071,7 @@
       <c r="A32" s="92">
         <v>29</v>
       </c>
-      <c r="B32" s="181"/>
+      <c r="B32" s="186"/>
       <c r="C32" s="64" t="s">
         <v>469</v>
       </c>
@@ -14880,10 +15283,10 @@
       <c r="BU32" s="115" t="s">
         <v>703</v>
       </c>
-      <c r="BV32" s="161" t="s">
+      <c r="BV32" s="160" t="s">
         <v>702</v>
       </c>
-      <c r="BW32" s="161" t="s">
+      <c r="BW32" s="160" t="s">
         <v>700</v>
       </c>
       <c r="BX32" s="115" t="s">
@@ -14893,14 +15296,14 @@
         <v>699</v>
       </c>
       <c r="BZ32" s="115" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="33" spans="1:78" s="68" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A33" s="92">
         <v>30</v>
       </c>
-      <c r="B33" s="181"/>
+      <c r="B33" s="186"/>
       <c r="C33" s="64" t="s">
         <v>470</v>
       </c>
@@ -15112,10 +15515,10 @@
       <c r="BU33" s="115">
         <v>8</v>
       </c>
-      <c r="BV33" s="161">
+      <c r="BV33" s="160">
         <v>3</v>
       </c>
-      <c r="BW33" s="161">
+      <c r="BW33" s="160">
         <v>6</v>
       </c>
       <c r="BX33" s="115">
@@ -15132,7 +15535,7 @@
       <c r="A34" s="92">
         <v>31</v>
       </c>
-      <c r="B34" s="181"/>
+      <c r="B34" s="186"/>
       <c r="C34" s="64" t="s">
         <v>471</v>
       </c>
@@ -15342,12 +15745,12 @@
         <v>11</v>
       </c>
       <c r="BU34" s="115" t="s">
-        <v>1442</v>
-      </c>
-      <c r="BV34" s="161" t="s">
+        <v>1441</v>
+      </c>
+      <c r="BV34" s="160" t="s">
         <v>703</v>
       </c>
-      <c r="BW34" s="161" t="s">
+      <c r="BW34" s="160" t="s">
         <v>698</v>
       </c>
       <c r="BX34" s="115" t="s">
@@ -15364,7 +15767,7 @@
       <c r="A35" s="92">
         <v>32</v>
       </c>
-      <c r="B35" s="181"/>
+      <c r="B35" s="186"/>
       <c r="C35" s="64" t="s">
         <v>472</v>
       </c>
@@ -15576,10 +15979,10 @@
       <c r="BU35" s="115">
         <v>78</v>
       </c>
-      <c r="BV35" s="161">
+      <c r="BV35" s="160">
         <v>8</v>
       </c>
-      <c r="BW35" s="161">
+      <c r="BW35" s="160">
         <v>2</v>
       </c>
       <c r="BX35" s="115">
@@ -15596,7 +15999,7 @@
       <c r="A36" s="92">
         <v>33</v>
       </c>
-      <c r="B36" s="181"/>
+      <c r="B36" s="186"/>
       <c r="C36" s="64" t="s">
         <v>473</v>
       </c>
@@ -15808,10 +16211,10 @@
       <c r="BU36" s="115" t="s">
         <v>702</v>
       </c>
-      <c r="BV36" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW36" s="161" t="s">
+      <c r="BV36" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW36" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX36" s="115" t="s">
@@ -15828,7 +16231,7 @@
       <c r="A37" s="92">
         <v>34</v>
       </c>
-      <c r="B37" s="181"/>
+      <c r="B37" s="186"/>
       <c r="C37" s="64" t="s">
         <v>474</v>
       </c>
@@ -16040,10 +16443,10 @@
       <c r="BU37" s="115">
         <v>3</v>
       </c>
-      <c r="BV37" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW37" s="161" t="s">
+      <c r="BV37" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW37" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX37" s="115">
@@ -16060,7 +16463,7 @@
       <c r="A38" s="92">
         <v>35</v>
       </c>
-      <c r="B38" s="181"/>
+      <c r="B38" s="186"/>
       <c r="C38" s="64" t="s">
         <v>475</v>
       </c>
@@ -16272,17 +16675,17 @@
       <c r="BU38" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV38" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW38" s="161" t="s">
+      <c r="BV38" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW38" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX38" s="115" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="BY38" s="115" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="BZ38" s="115" t="s">
         <v>703</v>
@@ -16292,7 +16695,7 @@
       <c r="A39" s="92">
         <v>36</v>
       </c>
-      <c r="B39" s="181"/>
+      <c r="B39" s="186"/>
       <c r="C39" s="64" t="s">
         <v>476</v>
       </c>
@@ -16504,10 +16907,10 @@
       <c r="BU39" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV39" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW39" s="161" t="s">
+      <c r="BV39" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW39" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX39" s="115">
@@ -16524,7 +16927,7 @@
       <c r="A40" s="92">
         <v>37</v>
       </c>
-      <c r="B40" s="181"/>
+      <c r="B40" s="186"/>
       <c r="C40" s="64" t="s">
         <v>477</v>
       </c>
@@ -16736,10 +17139,10 @@
       <c r="BU40" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV40" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW40" s="161" t="s">
+      <c r="BV40" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW40" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX40" s="115" t="s">
@@ -16749,14 +17152,14 @@
         <v>702</v>
       </c>
       <c r="BZ40" s="115" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="41" spans="1:78" s="68" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A41" s="92">
         <v>38</v>
       </c>
-      <c r="B41" s="181"/>
+      <c r="B41" s="186"/>
       <c r="C41" s="64" t="s">
         <v>478</v>
       </c>
@@ -16968,10 +17371,10 @@
       <c r="BU41" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV41" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW41" s="161" t="s">
+      <c r="BV41" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW41" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX41" s="115">
@@ -16988,7 +17391,7 @@
       <c r="A42" s="92">
         <v>39</v>
       </c>
-      <c r="B42" s="181"/>
+      <c r="B42" s="186"/>
       <c r="C42" s="64" t="s">
         <v>479</v>
       </c>
@@ -17200,10 +17603,10 @@
       <c r="BU42" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV42" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW42" s="161" t="s">
+      <c r="BV42" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW42" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX42" s="115" t="s">
@@ -17220,7 +17623,7 @@
       <c r="A43" s="92">
         <v>40</v>
       </c>
-      <c r="B43" s="181"/>
+      <c r="B43" s="186"/>
       <c r="C43" s="64" t="s">
         <v>480</v>
       </c>
@@ -17432,10 +17835,10 @@
       <c r="BU43" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV43" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW43" s="161" t="s">
+      <c r="BV43" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW43" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX43" s="115" t="s">
@@ -17452,7 +17855,7 @@
       <c r="A44" s="92">
         <v>41</v>
       </c>
-      <c r="B44" s="181"/>
+      <c r="B44" s="186"/>
       <c r="C44" s="64" t="s">
         <v>481</v>
       </c>
@@ -17664,10 +18067,10 @@
       <c r="BU44" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV44" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW44" s="161" t="s">
+      <c r="BV44" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW44" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX44" s="115" t="s">
@@ -17684,7 +18087,7 @@
       <c r="A45" s="92">
         <v>42</v>
       </c>
-      <c r="B45" s="181"/>
+      <c r="B45" s="186"/>
       <c r="C45" s="64" t="s">
         <v>482</v>
       </c>
@@ -17896,10 +18299,10 @@
       <c r="BU45" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV45" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW45" s="161" t="s">
+      <c r="BV45" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW45" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX45" s="115" t="s">
@@ -17916,7 +18319,7 @@
       <c r="A46" s="92">
         <v>43</v>
       </c>
-      <c r="B46" s="181"/>
+      <c r="B46" s="186"/>
       <c r="C46" s="64" t="s">
         <v>483</v>
       </c>
@@ -18128,10 +18531,10 @@
       <c r="BU46" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV46" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW46" s="161" t="s">
+      <c r="BV46" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW46" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX46" s="115" t="s">
@@ -18148,7 +18551,7 @@
       <c r="A47" s="92">
         <v>44</v>
       </c>
-      <c r="B47" s="181"/>
+      <c r="B47" s="186"/>
       <c r="C47" s="64" t="s">
         <v>484</v>
       </c>
@@ -18360,10 +18763,10 @@
       <c r="BU47" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV47" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW47" s="161" t="s">
+      <c r="BV47" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW47" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX47" s="115" t="s">
@@ -18380,7 +18783,7 @@
       <c r="A48" s="92">
         <v>45</v>
       </c>
-      <c r="B48" s="181"/>
+      <c r="B48" s="186"/>
       <c r="C48" s="64" t="s">
         <v>485</v>
       </c>
@@ -18592,10 +18995,10 @@
       <c r="BU48" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV48" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW48" s="161" t="s">
+      <c r="BV48" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW48" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX48" s="115" t="s">
@@ -18612,7 +19015,7 @@
       <c r="A49" s="92">
         <v>46</v>
       </c>
-      <c r="B49" s="181"/>
+      <c r="B49" s="186"/>
       <c r="C49" s="64" t="s">
         <v>486</v>
       </c>
@@ -18824,10 +19227,10 @@
       <c r="BU49" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BV49" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW49" s="161" t="s">
+      <c r="BV49" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW49" s="160" t="s">
         <v>11</v>
       </c>
       <c r="BX49" s="115" t="s">
@@ -18844,7 +19247,7 @@
       <c r="A50" s="92">
         <v>47</v>
       </c>
-      <c r="B50" s="181"/>
+      <c r="B50" s="186"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -19056,29 +19459,29 @@
         <v>1428</v>
       </c>
       <c r="BU50" s="115" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="BV50" s="115" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="BW50" s="115" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="BX50" s="115" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="BY50" s="115" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="BZ50" s="115" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="51" spans="1:78" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A51" s="92">
         <v>48</v>
       </c>
-      <c r="B51" s="181"/>
+      <c r="B51" s="186"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -19290,29 +19693,29 @@
         <v>1429</v>
       </c>
       <c r="BU51" s="115" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="BV51" s="115" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="BW51" s="115" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="BX51" s="115" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="BY51" s="115" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="BZ51" s="115" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="52" spans="1:78" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A52" s="92">
         <v>49</v>
       </c>
-      <c r="B52" s="181"/>
+      <c r="B52" s="186"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -19524,29 +19927,29 @@
         <v>1430</v>
       </c>
       <c r="BU52" s="115" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="BV52" s="115" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="BW52" s="115" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="BX52" s="115" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="BY52" s="115" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="BZ52" s="115" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="53" spans="1:78" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="92">
         <v>50</v>
       </c>
-      <c r="B53" s="182" t="s">
+      <c r="B53" s="187" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -19759,22 +20162,22 @@
       <c r="BT53" s="105" t="s">
         <v>860</v>
       </c>
-      <c r="BU53" s="157" t="s">
+      <c r="BU53" s="156" t="s">
         <v>206</v>
       </c>
-      <c r="BV53" s="157" t="s">
+      <c r="BV53" s="156" t="s">
         <v>206</v>
       </c>
       <c r="BW53" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="BX53" s="157" t="s">
+      <c r="BX53" s="156" t="s">
         <v>206</v>
       </c>
-      <c r="BY53" s="157" t="s">
+      <c r="BY53" s="156" t="s">
         <v>206</v>
       </c>
-      <c r="BZ53" s="157" t="s">
+      <c r="BZ53" s="156" t="s">
         <v>206</v>
       </c>
     </row>
@@ -19782,7 +20185,7 @@
       <c r="A54" s="92">
         <v>51</v>
       </c>
-      <c r="B54" s="182"/>
+      <c r="B54" s="187"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -20016,7 +20419,7 @@
       <c r="A55" s="92">
         <v>52</v>
       </c>
-      <c r="B55" s="182"/>
+      <c r="B55" s="187"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -20234,7 +20637,7 @@
         <v>30</v>
       </c>
       <c r="BW55" s="115" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="BX55" s="115" t="s">
         <v>30</v>
@@ -20250,7 +20653,7 @@
       <c r="A56" s="92">
         <v>53</v>
       </c>
-      <c r="B56" s="182"/>
+      <c r="B56" s="187"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -20459,30 +20862,30 @@
       <c r="BT56" s="105" t="s">
         <v>1401</v>
       </c>
-      <c r="BU56" s="158" t="s">
-        <v>1446</v>
-      </c>
-      <c r="BV56" s="158" t="s">
-        <v>1446</v>
+      <c r="BU56" s="157" t="s">
+        <v>1445</v>
+      </c>
+      <c r="BV56" s="157" t="s">
+        <v>1445</v>
       </c>
       <c r="BW56" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="BX56" s="158" t="s">
-        <v>1446</v>
-      </c>
-      <c r="BY56" s="158" t="s">
-        <v>1446</v>
-      </c>
-      <c r="BZ56" s="158" t="s">
-        <v>1446</v>
+      <c r="BX56" s="157" t="s">
+        <v>1445</v>
+      </c>
+      <c r="BY56" s="157" t="s">
+        <v>1445</v>
+      </c>
+      <c r="BZ56" s="157" t="s">
+        <v>1445</v>
       </c>
     </row>
     <row r="57" spans="1:78" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="92">
         <v>54</v>
       </c>
-      <c r="B57" s="182"/>
+      <c r="B57" s="187"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -20716,7 +21119,7 @@
       <c r="A58" s="92">
         <v>55</v>
       </c>
-      <c r="B58" s="182"/>
+      <c r="B58" s="187"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -20925,22 +21328,22 @@
       <c r="BT58" s="105" t="s">
         <v>1381</v>
       </c>
-      <c r="BU58" s="158" t="s">
+      <c r="BU58" s="157" t="s">
         <v>1381</v>
       </c>
-      <c r="BV58" s="158" t="s">
+      <c r="BV58" s="157" t="s">
         <v>1381</v>
       </c>
       <c r="BW58" s="115" t="s">
-        <v>1473</v>
-      </c>
-      <c r="BX58" s="158" t="s">
+        <v>1472</v>
+      </c>
+      <c r="BX58" s="157" t="s">
         <v>1381</v>
       </c>
-      <c r="BY58" s="158" t="s">
+      <c r="BY58" s="157" t="s">
         <v>1381</v>
       </c>
-      <c r="BZ58" s="158" t="s">
+      <c r="BZ58" s="157" t="s">
         <v>1381</v>
       </c>
     </row>
@@ -20948,7 +21351,7 @@
       <c r="A59" s="92">
         <v>56</v>
       </c>
-      <c r="B59" s="182"/>
+      <c r="B59" s="187"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -21159,22 +21562,22 @@
       <c r="BT59" s="105" t="s">
         <v>1401</v>
       </c>
-      <c r="BU59" s="158" t="s">
+      <c r="BU59" s="157" t="s">
         <v>1381</v>
       </c>
-      <c r="BV59" s="158" t="s">
+      <c r="BV59" s="157" t="s">
         <v>1381</v>
       </c>
       <c r="BW59" s="115" t="s">
-        <v>1473</v>
-      </c>
-      <c r="BX59" s="158" t="s">
+        <v>1472</v>
+      </c>
+      <c r="BX59" s="157" t="s">
         <v>1381</v>
       </c>
-      <c r="BY59" s="158" t="s">
+      <c r="BY59" s="157" t="s">
         <v>1381</v>
       </c>
-      <c r="BZ59" s="158" t="s">
+      <c r="BZ59" s="157" t="s">
         <v>1381</v>
       </c>
     </row>
@@ -21182,7 +21585,7 @@
       <c r="A60" s="92">
         <v>57</v>
       </c>
-      <c r="B60" s="182"/>
+      <c r="B60" s="187"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -21416,7 +21819,7 @@
       <c r="A61" s="92">
         <v>58</v>
       </c>
-      <c r="B61" s="183" t="s">
+      <c r="B61" s="188" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -21627,30 +22030,30 @@
       <c r="BT61" s="9">
         <v>44871</v>
       </c>
-      <c r="BU61" s="159" t="s">
-        <v>1447</v>
-      </c>
-      <c r="BV61" s="159" t="s">
-        <v>1459</v>
-      </c>
-      <c r="BW61" s="159">
+      <c r="BU61" s="158" t="s">
+        <v>1446</v>
+      </c>
+      <c r="BV61" s="158" t="s">
+        <v>1458</v>
+      </c>
+      <c r="BW61" s="158">
         <v>44871</v>
       </c>
-      <c r="BX61" s="159" t="s">
-        <v>1459</v>
-      </c>
-      <c r="BY61" s="159" t="s">
-        <v>1447</v>
-      </c>
-      <c r="BZ61" s="159" t="s">
-        <v>1447</v>
+      <c r="BX61" s="158" t="s">
+        <v>1458</v>
+      </c>
+      <c r="BY61" s="158" t="s">
+        <v>1446</v>
+      </c>
+      <c r="BZ61" s="158" t="s">
+        <v>1446</v>
       </c>
     </row>
     <row r="62" spans="1:78" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A62" s="92">
         <v>59</v>
       </c>
-      <c r="B62" s="183"/>
+      <c r="B62" s="188"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -21861,30 +22264,30 @@
       <c r="BT62" s="9">
         <v>44871</v>
       </c>
-      <c r="BU62" s="159" t="s">
-        <v>1447</v>
-      </c>
-      <c r="BV62" s="159" t="s">
-        <v>1459</v>
-      </c>
-      <c r="BW62" s="159">
+      <c r="BU62" s="158" t="s">
+        <v>1446</v>
+      </c>
+      <c r="BV62" s="158" t="s">
+        <v>1458</v>
+      </c>
+      <c r="BW62" s="158">
         <v>44871</v>
       </c>
-      <c r="BX62" s="159" t="s">
-        <v>1459</v>
-      </c>
-      <c r="BY62" s="159" t="s">
-        <v>1447</v>
-      </c>
-      <c r="BZ62" s="159" t="s">
-        <v>1447</v>
+      <c r="BX62" s="158" t="s">
+        <v>1458</v>
+      </c>
+      <c r="BY62" s="158" t="s">
+        <v>1446</v>
+      </c>
+      <c r="BZ62" s="158" t="s">
+        <v>1446</v>
       </c>
     </row>
     <row r="63" spans="1:78" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A63" s="92">
         <v>60</v>
       </c>
-      <c r="B63" s="183"/>
+      <c r="B63" s="188"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -22118,7 +22521,7 @@
       <c r="A64" s="92">
         <v>61</v>
       </c>
-      <c r="B64" s="183"/>
+      <c r="B64" s="188"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -22330,29 +22733,29 @@
         <v>1431</v>
       </c>
       <c r="BU64" s="115" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="BV64" s="115" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="BW64" s="115" t="s">
         <v>72</v>
       </c>
       <c r="BX64" s="115" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="BY64" s="115" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="BZ64" s="115" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="65" spans="1:105" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A65" s="92">
         <v>62</v>
       </c>
-      <c r="B65" s="183"/>
+      <c r="B65" s="188"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -22397,18 +22800,18 @@
       <c r="BR65" s="105"/>
       <c r="BS65" s="105"/>
       <c r="BT65" s="105"/>
-      <c r="BU65" s="158"/>
-      <c r="BV65" s="158"/>
-      <c r="BW65" s="158"/>
-      <c r="BX65" s="158"/>
-      <c r="BY65" s="158"/>
-      <c r="BZ65" s="158"/>
+      <c r="BU65" s="157"/>
+      <c r="BV65" s="157"/>
+      <c r="BW65" s="157"/>
+      <c r="BX65" s="157"/>
+      <c r="BY65" s="157"/>
+      <c r="BZ65" s="157"/>
     </row>
     <row r="66" spans="1:105" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A66" s="92">
         <v>63</v>
       </c>
-      <c r="B66" s="183"/>
+      <c r="B66" s="188"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -22453,18 +22856,18 @@
       <c r="BR66" s="105"/>
       <c r="BS66" s="105"/>
       <c r="BT66" s="105"/>
-      <c r="BU66" s="158"/>
-      <c r="BV66" s="158"/>
-      <c r="BW66" s="158"/>
-      <c r="BX66" s="158"/>
-      <c r="BY66" s="158"/>
-      <c r="BZ66" s="158"/>
+      <c r="BU66" s="157"/>
+      <c r="BV66" s="157"/>
+      <c r="BW66" s="157"/>
+      <c r="BX66" s="157"/>
+      <c r="BY66" s="157"/>
+      <c r="BZ66" s="157"/>
     </row>
     <row r="67" spans="1:105" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A67" s="92">
         <v>64</v>
       </c>
-      <c r="B67" s="183"/>
+      <c r="B67" s="188"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -22511,18 +22914,18 @@
       <c r="BR67" s="105"/>
       <c r="BS67" s="105"/>
       <c r="BT67" s="105"/>
-      <c r="BU67" s="158"/>
-      <c r="BV67" s="158"/>
-      <c r="BW67" s="158"/>
-      <c r="BX67" s="158"/>
-      <c r="BY67" s="158"/>
-      <c r="BZ67" s="158"/>
+      <c r="BU67" s="157"/>
+      <c r="BV67" s="157"/>
+      <c r="BW67" s="157"/>
+      <c r="BX67" s="157"/>
+      <c r="BY67" s="157"/>
+      <c r="BZ67" s="157"/>
     </row>
     <row r="68" spans="1:105" x14ac:dyDescent="0.35">
       <c r="A68" s="92">
         <v>65</v>
       </c>
-      <c r="B68" s="173" t="s">
+      <c r="B68" s="178" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -22549,18 +22952,18 @@
       </c>
       <c r="BS68" s="105"/>
       <c r="BT68" s="105"/>
-      <c r="BU68" s="158"/>
-      <c r="BV68" s="158"/>
-      <c r="BW68" s="158"/>
-      <c r="BX68" s="158"/>
-      <c r="BY68" s="158"/>
-      <c r="BZ68" s="158"/>
+      <c r="BU68" s="157"/>
+      <c r="BV68" s="157"/>
+      <c r="BW68" s="157"/>
+      <c r="BX68" s="157"/>
+      <c r="BY68" s="157"/>
+      <c r="BZ68" s="157"/>
     </row>
     <row r="69" spans="1:105" x14ac:dyDescent="0.35">
       <c r="A69" s="92">
         <v>66</v>
       </c>
-      <c r="B69" s="173"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -22582,18 +22985,18 @@
       <c r="BR69" s="105"/>
       <c r="BS69" s="105"/>
       <c r="BT69" s="105"/>
-      <c r="BU69" s="158"/>
-      <c r="BV69" s="158"/>
-      <c r="BW69" s="158"/>
-      <c r="BX69" s="158"/>
-      <c r="BY69" s="158"/>
-      <c r="BZ69" s="158"/>
+      <c r="BU69" s="157"/>
+      <c r="BV69" s="157"/>
+      <c r="BW69" s="157"/>
+      <c r="BX69" s="157"/>
+      <c r="BY69" s="157"/>
+      <c r="BZ69" s="157"/>
     </row>
     <row r="70" spans="1:105" x14ac:dyDescent="0.35">
       <c r="A70" s="92">
         <v>67</v>
       </c>
-      <c r="B70" s="173"/>
+      <c r="B70" s="178"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -22614,18 +23017,18 @@
       <c r="BR70" s="105"/>
       <c r="BS70" s="105"/>
       <c r="BT70" s="105"/>
-      <c r="BU70" s="158"/>
-      <c r="BV70" s="158"/>
-      <c r="BW70" s="158"/>
-      <c r="BX70" s="158"/>
-      <c r="BY70" s="158"/>
-      <c r="BZ70" s="158"/>
+      <c r="BU70" s="157"/>
+      <c r="BV70" s="157"/>
+      <c r="BW70" s="157"/>
+      <c r="BX70" s="157"/>
+      <c r="BY70" s="157"/>
+      <c r="BZ70" s="157"/>
     </row>
     <row r="71" spans="1:105" x14ac:dyDescent="0.35">
       <c r="A71" s="92">
         <v>68</v>
       </c>
-      <c r="B71" s="173"/>
+      <c r="B71" s="178"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -22646,18 +23049,18 @@
       <c r="BR71" s="105"/>
       <c r="BS71" s="105"/>
       <c r="BT71" s="105"/>
-      <c r="BU71" s="158"/>
-      <c r="BV71" s="158"/>
-      <c r="BW71" s="158"/>
-      <c r="BX71" s="158"/>
-      <c r="BY71" s="158"/>
-      <c r="BZ71" s="158"/>
+      <c r="BU71" s="157"/>
+      <c r="BV71" s="157"/>
+      <c r="BW71" s="157"/>
+      <c r="BX71" s="157"/>
+      <c r="BY71" s="157"/>
+      <c r="BZ71" s="157"/>
     </row>
     <row r="72" spans="1:105" x14ac:dyDescent="0.35">
       <c r="A72" s="92">
         <v>69</v>
       </c>
-      <c r="B72" s="174"/>
+      <c r="B72" s="179"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -22678,12 +23081,12 @@
       <c r="BR72" s="105"/>
       <c r="BS72" s="105"/>
       <c r="BT72" s="105"/>
-      <c r="BU72" s="160"/>
-      <c r="BV72" s="160"/>
-      <c r="BW72" s="160"/>
-      <c r="BX72" s="160"/>
-      <c r="BY72" s="160"/>
-      <c r="BZ72" s="160"/>
+      <c r="BU72" s="159"/>
+      <c r="BV72" s="159"/>
+      <c r="BW72" s="159"/>
+      <c r="BX72" s="159"/>
+      <c r="BY72" s="159"/>
+      <c r="BZ72" s="159"/>
     </row>
     <row r="73" spans="1:105" x14ac:dyDescent="0.35">
       <c r="U73" s="12"/>
@@ -23253,7 +23656,7 @@
       <c r="BT3" s="36"/>
     </row>
     <row r="4" spans="2:72" x14ac:dyDescent="0.35">
-      <c r="B4" s="175" t="s">
+      <c r="B4" s="180" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -23422,7 +23825,7 @@
       <c r="BT4" s="12"/>
     </row>
     <row r="5" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="176"/>
+      <c r="B5" s="181"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -23754,7 +24157,7 @@
       <c r="BT6" s="2"/>
     </row>
     <row r="7" spans="2:72" x14ac:dyDescent="0.35">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="182" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -23921,7 +24324,7 @@
       <c r="BT7" s="37"/>
     </row>
     <row r="8" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="177"/>
+      <c r="B8" s="182"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -24088,7 +24491,7 @@
       <c r="BT8" s="1"/>
     </row>
     <row r="9" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="177"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -24255,7 +24658,7 @@
       <c r="BT9" s="1"/>
     </row>
     <row r="10" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="177"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -24422,7 +24825,7 @@
       <c r="BT10" s="1"/>
     </row>
     <row r="11" spans="2:72" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="183" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -24589,7 +24992,7 @@
       <c r="BT11" s="106"/>
     </row>
     <row r="12" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="179"/>
+      <c r="B12" s="184"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -24754,7 +25157,7 @@
       <c r="BT12" s="2"/>
     </row>
     <row r="13" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="179"/>
+      <c r="B13" s="184"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -24919,7 +25322,7 @@
       <c r="BT13" s="106"/>
     </row>
     <row r="14" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="179"/>
+      <c r="B14" s="184"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -25084,7 +25487,7 @@
       <c r="BT14" s="2"/>
     </row>
     <row r="15" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="179"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -25249,7 +25652,7 @@
       <c r="BT15" s="2"/>
     </row>
     <row r="16" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="179"/>
+      <c r="B16" s="184"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -25414,7 +25817,7 @@
       <c r="BT16" s="2"/>
     </row>
     <row r="17" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="179"/>
+      <c r="B17" s="184"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -25579,7 +25982,7 @@
       <c r="BT17" s="2"/>
     </row>
     <row r="18" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="179"/>
+      <c r="B18" s="184"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -25744,7 +26147,7 @@
       <c r="BT18" s="2"/>
     </row>
     <row r="19" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="179"/>
+      <c r="B19" s="184"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -25909,7 +26312,7 @@
       <c r="BT19" s="2"/>
     </row>
     <row r="20" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="179"/>
+      <c r="B20" s="184"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -26074,7 +26477,7 @@
       <c r="BT20" s="2"/>
     </row>
     <row r="21" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="185" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -26282,7 +26685,7 @@
       <c r="BT21" s="106"/>
     </row>
     <row r="22" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="180"/>
+      <c r="B22" s="185"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -26490,7 +26893,7 @@
       <c r="BT22" s="106"/>
     </row>
     <row r="23" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="180"/>
+      <c r="B23" s="185"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -26657,7 +27060,7 @@
       <c r="BT23" s="2"/>
     </row>
     <row r="24" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B24" s="180"/>
+      <c r="B24" s="185"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -26824,7 +27227,7 @@
       <c r="BT24" s="105"/>
     </row>
     <row r="25" spans="2:72" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="B25" s="180"/>
+      <c r="B25" s="185"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -26989,7 +27392,7 @@
       <c r="BT25" s="6"/>
     </row>
     <row r="26" spans="2:72" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="181" t="s">
+      <c r="B26" s="186" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -27158,7 +27561,7 @@
       <c r="BT26" s="38"/>
     </row>
     <row r="27" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="181"/>
+      <c r="B27" s="186"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -27325,7 +27728,7 @@
       <c r="BT27" s="42"/>
     </row>
     <row r="28" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="181"/>
+      <c r="B28" s="186"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -27490,7 +27893,7 @@
       <c r="BT28" s="66"/>
     </row>
     <row r="29" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="181"/>
+      <c r="B29" s="186"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -27655,7 +28058,7 @@
       <c r="BT29" s="42"/>
     </row>
     <row r="30" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="181"/>
+      <c r="B30" s="186"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -27820,7 +28223,7 @@
       <c r="BT30" s="38"/>
     </row>
     <row r="31" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="181"/>
+      <c r="B31" s="186"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -27985,7 +28388,7 @@
       <c r="BT31" s="42"/>
     </row>
     <row r="32" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="181"/>
+      <c r="B32" s="186"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -28150,7 +28553,7 @@
       <c r="BT32" s="88"/>
     </row>
     <row r="33" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="181"/>
+      <c r="B33" s="186"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -28315,7 +28718,7 @@
       <c r="BT33" s="28"/>
     </row>
     <row r="34" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="181"/>
+      <c r="B34" s="186"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -28480,7 +28883,7 @@
       <c r="BT34" s="38"/>
     </row>
     <row r="35" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="181"/>
+      <c r="B35" s="186"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -28645,7 +29048,7 @@
       <c r="BT35" s="42"/>
     </row>
     <row r="36" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="181"/>
+      <c r="B36" s="186"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -28810,7 +29213,7 @@
       <c r="BT36" s="38"/>
     </row>
     <row r="37" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="181"/>
+      <c r="B37" s="186"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -28975,7 +29378,7 @@
       <c r="BT37" s="42"/>
     </row>
     <row r="38" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="181"/>
+      <c r="B38" s="186"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -29140,7 +29543,7 @@
       <c r="BT38" s="38"/>
     </row>
     <row r="39" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="181"/>
+      <c r="B39" s="186"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -29305,7 +29708,7 @@
       <c r="BT39" s="38"/>
     </row>
     <row r="40" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="181"/>
+      <c r="B40" s="186"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -29470,7 +29873,7 @@
       <c r="BT40" s="38"/>
     </row>
     <row r="41" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="181"/>
+      <c r="B41" s="186"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -29635,7 +30038,7 @@
       <c r="BT41" s="38"/>
     </row>
     <row r="42" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="181"/>
+      <c r="B42" s="186"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -29800,7 +30203,7 @@
       <c r="BT42" s="38"/>
     </row>
     <row r="43" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B43" s="181"/>
+      <c r="B43" s="186"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -29965,7 +30368,7 @@
       <c r="BT43" s="38"/>
     </row>
     <row r="44" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B44" s="181"/>
+      <c r="B44" s="186"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -30130,7 +30533,7 @@
       <c r="BT44" s="38"/>
     </row>
     <row r="45" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B45" s="181"/>
+      <c r="B45" s="186"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -30295,7 +30698,7 @@
       <c r="BT45" s="38"/>
     </row>
     <row r="46" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B46" s="181"/>
+      <c r="B46" s="186"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -30460,7 +30863,7 @@
       <c r="BT46" s="38"/>
     </row>
     <row r="47" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B47" s="181"/>
+      <c r="B47" s="186"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -30625,7 +31028,7 @@
       <c r="BT47" s="38"/>
     </row>
     <row r="48" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B48" s="181"/>
+      <c r="B48" s="186"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -30790,7 +31193,7 @@
       <c r="BT48" s="38"/>
     </row>
     <row r="49" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B49" s="181"/>
+      <c r="B49" s="186"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -30955,7 +31358,7 @@
       <c r="BT49" s="38"/>
     </row>
     <row r="50" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B50" s="181"/>
+      <c r="B50" s="186"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -31122,7 +31525,7 @@
       <c r="BT50" s="2"/>
     </row>
     <row r="51" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B51" s="181"/>
+      <c r="B51" s="186"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -31289,7 +31692,7 @@
       <c r="BT51" s="2"/>
     </row>
     <row r="52" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B52" s="181"/>
+      <c r="B52" s="186"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -31456,7 +31859,7 @@
       <c r="BT52" s="2"/>
     </row>
     <row r="53" spans="2:72" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="182" t="s">
+      <c r="B53" s="187" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -31625,7 +32028,7 @@
       <c r="BT53" s="105"/>
     </row>
     <row r="54" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B54" s="182"/>
+      <c r="B54" s="187"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -31792,7 +32195,7 @@
       <c r="BT54" s="5"/>
     </row>
     <row r="55" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B55" s="182"/>
+      <c r="B55" s="187"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -31959,7 +32362,7 @@
       <c r="BT55" s="5"/>
     </row>
     <row r="56" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B56" s="182"/>
+      <c r="B56" s="187"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -32124,7 +32527,7 @@
       <c r="BT56" s="3"/>
     </row>
     <row r="57" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B57" s="182"/>
+      <c r="B57" s="187"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -32291,7 +32694,7 @@
       <c r="BT57" s="2"/>
     </row>
     <row r="58" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B58" s="182"/>
+      <c r="B58" s="187"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -32456,7 +32859,7 @@
       <c r="BT58" s="7"/>
     </row>
     <row r="59" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B59" s="182"/>
+      <c r="B59" s="187"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -32623,7 +33026,7 @@
       <c r="BT59" s="5"/>
     </row>
     <row r="60" spans="2:72" x14ac:dyDescent="0.35">
-      <c r="B60" s="182"/>
+      <c r="B60" s="187"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -32790,7 +33193,7 @@
       <c r="BT60" s="12"/>
     </row>
     <row r="61" spans="2:72" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="183" t="s">
+      <c r="B61" s="188" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -32957,7 +33360,7 @@
       <c r="BT61" s="9"/>
     </row>
     <row r="62" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="183"/>
+      <c r="B62" s="188"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -33124,7 +33527,7 @@
       <c r="BT62" s="9"/>
     </row>
     <row r="63" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="183"/>
+      <c r="B63" s="188"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -33291,7 +33694,7 @@
       <c r="BT63" s="5"/>
     </row>
     <row r="64" spans="2:72" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B64" s="183"/>
+      <c r="B64" s="188"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -33458,7 +33861,7 @@
       <c r="BT64" s="2"/>
     </row>
     <row r="65" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="183"/>
+      <c r="B65" s="188"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -33475,7 +33878,7 @@
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B66" s="183"/>
+      <c r="B66" s="188"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -33494,7 +33897,7 @@
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B67" s="183"/>
+      <c r="B67" s="188"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -33513,7 +33916,7 @@
       <c r="P67" s="1"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B68" s="173" t="s">
+      <c r="B68" s="178" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -33523,7 +33926,7 @@
       <c r="L68" s="105"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B69" s="173"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -33531,7 +33934,7 @@
       <c r="K69" s="12"/>
     </row>
     <row r="70" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B70" s="173"/>
+      <c r="B70" s="178"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -33539,7 +33942,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:16" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B71" s="173"/>
+      <c r="B71" s="178"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -33551,7 +33954,7 @@
       <c r="L71" s="105"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B72" s="174"/>
+      <c r="B72" s="179"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -33929,10 +34332,10 @@
   <dimension ref="B1:AA72"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="R28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="R90" sqref="R90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -34131,7 +34534,7 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B4" s="175" t="s">
+      <c r="B4" s="180" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -34211,7 +34614,7 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="176"/>
+      <c r="B5" s="181"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -34365,7 +34768,7 @@
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="182" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -34443,7 +34846,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="177"/>
+      <c r="B8" s="182"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -34521,7 +34924,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="177"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -34599,7 +35002,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="177"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -34677,7 +35080,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="183" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -34755,7 +35158,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="179"/>
+      <c r="B12" s="184"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -34831,7 +35234,7 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="179"/>
+      <c r="B13" s="184"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -34907,7 +35310,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="179"/>
+      <c r="B14" s="184"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -34983,7 +35386,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="179"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -35059,7 +35462,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="179"/>
+      <c r="B16" s="184"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -35135,7 +35538,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="179"/>
+      <c r="B17" s="184"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -35211,7 +35614,7 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="179"/>
+      <c r="B18" s="184"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -35287,7 +35690,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="179"/>
+      <c r="B19" s="184"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -35363,7 +35766,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="179"/>
+      <c r="B20" s="184"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -35439,7 +35842,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="185" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -35517,7 +35920,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="180"/>
+      <c r="B22" s="185"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -35595,7 +35998,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="180"/>
+      <c r="B23" s="185"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -35673,7 +36076,7 @@
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B24" s="180"/>
+      <c r="B24" s="185"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -35751,7 +36154,7 @@
       </c>
     </row>
     <row r="25" spans="2:27" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="B25" s="180"/>
+      <c r="B25" s="185"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -35827,7 +36230,7 @@
       </c>
     </row>
     <row r="26" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="181" t="s">
+      <c r="B26" s="186" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -35907,7 +36310,7 @@
       </c>
     </row>
     <row r="27" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="181"/>
+      <c r="B27" s="186"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -35985,7 +36388,7 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="181"/>
+      <c r="B28" s="186"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -36061,7 +36464,7 @@
       </c>
     </row>
     <row r="29" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="181"/>
+      <c r="B29" s="186"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -36137,7 +36540,7 @@
       </c>
     </row>
     <row r="30" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="181"/>
+      <c r="B30" s="186"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -36213,7 +36616,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="181"/>
+      <c r="B31" s="186"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -36289,7 +36692,7 @@
       </c>
     </row>
     <row r="32" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="181"/>
+      <c r="B32" s="186"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -36365,7 +36768,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="181"/>
+      <c r="B33" s="186"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -36441,7 +36844,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="181"/>
+      <c r="B34" s="186"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -36517,7 +36920,7 @@
       </c>
     </row>
     <row r="35" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="181"/>
+      <c r="B35" s="186"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -36593,7 +36996,7 @@
       </c>
     </row>
     <row r="36" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="181"/>
+      <c r="B36" s="186"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -36669,7 +37072,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="181"/>
+      <c r="B37" s="186"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -36745,7 +37148,7 @@
       </c>
     </row>
     <row r="38" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="181"/>
+      <c r="B38" s="186"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -36821,7 +37224,7 @@
       </c>
     </row>
     <row r="39" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="181"/>
+      <c r="B39" s="186"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -36897,7 +37300,7 @@
       </c>
     </row>
     <row r="40" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="181"/>
+      <c r="B40" s="186"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -36973,7 +37376,7 @@
       </c>
     </row>
     <row r="41" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="181"/>
+      <c r="B41" s="186"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -37049,7 +37452,7 @@
       </c>
     </row>
     <row r="42" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="181"/>
+      <c r="B42" s="186"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -37125,7 +37528,7 @@
       </c>
     </row>
     <row r="43" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B43" s="181"/>
+      <c r="B43" s="186"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -37201,7 +37604,7 @@
       </c>
     </row>
     <row r="44" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B44" s="181"/>
+      <c r="B44" s="186"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -37277,7 +37680,7 @@
       </c>
     </row>
     <row r="45" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B45" s="181"/>
+      <c r="B45" s="186"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -37353,7 +37756,7 @@
       </c>
     </row>
     <row r="46" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B46" s="181"/>
+      <c r="B46" s="186"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -37429,7 +37832,7 @@
       </c>
     </row>
     <row r="47" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B47" s="181"/>
+      <c r="B47" s="186"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -37505,7 +37908,7 @@
       </c>
     </row>
     <row r="48" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B48" s="181"/>
+      <c r="B48" s="186"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -37581,7 +37984,7 @@
       </c>
     </row>
     <row r="49" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B49" s="181"/>
+      <c r="B49" s="186"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -37657,7 +38060,7 @@
       </c>
     </row>
     <row r="50" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B50" s="181"/>
+      <c r="B50" s="186"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -37735,7 +38138,7 @@
       </c>
     </row>
     <row r="51" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B51" s="181"/>
+      <c r="B51" s="186"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -37813,7 +38216,7 @@
       </c>
     </row>
     <row r="52" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B52" s="181"/>
+      <c r="B52" s="186"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -37891,7 +38294,7 @@
       </c>
     </row>
     <row r="53" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B53" s="182" t="s">
+      <c r="B53" s="187" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -37971,7 +38374,7 @@
       </c>
     </row>
     <row r="54" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B54" s="182"/>
+      <c r="B54" s="187"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -38049,7 +38452,7 @@
       </c>
     </row>
     <row r="55" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B55" s="182"/>
+      <c r="B55" s="187"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -38127,7 +38530,7 @@
       </c>
     </row>
     <row r="56" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B56" s="182"/>
+      <c r="B56" s="187"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -38203,7 +38606,7 @@
       </c>
     </row>
     <row r="57" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B57" s="182"/>
+      <c r="B57" s="187"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -38281,7 +38684,7 @@
       </c>
     </row>
     <row r="58" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B58" s="182"/>
+      <c r="B58" s="187"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -38357,7 +38760,7 @@
       </c>
     </row>
     <row r="59" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B59" s="182"/>
+      <c r="B59" s="187"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -38435,7 +38838,7 @@
       </c>
     </row>
     <row r="60" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B60" s="182"/>
+      <c r="B60" s="187"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -38513,7 +38916,7 @@
       </c>
     </row>
     <row r="61" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B61" s="183" t="s">
+      <c r="B61" s="188" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -38591,7 +38994,7 @@
       </c>
     </row>
     <row r="62" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="183"/>
+      <c r="B62" s="188"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -38669,7 +39072,7 @@
       </c>
     </row>
     <row r="63" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="183"/>
+      <c r="B63" s="188"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -38747,7 +39150,7 @@
       </c>
     </row>
     <row r="64" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B64" s="183"/>
+      <c r="B64" s="188"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -38825,7 +39228,7 @@
       </c>
     </row>
     <row r="65" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="183"/>
+      <c r="B65" s="188"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -38855,7 +39258,7 @@
       <c r="AA65" s="5"/>
     </row>
     <row r="66" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B66" s="183"/>
+      <c r="B66" s="188"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -38885,7 +39288,7 @@
       <c r="AA66" s="5"/>
     </row>
     <row r="67" spans="2:27" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B67" s="183"/>
+      <c r="B67" s="188"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -38915,7 +39318,7 @@
       <c r="AA67" s="1"/>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B68" s="173" t="s">
+      <c r="B68" s="178" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -38936,7 +39339,7 @@
       <c r="Q68" s="105"/>
     </row>
     <row r="69" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B69" s="173"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -38955,7 +39358,7 @@
       <c r="Q69" s="105"/>
     </row>
     <row r="70" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B70" s="173"/>
+      <c r="B70" s="178"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -38974,7 +39377,7 @@
       <c r="Q70" s="105"/>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B71" s="173"/>
+      <c r="B71" s="178"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -38993,7 +39396,7 @@
       <c r="Q71" s="105"/>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B72" s="174"/>
+      <c r="B72" s="179"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>

</xml_diff>

<commit_message>
New classifications, datagroups, and projects.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8130" uniqueCount="1543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8158" uniqueCount="1558">
   <si>
     <t>Description</t>
   </si>
@@ -4652,6 +4652,51 @@
   </si>
   <si>
     <t>entire industry, waste management</t>
+  </si>
+  <si>
+    <t>Meng_PNAS_2023_Global_Plastics_Pathways_Process_Data</t>
+  </si>
+  <si>
+    <t>unit process inventories, process parameters, yield factors</t>
+  </si>
+  <si>
+    <t>plastic monomer production processes</t>
+  </si>
+  <si>
+    <t>process inventories for ethylene, propylene, and butadiene</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.221829412</t>
+  </si>
+  <si>
+    <t>Fanran MENG</t>
+  </si>
+  <si>
+    <t>ethylene, propylene, and butadiene</t>
+  </si>
+  <si>
+    <t>2020-2080</t>
+  </si>
+  <si>
+    <t>GNU General Public License v3.0</t>
+  </si>
+  <si>
+    <t>mass, energy, monetary, lifetime, capacity</t>
+  </si>
+  <si>
+    <t>unit process inventories, process parameters, yield factors for ethylene, propylene, and butadiene</t>
+  </si>
+  <si>
+    <t>ethylene; propylene; butadiene; unit process inventories; process parameters; yield factors</t>
+  </si>
+  <si>
+    <t>dataset contains more technologies (ammonia, urea, benzene, etc.) but only the major plastic monomers where converted</t>
+  </si>
+  <si>
+    <t>intensive process properties, extensive process properties</t>
+  </si>
+  <si>
+    <t>one representative value, constant time series</t>
   </si>
 </sst>
 </file>
@@ -5024,7 +5069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -5366,6 +5411,10 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -6170,13 +6219,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T39"/>
+  <dimension ref="B2:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomRight" activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -6196,16 +6245,17 @@
     <col min="18" max="18" width="39.265625" customWidth="1"/>
     <col min="19" max="19" width="37.3984375" customWidth="1"/>
     <col min="20" max="20" width="34.53125" customWidth="1"/>
+    <col min="21" max="21" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:21" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:20" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:21" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="32"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -6261,8 +6311,11 @@
       <c r="T3" s="163" t="s">
         <v>1510</v>
       </c>
+      <c r="U3" s="163" t="s">
+        <v>1543</v>
+      </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" s="175" t="s">
         <v>2</v>
       </c>
@@ -6320,8 +6373,11 @@
       <c r="T4" s="141">
         <v>16</v>
       </c>
+      <c r="U4" s="141">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="176"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
@@ -6374,11 +6430,14 @@
       <c r="S5" s="164" t="s">
         <v>1509</v>
       </c>
-      <c r="T5" s="164" t="s">
+      <c r="T5" s="190" t="s">
         <v>1510</v>
       </c>
+      <c r="U5" s="190" t="s">
+        <v>1543</v>
+      </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="33"/>
       <c r="C6" s="54" t="s">
         <v>453</v>
@@ -6429,11 +6488,14 @@
       <c r="S6" s="164" t="s">
         <v>1150</v>
       </c>
-      <c r="T6" s="164" t="s">
+      <c r="T6" s="190" t="s">
         <v>1150</v>
       </c>
+      <c r="U6" s="190" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
@@ -6486,11 +6548,14 @@
       <c r="S7" s="40" t="s">
         <v>1505</v>
       </c>
-      <c r="T7" s="40" t="s">
+      <c r="T7" s="23" t="s">
         <v>1511</v>
       </c>
+      <c r="U7" s="23" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="2:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:21" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="171" t="s">
         <v>6</v>
       </c>
@@ -6543,11 +6608,14 @@
       <c r="S8" s="40" t="s">
         <v>1519</v>
       </c>
-      <c r="T8" s="164" t="s">
+      <c r="T8" s="190" t="s">
         <v>1533</v>
       </c>
+      <c r="U8" s="190" t="s">
+        <v>1556</v>
+      </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" s="171"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
@@ -6598,11 +6666,14 @@
       <c r="S9" s="40" t="s">
         <v>1521</v>
       </c>
-      <c r="T9" s="164" t="s">
+      <c r="T9" s="190" t="s">
         <v>1532</v>
       </c>
+      <c r="U9" s="190" t="s">
+        <v>1544</v>
+      </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" s="171"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
@@ -6653,11 +6724,14 @@
       <c r="S10" s="40" t="s">
         <v>1520</v>
       </c>
-      <c r="T10" s="164" t="s">
+      <c r="T10" s="190" t="s">
         <v>199</v>
       </c>
+      <c r="U10" s="190" t="s">
+        <v>1552</v>
+      </c>
     </row>
-    <row r="11" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B11" s="171"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
@@ -6708,11 +6782,14 @@
       <c r="S11" s="40" t="s">
         <v>1522</v>
       </c>
-      <c r="T11" s="164" t="s">
+      <c r="T11" s="190" t="s">
         <v>1542</v>
       </c>
+      <c r="U11" s="190" t="s">
+        <v>1545</v>
+      </c>
     </row>
-    <row r="12" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B12" s="171"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
@@ -6763,11 +6840,14 @@
       <c r="S12" s="164" t="s">
         <v>1516</v>
       </c>
-      <c r="T12" s="164" t="s">
+      <c r="T12" s="190" t="s">
         <v>1534</v>
       </c>
+      <c r="U12" s="190" t="s">
+        <v>1546</v>
+      </c>
     </row>
-    <row r="13" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B13" s="171"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
@@ -6818,11 +6898,14 @@
       <c r="S13" s="40" t="s">
         <v>1523</v>
       </c>
-      <c r="T13" s="164" t="s">
+      <c r="T13" s="190" t="s">
         <v>1094</v>
       </c>
+      <c r="U13" s="190" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="14" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B14" s="171"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
@@ -6873,11 +6956,14 @@
       <c r="S14" s="40" t="s">
         <v>1524</v>
       </c>
-      <c r="T14" s="164" t="s">
+      <c r="T14" s="190" t="s">
         <v>1535</v>
       </c>
+      <c r="U14" s="190" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="15" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B15" s="171"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
@@ -6928,11 +7014,14 @@
       <c r="S15" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="T15" s="164" t="s">
+      <c r="T15" s="190" t="s">
         <v>1536</v>
       </c>
+      <c r="U15" s="190" t="s">
+        <v>1545</v>
+      </c>
     </row>
-    <row r="16" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B16" s="171"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
@@ -6983,11 +7072,14 @@
       <c r="S16" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="T16" s="164" t="s">
+      <c r="T16" s="190" t="s">
         <v>1535</v>
       </c>
+      <c r="U16" s="190" t="s">
+        <v>1549</v>
+      </c>
     </row>
-    <row r="17" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B17" s="171"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
@@ -7038,11 +7130,14 @@
       <c r="S17" s="164" t="s">
         <v>819</v>
       </c>
-      <c r="T17" s="164" t="s">
+      <c r="T17" s="190" t="s">
         <v>1531</v>
       </c>
+      <c r="U17" s="190" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B18" s="171"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
@@ -7093,11 +7188,14 @@
       <c r="S18" s="164" t="s">
         <v>1517</v>
       </c>
-      <c r="T18" s="164" t="s">
+      <c r="T18" s="190" t="s">
         <v>1530</v>
       </c>
+      <c r="U18" s="190" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="171"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
@@ -7148,11 +7246,14 @@
       <c r="S19" s="164" t="s">
         <v>1518</v>
       </c>
-      <c r="T19" s="164" t="s">
+      <c r="T19" s="190" t="s">
         <v>1518</v>
       </c>
+      <c r="U19" s="190" t="s">
+        <v>1550</v>
+      </c>
     </row>
-    <row r="20" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B20" s="171"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
@@ -7203,11 +7304,14 @@
       <c r="S20" s="29" t="s">
         <v>1278</v>
       </c>
-      <c r="T20" s="164" t="s">
+      <c r="T20" s="190" t="s">
         <v>1278</v>
       </c>
+      <c r="U20" s="190" t="s">
+        <v>1557</v>
+      </c>
     </row>
-    <row r="21" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B21" s="172" t="s">
         <v>0</v>
       </c>
@@ -7260,11 +7364,14 @@
       <c r="S21" s="40" t="s">
         <v>1525</v>
       </c>
-      <c r="T21" s="164" t="s">
+      <c r="T21" s="190" t="s">
         <v>1537</v>
       </c>
+      <c r="U21" s="190" t="s">
+        <v>1553</v>
+      </c>
     </row>
-    <row r="22" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B22" s="172"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
@@ -7317,11 +7424,14 @@
       <c r="S22" s="40" t="s">
         <v>1526</v>
       </c>
-      <c r="T22" s="164" t="s">
+      <c r="T22" s="190" t="s">
         <v>1538</v>
       </c>
+      <c r="U22" s="190" t="s">
+        <v>1554</v>
+      </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B23" s="172"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
@@ -7369,14 +7479,17 @@
       <c r="R23" s="154" t="s">
         <v>1388</v>
       </c>
-      <c r="S23" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="T23" s="164" t="s">
+      <c r="S23" s="189" t="s">
+        <v>11</v>
+      </c>
+      <c r="T23" s="190" t="s">
+        <v>11</v>
+      </c>
+      <c r="U23" s="190" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B24" s="172"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
@@ -7427,11 +7540,14 @@
       <c r="S24" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="T24" s="164" t="s">
-        <v>11</v>
+      <c r="T24" s="190" t="s">
+        <v>11</v>
+      </c>
+      <c r="U24" s="190" t="s">
+        <v>1555</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:21" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="173" t="s">
         <v>8</v>
       </c>
@@ -7484,11 +7600,14 @@
       <c r="S25" s="40" t="s">
         <v>861</v>
       </c>
-      <c r="T25" s="40" t="s">
+      <c r="T25" s="23" t="s">
         <v>861</v>
       </c>
+      <c r="U25" s="23" t="s">
+        <v>860</v>
+      </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B26" s="173"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
@@ -7539,11 +7658,14 @@
       <c r="S26" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="T26" s="164" t="s">
+      <c r="T26" s="190" t="s">
         <v>1541</v>
       </c>
+      <c r="U26" s="190" t="s">
+        <v>1551</v>
+      </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B27" s="173"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
@@ -7594,11 +7716,14 @@
       <c r="S27" s="40" t="s">
         <v>1527</v>
       </c>
-      <c r="T27" s="164" t="s">
+      <c r="T27" s="190" t="s">
         <v>1511</v>
       </c>
+      <c r="U27" s="190" t="s">
+        <v>1548</v>
+      </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="173"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
@@ -7646,14 +7771,17 @@
       <c r="R28" s="154" t="s">
         <v>1388</v>
       </c>
-      <c r="S28" s="90" t="s">
+      <c r="S28" s="157" t="s">
         <v>1529</v>
       </c>
-      <c r="T28" s="90" t="s">
+      <c r="T28" s="47" t="s">
         <v>1539</v>
       </c>
+      <c r="U28" s="47" t="s">
+        <v>1547</v>
+      </c>
     </row>
-    <row r="29" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B29" s="173"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
@@ -7701,14 +7829,17 @@
       <c r="R29" s="154" t="s">
         <v>1388</v>
       </c>
-      <c r="S29" s="90" t="s">
+      <c r="S29" s="157" t="s">
         <v>1529</v>
       </c>
-      <c r="T29" s="62" t="s">
+      <c r="T29" s="191" t="s">
         <v>1539</v>
       </c>
+      <c r="U29" s="47" t="s">
+        <v>1547</v>
+      </c>
     </row>
-    <row r="30" spans="2:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:21" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B30" s="173"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
@@ -7756,14 +7887,17 @@
       <c r="R30" s="154" t="s">
         <v>1388</v>
       </c>
-      <c r="S30" s="62" t="s">
+      <c r="S30" s="189" t="s">
         <v>1528</v>
       </c>
-      <c r="T30" s="62" t="s">
+      <c r="T30" s="191" t="s">
         <v>1540</v>
       </c>
+      <c r="U30" s="47" t="s">
+        <v>1547</v>
+      </c>
     </row>
-    <row r="31" spans="2:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:21" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="174" t="s">
         <v>9</v>
       </c>
@@ -7821,8 +7955,11 @@
       <c r="T31" s="165">
         <v>45164</v>
       </c>
+      <c r="U31" s="165">
+        <v>45182</v>
+      </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B32" s="177"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
@@ -7875,11 +8012,14 @@
       <c r="S32" s="164" t="s">
         <v>30</v>
       </c>
-      <c r="T32" s="164" t="s">
+      <c r="T32" s="190" t="s">
         <v>30</v>
       </c>
+      <c r="U32" s="190" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B33" s="167" t="s">
         <v>185</v>
       </c>
@@ -7902,9 +8042,10 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="29"/>
       <c r="S33" s="164"/>
-      <c r="T33" s="164"/>
+      <c r="T33" s="190"/>
+      <c r="U33" s="190"/>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B34" s="168"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
@@ -7925,9 +8066,10 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="29"/>
       <c r="S34" s="164"/>
-      <c r="T34" s="164"/>
+      <c r="T34" s="190"/>
+      <c r="U34" s="190"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B35" s="169"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
@@ -7948,9 +8090,10 @@
       <c r="Q35" s="152"/>
       <c r="R35" s="30"/>
       <c r="S35" s="166"/>
-      <c r="T35" s="166"/>
+      <c r="T35" s="192"/>
+      <c r="U35" s="192"/>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
       <c r="I39" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
March 2025 lookup table and classification items update. New projects and data groups.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF02CC2-A31F-4EF0-B730-F0B28AF5EF72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3332DB-4D3C-45E6-9D48-FE4482CBD019}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="13" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="DataSets_SteelCycle" sheetId="20" r:id="rId4"/>
     <sheet name="DataSets_YSTAFDB_stocks&amp;flows" sheetId="21" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10650" uniqueCount="2108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10885" uniqueCount="2177">
   <si>
     <t>Description</t>
   </si>
@@ -6348,6 +6348,213 @@
   </si>
   <si>
     <t>Numbers manually reformatted from original source (xlsx) to Excel spreadsheet</t>
+  </si>
+  <si>
+    <t>dataset entry does not exist yet, needs to be created, no upload of data, just link!</t>
+  </si>
+  <si>
+    <t>1_F_MaterialFlows_UNEP_IRP</t>
+  </si>
+  <si>
+    <t>v2024</t>
+  </si>
+  <si>
+    <t>The full dataset used herein can be downloaded from the Global Material Flow Database hosted by the United Nations Environment Program International Resource Panel.</t>
+  </si>
+  <si>
+    <t>Heinz SCHANDL</t>
+  </si>
+  <si>
+    <t>United Nations Environment Programme, International Resource Panel, Global Material Flows Database” or “UNEP IRP Global Material Flows Database</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/jiec.13593</t>
+  </si>
+  <si>
+    <t>https://www.resourcepanel.org/global-material-flows-database</t>
+  </si>
+  <si>
+    <t>Data not converted for iedc, can be downloaded from UNEP-IRP directly</t>
+  </si>
+  <si>
+    <t>ecomomy-wide data</t>
+  </si>
+  <si>
+    <t>11 major material groups</t>
+  </si>
+  <si>
+    <t>single country data</t>
+  </si>
+  <si>
+    <t>1970-2024</t>
+  </si>
+  <si>
+    <t>THE global single-country database for global primary material extraction, trade of primary materials and products, material use, and waste. Contains DE; DMC; DMI; IMP; EXP; MF; PTB; RME_IMP; RME_EXP;</t>
+  </si>
+  <si>
+    <t>Material flow accounting; UNEP-IRP material flow database; MFA; biomass; fossil fuels; metal ores; minerals; DE; DMC; DMI; IMP; EXP; MF; PTB; RME_IMP; RME_EXP;</t>
+  </si>
+  <si>
+    <t>Value(r,m,o,d,X,t)</t>
+  </si>
+  <si>
+    <t>Dry mass of domestic extraction (DE) from environment to industrial metabolism of biomass in Afghanistan in 2024 was 38628527 tons.</t>
+  </si>
+  <si>
+    <t>[Layer] of [data type] of [Aspect 5] of [Aspect 2] from [Aspect ] to [Aspect 4] in [Aspect 1] in [Aspect 6] is [Value].</t>
+  </si>
+  <si>
+    <t>CIRCOMOD</t>
+  </si>
+  <si>
+    <t>https://circomod.eu/</t>
+  </si>
+  <si>
+    <t>CIRCOMOD = Circular Economy Modelling for Climate Change Mitigation</t>
+  </si>
+  <si>
+    <t>circular economy; materials; material cycles; MFA; CGE; IAM; resource efficiency</t>
+  </si>
+  <si>
+    <t>The current scenario models for policy pathways do not include circular economy options. CIRCOMOD will develop a new generation of models that will address this gap.</t>
+  </si>
+  <si>
+    <t>CIRCOMOD_scenario_drivers</t>
+  </si>
+  <si>
+    <t>CIRCOMOD project team</t>
+  </si>
+  <si>
+    <t>population, GDP, service demand etc. as exogenous input to scenario modelling</t>
+  </si>
+  <si>
+    <t>economic and physical</t>
+  </si>
+  <si>
+    <t>national to global level</t>
+  </si>
+  <si>
+    <t>population, economy</t>
+  </si>
+  <si>
+    <t>1970-2100</t>
+  </si>
+  <si>
+    <t>CIRCOMOD project input database of exogenous parameters to drive the different scenario models</t>
+  </si>
+  <si>
+    <t>Data will be available on Zenodo as of 2026</t>
+  </si>
+  <si>
+    <t>CIRCOMOD_technologies_strategies</t>
+  </si>
+  <si>
+    <t>CIRCOMOD_historic_data</t>
+  </si>
+  <si>
+    <t>CIRCOMOD_project_results</t>
+  </si>
+  <si>
+    <t>technology parameters, CE parameters, etc. as exogenous input to scenario modelling</t>
+  </si>
+  <si>
+    <t>manufacturing, use phase, waste management industries</t>
+  </si>
+  <si>
+    <t>all major end-use sectors</t>
+  </si>
+  <si>
+    <t>climate-relevant materials concrete, steel, plastics, wood, aluminium, and copper</t>
+  </si>
+  <si>
+    <t>2000-2060</t>
+  </si>
+  <si>
+    <t>CIRCOMOD project input database of technology parameters, CE parameters, etc. to describe manufacturing, use phase, waste management industries, as exogenous input to scenario modelling</t>
+  </si>
+  <si>
+    <t>population, GDP, service demand, technology parameters etc. as exogenous input to scenario modelling</t>
+  </si>
+  <si>
+    <t>population, economy, technology</t>
+  </si>
+  <si>
+    <t>CIRCOMOD historic information database of exogenous parameters to calibrate the different scenario models</t>
+  </si>
+  <si>
+    <t>2020-2100</t>
+  </si>
+  <si>
+    <t>Material stocks and demand, recycling, GVA, labour, GHG, CED, RMI, land use, water use, as result of scenario modelling</t>
+  </si>
+  <si>
+    <t>material cycles, economy, env. pressure indicators</t>
+  </si>
+  <si>
+    <t>CIRCOMOD result database of material stocks and demand, recycling, GVA, labour, GHG, CED, RMI, land use, water use, as result of scenario modelling of the different scenario models</t>
+  </si>
+  <si>
+    <t>CIRCOMOD_CE_profile_data</t>
+  </si>
+  <si>
+    <t>Material production, GHG by sector, waste statistics, etc.</t>
+  </si>
+  <si>
+    <t>ca. 2020</t>
+  </si>
+  <si>
+    <t>CIRCOMOD CE profile data for the status quo in different end-use sectors, materials, and regions: Material production, GHG by sector, waste statistics, etc.</t>
+  </si>
+  <si>
+    <t>SOUVERAEN</t>
+  </si>
+  <si>
+    <t>Tbd.</t>
+  </si>
+  <si>
+    <t>energy transition; materials; critical materials; EU; supply chains</t>
+  </si>
+  <si>
+    <t>SOUVERAEN is a joint project of Fraunhofer ISE, Uni Bayreuth, and Uni Freiburg</t>
+  </si>
+  <si>
+    <t>SOUVERÄN: Sovereign and sustainable supply chains for key energy transition technologies in the EU</t>
+  </si>
+  <si>
+    <t>SOUVERAEN_Database</t>
+  </si>
+  <si>
+    <t>SOUVERAEN project team</t>
+  </si>
+  <si>
+    <t>Data will be available on Zenodo as of 2027</t>
+  </si>
+  <si>
+    <t>SOUVERAEN datase on energy transition technologies; material demand; critical materials; EU supply chains; CE potentials</t>
+  </si>
+  <si>
+    <t>2020-2060</t>
+  </si>
+  <si>
+    <t>single country level</t>
+  </si>
+  <si>
+    <t>stocks, flows, intensive, and extensive properties</t>
+  </si>
+  <si>
+    <t>production and trade flows, production and installed capacity, material composition, unit process inventories, criticality metrics</t>
+  </si>
+  <si>
+    <t>major technology and critical materials</t>
+  </si>
+  <si>
+    <t>four energy conversion technologies</t>
+  </si>
+  <si>
+    <t>PV, wind turbines, batteries, and electrolysers</t>
+  </si>
+  <si>
+    <t>major processes in global supply chains and in the EU use phase and waste management industries</t>
   </si>
 </sst>
 </file>
@@ -6726,7 +6933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -7021,6 +7228,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7087,6 +7296,11 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -7374,10 +7588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I32"/>
+  <dimension ref="B2:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -7389,14 +7603,14 @@
     <col min="8" max="8" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>186</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B3" s="32"/>
       <c r="C3" s="31" t="s">
         <v>181</v>
@@ -7419,9 +7633,15 @@
       <c r="I3" s="39" t="s">
         <v>1503</v>
       </c>
+      <c r="J3" s="39" t="s">
+        <v>2126</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>2160</v>
+      </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B4" s="183" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B4" s="185" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -7445,9 +7665,15 @@
       <c r="I4" s="57">
         <v>5</v>
       </c>
+      <c r="J4" s="141">
+        <v>6</v>
+      </c>
+      <c r="K4" s="141">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B5" s="183"/>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B5" s="185"/>
       <c r="C5" s="26" t="s">
         <v>422</v>
       </c>
@@ -7469,9 +7695,15 @@
       <c r="I5" s="119" t="s">
         <v>1505</v>
       </c>
+      <c r="J5" s="118" t="s">
+        <v>2126</v>
+      </c>
+      <c r="K5" s="118" t="s">
+        <v>2160</v>
+      </c>
     </row>
-    <row r="6" spans="2:9" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="184" t="s">
+    <row r="6" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="186" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -7483,9 +7715,11 @@
       <c r="G6" s="52"/>
       <c r="H6" s="52"/>
       <c r="I6" s="52"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B7" s="184"/>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B7" s="186"/>
       <c r="C7" s="26" t="s">
         <v>424</v>
       </c>
@@ -7495,9 +7729,11 @@
       <c r="G7" s="52"/>
       <c r="H7" s="52"/>
       <c r="I7" s="52"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B8" s="184"/>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B8" s="186"/>
       <c r="C8" s="26" t="s">
         <v>425</v>
       </c>
@@ -7507,9 +7743,11 @@
       <c r="G8" s="52"/>
       <c r="H8" s="52"/>
       <c r="I8" s="52"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B9" s="184"/>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B9" s="186"/>
       <c r="C9" s="28" t="s">
         <v>426</v>
       </c>
@@ -7519,9 +7757,11 @@
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
       <c r="I9" s="52"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B10" s="184"/>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B10" s="186"/>
       <c r="C10" s="27" t="s">
         <v>427</v>
       </c>
@@ -7531,9 +7771,11 @@
       <c r="G10" s="52"/>
       <c r="H10" s="52"/>
       <c r="I10" s="52"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B11" s="184"/>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B11" s="186"/>
       <c r="C11" s="27" t="s">
         <v>428</v>
       </c>
@@ -7543,9 +7785,11 @@
       <c r="G11" s="52"/>
       <c r="H11" s="52"/>
       <c r="I11" s="52"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="121"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B12" s="184"/>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B12" s="186"/>
       <c r="C12" s="27" t="s">
         <v>429</v>
       </c>
@@ -7555,9 +7799,11 @@
       <c r="G12" s="52"/>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B13" s="184"/>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B13" s="186"/>
       <c r="C13" s="27" t="s">
         <v>430</v>
       </c>
@@ -7567,9 +7813,11 @@
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
       <c r="I13" s="52"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B14" s="184"/>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B14" s="186"/>
       <c r="C14" s="27" t="s">
         <v>431</v>
       </c>
@@ -7579,9 +7827,11 @@
       <c r="G14" s="52"/>
       <c r="H14" s="52"/>
       <c r="I14" s="52"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B15" s="184"/>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B15" s="186"/>
       <c r="C15" s="27" t="s">
         <v>432</v>
       </c>
@@ -7591,9 +7841,11 @@
       <c r="G15" s="52"/>
       <c r="H15" s="52"/>
       <c r="I15" s="52"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="121"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B16" s="184"/>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B16" s="186"/>
       <c r="C16" s="27" t="s">
         <v>433</v>
       </c>
@@ -7603,9 +7855,11 @@
       <c r="G16" s="52"/>
       <c r="H16" s="52"/>
       <c r="I16" s="52"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="184"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B17" s="186"/>
       <c r="C17" s="27" t="s">
         <v>434</v>
       </c>
@@ -7615,9 +7869,11 @@
       <c r="G17" s="52"/>
       <c r="H17" s="52"/>
       <c r="I17" s="52"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="184"/>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B18" s="186"/>
       <c r="C18" s="27" t="s">
         <v>435</v>
       </c>
@@ -7627,9 +7883,11 @@
       <c r="G18" s="52"/>
       <c r="H18" s="52"/>
       <c r="I18" s="52"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="121"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="185" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B19" s="187" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -7649,9 +7907,15 @@
       <c r="I19" s="119" t="s">
         <v>1504</v>
       </c>
+      <c r="J19" s="118" t="s">
+        <v>2130</v>
+      </c>
+      <c r="K19" s="118" t="s">
+        <v>2164</v>
+      </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="185"/>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B20" s="187"/>
       <c r="C20" s="27" t="s">
         <v>437</v>
       </c>
@@ -7673,9 +7937,15 @@
       <c r="I20" s="119" t="s">
         <v>1508</v>
       </c>
+      <c r="J20" s="118" t="s">
+        <v>2129</v>
+      </c>
+      <c r="K20" s="118" t="s">
+        <v>2162</v>
+      </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="185"/>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B21" s="187"/>
       <c r="C21" s="27" t="s">
         <v>438</v>
       </c>
@@ -7693,9 +7963,15 @@
       <c r="I21" s="119" t="s">
         <v>1507</v>
       </c>
+      <c r="J21" s="118" t="s">
+        <v>2128</v>
+      </c>
+      <c r="K21" s="118" t="s">
+        <v>2163</v>
+      </c>
     </row>
-    <row r="22" spans="2:9" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="186" t="s">
+    <row r="22" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="188" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -7717,9 +7993,15 @@
       <c r="I22" s="119" t="s">
         <v>861</v>
       </c>
+      <c r="J22" s="121" t="s">
+        <v>860</v>
+      </c>
+      <c r="K22" s="121" t="s">
+        <v>860</v>
+      </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="186"/>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B23" s="188"/>
       <c r="C23" s="26" t="s">
         <v>440</v>
       </c>
@@ -7729,9 +8011,11 @@
       <c r="G23" s="52"/>
       <c r="H23" s="52"/>
       <c r="I23" s="52"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="121"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="186"/>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B24" s="188"/>
       <c r="C24" s="25" t="s">
         <v>441</v>
       </c>
@@ -7741,9 +8025,11 @@
       <c r="G24" s="52"/>
       <c r="H24" s="52"/>
       <c r="I24" s="52"/>
+      <c r="J24" s="121"/>
+      <c r="K24" s="121"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B25" s="186"/>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B25" s="188"/>
       <c r="C25" s="25" t="s">
         <v>443</v>
       </c>
@@ -7761,9 +8047,15 @@
       <c r="I25" s="90" t="s">
         <v>1506</v>
       </c>
+      <c r="J25" s="171" t="s">
+        <v>2127</v>
+      </c>
+      <c r="K25" s="171" t="s">
+        <v>2161</v>
+      </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B26" s="186"/>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B26" s="188"/>
       <c r="C26" s="25" t="s">
         <v>444</v>
       </c>
@@ -7775,9 +8067,11 @@
       <c r="G26" s="52"/>
       <c r="H26" s="52"/>
       <c r="I26" s="52"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="121"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B27" s="186"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B27" s="188"/>
       <c r="C27" s="25" t="s">
         <v>445</v>
       </c>
@@ -7787,9 +8081,11 @@
       <c r="G27" s="52"/>
       <c r="H27" s="52"/>
       <c r="I27" s="52"/>
+      <c r="J27" s="121"/>
+      <c r="K27" s="121"/>
     </row>
-    <row r="28" spans="2:9" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="187" t="s">
+    <row r="28" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="189" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -7813,9 +8109,15 @@
       <c r="I28" s="123">
         <v>45144</v>
       </c>
+      <c r="J28" s="204">
+        <v>45704</v>
+      </c>
+      <c r="K28" s="204">
+        <v>45705</v>
+      </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B29" s="187"/>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B29" s="189"/>
       <c r="C29" s="25" t="s">
         <v>447</v>
       </c>
@@ -7837,9 +8139,15 @@
       <c r="I29" s="124" t="s">
         <v>30</v>
       </c>
+      <c r="J29" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="125" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B30" s="180" t="s">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B30" s="182" t="s">
         <v>185</v>
       </c>
       <c r="C30" s="107" t="s">
@@ -7851,9 +8159,11 @@
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
+      <c r="J30" s="205"/>
+      <c r="K30" s="205"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B31" s="181"/>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B31" s="183"/>
       <c r="C31" s="108" t="s">
         <v>449</v>
       </c>
@@ -7863,9 +8173,11 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
+      <c r="J31" s="165"/>
+      <c r="K31" s="165"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B32" s="182"/>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B32" s="184"/>
       <c r="C32" s="109" t="s">
         <v>450</v>
       </c>
@@ -7875,6 +8187,8 @@
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
+      <c r="J32" s="167"/>
+      <c r="K32" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7891,13 +8205,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:V39"/>
+  <dimension ref="B2:AB39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -7919,16 +8233,17 @@
     <col min="20" max="20" width="34.5546875" customWidth="1"/>
     <col min="21" max="21" width="52.6640625" customWidth="1"/>
     <col min="22" max="22" width="40.71875" customWidth="1"/>
+    <col min="23" max="23" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B3" s="32"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -7990,9 +8305,27 @@
       <c r="V3" s="82" t="s">
         <v>1994</v>
       </c>
+      <c r="W3" s="82" t="s">
+        <v>2131</v>
+      </c>
+      <c r="X3" s="82" t="s">
+        <v>2140</v>
+      </c>
+      <c r="Y3" s="82" t="s">
+        <v>2141</v>
+      </c>
+      <c r="Z3" s="82" t="s">
+        <v>2156</v>
+      </c>
+      <c r="AA3" s="82" t="s">
+        <v>2142</v>
+      </c>
+      <c r="AB3" s="82" t="s">
+        <v>2165</v>
+      </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B4" s="188" t="s">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B4" s="190" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -8055,9 +8388,27 @@
       <c r="V4" s="141">
         <v>18</v>
       </c>
+      <c r="W4" s="141">
+        <v>19</v>
+      </c>
+      <c r="X4" s="141">
+        <v>20</v>
+      </c>
+      <c r="Y4" s="141">
+        <v>21</v>
+      </c>
+      <c r="Z4" s="141">
+        <v>22</v>
+      </c>
+      <c r="AA4" s="141">
+        <v>23</v>
+      </c>
+      <c r="AB4" s="141">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B5" s="189"/>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B5" s="191"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
       </c>
@@ -8118,8 +8469,26 @@
       <c r="V5" s="165" t="s">
         <v>1994</v>
       </c>
+      <c r="W5" s="165" t="s">
+        <v>2131</v>
+      </c>
+      <c r="X5" s="165" t="s">
+        <v>2140</v>
+      </c>
+      <c r="Y5" s="165" t="s">
+        <v>2141</v>
+      </c>
+      <c r="Z5" s="165" t="s">
+        <v>2156</v>
+      </c>
+      <c r="AA5" s="165" t="s">
+        <v>2142</v>
+      </c>
+      <c r="AB5" s="165" t="s">
+        <v>2165</v>
+      </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B6" s="33"/>
       <c r="C6" s="54" t="s">
         <v>453</v>
@@ -8179,8 +8548,26 @@
       <c r="V6" s="165" t="s">
         <v>2018</v>
       </c>
+      <c r="W6" s="165" t="s">
+        <v>2018</v>
+      </c>
+      <c r="X6" s="165" t="s">
+        <v>2018</v>
+      </c>
+      <c r="Y6" s="165" t="s">
+        <v>2018</v>
+      </c>
+      <c r="Z6" s="165" t="s">
+        <v>2018</v>
+      </c>
+      <c r="AA6" s="165" t="s">
+        <v>2018</v>
+      </c>
+      <c r="AB6" s="165" t="s">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
@@ -8242,9 +8629,27 @@
       <c r="V7" s="23" t="s">
         <v>11</v>
       </c>
+      <c r="W7" s="23" t="s">
+        <v>2126</v>
+      </c>
+      <c r="X7" s="23" t="s">
+        <v>2126</v>
+      </c>
+      <c r="Y7" s="23" t="s">
+        <v>2126</v>
+      </c>
+      <c r="Z7" s="23" t="s">
+        <v>2126</v>
+      </c>
+      <c r="AA7" s="23" t="s">
+        <v>2126</v>
+      </c>
+      <c r="AB7" s="165" t="s">
+        <v>2160</v>
+      </c>
     </row>
-    <row r="8" spans="2:22" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="184" t="s">
+    <row r="8" spans="2:28" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="186" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="54" t="s">
@@ -8305,9 +8710,27 @@
       <c r="V8" s="165" t="s">
         <v>1995</v>
       </c>
+      <c r="W8" s="165" t="s">
+        <v>2133</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>2143</v>
+      </c>
+      <c r="Y8" s="23" t="s">
+        <v>2149</v>
+      </c>
+      <c r="Z8" s="23" t="s">
+        <v>2157</v>
+      </c>
+      <c r="AA8" s="23" t="s">
+        <v>2153</v>
+      </c>
+      <c r="AB8" s="23" t="s">
+        <v>2171</v>
+      </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B9" s="184"/>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B9" s="186"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
       </c>
@@ -8366,9 +8789,27 @@
       <c r="V9" s="165" t="s">
         <v>1996</v>
       </c>
+      <c r="W9" s="165" t="s">
+        <v>2133</v>
+      </c>
+      <c r="X9" s="23" t="s">
+        <v>2143</v>
+      </c>
+      <c r="Y9" s="23" t="s">
+        <v>2149</v>
+      </c>
+      <c r="Z9" s="23" t="s">
+        <v>2157</v>
+      </c>
+      <c r="AA9" s="23" t="s">
+        <v>2153</v>
+      </c>
+      <c r="AB9" s="23" t="s">
+        <v>2172</v>
+      </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B10" s="184"/>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B10" s="186"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
       </c>
@@ -8427,9 +8868,27 @@
       <c r="V10" s="165" t="s">
         <v>199</v>
       </c>
+      <c r="W10" s="165" t="s">
+        <v>2134</v>
+      </c>
+      <c r="X10" s="165" t="s">
+        <v>2134</v>
+      </c>
+      <c r="Y10" s="165" t="s">
+        <v>2134</v>
+      </c>
+      <c r="Z10" s="165" t="s">
+        <v>2134</v>
+      </c>
+      <c r="AA10" s="165" t="s">
+        <v>2134</v>
+      </c>
+      <c r="AB10" s="165" t="s">
+        <v>2134</v>
+      </c>
     </row>
-    <row r="11" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="184"/>
+    <row r="11" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B11" s="186"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
       </c>
@@ -8488,9 +8947,27 @@
       <c r="V11" s="165" t="s">
         <v>1997</v>
       </c>
+      <c r="W11" s="165" t="s">
+        <v>2136</v>
+      </c>
+      <c r="X11" s="23" t="s">
+        <v>2144</v>
+      </c>
+      <c r="Y11" s="23" t="s">
+        <v>2150</v>
+      </c>
+      <c r="Z11" s="23" t="s">
+        <v>2154</v>
+      </c>
+      <c r="AA11" s="23" t="s">
+        <v>2154</v>
+      </c>
+      <c r="AB11" s="23" t="s">
+        <v>2154</v>
+      </c>
     </row>
-    <row r="12" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="184"/>
+    <row r="12" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B12" s="186"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -8549,9 +9026,27 @@
       <c r="V12" s="165" t="s">
         <v>1998</v>
       </c>
+      <c r="W12" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="X12" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="Y12" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="Z12" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="AA12" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="AB12" s="165" t="s">
+        <v>2176</v>
+      </c>
     </row>
-    <row r="13" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="184"/>
+    <row r="13" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B13" s="186"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -8610,9 +9105,27 @@
       <c r="V13" s="165" t="s">
         <v>11</v>
       </c>
+      <c r="W13" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="Y13" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="Z13" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="AB13" s="23" t="s">
+        <v>2174</v>
+      </c>
     </row>
-    <row r="14" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="184"/>
+    <row r="14" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B14" s="186"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -8671,9 +9184,27 @@
       <c r="V14" s="165" t="s">
         <v>11</v>
       </c>
+      <c r="W14" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="X14" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="Y14" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="Z14" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="AA14" s="23" t="s">
+        <v>2145</v>
+      </c>
+      <c r="AB14" s="23" t="s">
+        <v>2175</v>
+      </c>
     </row>
-    <row r="15" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="184"/>
+    <row r="15" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B15" s="186"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -8732,9 +9263,27 @@
       <c r="V15" s="165" t="s">
         <v>1679</v>
       </c>
+      <c r="W15" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="X15" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="Y15" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="Z15" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="AA15" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="AB15" s="23" t="s">
+        <v>2173</v>
+      </c>
     </row>
-    <row r="16" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="184"/>
+    <row r="16" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B16" s="186"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -8793,9 +9342,27 @@
       <c r="V16" s="165" t="s">
         <v>1999</v>
       </c>
+      <c r="W16" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="X16" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="Y16" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="Z16" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="AA16" s="23" t="s">
+        <v>2146</v>
+      </c>
+      <c r="AB16" s="23" t="s">
+        <v>2173</v>
+      </c>
     </row>
-    <row r="17" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="184"/>
+    <row r="17" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B17" s="186"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -8854,9 +9421,27 @@
       <c r="V17" s="165" t="s">
         <v>19</v>
       </c>
+      <c r="W17" s="165" t="s">
+        <v>819</v>
+      </c>
+      <c r="X17" s="165" t="s">
+        <v>819</v>
+      </c>
+      <c r="Y17" s="165" t="s">
+        <v>819</v>
+      </c>
+      <c r="Z17" s="165" t="s">
+        <v>819</v>
+      </c>
+      <c r="AA17" s="165" t="s">
+        <v>819</v>
+      </c>
+      <c r="AB17" s="165" t="s">
+        <v>1422</v>
+      </c>
     </row>
-    <row r="18" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="184"/>
+    <row r="18" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B18" s="186"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -8915,9 +9500,27 @@
       <c r="V18" s="165" t="s">
         <v>2000</v>
       </c>
+      <c r="W18" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="X18" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="Y18" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="Z18" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="AA18" s="165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="AB18" s="165" t="s">
+        <v>2170</v>
+      </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B19" s="184"/>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B19" s="186"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -8976,9 +9579,27 @@
       <c r="V19" s="165" t="s">
         <v>2001</v>
       </c>
+      <c r="W19" s="165" t="s">
+        <v>2137</v>
+      </c>
+      <c r="X19" s="23" t="s">
+        <v>2147</v>
+      </c>
+      <c r="Y19" s="23" t="s">
+        <v>1410</v>
+      </c>
+      <c r="Z19" s="23" t="s">
+        <v>2158</v>
+      </c>
+      <c r="AA19" s="23" t="s">
+        <v>2152</v>
+      </c>
+      <c r="AB19" s="23" t="s">
+        <v>2169</v>
+      </c>
     </row>
-    <row r="20" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="184"/>
+    <row r="20" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B20" s="186"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -9037,9 +9658,27 @@
       <c r="V20" s="165" t="s">
         <v>1278</v>
       </c>
+      <c r="W20" s="165" t="s">
+        <v>1278</v>
+      </c>
+      <c r="X20" s="165" t="s">
+        <v>1278</v>
+      </c>
+      <c r="Y20" s="165" t="s">
+        <v>1278</v>
+      </c>
+      <c r="Z20" s="165" t="s">
+        <v>1278</v>
+      </c>
+      <c r="AA20" s="165" t="s">
+        <v>1278</v>
+      </c>
+      <c r="AB20" s="165" t="s">
+        <v>1278</v>
+      </c>
     </row>
-    <row r="21" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="185" t="s">
+    <row r="21" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B21" s="187" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -9100,9 +9739,27 @@
       <c r="V21" s="165" t="s">
         <v>2002</v>
       </c>
+      <c r="W21" s="165" t="s">
+        <v>2138</v>
+      </c>
+      <c r="X21" s="23" t="s">
+        <v>2148</v>
+      </c>
+      <c r="Y21" s="23" t="s">
+        <v>2151</v>
+      </c>
+      <c r="Z21" s="206" t="s">
+        <v>2159</v>
+      </c>
+      <c r="AA21" s="23" t="s">
+        <v>2155</v>
+      </c>
+      <c r="AB21" s="23" t="s">
+        <v>2168</v>
+      </c>
     </row>
-    <row r="22" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="185"/>
+    <row r="22" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B22" s="187"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -9163,9 +9820,27 @@
       <c r="V22" s="165" t="s">
         <v>2003</v>
       </c>
+      <c r="W22" s="165" t="s">
+        <v>2126</v>
+      </c>
+      <c r="X22" s="165" t="s">
+        <v>2126</v>
+      </c>
+      <c r="Y22" s="165" t="s">
+        <v>2126</v>
+      </c>
+      <c r="Z22" s="165" t="s">
+        <v>2126</v>
+      </c>
+      <c r="AA22" s="165" t="s">
+        <v>2126</v>
+      </c>
+      <c r="AB22" s="165" t="s">
+        <v>2160</v>
+      </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B23" s="185"/>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B23" s="187"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
       </c>
@@ -9224,9 +9899,27 @@
       <c r="V23" s="165" t="s">
         <v>2004</v>
       </c>
+      <c r="W23" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="X23" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y23" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z23" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA23" s="165" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB23" s="165" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="24" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="185"/>
+    <row r="24" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B24" s="187"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
       </c>
@@ -9285,9 +9978,27 @@
       <c r="V24" s="165" t="s">
         <v>2008</v>
       </c>
+      <c r="W24" s="165" t="s">
+        <v>2139</v>
+      </c>
+      <c r="X24" s="165" t="s">
+        <v>2139</v>
+      </c>
+      <c r="Y24" s="165" t="s">
+        <v>2139</v>
+      </c>
+      <c r="Z24" s="165" t="s">
+        <v>2139</v>
+      </c>
+      <c r="AA24" s="165" t="s">
+        <v>2139</v>
+      </c>
+      <c r="AB24" s="165" t="s">
+        <v>2167</v>
+      </c>
     </row>
-    <row r="25" spans="2:22" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="186" t="s">
+    <row r="25" spans="2:28" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="188" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -9348,9 +10059,27 @@
       <c r="V25" s="23" t="s">
         <v>860</v>
       </c>
+      <c r="W25" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="X25" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="Y25" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="Z25" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="AA25" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="AB25" s="23" t="s">
+        <v>860</v>
+      </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B26" s="186"/>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B26" s="188"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
       </c>
@@ -9406,12 +10135,30 @@
       <c r="U26" s="165" t="s">
         <v>1551</v>
       </c>
-      <c r="V26" s="37" t="s">
+      <c r="V26" s="165" t="s">
         <v>857</v>
       </c>
+      <c r="W26" s="165" t="s">
+        <v>857</v>
+      </c>
+      <c r="X26" s="165" t="s">
+        <v>857</v>
+      </c>
+      <c r="Y26" s="165" t="s">
+        <v>857</v>
+      </c>
+      <c r="Z26" s="165" t="s">
+        <v>857</v>
+      </c>
+      <c r="AA26" s="165" t="s">
+        <v>857</v>
+      </c>
+      <c r="AB26" s="165" t="s">
+        <v>857</v>
+      </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B27" s="186"/>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B27" s="188"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
       </c>
@@ -9470,9 +10217,27 @@
       <c r="V27" s="165" t="s">
         <v>1315</v>
       </c>
+      <c r="W27" s="165" t="s">
+        <v>2132</v>
+      </c>
+      <c r="X27" s="165" t="s">
+        <v>2132</v>
+      </c>
+      <c r="Y27" s="165" t="s">
+        <v>2132</v>
+      </c>
+      <c r="Z27" s="165" t="s">
+        <v>2132</v>
+      </c>
+      <c r="AA27" s="165" t="s">
+        <v>2132</v>
+      </c>
+      <c r="AB27" s="165" t="s">
+        <v>2166</v>
+      </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B28" s="186"/>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B28" s="188"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
       </c>
@@ -9528,12 +10293,30 @@
       <c r="U28" s="47" t="s">
         <v>1547</v>
       </c>
-      <c r="V28" s="153" t="s">
+      <c r="V28" s="181" t="s">
         <v>2007</v>
       </c>
+      <c r="W28" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="X28" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Y28" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Z28" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="AA28" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="AB28" s="181" t="s">
+        <v>2161</v>
+      </c>
     </row>
-    <row r="29" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="186"/>
+    <row r="29" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B29" s="188"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
       </c>
@@ -9589,12 +10372,30 @@
       <c r="U29" s="47" t="s">
         <v>1547</v>
       </c>
-      <c r="V29" s="153" t="s">
+      <c r="V29" s="181" t="s">
         <v>2006</v>
       </c>
+      <c r="W29" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="X29" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Y29" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Z29" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="AA29" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="AB29" s="181" t="s">
+        <v>2161</v>
+      </c>
     </row>
-    <row r="30" spans="2:22" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="186"/>
+    <row r="30" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="B30" s="188"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
       </c>
@@ -9650,12 +10451,30 @@
       <c r="U30" s="47" t="s">
         <v>1547</v>
       </c>
-      <c r="V30" s="153" t="s">
+      <c r="V30" s="181" t="s">
         <v>2006</v>
       </c>
+      <c r="W30" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="X30" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Y30" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Z30" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="AA30" s="181" t="s">
+        <v>2127</v>
+      </c>
+      <c r="AB30" s="181" t="s">
+        <v>2161</v>
+      </c>
     </row>
-    <row r="31" spans="2:22" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="187" t="s">
+    <row r="31" spans="2:28" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="189" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -9718,9 +10537,27 @@
       <c r="V31" s="162">
         <v>45611</v>
       </c>
+      <c r="W31" s="162">
+        <v>45704</v>
+      </c>
+      <c r="X31" s="162">
+        <v>45704</v>
+      </c>
+      <c r="Y31" s="162">
+        <v>45704</v>
+      </c>
+      <c r="Z31" s="162">
+        <v>45704</v>
+      </c>
+      <c r="AA31" s="162">
+        <v>45704</v>
+      </c>
+      <c r="AB31" s="162">
+        <v>45705</v>
+      </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B32" s="190"/>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B32" s="192"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
       </c>
@@ -9781,9 +10618,27 @@
       <c r="V32" s="165" t="s">
         <v>30</v>
       </c>
+      <c r="W32" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="X32" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y32" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z32" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA32" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB32" s="165" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B33" s="180" t="s">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B33" s="182" t="s">
         <v>185</v>
       </c>
       <c r="C33" s="83" t="s">
@@ -9808,9 +10663,15 @@
       <c r="T33" s="165"/>
       <c r="U33" s="165"/>
       <c r="V33" s="165"/>
+      <c r="W33" s="165"/>
+      <c r="X33" s="165"/>
+      <c r="Y33" s="165"/>
+      <c r="Z33" s="165"/>
+      <c r="AA33" s="165"/>
+      <c r="AB33" s="165"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B34" s="181"/>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B34" s="183"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
       </c>
@@ -9833,9 +10694,15 @@
       <c r="T34" s="165"/>
       <c r="U34" s="165"/>
       <c r="V34" s="165"/>
+      <c r="W34" s="165"/>
+      <c r="X34" s="165"/>
+      <c r="Y34" s="165"/>
+      <c r="Z34" s="165"/>
+      <c r="AA34" s="165"/>
+      <c r="AB34" s="165"/>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B35" s="182"/>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="B35" s="184"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
       </c>
@@ -9858,8 +10725,17 @@
       <c r="T35" s="167"/>
       <c r="U35" s="167"/>
       <c r="V35" s="167"/>
+      <c r="W35" s="167"/>
+      <c r="X35" s="167"/>
+      <c r="Y35" s="167"/>
+      <c r="Z35" s="167"/>
+      <c r="AA35" s="167"/>
+      <c r="AB35" s="167"/>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="W36" s="105"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.4">
       <c r="I39" s="12"/>
     </row>
   </sheetData>
@@ -9875,6 +10751,7 @@
     <hyperlink ref="G28" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9882,11 +10759,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:EO74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="DJ39" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="DP6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="EE2" sqref="EE2"/>
+      <selection pane="bottomRight" activeCell="DW2" sqref="DW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -9947,7 +10824,7 @@
     <col min="70" max="16384" width="11.5546875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:126" x14ac:dyDescent="0.4">
       <c r="C1" s="73" t="s">
         <v>269</v>
       </c>
@@ -10314,8 +11191,11 @@
       <c r="DU1" s="155" t="s">
         <v>1989</v>
       </c>
+      <c r="DV1" s="180" t="s">
+        <v>2108</v>
+      </c>
     </row>
-    <row r="2" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B2" s="34" t="s">
         <v>183</v>
       </c>
@@ -10506,8 +11386,11 @@
       <c r="DU2" s="176" t="s">
         <v>1967</v>
       </c>
+      <c r="DV2" s="180" t="s">
+        <v>1967</v>
+      </c>
     </row>
-    <row r="3" spans="1:125" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:126" x14ac:dyDescent="0.4">
       <c r="B3" s="58"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -10760,11 +11643,11 @@
       <c r="DS3" s="105"/>
       <c r="DT3" s="105"/>
     </row>
-    <row r="4" spans="1:125" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:126" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>1</v>
       </c>
-      <c r="B4" s="193" t="s">
+      <c r="B4" s="195" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -11018,11 +11901,11 @@
       <c r="DS4" s="105"/>
       <c r="DT4" s="105"/>
     </row>
-    <row r="5" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="194"/>
+      <c r="B5" s="196"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -11392,8 +12275,11 @@
       <c r="DU5" s="41" t="s">
         <v>2092</v>
       </c>
+      <c r="DV5" s="105" t="s">
+        <v>2109</v>
+      </c>
     </row>
-    <row r="6" spans="1:125" ht="14.1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:126" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A6" s="92">
         <v>3</v>
       </c>
@@ -11765,12 +12651,15 @@
       <c r="DU6" s="41" t="s">
         <v>2093</v>
       </c>
+      <c r="DV6" s="105" t="s">
+        <v>2110</v>
+      </c>
     </row>
-    <row r="7" spans="1:125" ht="14.1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:126" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A7" s="92">
         <v>4</v>
       </c>
-      <c r="B7" s="195" t="s">
+      <c r="B7" s="197" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -12140,12 +13029,15 @@
       <c r="DU7" s="41" t="s">
         <v>845</v>
       </c>
+      <c r="DV7" s="105" t="s">
+        <v>845</v>
+      </c>
     </row>
-    <row r="8" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A8" s="92">
         <v>5</v>
       </c>
-      <c r="B8" s="195"/>
+      <c r="B8" s="197"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -12515,12 +13407,15 @@
       <c r="DU8" s="41">
         <v>3</v>
       </c>
+      <c r="DV8" s="105">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A9" s="92">
         <v>6</v>
       </c>
-      <c r="B9" s="195"/>
+      <c r="B9" s="197"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -12890,12 +13785,15 @@
       <c r="DU9" s="41" t="s">
         <v>846</v>
       </c>
+      <c r="DV9" s="172" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A10" s="92">
         <v>7</v>
       </c>
-      <c r="B10" s="195"/>
+      <c r="B10" s="197"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -13265,12 +14163,15 @@
       <c r="DU10" s="41" t="s">
         <v>151</v>
       </c>
+      <c r="DV10" s="172" t="s">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="11" spans="1:125" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:126" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="92">
         <v>8</v>
       </c>
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="198" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -13640,12 +14541,15 @@
       <c r="DU11" s="41" t="s">
         <v>32</v>
       </c>
+      <c r="DV11" s="172" t="s">
+        <v>2117</v>
+      </c>
     </row>
-    <row r="12" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="92">
         <v>9</v>
       </c>
-      <c r="B12" s="197"/>
+      <c r="B12" s="199"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -14013,12 +14917,15 @@
       <c r="DU12" s="41" t="s">
         <v>152</v>
       </c>
+      <c r="DV12" s="172" t="s">
+        <v>779</v>
+      </c>
     </row>
-    <row r="13" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="92">
         <v>10</v>
       </c>
-      <c r="B13" s="197"/>
+      <c r="B13" s="199"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -14386,12 +15293,15 @@
       <c r="DU13" s="41" t="s">
         <v>2094</v>
       </c>
+      <c r="DV13" s="172" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="14" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="92">
         <v>11</v>
       </c>
-      <c r="B14" s="197"/>
+      <c r="B14" s="199"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -14759,12 +15669,15 @@
       <c r="DU14" s="41" t="s">
         <v>2095</v>
       </c>
+      <c r="DV14" s="172" t="s">
+        <v>1392</v>
+      </c>
     </row>
-    <row r="15" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="92">
         <v>12</v>
       </c>
-      <c r="B15" s="197"/>
+      <c r="B15" s="199"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -15132,12 +16045,15 @@
       <c r="DU15" s="41" t="s">
         <v>347</v>
       </c>
+      <c r="DV15" s="172" t="s">
+        <v>1679</v>
+      </c>
     </row>
-    <row r="16" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="92">
         <v>13</v>
       </c>
-      <c r="B16" s="197"/>
+      <c r="B16" s="199"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -15505,12 +16421,15 @@
       <c r="DU16" s="41" t="s">
         <v>508</v>
       </c>
+      <c r="DV16" s="172" t="s">
+        <v>2118</v>
+      </c>
     </row>
-    <row r="17" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="92">
         <v>14</v>
       </c>
-      <c r="B17" s="197"/>
+      <c r="B17" s="199"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -15878,12 +16797,15 @@
       <c r="DU17" s="41" t="s">
         <v>156</v>
       </c>
+      <c r="DV17" s="176" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="92">
         <v>15</v>
       </c>
-      <c r="B18" s="197"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -16251,12 +17173,15 @@
       <c r="DU18" s="41" t="s">
         <v>2096</v>
       </c>
+      <c r="DV18" s="172" t="s">
+        <v>2119</v>
+      </c>
     </row>
-    <row r="19" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="92">
         <v>16</v>
       </c>
-      <c r="B19" s="197"/>
+      <c r="B19" s="199"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -16624,12 +17549,15 @@
       <c r="DU19" s="41" t="s">
         <v>2097</v>
       </c>
+      <c r="DV19" s="172" t="s">
+        <v>2120</v>
+      </c>
     </row>
-    <row r="20" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="92">
         <v>17</v>
       </c>
-      <c r="B20" s="197"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -16997,12 +17925,15 @@
       <c r="DU20" s="41" t="s">
         <v>2098</v>
       </c>
+      <c r="DV20" s="172" t="s">
+        <v>2015</v>
+      </c>
     </row>
-    <row r="21" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="92">
         <v>18</v>
       </c>
-      <c r="B21" s="198" t="s">
+      <c r="B21" s="200" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -17366,12 +18297,15 @@
       <c r="DU21" s="41" t="s">
         <v>2099</v>
       </c>
+      <c r="DV21" s="172" t="s">
+        <v>2121</v>
+      </c>
     </row>
-    <row r="22" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="92">
         <v>19</v>
       </c>
-      <c r="B22" s="198"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -17741,12 +18675,15 @@
       <c r="DU22" s="41" t="s">
         <v>2100</v>
       </c>
+      <c r="DV22" s="172" t="s">
+        <v>2122</v>
+      </c>
     </row>
-    <row r="23" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A23" s="92">
         <v>20</v>
       </c>
-      <c r="B23" s="198"/>
+      <c r="B23" s="200"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -18116,12 +19053,15 @@
       <c r="DU23" s="41" t="s">
         <v>24</v>
       </c>
+      <c r="DV23" s="105" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="1:125" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:126" x14ac:dyDescent="0.4">
       <c r="A24" s="92">
         <v>21</v>
       </c>
-      <c r="B24" s="198"/>
+      <c r="B24" s="200"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -18491,12 +19431,15 @@
       <c r="DU24" s="41">
         <v>8130</v>
       </c>
+      <c r="DV24" s="105">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:125" ht="14.1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:126" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A25" s="92">
         <v>22</v>
       </c>
-      <c r="B25" s="198"/>
+      <c r="B25" s="200"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -18864,12 +19807,15 @@
       <c r="DU25" s="41" t="s">
         <v>11</v>
       </c>
+      <c r="DV25" s="105" t="s">
+        <v>2111</v>
+      </c>
     </row>
-    <row r="26" spans="1:125" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:126" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="92">
         <v>23</v>
       </c>
-      <c r="B26" s="199" t="s">
+      <c r="B26" s="201" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="64" t="s">
@@ -19241,12 +20187,15 @@
       <c r="DU26" s="68" t="s">
         <v>698</v>
       </c>
+      <c r="DV26" s="68" t="s">
+        <v>698</v>
+      </c>
     </row>
-    <row r="27" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A27" s="92">
         <v>24</v>
       </c>
-      <c r="B27" s="199"/>
+      <c r="B27" s="201"/>
       <c r="C27" s="64" t="s">
         <v>464</v>
       </c>
@@ -19616,12 +20565,15 @@
       <c r="DU27" s="68">
         <v>85</v>
       </c>
+      <c r="DV27" s="68">
+        <v>2</v>
+      </c>
     </row>
-    <row r="28" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A28" s="92">
         <v>25</v>
       </c>
-      <c r="B28" s="199"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="64" t="s">
         <v>465</v>
       </c>
@@ -19989,12 +20941,15 @@
       <c r="DU28" s="68" t="s">
         <v>851</v>
       </c>
+      <c r="DV28" s="68" t="s">
+        <v>1033</v>
+      </c>
     </row>
-    <row r="29" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A29" s="92">
         <v>26</v>
       </c>
-      <c r="B29" s="199"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="64" t="s">
         <v>466</v>
       </c>
@@ -20362,12 +21317,15 @@
       <c r="DU29" s="68">
         <v>13</v>
       </c>
+      <c r="DV29" s="68">
+        <v>72</v>
+      </c>
     </row>
-    <row r="30" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A30" s="92">
         <v>27</v>
       </c>
-      <c r="B30" s="199"/>
+      <c r="B30" s="201"/>
       <c r="C30" s="64" t="s">
         <v>467</v>
       </c>
@@ -20735,12 +21693,15 @@
       <c r="DU30" s="68" t="s">
         <v>696</v>
       </c>
+      <c r="DV30" s="68" t="s">
+        <v>699</v>
+      </c>
     </row>
-    <row r="31" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A31" s="92">
         <v>28</v>
       </c>
-      <c r="B31" s="199"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="64" t="s">
         <v>468</v>
       </c>
@@ -21108,12 +22069,15 @@
       <c r="DU31" s="68">
         <v>13</v>
       </c>
+      <c r="DV31" s="68">
+        <v>6</v>
+      </c>
     </row>
-    <row r="32" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A32" s="92">
         <v>29</v>
       </c>
-      <c r="B32" s="199"/>
+      <c r="B32" s="201"/>
       <c r="C32" s="64" t="s">
         <v>469</v>
       </c>
@@ -21481,12 +22445,15 @@
       <c r="DU32" s="68" t="s">
         <v>704</v>
       </c>
+      <c r="DV32" s="68" t="s">
+        <v>700</v>
+      </c>
     </row>
-    <row r="33" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A33" s="92">
         <v>30</v>
       </c>
-      <c r="B33" s="199"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="64" t="s">
         <v>470</v>
       </c>
@@ -21854,12 +22821,15 @@
       <c r="DU33" s="174">
         <v>14</v>
       </c>
+      <c r="DV33" s="68">
+        <v>6</v>
+      </c>
     </row>
-    <row r="34" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A34" s="92">
         <v>31</v>
       </c>
-      <c r="B34" s="199"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="64" t="s">
         <v>471</v>
       </c>
@@ -22227,12 +23197,15 @@
       <c r="DU34" s="68" t="s">
         <v>849</v>
       </c>
+      <c r="DV34" s="68" t="s">
+        <v>1467</v>
+      </c>
     </row>
-    <row r="35" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A35" s="92">
         <v>32</v>
       </c>
-      <c r="B35" s="199"/>
+      <c r="B35" s="201"/>
       <c r="C35" s="64" t="s">
         <v>472</v>
       </c>
@@ -22600,12 +23573,15 @@
       <c r="DU35" s="68">
         <v>4</v>
       </c>
+      <c r="DV35" s="68">
+        <v>79</v>
+      </c>
     </row>
-    <row r="36" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A36" s="92">
         <v>33</v>
       </c>
-      <c r="B36" s="199"/>
+      <c r="B36" s="201"/>
       <c r="C36" s="64" t="s">
         <v>473</v>
       </c>
@@ -22973,12 +23949,15 @@
       <c r="DU36" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV36" s="68" t="s">
+        <v>702</v>
+      </c>
     </row>
-    <row r="37" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A37" s="92">
         <v>34</v>
       </c>
-      <c r="B37" s="199"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="64" t="s">
         <v>474</v>
       </c>
@@ -23346,12 +24325,15 @@
       <c r="DU37" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV37" s="68">
+        <v>3</v>
+      </c>
     </row>
-    <row r="38" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A38" s="92">
         <v>35</v>
       </c>
-      <c r="B38" s="199"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="64" t="s">
         <v>475</v>
       </c>
@@ -23719,12 +24701,15 @@
       <c r="DU38" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV38" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="39" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A39" s="92">
         <v>36</v>
       </c>
-      <c r="B39" s="199"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="64" t="s">
         <v>476</v>
       </c>
@@ -24092,12 +25077,15 @@
       <c r="DU39" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV39" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="40" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A40" s="92">
         <v>37</v>
       </c>
-      <c r="B40" s="199"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="64" t="s">
         <v>477</v>
       </c>
@@ -24465,12 +25453,15 @@
       <c r="DU40" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV40" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A41" s="92">
         <v>38</v>
       </c>
-      <c r="B41" s="199"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="64" t="s">
         <v>478</v>
       </c>
@@ -24838,12 +25829,15 @@
       <c r="DU41" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV41" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="42" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A42" s="92">
         <v>39</v>
       </c>
-      <c r="B42" s="199"/>
+      <c r="B42" s="201"/>
       <c r="C42" s="64" t="s">
         <v>479</v>
       </c>
@@ -25211,12 +26205,15 @@
       <c r="DU42" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV42" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A43" s="92">
         <v>40</v>
       </c>
-      <c r="B43" s="199"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="64" t="s">
         <v>480</v>
       </c>
@@ -25584,12 +26581,15 @@
       <c r="DU43" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV43" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="44" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A44" s="92">
         <v>41</v>
       </c>
-      <c r="B44" s="199"/>
+      <c r="B44" s="201"/>
       <c r="C44" s="64" t="s">
         <v>481</v>
       </c>
@@ -25957,12 +26957,15 @@
       <c r="DU44" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV44" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="45" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A45" s="92">
         <v>42</v>
       </c>
-      <c r="B45" s="199"/>
+      <c r="B45" s="201"/>
       <c r="C45" s="64" t="s">
         <v>482</v>
       </c>
@@ -26330,12 +27333,15 @@
       <c r="DU45" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV45" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="46" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A46" s="92">
         <v>43</v>
       </c>
-      <c r="B46" s="199"/>
+      <c r="B46" s="201"/>
       <c r="C46" s="64" t="s">
         <v>483</v>
       </c>
@@ -26703,12 +27709,15 @@
       <c r="DU46" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV46" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="47" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A47" s="92">
         <v>44</v>
       </c>
-      <c r="B47" s="199"/>
+      <c r="B47" s="201"/>
       <c r="C47" s="64" t="s">
         <v>484</v>
       </c>
@@ -27076,12 +28085,15 @@
       <c r="DU47" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV47" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="48" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A48" s="92">
         <v>45</v>
       </c>
-      <c r="B48" s="199"/>
+      <c r="B48" s="201"/>
       <c r="C48" s="64" t="s">
         <v>485</v>
       </c>
@@ -27449,12 +28461,15 @@
       <c r="DU48" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV48" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="49" spans="1:125" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:126" s="68" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A49" s="92">
         <v>46</v>
       </c>
-      <c r="B49" s="199"/>
+      <c r="B49" s="201"/>
       <c r="C49" s="64" t="s">
         <v>486</v>
       </c>
@@ -27822,12 +28837,15 @@
       <c r="DU49" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="DV49" s="68" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="50" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A50" s="92">
         <v>47</v>
       </c>
-      <c r="B50" s="199"/>
+      <c r="B50" s="201"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -28197,12 +29215,15 @@
       <c r="DU50" s="41" t="s">
         <v>2101</v>
       </c>
+      <c r="DV50" s="105" t="s">
+        <v>2123</v>
+      </c>
     </row>
-    <row r="51" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="92">
         <v>48</v>
       </c>
-      <c r="B51" s="199"/>
+      <c r="B51" s="201"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -28572,12 +29593,15 @@
       <c r="DU51" s="41" t="s">
         <v>2102</v>
       </c>
+      <c r="DV51" s="12" t="s">
+        <v>2124</v>
+      </c>
     </row>
-    <row r="52" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A52" s="92">
         <v>49</v>
       </c>
-      <c r="B52" s="199"/>
+      <c r="B52" s="201"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -28947,12 +29971,15 @@
       <c r="DU52" s="41" t="s">
         <v>2103</v>
       </c>
+      <c r="DV52" s="105" t="s">
+        <v>2125</v>
+      </c>
     </row>
-    <row r="53" spans="1:125" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:126" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="92">
         <v>50</v>
       </c>
-      <c r="B53" s="200" t="s">
+      <c r="B53" s="202" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -29324,12 +30351,15 @@
       <c r="DU53" s="41" t="s">
         <v>860</v>
       </c>
+      <c r="DV53" s="105" t="s">
+        <v>861</v>
+      </c>
     </row>
-    <row r="54" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A54" s="92">
         <v>51</v>
       </c>
-      <c r="B54" s="200"/>
+      <c r="B54" s="202"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -29699,12 +30729,15 @@
       <c r="DU54" s="41" t="s">
         <v>61</v>
       </c>
+      <c r="DV54" s="4" t="s">
+        <v>858</v>
+      </c>
     </row>
-    <row r="55" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A55" s="92">
         <v>52</v>
       </c>
-      <c r="B55" s="200"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -30074,12 +31107,15 @@
       <c r="DU55" s="41" t="s">
         <v>2104</v>
       </c>
+      <c r="DV55" s="105" t="s">
+        <v>2112</v>
+      </c>
     </row>
-    <row r="56" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="92">
         <v>53</v>
       </c>
-      <c r="B56" s="200"/>
+      <c r="B56" s="202"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -30447,12 +31483,15 @@
       <c r="DU56" s="41" t="s">
         <v>2105</v>
       </c>
+      <c r="DV56" s="105" t="s">
+        <v>2115</v>
+      </c>
     </row>
-    <row r="57" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A57" s="92">
         <v>54</v>
       </c>
-      <c r="B57" s="200"/>
+      <c r="B57" s="202"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -30822,12 +31861,15 @@
       <c r="DU57" s="41" t="s">
         <v>1593</v>
       </c>
+      <c r="DV57" s="105" t="s">
+        <v>1980</v>
+      </c>
     </row>
-    <row r="58" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="92">
         <v>55</v>
       </c>
-      <c r="B58" s="200"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -31168,12 +32210,15 @@
       <c r="DU58" s="41" t="s">
         <v>2105</v>
       </c>
+      <c r="DV58" s="171" t="s">
+        <v>2114</v>
+      </c>
     </row>
-    <row r="59" spans="1:125" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:126" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="92">
         <v>56</v>
       </c>
-      <c r="B59" s="200"/>
+      <c r="B59" s="202"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -31543,12 +32588,15 @@
       <c r="DU59" s="41" t="s">
         <v>2106</v>
       </c>
+      <c r="DV59" t="s">
+        <v>2113</v>
+      </c>
     </row>
-    <row r="60" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A60" s="92">
         <v>57</v>
       </c>
-      <c r="B60" s="200"/>
+      <c r="B60" s="202"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -31918,12 +32966,15 @@
       <c r="DU60" s="41">
         <v>1</v>
       </c>
+      <c r="DV60" s="105">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:125" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:126" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="92">
         <v>58</v>
       </c>
-      <c r="B61" s="201" t="s">
+      <c r="B61" s="203" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -32293,12 +33344,15 @@
       <c r="DU61" s="173">
         <v>45611</v>
       </c>
+      <c r="DV61" s="173">
+        <v>45628</v>
+      </c>
     </row>
-    <row r="62" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A62" s="92">
         <v>59</v>
       </c>
-      <c r="B62" s="201"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -32668,12 +33722,15 @@
       <c r="DU62" s="173">
         <v>45611</v>
       </c>
+      <c r="DV62" s="173">
+        <v>45628</v>
+      </c>
     </row>
-    <row r="63" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A63" s="92">
         <v>60</v>
       </c>
-      <c r="B63" s="201"/>
+      <c r="B63" s="203"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -33043,12 +34100,15 @@
       <c r="DU63" s="41" t="s">
         <v>30</v>
       </c>
+      <c r="DV63" s="105" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="64" spans="1:125" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:126" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A64" s="92">
         <v>61</v>
       </c>
-      <c r="B64" s="201"/>
+      <c r="B64" s="203"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -33417,13 +34477,16 @@
       </c>
       <c r="DU64" s="41" t="s">
         <v>2107</v>
+      </c>
+      <c r="DV64" s="105" t="s">
+        <v>2116</v>
       </c>
     </row>
     <row r="65" spans="1:145" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A65" s="92">
         <v>62</v>
       </c>
-      <c r="B65" s="201"/>
+      <c r="B65" s="203"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -33533,7 +34596,7 @@
       <c r="A66" s="92">
         <v>63</v>
       </c>
-      <c r="B66" s="201"/>
+      <c r="B66" s="203"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -33643,7 +34706,7 @@
       <c r="A67" s="92">
         <v>64</v>
       </c>
-      <c r="B67" s="201"/>
+      <c r="B67" s="203"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -33706,7 +34769,7 @@
       <c r="A68" s="92">
         <v>65</v>
       </c>
-      <c r="B68" s="191" t="s">
+      <c r="B68" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -33748,7 +34811,7 @@
       <c r="A69" s="92">
         <v>66</v>
       </c>
-      <c r="B69" s="191"/>
+      <c r="B69" s="193"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -33783,7 +34846,7 @@
       <c r="A70" s="92">
         <v>67</v>
       </c>
-      <c r="B70" s="191"/>
+      <c r="B70" s="193"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -33816,7 +34879,7 @@
       <c r="A71" s="92">
         <v>68</v>
       </c>
-      <c r="B71" s="191"/>
+      <c r="B71" s="193"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -33848,7 +34911,7 @@
       <c r="A72" s="92">
         <v>69</v>
       </c>
-      <c r="B72" s="192"/>
+      <c r="B72" s="194"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -34566,7 +35629,7 @@
       <c r="BT3" s="36"/>
     </row>
     <row r="4" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B4" s="193" t="s">
+      <c r="B4" s="195" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -34735,7 +35798,7 @@
       <c r="BT4" s="12"/>
     </row>
     <row r="5" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="194"/>
+      <c r="B5" s="196"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -35067,7 +36130,7 @@
       <c r="BT6" s="2"/>
     </row>
     <row r="7" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B7" s="195" t="s">
+      <c r="B7" s="197" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -35234,7 +36297,7 @@
       <c r="BT7" s="37"/>
     </row>
     <row r="8" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="195"/>
+      <c r="B8" s="197"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -35401,7 +36464,7 @@
       <c r="BT8" s="1"/>
     </row>
     <row r="9" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="195"/>
+      <c r="B9" s="197"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -35568,7 +36631,7 @@
       <c r="BT9" s="1"/>
     </row>
     <row r="10" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="195"/>
+      <c r="B10" s="197"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -35735,7 +36798,7 @@
       <c r="BT10" s="1"/>
     </row>
     <row r="11" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="198" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -35902,7 +36965,7 @@
       <c r="BT11" s="106"/>
     </row>
     <row r="12" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="197"/>
+      <c r="B12" s="199"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -36067,7 +37130,7 @@
       <c r="BT12" s="2"/>
     </row>
     <row r="13" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="197"/>
+      <c r="B13" s="199"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -36232,7 +37295,7 @@
       <c r="BT13" s="106"/>
     </row>
     <row r="14" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="197"/>
+      <c r="B14" s="199"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -36397,7 +37460,7 @@
       <c r="BT14" s="2"/>
     </row>
     <row r="15" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="197"/>
+      <c r="B15" s="199"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -36562,7 +37625,7 @@
       <c r="BT15" s="2"/>
     </row>
     <row r="16" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="197"/>
+      <c r="B16" s="199"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -36727,7 +37790,7 @@
       <c r="BT16" s="2"/>
     </row>
     <row r="17" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="197"/>
+      <c r="B17" s="199"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -36892,7 +37955,7 @@
       <c r="BT17" s="2"/>
     </row>
     <row r="18" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="197"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -37057,7 +38120,7 @@
       <c r="BT18" s="2"/>
     </row>
     <row r="19" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="197"/>
+      <c r="B19" s="199"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -37222,7 +38285,7 @@
       <c r="BT19" s="2"/>
     </row>
     <row r="20" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="197"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -37387,7 +38450,7 @@
       <c r="BT20" s="2"/>
     </row>
     <row r="21" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="198" t="s">
+      <c r="B21" s="200" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -37595,7 +38658,7 @@
       <c r="BT21" s="106"/>
     </row>
     <row r="22" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="198"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -37803,7 +38866,7 @@
       <c r="BT22" s="106"/>
     </row>
     <row r="23" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="198"/>
+      <c r="B23" s="200"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -37970,7 +39033,7 @@
       <c r="BT23" s="2"/>
     </row>
     <row r="24" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="198"/>
+      <c r="B24" s="200"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -38137,7 +39200,7 @@
       <c r="BT24" s="105"/>
     </row>
     <row r="25" spans="2:72" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="198"/>
+      <c r="B25" s="200"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -38302,7 +39365,7 @@
       <c r="BT25" s="6"/>
     </row>
     <row r="26" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="199" t="s">
+      <c r="B26" s="201" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -38471,7 +39534,7 @@
       <c r="BT26" s="38"/>
     </row>
     <row r="27" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="199"/>
+      <c r="B27" s="201"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -38638,7 +39701,7 @@
       <c r="BT27" s="42"/>
     </row>
     <row r="28" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="199"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -38803,7 +39866,7 @@
       <c r="BT28" s="66"/>
     </row>
     <row r="29" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="199"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -38968,7 +40031,7 @@
       <c r="BT29" s="42"/>
     </row>
     <row r="30" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="199"/>
+      <c r="B30" s="201"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -39133,7 +40196,7 @@
       <c r="BT30" s="38"/>
     </row>
     <row r="31" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="199"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -39298,7 +40361,7 @@
       <c r="BT31" s="42"/>
     </row>
     <row r="32" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="199"/>
+      <c r="B32" s="201"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -39463,7 +40526,7 @@
       <c r="BT32" s="88"/>
     </row>
     <row r="33" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="199"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -39628,7 +40691,7 @@
       <c r="BT33" s="28"/>
     </row>
     <row r="34" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="199"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -39793,7 +40856,7 @@
       <c r="BT34" s="38"/>
     </row>
     <row r="35" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="199"/>
+      <c r="B35" s="201"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -39958,7 +41021,7 @@
       <c r="BT35" s="42"/>
     </row>
     <row r="36" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="199"/>
+      <c r="B36" s="201"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -40123,7 +41186,7 @@
       <c r="BT36" s="38"/>
     </row>
     <row r="37" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="199"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -40288,7 +41351,7 @@
       <c r="BT37" s="42"/>
     </row>
     <row r="38" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="199"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -40453,7 +41516,7 @@
       <c r="BT38" s="38"/>
     </row>
     <row r="39" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="199"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -40618,7 +41681,7 @@
       <c r="BT39" s="38"/>
     </row>
     <row r="40" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="199"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -40783,7 +41846,7 @@
       <c r="BT40" s="38"/>
     </row>
     <row r="41" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="199"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -40948,7 +42011,7 @@
       <c r="BT41" s="38"/>
     </row>
     <row r="42" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="199"/>
+      <c r="B42" s="201"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -41113,7 +42176,7 @@
       <c r="BT42" s="38"/>
     </row>
     <row r="43" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="199"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -41278,7 +42341,7 @@
       <c r="BT43" s="38"/>
     </row>
     <row r="44" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="199"/>
+      <c r="B44" s="201"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -41443,7 +42506,7 @@
       <c r="BT44" s="38"/>
     </row>
     <row r="45" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="199"/>
+      <c r="B45" s="201"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -41608,7 +42671,7 @@
       <c r="BT45" s="38"/>
     </row>
     <row r="46" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="199"/>
+      <c r="B46" s="201"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -41773,7 +42836,7 @@
       <c r="BT46" s="38"/>
     </row>
     <row r="47" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="199"/>
+      <c r="B47" s="201"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -41938,7 +43001,7 @@
       <c r="BT47" s="38"/>
     </row>
     <row r="48" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="199"/>
+      <c r="B48" s="201"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -42103,7 +43166,7 @@
       <c r="BT48" s="38"/>
     </row>
     <row r="49" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="199"/>
+      <c r="B49" s="201"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -42268,7 +43331,7 @@
       <c r="BT49" s="38"/>
     </row>
     <row r="50" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="199"/>
+      <c r="B50" s="201"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -42435,7 +43498,7 @@
       <c r="BT50" s="2"/>
     </row>
     <row r="51" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="199"/>
+      <c r="B51" s="201"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -42602,7 +43665,7 @@
       <c r="BT51" s="2"/>
     </row>
     <row r="52" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="199"/>
+      <c r="B52" s="201"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -42769,7 +43832,7 @@
       <c r="BT52" s="2"/>
     </row>
     <row r="53" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="200" t="s">
+      <c r="B53" s="202" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -42938,7 +44001,7 @@
       <c r="BT53" s="105"/>
     </row>
     <row r="54" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="200"/>
+      <c r="B54" s="202"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -43105,7 +44168,7 @@
       <c r="BT54" s="5"/>
     </row>
     <row r="55" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="200"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -43272,7 +44335,7 @@
       <c r="BT55" s="5"/>
     </row>
     <row r="56" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="200"/>
+      <c r="B56" s="202"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -43437,7 +44500,7 @@
       <c r="BT56" s="3"/>
     </row>
     <row r="57" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="200"/>
+      <c r="B57" s="202"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -43604,7 +44667,7 @@
       <c r="BT57" s="2"/>
     </row>
     <row r="58" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B58" s="200"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -43769,7 +44832,7 @@
       <c r="BT58" s="7"/>
     </row>
     <row r="59" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="200"/>
+      <c r="B59" s="202"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -43936,7 +44999,7 @@
       <c r="BT59" s="5"/>
     </row>
     <row r="60" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B60" s="200"/>
+      <c r="B60" s="202"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -44103,7 +45166,7 @@
       <c r="BT60" s="12"/>
     </row>
     <row r="61" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="201" t="s">
+      <c r="B61" s="203" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -44270,7 +45333,7 @@
       <c r="BT61" s="9"/>
     </row>
     <row r="62" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="201"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -44437,7 +45500,7 @@
       <c r="BT62" s="9"/>
     </row>
     <row r="63" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="201"/>
+      <c r="B63" s="203"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -44604,7 +45667,7 @@
       <c r="BT63" s="5"/>
     </row>
     <row r="64" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="201"/>
+      <c r="B64" s="203"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -44771,7 +45834,7 @@
       <c r="BT64" s="2"/>
     </row>
     <row r="65" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="201"/>
+      <c r="B65" s="203"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -44788,7 +45851,7 @@
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="201"/>
+      <c r="B66" s="203"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -44807,7 +45870,7 @@
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="201"/>
+      <c r="B67" s="203"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -44826,7 +45889,7 @@
       <c r="P67" s="1"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B68" s="191" t="s">
+      <c r="B68" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -44836,7 +45899,7 @@
       <c r="L68" s="105"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B69" s="191"/>
+      <c r="B69" s="193"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -44844,7 +45907,7 @@
       <c r="K69" s="12"/>
     </row>
     <row r="70" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B70" s="191"/>
+      <c r="B70" s="193"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -44852,7 +45915,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B71" s="191"/>
+      <c r="B71" s="193"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -44864,7 +45927,7 @@
       <c r="L71" s="105"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B72" s="192"/>
+      <c r="B72" s="194"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -45444,7 +46507,7 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B4" s="193" t="s">
+      <c r="B4" s="195" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -45524,7 +46587,7 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="194"/>
+      <c r="B5" s="196"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -45678,7 +46741,7 @@
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B7" s="195" t="s">
+      <c r="B7" s="197" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -45756,7 +46819,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="195"/>
+      <c r="B8" s="197"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -45834,7 +46897,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="195"/>
+      <c r="B9" s="197"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -45912,7 +46975,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="195"/>
+      <c r="B10" s="197"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -45990,7 +47053,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="198" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -46068,7 +47131,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="197"/>
+      <c r="B12" s="199"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -46144,7 +47207,7 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="197"/>
+      <c r="B13" s="199"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -46220,7 +47283,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="197"/>
+      <c r="B14" s="199"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -46296,7 +47359,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="197"/>
+      <c r="B15" s="199"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -46372,7 +47435,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="197"/>
+      <c r="B16" s="199"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -46448,7 +47511,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="197"/>
+      <c r="B17" s="199"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -46524,7 +47587,7 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="197"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -46600,7 +47663,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="197"/>
+      <c r="B19" s="199"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -46676,7 +47739,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="197"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -46752,7 +47815,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="198" t="s">
+      <c r="B21" s="200" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -46830,7 +47893,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="198"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -46908,7 +47971,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="198"/>
+      <c r="B23" s="200"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -46986,7 +48049,7 @@
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B24" s="198"/>
+      <c r="B24" s="200"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -47064,7 +48127,7 @@
       </c>
     </row>
     <row r="25" spans="2:27" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="198"/>
+      <c r="B25" s="200"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -47140,7 +48203,7 @@
       </c>
     </row>
     <row r="26" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B26" s="199" t="s">
+      <c r="B26" s="201" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -47220,7 +48283,7 @@
       </c>
     </row>
     <row r="27" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="199"/>
+      <c r="B27" s="201"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -47298,7 +48361,7 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="199"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -47374,7 +48437,7 @@
       </c>
     </row>
     <row r="29" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="199"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -47450,7 +48513,7 @@
       </c>
     </row>
     <row r="30" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="199"/>
+      <c r="B30" s="201"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -47526,7 +48589,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="199"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -47602,7 +48665,7 @@
       </c>
     </row>
     <row r="32" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="199"/>
+      <c r="B32" s="201"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -47678,7 +48741,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="199"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -47754,7 +48817,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="199"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -47830,7 +48893,7 @@
       </c>
     </row>
     <row r="35" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="199"/>
+      <c r="B35" s="201"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -47906,7 +48969,7 @@
       </c>
     </row>
     <row r="36" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="199"/>
+      <c r="B36" s="201"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -47982,7 +49045,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="199"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -48058,7 +49121,7 @@
       </c>
     </row>
     <row r="38" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="199"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -48134,7 +49197,7 @@
       </c>
     </row>
     <row r="39" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="199"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -48210,7 +49273,7 @@
       </c>
     </row>
     <row r="40" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="199"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -48286,7 +49349,7 @@
       </c>
     </row>
     <row r="41" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="199"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -48362,7 +49425,7 @@
       </c>
     </row>
     <row r="42" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="199"/>
+      <c r="B42" s="201"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -48438,7 +49501,7 @@
       </c>
     </row>
     <row r="43" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="199"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -48514,7 +49577,7 @@
       </c>
     </row>
     <row r="44" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="199"/>
+      <c r="B44" s="201"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -48590,7 +49653,7 @@
       </c>
     </row>
     <row r="45" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="199"/>
+      <c r="B45" s="201"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -48666,7 +49729,7 @@
       </c>
     </row>
     <row r="46" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="199"/>
+      <c r="B46" s="201"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -48742,7 +49805,7 @@
       </c>
     </row>
     <row r="47" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="199"/>
+      <c r="B47" s="201"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -48818,7 +49881,7 @@
       </c>
     </row>
     <row r="48" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="199"/>
+      <c r="B48" s="201"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -48894,7 +49957,7 @@
       </c>
     </row>
     <row r="49" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="199"/>
+      <c r="B49" s="201"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -48970,7 +50033,7 @@
       </c>
     </row>
     <row r="50" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="199"/>
+      <c r="B50" s="201"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -49048,7 +50111,7 @@
       </c>
     </row>
     <row r="51" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="199"/>
+      <c r="B51" s="201"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -49126,7 +50189,7 @@
       </c>
     </row>
     <row r="52" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="199"/>
+      <c r="B52" s="201"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -49204,7 +50267,7 @@
       </c>
     </row>
     <row r="53" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B53" s="200" t="s">
+      <c r="B53" s="202" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -49284,7 +50347,7 @@
       </c>
     </row>
     <row r="54" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="200"/>
+      <c r="B54" s="202"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -49362,7 +50425,7 @@
       </c>
     </row>
     <row r="55" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="200"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -49440,7 +50503,7 @@
       </c>
     </row>
     <row r="56" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="200"/>
+      <c r="B56" s="202"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -49516,7 +50579,7 @@
       </c>
     </row>
     <row r="57" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="200"/>
+      <c r="B57" s="202"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -49594,7 +50657,7 @@
       </c>
     </row>
     <row r="58" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B58" s="200"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -49670,7 +50733,7 @@
       </c>
     </row>
     <row r="59" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="200"/>
+      <c r="B59" s="202"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -49748,7 +50811,7 @@
       </c>
     </row>
     <row r="60" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B60" s="200"/>
+      <c r="B60" s="202"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -49826,7 +50889,7 @@
       </c>
     </row>
     <row r="61" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B61" s="201" t="s">
+      <c r="B61" s="203" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -49904,7 +50967,7 @@
       </c>
     </row>
     <row r="62" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="201"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -49982,7 +51045,7 @@
       </c>
     </row>
     <row r="63" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="201"/>
+      <c r="B63" s="203"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -50060,7 +51123,7 @@
       </c>
     </row>
     <row r="64" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="201"/>
+      <c r="B64" s="203"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -50138,7 +51201,7 @@
       </c>
     </row>
     <row r="65" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="201"/>
+      <c r="B65" s="203"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -50168,7 +51231,7 @@
       <c r="AA65" s="5"/>
     </row>
     <row r="66" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="201"/>
+      <c r="B66" s="203"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -50198,7 +51261,7 @@
       <c r="AA66" s="5"/>
     </row>
     <row r="67" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="201"/>
+      <c r="B67" s="203"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -50228,7 +51291,7 @@
       <c r="AA67" s="1"/>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B68" s="191" t="s">
+      <c r="B68" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -50249,7 +51312,7 @@
       <c r="Q68" s="105"/>
     </row>
     <row r="69" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B69" s="191"/>
+      <c r="B69" s="193"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -50268,7 +51331,7 @@
       <c r="Q69" s="105"/>
     </row>
     <row r="70" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B70" s="191"/>
+      <c r="B70" s="193"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -50287,7 +51350,7 @@
       <c r="Q70" s="105"/>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B71" s="191"/>
+      <c r="B71" s="193"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -50306,7 +51369,7 @@
       <c r="Q71" s="105"/>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B72" s="192"/>
+      <c r="B72" s="194"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>

</xml_diff>

<commit_message>
uploaded 30 datasets and made a few fixed related to this upload.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A65652-BFE7-4BFD-9BC6-04C47D25263B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C41E91-0665-48DF-92D3-FADDDC3F6D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12453" uniqueCount="2573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12483" uniqueCount="2573">
   <si>
     <t>Description</t>
   </si>
@@ -7742,7 +7742,7 @@
     <t>3_MC_nonresidential_buildings_Germany_per_volume_IOER</t>
   </si>
   <si>
-    <t>dataset entry created, data still need to be uploaded</t>
+    <t>dataset entry created, data uploaded on March 17, 2025.</t>
   </si>
 </sst>
 </file>
@@ -7884,7 +7884,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7948,12 +7948,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8140,7 +8134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -8474,7 +8468,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8882,7 +8875,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="203" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -8914,7 +8907,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B5" s="204"/>
+      <c r="B5" s="203"/>
       <c r="C5" s="26" t="s">
         <v>422</v>
       </c>
@@ -8944,7 +8937,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="205" t="s">
+      <c r="B6" s="204" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -8960,7 +8953,7 @@
       <c r="K6" s="121"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B7" s="205"/>
+      <c r="B7" s="204"/>
       <c r="C7" s="26" t="s">
         <v>424</v>
       </c>
@@ -8974,7 +8967,7 @@
       <c r="K7" s="121"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B8" s="205"/>
+      <c r="B8" s="204"/>
       <c r="C8" s="26" t="s">
         <v>425</v>
       </c>
@@ -8988,7 +8981,7 @@
       <c r="K8" s="121"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B9" s="205"/>
+      <c r="B9" s="204"/>
       <c r="C9" s="28" t="s">
         <v>426</v>
       </c>
@@ -9002,7 +8995,7 @@
       <c r="K9" s="121"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B10" s="205"/>
+      <c r="B10" s="204"/>
       <c r="C10" s="27" t="s">
         <v>427</v>
       </c>
@@ -9016,7 +9009,7 @@
       <c r="K10" s="121"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B11" s="205"/>
+      <c r="B11" s="204"/>
       <c r="C11" s="27" t="s">
         <v>428</v>
       </c>
@@ -9030,7 +9023,7 @@
       <c r="K11" s="121"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B12" s="205"/>
+      <c r="B12" s="204"/>
       <c r="C12" s="27" t="s">
         <v>429</v>
       </c>
@@ -9044,7 +9037,7 @@
       <c r="K12" s="121"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B13" s="205"/>
+      <c r="B13" s="204"/>
       <c r="C13" s="27" t="s">
         <v>430</v>
       </c>
@@ -9058,7 +9051,7 @@
       <c r="K13" s="121"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B14" s="205"/>
+      <c r="B14" s="204"/>
       <c r="C14" s="27" t="s">
         <v>431</v>
       </c>
@@ -9072,7 +9065,7 @@
       <c r="K14" s="121"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B15" s="205"/>
+      <c r="B15" s="204"/>
       <c r="C15" s="27" t="s">
         <v>432</v>
       </c>
@@ -9086,7 +9079,7 @@
       <c r="K15" s="121"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B16" s="205"/>
+      <c r="B16" s="204"/>
       <c r="C16" s="27" t="s">
         <v>433</v>
       </c>
@@ -9100,7 +9093,7 @@
       <c r="K16" s="121"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B17" s="205"/>
+      <c r="B17" s="204"/>
       <c r="C17" s="27" t="s">
         <v>434</v>
       </c>
@@ -9114,7 +9107,7 @@
       <c r="K17" s="121"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B18" s="205"/>
+      <c r="B18" s="204"/>
       <c r="C18" s="27" t="s">
         <v>435</v>
       </c>
@@ -9128,7 +9121,7 @@
       <c r="K18" s="121"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B19" s="206" t="s">
+      <c r="B19" s="205" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -9156,7 +9149,7 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B20" s="206"/>
+      <c r="B20" s="205"/>
       <c r="C20" s="27" t="s">
         <v>437</v>
       </c>
@@ -9186,7 +9179,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B21" s="206"/>
+      <c r="B21" s="205"/>
       <c r="C21" s="27" t="s">
         <v>438</v>
       </c>
@@ -9212,7 +9205,7 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="207" t="s">
+      <c r="B22" s="206" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -9242,7 +9235,7 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B23" s="207"/>
+      <c r="B23" s="206"/>
       <c r="C23" s="26" t="s">
         <v>440</v>
       </c>
@@ -9256,7 +9249,7 @@
       <c r="K23" s="121"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B24" s="207"/>
+      <c r="B24" s="206"/>
       <c r="C24" s="25" t="s">
         <v>441</v>
       </c>
@@ -9270,7 +9263,7 @@
       <c r="K24" s="121"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B25" s="207"/>
+      <c r="B25" s="206"/>
       <c r="C25" s="25" t="s">
         <v>443</v>
       </c>
@@ -9296,7 +9289,7 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B26" s="207"/>
+      <c r="B26" s="206"/>
       <c r="C26" s="25" t="s">
         <v>444</v>
       </c>
@@ -9312,7 +9305,7 @@
       <c r="K26" s="121"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B27" s="207"/>
+      <c r="B27" s="206"/>
       <c r="C27" s="25" t="s">
         <v>445</v>
       </c>
@@ -9326,7 +9319,7 @@
       <c r="K27" s="121"/>
     </row>
     <row r="28" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="208" t="s">
+      <c r="B28" s="207" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -9358,7 +9351,7 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B29" s="208"/>
+      <c r="B29" s="207"/>
       <c r="C29" s="25" t="s">
         <v>447</v>
       </c>
@@ -9388,7 +9381,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B30" s="201" t="s">
+      <c r="B30" s="200" t="s">
         <v>185</v>
       </c>
       <c r="C30" s="107" t="s">
@@ -9404,7 +9397,7 @@
       <c r="K30" s="181"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B31" s="202"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="108" t="s">
         <v>449</v>
       </c>
@@ -9418,7 +9411,7 @@
       <c r="K31" s="164"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B32" s="203"/>
+      <c r="B32" s="202"/>
       <c r="C32" s="109" t="s">
         <v>450</v>
       </c>
@@ -9448,11 +9441,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S38" sqref="S38"/>
+      <selection pane="bottomRight" activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -9566,7 +9559,7 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B4" s="209" t="s">
+      <c r="B4" s="208" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -9649,7 +9642,7 @@
       </c>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B5" s="210"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
       </c>
@@ -9890,7 +9883,7 @@
       </c>
     </row>
     <row r="8" spans="2:28" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="205" t="s">
+      <c r="B8" s="204" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="54" t="s">
@@ -9971,7 +9964,7 @@
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B9" s="205"/>
+      <c r="B9" s="204"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
       </c>
@@ -10050,7 +10043,7 @@
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B10" s="205"/>
+      <c r="B10" s="204"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
       </c>
@@ -10129,7 +10122,7 @@
       </c>
     </row>
     <row r="11" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="205"/>
+      <c r="B11" s="204"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
       </c>
@@ -10208,7 +10201,7 @@
       </c>
     </row>
     <row r="12" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="205"/>
+      <c r="B12" s="204"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -10287,7 +10280,7 @@
       </c>
     </row>
     <row r="13" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="205"/>
+      <c r="B13" s="204"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -10366,7 +10359,7 @@
       </c>
     </row>
     <row r="14" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="205"/>
+      <c r="B14" s="204"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -10445,7 +10438,7 @@
       </c>
     </row>
     <row r="15" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="205"/>
+      <c r="B15" s="204"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -10524,7 +10517,7 @@
       </c>
     </row>
     <row r="16" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="205"/>
+      <c r="B16" s="204"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -10603,7 +10596,7 @@
       </c>
     </row>
     <row r="17" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="205"/>
+      <c r="B17" s="204"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -10682,7 +10675,7 @@
       </c>
     </row>
     <row r="18" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="205"/>
+      <c r="B18" s="204"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -10761,7 +10754,7 @@
       </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B19" s="205"/>
+      <c r="B19" s="204"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -10840,7 +10833,7 @@
       </c>
     </row>
     <row r="20" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="205"/>
+      <c r="B20" s="204"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -10919,7 +10912,7 @@
       </c>
     </row>
     <row r="21" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="206" t="s">
+      <c r="B21" s="205" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -11000,7 +10993,7 @@
       </c>
     </row>
     <row r="22" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="206"/>
+      <c r="B22" s="205"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -11081,7 +11074,7 @@
       </c>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B23" s="206"/>
+      <c r="B23" s="205"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
       </c>
@@ -11160,7 +11153,7 @@
       </c>
     </row>
     <row r="24" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="206"/>
+      <c r="B24" s="205"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
       </c>
@@ -11239,7 +11232,7 @@
       </c>
     </row>
     <row r="25" spans="2:28" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="207" t="s">
+      <c r="B25" s="206" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -11320,7 +11313,7 @@
       </c>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B26" s="207"/>
+      <c r="B26" s="206"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
       </c>
@@ -11399,7 +11392,7 @@
       </c>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B27" s="207"/>
+      <c r="B27" s="206"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
       </c>
@@ -11478,7 +11471,7 @@
       </c>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B28" s="207"/>
+      <c r="B28" s="206"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
       </c>
@@ -11557,7 +11550,7 @@
       </c>
     </row>
     <row r="29" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="207"/>
+      <c r="B29" s="206"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
       </c>
@@ -11636,7 +11629,7 @@
       </c>
     </row>
     <row r="30" spans="2:28" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="207"/>
+      <c r="B30" s="206"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
       </c>
@@ -11715,7 +11708,7 @@
       </c>
     </row>
     <row r="31" spans="2:28" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="208" t="s">
+      <c r="B31" s="207" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -11798,7 +11791,7 @@
       </c>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B32" s="211"/>
+      <c r="B32" s="210"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
       </c>
@@ -11879,7 +11872,7 @@
       </c>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B33" s="201" t="s">
+      <c r="B33" s="200" t="s">
         <v>185</v>
       </c>
       <c r="C33" s="83" t="s">
@@ -11912,7 +11905,7 @@
       <c r="AB33" s="164"/>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B34" s="202"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
       </c>
@@ -11943,7 +11936,7 @@
       <c r="AB34" s="164"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B35" s="203"/>
+      <c r="B35" s="202"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
       </c>
@@ -11997,11 +11990,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:FG74"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="DU48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="ED6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="ED5" sqref="ED5"/>
+      <selection pane="bottomRight" activeCell="FA9" sqref="FA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -12432,94 +12425,94 @@
       <c r="DV1" s="154" t="s">
         <v>2569</v>
       </c>
-      <c r="DW1" s="199" t="s">
+      <c r="DW1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="DX1" s="199" t="s">
+      <c r="DX1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="DY1" s="199" t="s">
+      <c r="DY1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="DZ1" s="199" t="s">
+      <c r="DZ1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EA1" s="199" t="s">
+      <c r="EA1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EB1" s="199" t="s">
+      <c r="EB1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EC1" s="199" t="s">
+      <c r="EC1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="ED1" s="199" t="s">
+      <c r="ED1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EE1" s="199" t="s">
+      <c r="EE1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EF1" s="199" t="s">
+      <c r="EF1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EG1" s="199" t="s">
+      <c r="EG1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EH1" s="199" t="s">
+      <c r="EH1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EI1" s="199" t="s">
+      <c r="EI1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EJ1" s="199" t="s">
+      <c r="EJ1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EK1" s="199" t="s">
+      <c r="EK1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EL1" s="199" t="s">
+      <c r="EL1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EM1" s="199" t="s">
+      <c r="EM1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EN1" s="199" t="s">
+      <c r="EN1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EO1" s="199" t="s">
+      <c r="EO1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EP1" s="199" t="s">
+      <c r="EP1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EQ1" s="199" t="s">
+      <c r="EQ1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="ER1" s="199" t="s">
+      <c r="ER1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="ES1" s="199" t="s">
+      <c r="ES1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="ET1" s="199" t="s">
+      <c r="ET1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EU1" s="199" t="s">
+      <c r="EU1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EV1" s="199" t="s">
+      <c r="EV1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EW1" s="199" t="s">
+      <c r="EW1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EX1" s="199" t="s">
+      <c r="EX1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EY1" s="199" t="s">
+      <c r="EY1" s="154" t="s">
         <v>2572</v>
       </c>
-      <c r="EZ1" s="199" t="s">
+      <c r="EZ1" s="154" t="s">
         <v>2572</v>
       </c>
     </row>
@@ -12546,31 +12539,31 @@
       <c r="BO2" s="105"/>
       <c r="BP2" s="105"/>
       <c r="BQ2" s="105"/>
-      <c r="BR2" s="200" t="s">
+      <c r="BR2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BS2" s="200" t="s">
+      <c r="BS2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BT2" s="200" t="s">
+      <c r="BT2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BU2" s="200" t="s">
+      <c r="BU2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BV2" s="200" t="s">
+      <c r="BV2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BW2" s="200" t="s">
+      <c r="BW2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BX2" s="200" t="s">
+      <c r="BX2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BY2" s="200" t="s">
+      <c r="BY2" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="BZ2" s="200" t="s">
+      <c r="BZ2" s="199" t="s">
         <v>1432</v>
       </c>
       <c r="CA2" s="154" t="s">
@@ -12715,6 +12708,96 @@
         <v>2568</v>
       </c>
       <c r="DV2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="DW2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="DX2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="DY2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="DZ2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EA2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EB2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EC2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="ED2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EE2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EF2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EG2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EH2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EI2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EJ2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EK2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EL2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EM2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EN2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EO2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EP2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EQ2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="ER2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="ES2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="ET2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EU2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EV2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EW2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EX2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EY2" s="154" t="s">
+        <v>2570</v>
+      </c>
+      <c r="EZ2" s="154" t="s">
         <v>2570</v>
       </c>
     </row>
@@ -12975,7 +13058,7 @@
       <c r="A4" s="41">
         <v>1</v>
       </c>
-      <c r="B4" s="214" t="s">
+      <c r="B4" s="213" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -13233,7 +13316,7 @@
       <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="215"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -14167,7 +14250,7 @@
       <c r="A7" s="92">
         <v>4</v>
       </c>
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="215" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -14635,7 +14718,7 @@
       <c r="A8" s="92">
         <v>5</v>
       </c>
-      <c r="B8" s="216"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -15103,7 +15186,7 @@
       <c r="A9" s="92">
         <v>6</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="215"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -15571,7 +15654,7 @@
       <c r="A10" s="92">
         <v>7</v>
       </c>
-      <c r="B10" s="216"/>
+      <c r="B10" s="215"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -16039,7 +16122,7 @@
       <c r="A11" s="92">
         <v>8</v>
       </c>
-      <c r="B11" s="217" t="s">
+      <c r="B11" s="216" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -16507,7 +16590,7 @@
       <c r="A12" s="92">
         <v>9</v>
       </c>
-      <c r="B12" s="218"/>
+      <c r="B12" s="217"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -16973,7 +17056,7 @@
       <c r="A13" s="92">
         <v>10</v>
       </c>
-      <c r="B13" s="218"/>
+      <c r="B13" s="217"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -17439,7 +17522,7 @@
       <c r="A14" s="92">
         <v>11</v>
       </c>
-      <c r="B14" s="218"/>
+      <c r="B14" s="217"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -17905,7 +17988,7 @@
       <c r="A15" s="92">
         <v>12</v>
       </c>
-      <c r="B15" s="218"/>
+      <c r="B15" s="217"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -18371,7 +18454,7 @@
       <c r="A16" s="92">
         <v>13</v>
       </c>
-      <c r="B16" s="218"/>
+      <c r="B16" s="217"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -18837,7 +18920,7 @@
       <c r="A17" s="92">
         <v>14</v>
       </c>
-      <c r="B17" s="218"/>
+      <c r="B17" s="217"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -19303,7 +19386,7 @@
       <c r="A18" s="92">
         <v>15</v>
       </c>
-      <c r="B18" s="218"/>
+      <c r="B18" s="217"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -19769,7 +19852,7 @@
       <c r="A19" s="92">
         <v>16</v>
       </c>
-      <c r="B19" s="218"/>
+      <c r="B19" s="217"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -20235,7 +20318,7 @@
       <c r="A20" s="92">
         <v>17</v>
       </c>
-      <c r="B20" s="218"/>
+      <c r="B20" s="217"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -20701,7 +20784,7 @@
       <c r="A21" s="92">
         <v>18</v>
       </c>
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="218" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -21163,7 +21246,7 @@
       <c r="A22" s="92">
         <v>19</v>
       </c>
-      <c r="B22" s="219"/>
+      <c r="B22" s="218"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -21631,7 +21714,7 @@
       <c r="A23" s="92">
         <v>20</v>
       </c>
-      <c r="B23" s="219"/>
+      <c r="B23" s="218"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -22099,7 +22182,7 @@
       <c r="A24" s="92">
         <v>21</v>
       </c>
-      <c r="B24" s="219"/>
+      <c r="B24" s="218"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -22567,7 +22650,7 @@
       <c r="A25" s="92">
         <v>22</v>
       </c>
-      <c r="B25" s="219"/>
+      <c r="B25" s="218"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -23033,7 +23116,7 @@
       <c r="A26" s="92">
         <v>23</v>
       </c>
-      <c r="B26" s="220" t="s">
+      <c r="B26" s="219" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="64" t="s">
@@ -23503,7 +23586,7 @@
       <c r="A27" s="92">
         <v>24</v>
       </c>
-      <c r="B27" s="220"/>
+      <c r="B27" s="219"/>
       <c r="C27" s="64" t="s">
         <v>464</v>
       </c>
@@ -23971,7 +24054,7 @@
       <c r="A28" s="92">
         <v>25</v>
       </c>
-      <c r="B28" s="220"/>
+      <c r="B28" s="219"/>
       <c r="C28" s="64" t="s">
         <v>465</v>
       </c>
@@ -24437,7 +24520,7 @@
       <c r="A29" s="92">
         <v>26</v>
       </c>
-      <c r="B29" s="220"/>
+      <c r="B29" s="219"/>
       <c r="C29" s="64" t="s">
         <v>466</v>
       </c>
@@ -24903,7 +24986,7 @@
       <c r="A30" s="92">
         <v>27</v>
       </c>
-      <c r="B30" s="220"/>
+      <c r="B30" s="219"/>
       <c r="C30" s="64" t="s">
         <v>467</v>
       </c>
@@ -25369,7 +25452,7 @@
       <c r="A31" s="92">
         <v>28</v>
       </c>
-      <c r="B31" s="220"/>
+      <c r="B31" s="219"/>
       <c r="C31" s="64" t="s">
         <v>468</v>
       </c>
@@ -25835,7 +25918,7 @@
       <c r="A32" s="92">
         <v>29</v>
       </c>
-      <c r="B32" s="220"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="64" t="s">
         <v>469</v>
       </c>
@@ -26301,7 +26384,7 @@
       <c r="A33" s="92">
         <v>30</v>
       </c>
-      <c r="B33" s="220"/>
+      <c r="B33" s="219"/>
       <c r="C33" s="64" t="s">
         <v>470</v>
       </c>
@@ -26767,7 +26850,7 @@
       <c r="A34" s="92">
         <v>31</v>
       </c>
-      <c r="B34" s="220"/>
+      <c r="B34" s="219"/>
       <c r="C34" s="64" t="s">
         <v>471</v>
       </c>
@@ -27233,7 +27316,7 @@
       <c r="A35" s="92">
         <v>32</v>
       </c>
-      <c r="B35" s="220"/>
+      <c r="B35" s="219"/>
       <c r="C35" s="64" t="s">
         <v>472</v>
       </c>
@@ -27699,7 +27782,7 @@
       <c r="A36" s="92">
         <v>33</v>
       </c>
-      <c r="B36" s="220"/>
+      <c r="B36" s="219"/>
       <c r="C36" s="64" t="s">
         <v>473</v>
       </c>
@@ -28165,7 +28248,7 @@
       <c r="A37" s="92">
         <v>34</v>
       </c>
-      <c r="B37" s="220"/>
+      <c r="B37" s="219"/>
       <c r="C37" s="64" t="s">
         <v>474</v>
       </c>
@@ -28631,7 +28714,7 @@
       <c r="A38" s="92">
         <v>35</v>
       </c>
-      <c r="B38" s="220"/>
+      <c r="B38" s="219"/>
       <c r="C38" s="64" t="s">
         <v>475</v>
       </c>
@@ -29097,7 +29180,7 @@
       <c r="A39" s="92">
         <v>36</v>
       </c>
-      <c r="B39" s="220"/>
+      <c r="B39" s="219"/>
       <c r="C39" s="64" t="s">
         <v>476</v>
       </c>
@@ -29563,7 +29646,7 @@
       <c r="A40" s="92">
         <v>37</v>
       </c>
-      <c r="B40" s="220"/>
+      <c r="B40" s="219"/>
       <c r="C40" s="64" t="s">
         <v>477</v>
       </c>
@@ -30029,7 +30112,7 @@
       <c r="A41" s="92">
         <v>38</v>
       </c>
-      <c r="B41" s="220"/>
+      <c r="B41" s="219"/>
       <c r="C41" s="64" t="s">
         <v>478</v>
       </c>
@@ -30495,7 +30578,7 @@
       <c r="A42" s="92">
         <v>39</v>
       </c>
-      <c r="B42" s="220"/>
+      <c r="B42" s="219"/>
       <c r="C42" s="64" t="s">
         <v>479</v>
       </c>
@@ -30961,7 +31044,7 @@
       <c r="A43" s="92">
         <v>40</v>
       </c>
-      <c r="B43" s="220"/>
+      <c r="B43" s="219"/>
       <c r="C43" s="64" t="s">
         <v>480</v>
       </c>
@@ -31427,7 +31510,7 @@
       <c r="A44" s="92">
         <v>41</v>
       </c>
-      <c r="B44" s="220"/>
+      <c r="B44" s="219"/>
       <c r="C44" s="64" t="s">
         <v>481</v>
       </c>
@@ -31893,7 +31976,7 @@
       <c r="A45" s="92">
         <v>42</v>
       </c>
-      <c r="B45" s="220"/>
+      <c r="B45" s="219"/>
       <c r="C45" s="64" t="s">
         <v>482</v>
       </c>
@@ -32359,7 +32442,7 @@
       <c r="A46" s="92">
         <v>43</v>
       </c>
-      <c r="B46" s="220"/>
+      <c r="B46" s="219"/>
       <c r="C46" s="64" t="s">
         <v>483</v>
       </c>
@@ -32825,7 +32908,7 @@
       <c r="A47" s="92">
         <v>44</v>
       </c>
-      <c r="B47" s="220"/>
+      <c r="B47" s="219"/>
       <c r="C47" s="64" t="s">
         <v>484</v>
       </c>
@@ -33291,7 +33374,7 @@
       <c r="A48" s="92">
         <v>45</v>
       </c>
-      <c r="B48" s="220"/>
+      <c r="B48" s="219"/>
       <c r="C48" s="64" t="s">
         <v>485</v>
       </c>
@@ -33757,7 +33840,7 @@
       <c r="A49" s="92">
         <v>46</v>
       </c>
-      <c r="B49" s="220"/>
+      <c r="B49" s="219"/>
       <c r="C49" s="64" t="s">
         <v>486</v>
       </c>
@@ -34223,7 +34306,7 @@
       <c r="A50" s="92">
         <v>47</v>
       </c>
-      <c r="B50" s="220"/>
+      <c r="B50" s="219"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -34691,7 +34774,7 @@
       <c r="A51" s="92">
         <v>48</v>
       </c>
-      <c r="B51" s="220"/>
+      <c r="B51" s="219"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -35159,7 +35242,7 @@
       <c r="A52" s="92">
         <v>49</v>
       </c>
-      <c r="B52" s="220"/>
+      <c r="B52" s="219"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -35627,7 +35710,7 @@
       <c r="A53" s="92">
         <v>50</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="220" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -36097,7 +36180,7 @@
       <c r="A54" s="92">
         <v>51</v>
       </c>
-      <c r="B54" s="221"/>
+      <c r="B54" s="220"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -36565,7 +36648,7 @@
       <c r="A55" s="92">
         <v>52</v>
       </c>
-      <c r="B55" s="221"/>
+      <c r="B55" s="220"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -37033,7 +37116,7 @@
       <c r="A56" s="92">
         <v>53</v>
       </c>
-      <c r="B56" s="221"/>
+      <c r="B56" s="220"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -37499,7 +37582,7 @@
       <c r="A57" s="92">
         <v>54</v>
       </c>
-      <c r="B57" s="221"/>
+      <c r="B57" s="220"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -37967,7 +38050,7 @@
       <c r="A58" s="92">
         <v>55</v>
       </c>
-      <c r="B58" s="221"/>
+      <c r="B58" s="220"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -38406,7 +38489,7 @@
       <c r="A59" s="92">
         <v>56</v>
       </c>
-      <c r="B59" s="221"/>
+      <c r="B59" s="220"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -38874,7 +38957,7 @@
       <c r="A60" s="92">
         <v>57</v>
       </c>
-      <c r="B60" s="221"/>
+      <c r="B60" s="220"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -39342,7 +39425,7 @@
       <c r="A61" s="92">
         <v>58</v>
       </c>
-      <c r="B61" s="222" t="s">
+      <c r="B61" s="221" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -39810,7 +39893,7 @@
       <c r="A62" s="92">
         <v>59</v>
       </c>
-      <c r="B62" s="222"/>
+      <c r="B62" s="221"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -40278,7 +40361,7 @@
       <c r="A63" s="92">
         <v>60</v>
       </c>
-      <c r="B63" s="222"/>
+      <c r="B63" s="221"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -40746,7 +40829,7 @@
       <c r="A64" s="92">
         <v>61</v>
       </c>
-      <c r="B64" s="222"/>
+      <c r="B64" s="221"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -41214,7 +41297,7 @@
       <c r="A65" s="92">
         <v>62</v>
       </c>
-      <c r="B65" s="222"/>
+      <c r="B65" s="221"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -41400,7 +41483,7 @@
       <c r="A66" s="92">
         <v>63</v>
       </c>
-      <c r="B66" s="222"/>
+      <c r="B66" s="221"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -41584,7 +41667,7 @@
       <c r="A67" s="92">
         <v>64</v>
       </c>
-      <c r="B67" s="222"/>
+      <c r="B67" s="221"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -41683,7 +41766,7 @@
       <c r="A68" s="92">
         <v>65</v>
       </c>
-      <c r="B68" s="212" t="s">
+      <c r="B68" s="211" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -41745,7 +41828,7 @@
       <c r="A69" s="92">
         <v>66</v>
       </c>
-      <c r="B69" s="212"/>
+      <c r="B69" s="211"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -41792,7 +41875,7 @@
       <c r="A70" s="92">
         <v>67</v>
       </c>
-      <c r="B70" s="212"/>
+      <c r="B70" s="211"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -41830,7 +41913,7 @@
       <c r="A71" s="92">
         <v>68</v>
       </c>
-      <c r="B71" s="212"/>
+      <c r="B71" s="211"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -41865,7 +41948,7 @@
       <c r="A72" s="92">
         <v>69</v>
       </c>
-      <c r="B72" s="213"/>
+      <c r="B72" s="212"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -42643,7 +42726,7 @@
       <c r="BT3" s="36"/>
     </row>
     <row r="4" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B4" s="214" t="s">
+      <c r="B4" s="213" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -42812,7 +42895,7 @@
       <c r="BT4" s="12"/>
     </row>
     <row r="5" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="215"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -43144,7 +43227,7 @@
       <c r="BT6" s="2"/>
     </row>
     <row r="7" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="215" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -43311,7 +43394,7 @@
       <c r="BT7" s="37"/>
     </row>
     <row r="8" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="216"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -43478,7 +43561,7 @@
       <c r="BT8" s="1"/>
     </row>
     <row r="9" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="216"/>
+      <c r="B9" s="215"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -43645,7 +43728,7 @@
       <c r="BT9" s="1"/>
     </row>
     <row r="10" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="216"/>
+      <c r="B10" s="215"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -43812,7 +43895,7 @@
       <c r="BT10" s="1"/>
     </row>
     <row r="11" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="217" t="s">
+      <c r="B11" s="216" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -43979,7 +44062,7 @@
       <c r="BT11" s="106"/>
     </row>
     <row r="12" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="218"/>
+      <c r="B12" s="217"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -44144,7 +44227,7 @@
       <c r="BT12" s="2"/>
     </row>
     <row r="13" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="218"/>
+      <c r="B13" s="217"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -44309,7 +44392,7 @@
       <c r="BT13" s="106"/>
     </row>
     <row r="14" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="218"/>
+      <c r="B14" s="217"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -44474,7 +44557,7 @@
       <c r="BT14" s="2"/>
     </row>
     <row r="15" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="218"/>
+      <c r="B15" s="217"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -44639,7 +44722,7 @@
       <c r="BT15" s="2"/>
     </row>
     <row r="16" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="218"/>
+      <c r="B16" s="217"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -44804,7 +44887,7 @@
       <c r="BT16" s="2"/>
     </row>
     <row r="17" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="218"/>
+      <c r="B17" s="217"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -44969,7 +45052,7 @@
       <c r="BT17" s="2"/>
     </row>
     <row r="18" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="218"/>
+      <c r="B18" s="217"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -45134,7 +45217,7 @@
       <c r="BT18" s="2"/>
     </row>
     <row r="19" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="218"/>
+      <c r="B19" s="217"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -45299,7 +45382,7 @@
       <c r="BT19" s="2"/>
     </row>
     <row r="20" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="218"/>
+      <c r="B20" s="217"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -45464,7 +45547,7 @@
       <c r="BT20" s="2"/>
     </row>
     <row r="21" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="218" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -45672,7 +45755,7 @@
       <c r="BT21" s="106"/>
     </row>
     <row r="22" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="219"/>
+      <c r="B22" s="218"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -45880,7 +45963,7 @@
       <c r="BT22" s="106"/>
     </row>
     <row r="23" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="219"/>
+      <c r="B23" s="218"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -46047,7 +46130,7 @@
       <c r="BT23" s="2"/>
     </row>
     <row r="24" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="219"/>
+      <c r="B24" s="218"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -46214,7 +46297,7 @@
       <c r="BT24" s="105"/>
     </row>
     <row r="25" spans="2:72" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="219"/>
+      <c r="B25" s="218"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -46379,7 +46462,7 @@
       <c r="BT25" s="6"/>
     </row>
     <row r="26" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="220" t="s">
+      <c r="B26" s="219" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -46548,7 +46631,7 @@
       <c r="BT26" s="38"/>
     </row>
     <row r="27" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="220"/>
+      <c r="B27" s="219"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -46715,7 +46798,7 @@
       <c r="BT27" s="42"/>
     </row>
     <row r="28" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="220"/>
+      <c r="B28" s="219"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -46880,7 +46963,7 @@
       <c r="BT28" s="66"/>
     </row>
     <row r="29" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="220"/>
+      <c r="B29" s="219"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -47045,7 +47128,7 @@
       <c r="BT29" s="42"/>
     </row>
     <row r="30" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="220"/>
+      <c r="B30" s="219"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -47210,7 +47293,7 @@
       <c r="BT30" s="38"/>
     </row>
     <row r="31" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="220"/>
+      <c r="B31" s="219"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -47375,7 +47458,7 @@
       <c r="BT31" s="42"/>
     </row>
     <row r="32" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="220"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -47540,7 +47623,7 @@
       <c r="BT32" s="88"/>
     </row>
     <row r="33" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="220"/>
+      <c r="B33" s="219"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -47705,7 +47788,7 @@
       <c r="BT33" s="28"/>
     </row>
     <row r="34" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="220"/>
+      <c r="B34" s="219"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -47870,7 +47953,7 @@
       <c r="BT34" s="38"/>
     </row>
     <row r="35" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="220"/>
+      <c r="B35" s="219"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -48035,7 +48118,7 @@
       <c r="BT35" s="42"/>
     </row>
     <row r="36" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="220"/>
+      <c r="B36" s="219"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -48200,7 +48283,7 @@
       <c r="BT36" s="38"/>
     </row>
     <row r="37" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="220"/>
+      <c r="B37" s="219"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -48365,7 +48448,7 @@
       <c r="BT37" s="42"/>
     </row>
     <row r="38" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="220"/>
+      <c r="B38" s="219"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -48530,7 +48613,7 @@
       <c r="BT38" s="38"/>
     </row>
     <row r="39" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="220"/>
+      <c r="B39" s="219"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -48695,7 +48778,7 @@
       <c r="BT39" s="38"/>
     </row>
     <row r="40" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="220"/>
+      <c r="B40" s="219"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -48860,7 +48943,7 @@
       <c r="BT40" s="38"/>
     </row>
     <row r="41" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="220"/>
+      <c r="B41" s="219"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -49025,7 +49108,7 @@
       <c r="BT41" s="38"/>
     </row>
     <row r="42" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="220"/>
+      <c r="B42" s="219"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -49190,7 +49273,7 @@
       <c r="BT42" s="38"/>
     </row>
     <row r="43" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="220"/>
+      <c r="B43" s="219"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -49355,7 +49438,7 @@
       <c r="BT43" s="38"/>
     </row>
     <row r="44" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="220"/>
+      <c r="B44" s="219"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -49520,7 +49603,7 @@
       <c r="BT44" s="38"/>
     </row>
     <row r="45" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="220"/>
+      <c r="B45" s="219"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -49685,7 +49768,7 @@
       <c r="BT45" s="38"/>
     </row>
     <row r="46" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="220"/>
+      <c r="B46" s="219"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -49850,7 +49933,7 @@
       <c r="BT46" s="38"/>
     </row>
     <row r="47" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="220"/>
+      <c r="B47" s="219"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -50015,7 +50098,7 @@
       <c r="BT47" s="38"/>
     </row>
     <row r="48" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="220"/>
+      <c r="B48" s="219"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -50180,7 +50263,7 @@
       <c r="BT48" s="38"/>
     </row>
     <row r="49" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="220"/>
+      <c r="B49" s="219"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -50345,7 +50428,7 @@
       <c r="BT49" s="38"/>
     </row>
     <row r="50" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="220"/>
+      <c r="B50" s="219"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -50512,7 +50595,7 @@
       <c r="BT50" s="2"/>
     </row>
     <row r="51" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="220"/>
+      <c r="B51" s="219"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -50679,7 +50762,7 @@
       <c r="BT51" s="2"/>
     </row>
     <row r="52" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="220"/>
+      <c r="B52" s="219"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -50846,7 +50929,7 @@
       <c r="BT52" s="2"/>
     </row>
     <row r="53" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="220" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -51015,7 +51098,7 @@
       <c r="BT53" s="105"/>
     </row>
     <row r="54" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="221"/>
+      <c r="B54" s="220"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -51182,7 +51265,7 @@
       <c r="BT54" s="5"/>
     </row>
     <row r="55" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="221"/>
+      <c r="B55" s="220"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -51349,7 +51432,7 @@
       <c r="BT55" s="5"/>
     </row>
     <row r="56" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="221"/>
+      <c r="B56" s="220"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -51514,7 +51597,7 @@
       <c r="BT56" s="3"/>
     </row>
     <row r="57" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="221"/>
+      <c r="B57" s="220"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -51681,7 +51764,7 @@
       <c r="BT57" s="2"/>
     </row>
     <row r="58" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B58" s="221"/>
+      <c r="B58" s="220"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -51846,7 +51929,7 @@
       <c r="BT58" s="7"/>
     </row>
     <row r="59" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="221"/>
+      <c r="B59" s="220"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -52013,7 +52096,7 @@
       <c r="BT59" s="5"/>
     </row>
     <row r="60" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B60" s="221"/>
+      <c r="B60" s="220"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -52180,7 +52263,7 @@
       <c r="BT60" s="12"/>
     </row>
     <row r="61" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="222" t="s">
+      <c r="B61" s="221" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -52347,7 +52430,7 @@
       <c r="BT61" s="9"/>
     </row>
     <row r="62" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="222"/>
+      <c r="B62" s="221"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -52514,7 +52597,7 @@
       <c r="BT62" s="9"/>
     </row>
     <row r="63" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="222"/>
+      <c r="B63" s="221"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -52681,7 +52764,7 @@
       <c r="BT63" s="5"/>
     </row>
     <row r="64" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="222"/>
+      <c r="B64" s="221"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -52848,7 +52931,7 @@
       <c r="BT64" s="2"/>
     </row>
     <row r="65" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="222"/>
+      <c r="B65" s="221"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -52865,7 +52948,7 @@
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="222"/>
+      <c r="B66" s="221"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -52884,7 +52967,7 @@
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="222"/>
+      <c r="B67" s="221"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -52903,7 +52986,7 @@
       <c r="P67" s="1"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B68" s="212" t="s">
+      <c r="B68" s="211" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -52913,7 +52996,7 @@
       <c r="L68" s="105"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B69" s="212"/>
+      <c r="B69" s="211"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -52921,7 +53004,7 @@
       <c r="K69" s="12"/>
     </row>
     <row r="70" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B70" s="212"/>
+      <c r="B70" s="211"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -52929,7 +53012,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B71" s="212"/>
+      <c r="B71" s="211"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -52941,7 +53024,7 @@
       <c r="L71" s="105"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B72" s="213"/>
+      <c r="B72" s="212"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -53521,7 +53604,7 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B4" s="214" t="s">
+      <c r="B4" s="213" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -53601,7 +53684,7 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="215"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -53755,7 +53838,7 @@
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="215" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -53833,7 +53916,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="216"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -53911,7 +53994,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="216"/>
+      <c r="B9" s="215"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -53989,7 +54072,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="216"/>
+      <c r="B10" s="215"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -54067,7 +54150,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="217" t="s">
+      <c r="B11" s="216" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -54145,7 +54228,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="218"/>
+      <c r="B12" s="217"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -54221,7 +54304,7 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="218"/>
+      <c r="B13" s="217"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -54297,7 +54380,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="218"/>
+      <c r="B14" s="217"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -54373,7 +54456,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="218"/>
+      <c r="B15" s="217"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -54449,7 +54532,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="218"/>
+      <c r="B16" s="217"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -54525,7 +54608,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="218"/>
+      <c r="B17" s="217"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -54601,7 +54684,7 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="218"/>
+      <c r="B18" s="217"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -54677,7 +54760,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="218"/>
+      <c r="B19" s="217"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -54753,7 +54836,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="218"/>
+      <c r="B20" s="217"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -54829,7 +54912,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="218" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -54907,7 +54990,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="219"/>
+      <c r="B22" s="218"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -54985,7 +55068,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="219"/>
+      <c r="B23" s="218"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -55063,7 +55146,7 @@
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B24" s="219"/>
+      <c r="B24" s="218"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -55141,7 +55224,7 @@
       </c>
     </row>
     <row r="25" spans="2:27" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="219"/>
+      <c r="B25" s="218"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -55217,7 +55300,7 @@
       </c>
     </row>
     <row r="26" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B26" s="220" t="s">
+      <c r="B26" s="219" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -55297,7 +55380,7 @@
       </c>
     </row>
     <row r="27" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="220"/>
+      <c r="B27" s="219"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -55375,7 +55458,7 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="220"/>
+      <c r="B28" s="219"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -55451,7 +55534,7 @@
       </c>
     </row>
     <row r="29" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="220"/>
+      <c r="B29" s="219"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -55527,7 +55610,7 @@
       </c>
     </row>
     <row r="30" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="220"/>
+      <c r="B30" s="219"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -55603,7 +55686,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="220"/>
+      <c r="B31" s="219"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -55679,7 +55762,7 @@
       </c>
     </row>
     <row r="32" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="220"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -55755,7 +55838,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="220"/>
+      <c r="B33" s="219"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -55831,7 +55914,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="220"/>
+      <c r="B34" s="219"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -55907,7 +55990,7 @@
       </c>
     </row>
     <row r="35" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="220"/>
+      <c r="B35" s="219"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -55983,7 +56066,7 @@
       </c>
     </row>
     <row r="36" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="220"/>
+      <c r="B36" s="219"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -56059,7 +56142,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="220"/>
+      <c r="B37" s="219"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -56135,7 +56218,7 @@
       </c>
     </row>
     <row r="38" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="220"/>
+      <c r="B38" s="219"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -56211,7 +56294,7 @@
       </c>
     </row>
     <row r="39" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="220"/>
+      <c r="B39" s="219"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -56287,7 +56370,7 @@
       </c>
     </row>
     <row r="40" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="220"/>
+      <c r="B40" s="219"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -56363,7 +56446,7 @@
       </c>
     </row>
     <row r="41" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="220"/>
+      <c r="B41" s="219"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -56439,7 +56522,7 @@
       </c>
     </row>
     <row r="42" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="220"/>
+      <c r="B42" s="219"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -56515,7 +56598,7 @@
       </c>
     </row>
     <row r="43" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="220"/>
+      <c r="B43" s="219"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -56591,7 +56674,7 @@
       </c>
     </row>
     <row r="44" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="220"/>
+      <c r="B44" s="219"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -56667,7 +56750,7 @@
       </c>
     </row>
     <row r="45" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="220"/>
+      <c r="B45" s="219"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -56743,7 +56826,7 @@
       </c>
     </row>
     <row r="46" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="220"/>
+      <c r="B46" s="219"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -56819,7 +56902,7 @@
       </c>
     </row>
     <row r="47" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="220"/>
+      <c r="B47" s="219"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -56895,7 +56978,7 @@
       </c>
     </row>
     <row r="48" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="220"/>
+      <c r="B48" s="219"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -56971,7 +57054,7 @@
       </c>
     </row>
     <row r="49" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="220"/>
+      <c r="B49" s="219"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -57047,7 +57130,7 @@
       </c>
     </row>
     <row r="50" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="220"/>
+      <c r="B50" s="219"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -57125,7 +57208,7 @@
       </c>
     </row>
     <row r="51" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="220"/>
+      <c r="B51" s="219"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -57203,7 +57286,7 @@
       </c>
     </row>
     <row r="52" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="220"/>
+      <c r="B52" s="219"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -57281,7 +57364,7 @@
       </c>
     </row>
     <row r="53" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="220" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -57361,7 +57444,7 @@
       </c>
     </row>
     <row r="54" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="221"/>
+      <c r="B54" s="220"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -57439,7 +57522,7 @@
       </c>
     </row>
     <row r="55" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="221"/>
+      <c r="B55" s="220"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -57517,7 +57600,7 @@
       </c>
     </row>
     <row r="56" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="221"/>
+      <c r="B56" s="220"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -57593,7 +57676,7 @@
       </c>
     </row>
     <row r="57" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="221"/>
+      <c r="B57" s="220"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -57671,7 +57754,7 @@
       </c>
     </row>
     <row r="58" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B58" s="221"/>
+      <c r="B58" s="220"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -57747,7 +57830,7 @@
       </c>
     </row>
     <row r="59" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="221"/>
+      <c r="B59" s="220"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -57825,7 +57908,7 @@
       </c>
     </row>
     <row r="60" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B60" s="221"/>
+      <c r="B60" s="220"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -57903,7 +57986,7 @@
       </c>
     </row>
     <row r="61" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B61" s="222" t="s">
+      <c r="B61" s="221" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -57981,7 +58064,7 @@
       </c>
     </row>
     <row r="62" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="222"/>
+      <c r="B62" s="221"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -58059,7 +58142,7 @@
       </c>
     </row>
     <row r="63" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="222"/>
+      <c r="B63" s="221"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -58137,7 +58220,7 @@
       </c>
     </row>
     <row r="64" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="222"/>
+      <c r="B64" s="221"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -58215,7 +58298,7 @@
       </c>
     </row>
     <row r="65" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="222"/>
+      <c r="B65" s="221"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -58245,7 +58328,7 @@
       <c r="AA65" s="5"/>
     </row>
     <row r="66" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="222"/>
+      <c r="B66" s="221"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -58275,7 +58358,7 @@
       <c r="AA66" s="5"/>
     </row>
     <row r="67" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="222"/>
+      <c r="B67" s="221"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -58305,7 +58388,7 @@
       <c r="AA67" s="1"/>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B68" s="212" t="s">
+      <c r="B68" s="211" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -58326,7 +58409,7 @@
       <c r="Q68" s="105"/>
     </row>
     <row r="69" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B69" s="212"/>
+      <c r="B69" s="211"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -58345,7 +58428,7 @@
       <c r="Q69" s="105"/>
     </row>
     <row r="70" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B70" s="212"/>
+      <c r="B70" s="211"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -58364,7 +58447,7 @@
       <c r="Q70" s="105"/>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B71" s="212"/>
+      <c r="B71" s="211"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -58383,7 +58466,7 @@
       <c r="Q71" s="105"/>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B72" s="213"/>
+      <c r="B72" s="212"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>

</xml_diff>

<commit_message>
May 7 2025 update.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45813923-1D42-4A7C-82F9-95A17FBF4196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C4A67-1304-4474-B428-600A2CF2FF71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13159" uniqueCount="2731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13410" uniqueCount="2797">
   <si>
     <t>Description</t>
   </si>
@@ -8217,6 +8217,204 @@
   </si>
   <si>
     <t>Jonas Golisch</t>
+  </si>
+  <si>
+    <t>2_IUS_Electricity_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>around 20 technologies</t>
+  </si>
+  <si>
+    <t>single country resolution</t>
+  </si>
+  <si>
+    <t>1970-2023</t>
+  </si>
+  <si>
+    <t>annual values, technology specific</t>
+  </si>
+  <si>
+    <t>In use stocks for the different technology groups included in the CIRCOMOD project. Electricity generation and distribution</t>
+  </si>
+  <si>
+    <t>in-use stocks; age-cohort; regional stocks; electricity infrastructure; electricity grid; electricity generation; electricity distribution</t>
+  </si>
+  <si>
+    <t>Value(U,g,t,r,L)</t>
+  </si>
+  <si>
+    <t>In-use stock of electricity transmission, 35 kV in use phase - electricity infrastructure in China in 2014 measured as lenght is 484295 km.</t>
+  </si>
+  <si>
+    <t>[Data type] of [Aspect 2] in [Aspect 1] in [Aspect 4] in [Aspect 3] measured as [Aspect 5] is [Value].</t>
+  </si>
+  <si>
+    <t>Marcel Geller and Stefan Pauliuk</t>
+  </si>
+  <si>
+    <t>3_MC_Furniture_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>furniture</t>
+  </si>
+  <si>
+    <t>five different types of furniture</t>
+  </si>
+  <si>
+    <t>typical furniture materials</t>
+  </si>
+  <si>
+    <t>15 material groups</t>
+  </si>
+  <si>
+    <t>Material composition of furniture, taken from Y. Ikeda (2023). Values are an average of existing data in literature, thus not really representing World data but rather unspecific to a region.</t>
+  </si>
+  <si>
+    <t>material; material composition; furniture</t>
+  </si>
+  <si>
+    <t>Taken from Ikeda, Y. (2023). Quantifying materials in household furniture: A case study of dynamic furniture stock in American homes. Values are an average of existing data in literature, thus not really representing World data but rather unspecific to a region.</t>
+  </si>
+  <si>
+    <t>Value(m,g,U,r,c)</t>
+  </si>
+  <si>
+    <t>Mass per unit of wood, solid, in chair, upholstered in use phase - furniture built in ca. 2020 in Global is 16.9113 kg/unit.</t>
+  </si>
+  <si>
+    <t>[Layer] of [Aspect 1] in [Aspect 2] in [Aspect 3] built in [Aspect 5] in [Aspect 4] is [Value].</t>
+  </si>
+  <si>
+    <t>Y. IKEDA</t>
+  </si>
+  <si>
+    <t>https://repository.tudelft.nl/islandora/object/uuid%3Afec8d24f-f856-43a4-8673-570cc6de9d01</t>
+  </si>
+  <si>
+    <t>tables and figures in original source</t>
+  </si>
+  <si>
+    <t>Ikeda, Y. (2023). Quantifying materials in household furniture: A case study of dynamic furniture stock in American homes.</t>
+  </si>
+  <si>
+    <t>4_PE_EnergyIntensity_Fabrication_Furniture_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>Energy per unit of output</t>
+  </si>
+  <si>
+    <t>furniture manufacturing</t>
+  </si>
+  <si>
+    <t>six different types of furniture</t>
+  </si>
+  <si>
+    <t>Germany, China, United States</t>
+  </si>
+  <si>
+    <t>country average</t>
+  </si>
+  <si>
+    <t>2005-2016</t>
+  </si>
+  <si>
+    <t>Per unit-of-output energy demand of furniture manufacturing</t>
+  </si>
+  <si>
+    <t>furniture; manufacturing; energy intensity; unit process;</t>
+  </si>
+  <si>
+    <t>Value(n,g,p,c,r)</t>
+  </si>
+  <si>
+    <t>Process extension of energy per unit of output of energy carrier all (unspecified) in manufacturing of furniture per unit of desk in United States in 2005 was 3490 MJ/item.</t>
+  </si>
+  <si>
+    <t>[Data type] of [Layer] of [Aspect 1] in [Aspect 3] for producing [Aspect 2] in [Aspect 5] in [Aspect 4] is [Value].</t>
+  </si>
+  <si>
+    <t>4_PY_Asphalt_Recycling_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>road maintenance</t>
+  </si>
+  <si>
+    <t>asphalt pavement</t>
+  </si>
+  <si>
+    <t>one infrastructure type</t>
+  </si>
+  <si>
+    <t>asphalt</t>
+  </si>
+  <si>
+    <t>one material category</t>
+  </si>
+  <si>
+    <t>USA, Europe</t>
+  </si>
+  <si>
+    <t>country-level values</t>
+  </si>
+  <si>
+    <t>2019-ca. 2050</t>
+  </si>
+  <si>
+    <t>most values for around 2020-2022</t>
+  </si>
+  <si>
+    <t>recycling yield for extracting asphalt from asphalt pavement in road maintenance</t>
+  </si>
+  <si>
+    <t>asphalt; pavement; recycling;</t>
+  </si>
+  <si>
+    <t>Value(v,b,B,f,p,t,r)</t>
+  </si>
+  <si>
+    <t>Mass ratio for strategy Recycle of asphalt in asphalt pavement into recycled asphalt in process road maintenance in 2022 in Croatia is 63%.</t>
+  </si>
+  <si>
+    <t>[Layer] for [Aspect 1] of [Aspect 2] in [Aspect 3] into [Aspect 4] in process [Aspect 5] in [Aspect 6] in [Aspect 7] is [Value].</t>
+  </si>
+  <si>
+    <t>4_PY_Fabrication_Furniture_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>furniture manufacturing processes</t>
+  </si>
+  <si>
+    <t>15 different types of furniture components</t>
+  </si>
+  <si>
+    <t>Wood yield factors for furniture manufacturing, 15 different components of furniture</t>
+  </si>
+  <si>
+    <t>furniture; manufacturing; yield factor; unit process; wood</t>
+  </si>
+  <si>
+    <t>Value(b,k,F,p,t,r)</t>
+  </si>
+  <si>
+    <t>Mass ratio of yield coefficient of wood into boards from butt log in furniture in manufacturing of furniture - sawing (3X) in Sweden in 2015 is 37%.</t>
+  </si>
+  <si>
+    <t>[Layer] of [Data type] of [Aspect 1] into [Aspect 2] in [Aspect 3] in process [Aspect 4] in [Aspect 5] in [Aspect 6] is [Value].</t>
+  </si>
+  <si>
+    <t>Broman &amp; Fredriksson</t>
+  </si>
+  <si>
+    <t>https://urn.kb.se/resolve?urn=urn:nbn:se:ltu:diva-28597</t>
+  </si>
+  <si>
+    <t>Table in report</t>
+  </si>
+  <si>
+    <t>Broman &amp; Fredriksson 2015. Effect of Raw Material on Yield in a Furniture Production Process. Proceedings of the 22nd International Wood Machining Seminar, June 14-17, 2015 Qebec City, Canada</t>
+  </si>
+  <si>
+    <t>May 7, 2025 update</t>
   </si>
 </sst>
 </file>
@@ -8608,7 +8806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -9009,6 +9207,21 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -12747,10 +12960,10 @@
   <dimension ref="A1:GW74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="ES27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="FA24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="FN40" sqref="FN40"/>
+      <selection pane="bottomRight" activeCell="FQ1" sqref="FQ1:FQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -12811,7 +13024,7 @@
     <col min="70" max="16384" width="11.5546875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:168" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:173" x14ac:dyDescent="0.4">
       <c r="C1" s="73" t="s">
         <v>269</v>
       </c>
@@ -13283,8 +13496,13 @@
       <c r="FJ1" s="174"/>
       <c r="FK1" s="174"/>
       <c r="FL1" s="174"/>
+      <c r="FM1" s="174"/>
+      <c r="FN1" s="174"/>
+      <c r="FO1" s="174"/>
+      <c r="FP1" s="174"/>
+      <c r="FQ1" s="174"/>
     </row>
-    <row r="2" spans="1:168" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B2" s="34" t="s">
         <v>183</v>
       </c>
@@ -13604,8 +13822,23 @@
       <c r="FL2" s="154" t="s">
         <v>2729</v>
       </c>
+      <c r="FM2" s="154" t="s">
+        <v>2796</v>
+      </c>
+      <c r="FN2" s="154" t="s">
+        <v>2796</v>
+      </c>
+      <c r="FO2" s="154" t="s">
+        <v>2796</v>
+      </c>
+      <c r="FP2" s="154" t="s">
+        <v>2796</v>
+      </c>
+      <c r="FQ2" s="154" t="s">
+        <v>2796</v>
+      </c>
     </row>
-    <row r="3" spans="1:168" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:173" x14ac:dyDescent="0.4">
       <c r="B3" s="58"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -13858,7 +14091,7 @@
       <c r="DS3" s="105"/>
       <c r="DT3" s="105"/>
     </row>
-    <row r="4" spans="1:168" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:173" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>1</v>
       </c>
@@ -14116,7 +14349,7 @@
       <c r="DS4" s="105"/>
       <c r="DT4" s="105"/>
     </row>
-    <row r="5" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="41">
         <v>2</v>
       </c>
@@ -14619,8 +14852,23 @@
       <c r="FL5" s="41" t="s">
         <v>2722</v>
       </c>
+      <c r="FM5" s="222" t="s">
+        <v>2731</v>
+      </c>
+      <c r="FN5" s="187" t="s">
+        <v>2742</v>
+      </c>
+      <c r="FO5" s="187" t="s">
+        <v>2757</v>
+      </c>
+      <c r="FP5" s="187" t="s">
+        <v>2769</v>
+      </c>
+      <c r="FQ5" s="187" t="s">
+        <v>2784</v>
+      </c>
     </row>
-    <row r="6" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="92">
         <v>3</v>
       </c>
@@ -15121,8 +15369,23 @@
       <c r="FL6" s="41" t="s">
         <v>11</v>
       </c>
+      <c r="FM6" s="222" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FN6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FO6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FP6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FQ6" s="187" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="7" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="92">
         <v>4</v>
       </c>
@@ -15625,8 +15888,23 @@
       <c r="FL7" s="41">
         <v>27</v>
       </c>
+      <c r="FM7" s="222">
+        <v>21</v>
+      </c>
+      <c r="FN7" s="187">
+        <v>20</v>
+      </c>
+      <c r="FO7" s="187">
+        <v>20</v>
+      </c>
+      <c r="FP7" s="187">
+        <v>20</v>
+      </c>
+      <c r="FQ7" s="187">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="92">
         <v>5</v>
       </c>
@@ -16129,8 +16407,23 @@
       <c r="FL8" s="41">
         <v>6</v>
       </c>
+      <c r="FM8" s="222">
+        <v>2</v>
+      </c>
+      <c r="FN8" s="187">
+        <v>3</v>
+      </c>
+      <c r="FO8" s="187">
+        <v>4</v>
+      </c>
+      <c r="FP8" s="187">
+        <v>4</v>
+      </c>
+      <c r="FQ8" s="187">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="92">
         <v>6</v>
       </c>
@@ -16633,8 +16926,23 @@
       <c r="FL9" s="41" t="s">
         <v>2708</v>
       </c>
+      <c r="FM9" s="222" t="s">
+        <v>31</v>
+      </c>
+      <c r="FN9" s="187" t="s">
+        <v>846</v>
+      </c>
+      <c r="FO9" s="187" t="s">
+        <v>179</v>
+      </c>
+      <c r="FP9" s="187" t="s">
+        <v>94</v>
+      </c>
+      <c r="FQ9" s="187" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="10" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="92">
         <v>7</v>
       </c>
@@ -17137,8 +17445,23 @@
       <c r="FL10" s="41" t="s">
         <v>1091</v>
       </c>
+      <c r="FM10" s="222" t="s">
+        <v>1025</v>
+      </c>
+      <c r="FN10" s="187" t="s">
+        <v>824</v>
+      </c>
+      <c r="FO10" s="187" t="s">
+        <v>2758</v>
+      </c>
+      <c r="FP10" s="187" t="s">
+        <v>5</v>
+      </c>
+      <c r="FQ10" s="187" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:168" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:173" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="92">
         <v>8</v>
       </c>
@@ -17641,8 +17964,23 @@
       <c r="FL11" s="41" t="s">
         <v>779</v>
       </c>
+      <c r="FM11" s="222" t="s">
+        <v>782</v>
+      </c>
+      <c r="FN11" s="188" t="s">
+        <v>782</v>
+      </c>
+      <c r="FO11" s="188" t="s">
+        <v>2759</v>
+      </c>
+      <c r="FP11" s="188" t="s">
+        <v>2770</v>
+      </c>
+      <c r="FQ11" s="188" t="s">
+        <v>2785</v>
+      </c>
     </row>
-    <row r="12" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="92">
         <v>9</v>
       </c>
@@ -18143,8 +18481,23 @@
       <c r="FL12" s="41" t="s">
         <v>868</v>
       </c>
+      <c r="FM12" s="222" t="s">
+        <v>152</v>
+      </c>
+      <c r="FN12" s="187" t="s">
+        <v>2274</v>
+      </c>
+      <c r="FO12" s="187" t="s">
+        <v>2274</v>
+      </c>
+      <c r="FP12" s="187" t="s">
+        <v>2274</v>
+      </c>
+      <c r="FQ12" s="187" t="s">
+        <v>2274</v>
+      </c>
     </row>
-    <row r="13" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="92">
         <v>10</v>
       </c>
@@ -18645,8 +18998,23 @@
       <c r="FL13" s="41" t="s">
         <v>11</v>
       </c>
+      <c r="FM13" s="222" t="s">
+        <v>2641</v>
+      </c>
+      <c r="FN13" s="187" t="s">
+        <v>2743</v>
+      </c>
+      <c r="FO13" s="188" t="s">
+        <v>2743</v>
+      </c>
+      <c r="FP13" s="188" t="s">
+        <v>2771</v>
+      </c>
+      <c r="FQ13" s="188" t="s">
+        <v>2743</v>
+      </c>
     </row>
-    <row r="14" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="92">
         <v>11</v>
       </c>
@@ -19147,8 +19515,23 @@
       <c r="FL14" s="41" t="s">
         <v>11</v>
       </c>
+      <c r="FM14" s="222" t="s">
+        <v>2732</v>
+      </c>
+      <c r="FN14" s="187" t="s">
+        <v>2744</v>
+      </c>
+      <c r="FO14" s="187" t="s">
+        <v>2760</v>
+      </c>
+      <c r="FP14" s="187" t="s">
+        <v>2772</v>
+      </c>
+      <c r="FQ14" s="187" t="s">
+        <v>2786</v>
+      </c>
     </row>
-    <row r="15" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="92">
         <v>12</v>
       </c>
@@ -19649,8 +20032,23 @@
       <c r="FL15" s="41" t="s">
         <v>2723</v>
       </c>
+      <c r="FM15" s="222" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN15" s="187" t="s">
+        <v>2745</v>
+      </c>
+      <c r="FO15" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP15" s="188" t="s">
+        <v>2773</v>
+      </c>
+      <c r="FQ15" s="187" t="s">
+        <v>565</v>
+      </c>
     </row>
-    <row r="16" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="92">
         <v>13</v>
       </c>
@@ -20151,8 +20549,23 @@
       <c r="FL16" s="41" t="s">
         <v>2724</v>
       </c>
+      <c r="FM16" s="222" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN16" s="187" t="s">
+        <v>2746</v>
+      </c>
+      <c r="FO16" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP16" s="187" t="s">
+        <v>2774</v>
+      </c>
+      <c r="FQ16" s="187" t="s">
+        <v>1680</v>
+      </c>
     </row>
-    <row r="17" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="92">
         <v>14</v>
       </c>
@@ -20653,8 +21066,23 @@
       <c r="FL17" s="41" t="s">
         <v>1422</v>
       </c>
+      <c r="FM17" s="222" t="s">
+        <v>819</v>
+      </c>
+      <c r="FN17" s="187" t="s">
+        <v>819</v>
+      </c>
+      <c r="FO17" s="187" t="s">
+        <v>2761</v>
+      </c>
+      <c r="FP17" s="187" t="s">
+        <v>2775</v>
+      </c>
+      <c r="FQ17" s="187" t="s">
+        <v>527</v>
+      </c>
     </row>
-    <row r="18" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="92">
         <v>15</v>
       </c>
@@ -21155,8 +21583,23 @@
       <c r="FL18" s="41" t="s">
         <v>2711</v>
       </c>
+      <c r="FM18" s="222" t="s">
+        <v>2733</v>
+      </c>
+      <c r="FN18" s="187" t="s">
+        <v>2050</v>
+      </c>
+      <c r="FO18" s="187" t="s">
+        <v>2762</v>
+      </c>
+      <c r="FP18" s="187" t="s">
+        <v>2776</v>
+      </c>
+      <c r="FQ18" s="187" t="s">
+        <v>2762</v>
+      </c>
     </row>
-    <row r="19" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="92">
         <v>16</v>
       </c>
@@ -21657,8 +22100,23 @@
       <c r="FL19" s="41">
         <v>2020</v>
       </c>
+      <c r="FM19" s="222" t="s">
+        <v>2734</v>
+      </c>
+      <c r="FN19" s="187" t="s">
+        <v>2154</v>
+      </c>
+      <c r="FO19" s="187" t="s">
+        <v>2763</v>
+      </c>
+      <c r="FP19" s="187" t="s">
+        <v>2777</v>
+      </c>
+      <c r="FQ19" s="187">
+        <v>2015</v>
+      </c>
     </row>
-    <row r="20" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="92">
         <v>17</v>
       </c>
@@ -22159,8 +22617,23 @@
       <c r="FL20" s="41" t="s">
         <v>2712</v>
       </c>
+      <c r="FM20" s="222" t="s">
+        <v>2735</v>
+      </c>
+      <c r="FN20" s="187" t="s">
+        <v>2154</v>
+      </c>
+      <c r="FO20" s="187" t="s">
+        <v>2349</v>
+      </c>
+      <c r="FP20" s="187" t="s">
+        <v>2778</v>
+      </c>
+      <c r="FQ20" s="187" t="s">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="21" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="92">
         <v>18</v>
       </c>
@@ -22657,8 +23130,23 @@
       <c r="FL21" s="41" t="s">
         <v>2725</v>
       </c>
+      <c r="FM21" s="222" t="s">
+        <v>2736</v>
+      </c>
+      <c r="FN21" s="187" t="s">
+        <v>2747</v>
+      </c>
+      <c r="FO21" s="187" t="s">
+        <v>2764</v>
+      </c>
+      <c r="FP21" s="187" t="s">
+        <v>2779</v>
+      </c>
+      <c r="FQ21" s="187" t="s">
+        <v>2787</v>
+      </c>
     </row>
-    <row r="22" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="92">
         <v>19</v>
       </c>
@@ -23161,8 +23649,23 @@
       <c r="FL22" s="41" t="s">
         <v>2714</v>
       </c>
+      <c r="FM22" s="222" t="s">
+        <v>2737</v>
+      </c>
+      <c r="FN22" s="187" t="s">
+        <v>2748</v>
+      </c>
+      <c r="FO22" s="187" t="s">
+        <v>2765</v>
+      </c>
+      <c r="FP22" s="187" t="s">
+        <v>2780</v>
+      </c>
+      <c r="FQ22" s="187" t="s">
+        <v>2788</v>
+      </c>
     </row>
-    <row r="23" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="92">
         <v>20</v>
       </c>
@@ -23665,8 +24168,23 @@
       <c r="FL23" s="41" t="s">
         <v>141</v>
       </c>
+      <c r="FM23" s="222" t="s">
+        <v>169</v>
+      </c>
+      <c r="FN23" s="187" t="s">
+        <v>24</v>
+      </c>
+      <c r="FO23" s="187" t="s">
+        <v>634</v>
+      </c>
+      <c r="FP23" s="187" t="s">
+        <v>24</v>
+      </c>
+      <c r="FQ23" s="187" t="s">
+        <v>634</v>
+      </c>
     </row>
-    <row r="24" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="92">
         <v>21</v>
       </c>
@@ -24169,8 +24687,23 @@
       <c r="FL24" s="41">
         <v>137</v>
       </c>
+      <c r="FM24" s="222">
+        <v>1111</v>
+      </c>
+      <c r="FN24" s="155">
+        <v>75</v>
+      </c>
+      <c r="FO24" s="187">
+        <v>7</v>
+      </c>
+      <c r="FP24" s="187">
+        <v>51</v>
+      </c>
+      <c r="FQ24" s="187">
+        <v>18</v>
+      </c>
     </row>
-    <row r="25" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="92">
         <v>22</v>
       </c>
@@ -24668,8 +25201,23 @@
       <c r="FL25" s="41" t="s">
         <v>2726</v>
       </c>
+      <c r="FM25" s="223" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN25" s="155" t="s">
+        <v>2749</v>
+      </c>
+      <c r="FO25" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP25" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ25" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="26" spans="1:168" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:173" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="92">
         <v>23</v>
       </c>
@@ -25174,8 +25722,23 @@
       <c r="FL26" s="68" t="s">
         <v>1033</v>
       </c>
+      <c r="FM26" s="222" t="s">
+        <v>1440</v>
+      </c>
+      <c r="FN26" s="156" t="s">
+        <v>849</v>
+      </c>
+      <c r="FO26" s="187" t="s">
+        <v>713</v>
+      </c>
+      <c r="FP26" s="156" t="s">
+        <v>1441</v>
+      </c>
+      <c r="FQ26" s="156" t="s">
+        <v>852</v>
+      </c>
     </row>
-    <row r="27" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="92">
         <v>24</v>
       </c>
@@ -25678,8 +26241,23 @@
       <c r="FL27" s="68">
         <v>4</v>
       </c>
+      <c r="FM27" s="223">
+        <v>6</v>
+      </c>
+      <c r="FN27" s="155">
+        <v>4</v>
+      </c>
+      <c r="FO27" s="187">
+        <v>10</v>
+      </c>
+      <c r="FP27" s="155">
+        <v>86</v>
+      </c>
+      <c r="FQ27" s="155">
+        <v>4</v>
+      </c>
     </row>
-    <row r="28" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="92">
         <v>25</v>
       </c>
@@ -26180,8 +26758,23 @@
       <c r="FL28" s="68" t="s">
         <v>1087</v>
       </c>
+      <c r="FM28" s="222" t="s">
+        <v>696</v>
+      </c>
+      <c r="FN28" s="187" t="s">
+        <v>696</v>
+      </c>
+      <c r="FO28" s="187" t="s">
+        <v>696</v>
+      </c>
+      <c r="FP28" s="156" t="s">
+        <v>852</v>
+      </c>
+      <c r="FQ28" s="187" t="s">
+        <v>1640</v>
+      </c>
     </row>
-    <row r="29" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="92">
         <v>26</v>
       </c>
@@ -26682,8 +27275,23 @@
       <c r="FL29" s="68">
         <v>18</v>
       </c>
+      <c r="FM29" s="222">
+        <v>7</v>
+      </c>
+      <c r="FN29" s="187">
+        <v>7</v>
+      </c>
+      <c r="FO29" s="187">
+        <v>7</v>
+      </c>
+      <c r="FP29" s="155">
+        <v>4</v>
+      </c>
+      <c r="FQ29" s="155">
+        <v>90</v>
+      </c>
     </row>
-    <row r="30" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="92">
         <v>27</v>
       </c>
@@ -27184,8 +27792,23 @@
       <c r="FL30" s="68" t="s">
         <v>1657</v>
       </c>
+      <c r="FM30" s="222" t="s">
+        <v>702</v>
+      </c>
+      <c r="FN30" s="156" t="s">
+        <v>1440</v>
+      </c>
+      <c r="FO30" s="187" t="s">
+        <v>697</v>
+      </c>
+      <c r="FP30" s="187" t="s">
+        <v>707</v>
+      </c>
+      <c r="FQ30" s="187" t="s">
+        <v>799</v>
+      </c>
     </row>
-    <row r="31" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="92">
         <v>28</v>
       </c>
@@ -27686,8 +28309,23 @@
       <c r="FL31" s="68">
         <v>93</v>
       </c>
+      <c r="FM31" s="222">
+        <v>3</v>
+      </c>
+      <c r="FN31" s="155">
+        <v>6</v>
+      </c>
+      <c r="FO31" s="187">
+        <v>6</v>
+      </c>
+      <c r="FP31" s="155">
+        <v>7</v>
+      </c>
+      <c r="FQ31" s="155">
+        <v>7</v>
+      </c>
     </row>
-    <row r="32" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="92">
         <v>29</v>
       </c>
@@ -28188,8 +28826,23 @@
       <c r="FL32" s="68" t="s">
         <v>698</v>
       </c>
+      <c r="FM32" s="222" t="s">
+        <v>698</v>
+      </c>
+      <c r="FN32" s="188" t="s">
+        <v>698</v>
+      </c>
+      <c r="FO32" s="187" t="s">
+        <v>704</v>
+      </c>
+      <c r="FP32" s="187" t="s">
+        <v>706</v>
+      </c>
+      <c r="FQ32" s="187" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="33" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="92">
         <v>30</v>
       </c>
@@ -28690,8 +29343,23 @@
       <c r="FL33" s="68">
         <v>2</v>
       </c>
+      <c r="FM33" s="222">
+        <v>89</v>
+      </c>
+      <c r="FN33" s="188">
+        <v>2</v>
+      </c>
+      <c r="FO33" s="187">
+        <v>14</v>
+      </c>
+      <c r="FP33" s="155">
+        <v>4</v>
+      </c>
+      <c r="FQ33" s="155">
+        <v>6</v>
+      </c>
     </row>
-    <row r="34" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="92">
         <v>31</v>
       </c>
@@ -29192,8 +29860,23 @@
       <c r="FL34" s="68" t="s">
         <v>702</v>
       </c>
+      <c r="FM34" s="224" t="s">
+        <v>1034</v>
+      </c>
+      <c r="FN34" s="188" t="s">
+        <v>704</v>
+      </c>
+      <c r="FO34" s="156" t="s">
+        <v>698</v>
+      </c>
+      <c r="FP34" s="187" t="s">
+        <v>697</v>
+      </c>
+      <c r="FQ34" s="187" t="s">
+        <v>702</v>
+      </c>
     </row>
-    <row r="35" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="92">
         <v>32</v>
       </c>
@@ -29694,8 +30377,23 @@
       <c r="FL35" s="68">
         <v>3</v>
       </c>
+      <c r="FM35" s="224">
+        <v>20</v>
+      </c>
+      <c r="FN35" s="188">
+        <v>9</v>
+      </c>
+      <c r="FO35" s="187">
+        <v>2</v>
+      </c>
+      <c r="FP35" s="155">
+        <v>6</v>
+      </c>
+      <c r="FQ35" s="155">
+        <v>3</v>
+      </c>
     </row>
-    <row r="36" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="92">
         <v>33</v>
       </c>
@@ -30196,8 +30894,23 @@
       <c r="FL36" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM36" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN36" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO36" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP36" s="187" t="s">
+        <v>702</v>
+      </c>
+      <c r="FQ36" s="187" t="s">
+        <v>698</v>
+      </c>
     </row>
-    <row r="37" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="92">
         <v>34</v>
       </c>
@@ -30698,8 +31411,23 @@
       <c r="FL37" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM37" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN37" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO37" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP37" s="155">
+        <v>3</v>
+      </c>
+      <c r="FQ37" s="155">
+        <v>2</v>
+      </c>
     </row>
-    <row r="38" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="92">
         <v>35</v>
       </c>
@@ -31200,8 +31928,23 @@
       <c r="FL38" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM38" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN38" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO38" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP38" s="187" t="s">
+        <v>698</v>
+      </c>
+      <c r="FQ38" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="39" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="92">
         <v>36</v>
       </c>
@@ -31702,8 +32445,23 @@
       <c r="FL39" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM39" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN39" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO39" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP39" s="155">
+        <v>2</v>
+      </c>
+      <c r="FQ39" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="40" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="92">
         <v>37</v>
       </c>
@@ -32204,8 +32962,23 @@
       <c r="FL40" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM40" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN40" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO40" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP40" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ40" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="92">
         <v>38</v>
       </c>
@@ -32706,8 +33479,23 @@
       <c r="FL41" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM41" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN41" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO41" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP41" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ41" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="42" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="92">
         <v>39</v>
       </c>
@@ -33208,8 +33996,23 @@
       <c r="FL42" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM42" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN42" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO42" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP42" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ42" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="92">
         <v>40</v>
       </c>
@@ -33710,8 +34513,23 @@
       <c r="FL43" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM43" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN43" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO43" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP43" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ43" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="44" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="92">
         <v>41</v>
       </c>
@@ -34212,8 +35030,23 @@
       <c r="FL44" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM44" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN44" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO44" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP44" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ44" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="45" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="92">
         <v>42</v>
       </c>
@@ -34714,8 +35547,23 @@
       <c r="FL45" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM45" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN45" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO45" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP45" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ45" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="46" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="92">
         <v>43</v>
       </c>
@@ -35216,8 +36064,23 @@
       <c r="FL46" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM46" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN46" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO46" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP46" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ46" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="47" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="92">
         <v>44</v>
       </c>
@@ -35718,8 +36581,23 @@
       <c r="FL47" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM47" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN47" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO47" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP47" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ47" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="48" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="92">
         <v>45</v>
       </c>
@@ -36220,8 +37098,23 @@
       <c r="FL48" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM48" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN48" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO48" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP48" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ48" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="49" spans="1:168" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="92">
         <v>46</v>
       </c>
@@ -36722,8 +37615,23 @@
       <c r="FL49" s="68" t="s">
         <v>11</v>
       </c>
+      <c r="FM49" s="120" t="s">
+        <v>11</v>
+      </c>
+      <c r="FN49" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO49" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP49" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ49" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="50" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="92">
         <v>47</v>
       </c>
@@ -37226,8 +38134,23 @@
       <c r="FL50" s="41" t="s">
         <v>2716</v>
       </c>
+      <c r="FM50" s="187" t="s">
+        <v>2738</v>
+      </c>
+      <c r="FN50" s="155" t="s">
+        <v>2750</v>
+      </c>
+      <c r="FO50" s="187" t="s">
+        <v>2766</v>
+      </c>
+      <c r="FP50" s="187" t="s">
+        <v>2781</v>
+      </c>
+      <c r="FQ50" s="187" t="s">
+        <v>2789</v>
+      </c>
     </row>
-    <row r="51" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="92">
         <v>48</v>
       </c>
@@ -37730,8 +38653,23 @@
       <c r="FL51" s="41" t="s">
         <v>2727</v>
       </c>
+      <c r="FM51" s="155" t="s">
+        <v>2739</v>
+      </c>
+      <c r="FN51" s="155" t="s">
+        <v>2751</v>
+      </c>
+      <c r="FO51" s="155" t="s">
+        <v>2767</v>
+      </c>
+      <c r="FP51" s="155" t="s">
+        <v>2782</v>
+      </c>
+      <c r="FQ51" s="155" t="s">
+        <v>2790</v>
+      </c>
     </row>
-    <row r="52" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="92">
         <v>49</v>
       </c>
@@ -38234,8 +39172,23 @@
       <c r="FL52" s="41" t="s">
         <v>2718</v>
       </c>
+      <c r="FM52" s="155" t="s">
+        <v>2740</v>
+      </c>
+      <c r="FN52" s="155" t="s">
+        <v>2752</v>
+      </c>
+      <c r="FO52" s="155" t="s">
+        <v>2768</v>
+      </c>
+      <c r="FP52" s="155" t="s">
+        <v>2783</v>
+      </c>
+      <c r="FQ52" s="155" t="s">
+        <v>2791</v>
+      </c>
     </row>
-    <row r="53" spans="1:168" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:173" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="92">
         <v>50</v>
       </c>
@@ -38740,8 +39693,23 @@
       <c r="FL53" s="41" t="s">
         <v>860</v>
       </c>
+      <c r="FM53" s="223" t="s">
+        <v>207</v>
+      </c>
+      <c r="FN53" s="155" t="s">
+        <v>206</v>
+      </c>
+      <c r="FO53" s="155" t="s">
+        <v>206</v>
+      </c>
+      <c r="FP53" s="155" t="s">
+        <v>206</v>
+      </c>
+      <c r="FQ53" s="155" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="54" spans="1:168" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A54" s="92">
         <v>51</v>
       </c>
@@ -39244,8 +40212,23 @@
       <c r="FL54" s="41" t="s">
         <v>858</v>
       </c>
+      <c r="FM54" s="223" t="s">
+        <v>858</v>
+      </c>
+      <c r="FN54" s="155" t="s">
+        <v>858</v>
+      </c>
+      <c r="FO54" s="155" t="s">
+        <v>858</v>
+      </c>
+      <c r="FP54" s="155" t="s">
+        <v>858</v>
+      </c>
+      <c r="FQ54" s="155" t="s">
+        <v>858</v>
+      </c>
     </row>
-    <row r="55" spans="1:168" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A55" s="92">
         <v>52</v>
       </c>
@@ -39748,8 +40731,23 @@
       <c r="FL55" s="41" t="s">
         <v>2606</v>
       </c>
+      <c r="FM55" s="223" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FN55" s="155" t="s">
+        <v>2753</v>
+      </c>
+      <c r="FO55" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FP55" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FQ55" s="155" t="s">
+        <v>2792</v>
+      </c>
     </row>
-    <row r="56" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="92">
         <v>53</v>
       </c>
@@ -40250,8 +41248,23 @@
       <c r="FL56" s="41" t="s">
         <v>2728</v>
       </c>
+      <c r="FM56" s="223" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FN56" s="155" t="s">
+        <v>2754</v>
+      </c>
+      <c r="FO56" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FP56" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FQ56" s="155" t="s">
+        <v>2793</v>
+      </c>
     </row>
-    <row r="57" spans="1:168" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A57" s="92">
         <v>54</v>
       </c>
@@ -40754,8 +41767,23 @@
       <c r="FL57" s="41" t="s">
         <v>2720</v>
       </c>
+      <c r="FM57" s="223" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FN57" s="155" t="s">
+        <v>2755</v>
+      </c>
+      <c r="FO57" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FP57" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FQ57" s="155" t="s">
+        <v>2794</v>
+      </c>
     </row>
-    <row r="58" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="92">
         <v>55</v>
       </c>
@@ -41229,8 +42257,23 @@
       <c r="FL58" s="41" t="s">
         <v>2728</v>
       </c>
+      <c r="FM58" s="223" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FN58" s="155" t="s">
+        <v>2756</v>
+      </c>
+      <c r="FO58" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FP58" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FQ58" s="155" t="s">
+        <v>2795</v>
+      </c>
     </row>
-    <row r="59" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="92">
         <v>56</v>
       </c>
@@ -41733,8 +42776,23 @@
       <c r="FL59" s="41" t="s">
         <v>2728</v>
       </c>
+      <c r="FM59" s="223" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FN59" s="155" t="s">
+        <v>2756</v>
+      </c>
+      <c r="FO59" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FP59" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FQ59" s="155" t="s">
+        <v>2795</v>
+      </c>
     </row>
-    <row r="60" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="92">
         <v>57</v>
       </c>
@@ -42237,8 +43295,23 @@
       <c r="FL60" s="41">
         <v>1</v>
       </c>
+      <c r="FM60" s="224">
+        <v>1</v>
+      </c>
+      <c r="FN60" s="188">
+        <v>1</v>
+      </c>
+      <c r="FO60" s="188">
+        <v>1</v>
+      </c>
+      <c r="FP60" s="188">
+        <v>1</v>
+      </c>
+      <c r="FQ60" s="188">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:168" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:173" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="92">
         <v>58</v>
       </c>
@@ -42741,8 +43814,23 @@
       <c r="FL61" s="157">
         <v>45727</v>
       </c>
+      <c r="FM61" s="225">
+        <v>45413</v>
+      </c>
+      <c r="FN61" s="189">
+        <v>45413</v>
+      </c>
+      <c r="FO61" s="189">
+        <v>45413</v>
+      </c>
+      <c r="FP61" s="189">
+        <v>45413</v>
+      </c>
+      <c r="FQ61" s="189">
+        <v>45413</v>
+      </c>
     </row>
-    <row r="62" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="92">
         <v>59</v>
       </c>
@@ -43245,8 +44333,23 @@
       <c r="FL62" s="157">
         <v>45769</v>
       </c>
+      <c r="FM62" s="226">
+        <v>45709</v>
+      </c>
+      <c r="FN62" s="190">
+        <v>45709</v>
+      </c>
+      <c r="FO62" s="190">
+        <v>45709</v>
+      </c>
+      <c r="FP62" s="190">
+        <v>45709</v>
+      </c>
+      <c r="FQ62" s="190">
+        <v>45709</v>
+      </c>
     </row>
-    <row r="63" spans="1:168" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="92">
         <v>60</v>
       </c>
@@ -43749,8 +44852,23 @@
       <c r="FL63" s="157" t="s">
         <v>2730</v>
       </c>
+      <c r="FM63" s="120" t="s">
+        <v>2331</v>
+      </c>
+      <c r="FN63" s="155" t="s">
+        <v>2386</v>
+      </c>
+      <c r="FO63" s="155" t="s">
+        <v>2386</v>
+      </c>
+      <c r="FP63" s="155" t="s">
+        <v>2386</v>
+      </c>
+      <c r="FQ63" s="155" t="s">
+        <v>2386</v>
+      </c>
     </row>
-    <row r="64" spans="1:168" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A64" s="92">
         <v>61</v>
       </c>
@@ -44252,6 +45370,21 @@
       </c>
       <c r="FL64" s="115" t="s">
         <v>2721</v>
+      </c>
+      <c r="FM64" s="120" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FN64" s="155" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FO64" s="155" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FP64" s="155" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FQ64" s="155" t="s">
+        <v>2332</v>
       </c>
     </row>
     <row r="65" spans="1:205" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -44460,6 +45593,21 @@
       <c r="FL65" s="157">
         <v>45772</v>
       </c>
+      <c r="FM65" s="226">
+        <v>45784</v>
+      </c>
+      <c r="FN65" s="190">
+        <v>45781</v>
+      </c>
+      <c r="FO65" s="190">
+        <v>45782</v>
+      </c>
+      <c r="FP65" s="190">
+        <v>45782</v>
+      </c>
+      <c r="FQ65" s="190">
+        <v>45782</v>
+      </c>
     </row>
     <row r="66" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A66" s="92">
@@ -44663,6 +45811,21 @@
         <v>30</v>
       </c>
       <c r="FL66" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="FM66" s="47" t="s">
+        <v>2741</v>
+      </c>
+      <c r="FN66" s="156" t="s">
+        <v>30</v>
+      </c>
+      <c r="FO66" s="156" t="s">
+        <v>30</v>
+      </c>
+      <c r="FP66" s="156" t="s">
+        <v>30</v>
+      </c>
+      <c r="FQ66" s="156" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Early May 2025 classification and lookup table update.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C4A67-1304-4474-B428-600A2CF2FF71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38410A87-9C6C-4D2B-9E07-A9E41C0D5864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13410" uniqueCount="2797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13608" uniqueCount="2847">
   <si>
     <t>Description</t>
   </si>
@@ -8415,6 +8415,156 @@
   </si>
   <si>
     <t>May 7, 2025 update</t>
+  </si>
+  <si>
+    <t>3_LT_CIRCOMOD_Infrastructure</t>
+  </si>
+  <si>
+    <t>infrastructure</t>
+  </si>
+  <si>
+    <t>ca. 100 different types of infrastructure</t>
+  </si>
+  <si>
+    <t>typical infrastructure materials</t>
+  </si>
+  <si>
+    <t>most data apply to the entire asset (all materials) but for some, specific lifetime apply for different materials</t>
+  </si>
+  <si>
+    <t>country- and region-specific values</t>
+  </si>
+  <si>
+    <t>no age-cohort information given</t>
+  </si>
+  <si>
+    <t>mean lifetime of infrastructure in the use phase, compiled by several colleagues from the CIRCOMOD EU project</t>
+  </si>
+  <si>
+    <t>lifetime; infrastructure; use phase; road; rail; pipes</t>
+  </si>
+  <si>
+    <t>See comment for each data entry for the reference/literature source</t>
+  </si>
+  <si>
+    <t>Value(m,g,p,r,c)</t>
+  </si>
+  <si>
+    <t>Cement in roads and runways in use phase - infrastructure in Global of age-cohort n.a. has lifetime of 33 yr with rel. standard deviation of +/- 15%.</t>
+  </si>
+  <si>
+    <t>[Aspect 1] in [Aspect 2] in [Aspect 3] in [Aspect 4] built in [Aspect 5] has [data type] of [value].</t>
+  </si>
+  <si>
+    <t>May 8, 2025 update</t>
+  </si>
+  <si>
+    <t>3_MC_Infrastructure_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>ca. 90 different materials</t>
+  </si>
+  <si>
+    <t>Global average plus single-country values for six larger economies, including Germany, USA, and China</t>
+  </si>
+  <si>
+    <t>1978-2024</t>
+  </si>
+  <si>
+    <t>product specific, single-year values</t>
+  </si>
+  <si>
+    <t>Material content of infrastructure, compiled by the CIRCOMOD project team</t>
+  </si>
+  <si>
+    <t>material; material content; material composition; infrastructure; road; rail; pipe;</t>
+  </si>
+  <si>
+    <t>Value(m,g,p,c,r,v,L)</t>
+  </si>
+  <si>
+    <t>Material composition for layer mass per area of all materials in road bridge in use phase - infrastructure built in n.a. in Austria for CE strategy none is 1.431 t/m².</t>
+  </si>
+  <si>
+    <t>[Data type] as [Layer/Aspect 7] of [Aspect 1] in [Aspect 2] in [Aspect 3] built in [Aspect 4] in [Aspect 5] for circular economy strategy [Aspect 6] is [Value].</t>
+  </si>
+  <si>
+    <t>3_MC_Electricity_Sector_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>45 different generation, distribution, and storage technologies</t>
+  </si>
+  <si>
+    <t>76 different engineering materials</t>
+  </si>
+  <si>
+    <t>Global values, plus values for China, Denmark, Germany, and the Netherlands</t>
+  </si>
+  <si>
+    <t>product specific, single year values</t>
+  </si>
+  <si>
+    <t>Material content of electricity generation, distribution, and storage technologies technologies</t>
+  </si>
+  <si>
+    <t>material; material content; electricity generation; electricity storage; electricity distribution</t>
+  </si>
+  <si>
+    <t>Compiled from different sources, see the comment for each data point</t>
+  </si>
+  <si>
+    <t>Value(p,g,k,c,r,m)</t>
+  </si>
+  <si>
+    <t>Mass per unit of silicon in module, buffer layer in electricity generation - PV CIGS (ground-mounted) in use phase - electricity infrastructure in China built in 2025 is 6.7 kg/MWp.</t>
+  </si>
+  <si>
+    <t>[Layer] of [Aspect 6] in [Aspect 3] in [Aspect 2] in [Aspect 1] in [Aspect 5] built in [Aspect 4] is [Value].</t>
+  </si>
+  <si>
+    <t>3_MC_Electricity_Sector_CIRCOMOD_LightWeighting_Potential_Relative</t>
+  </si>
+  <si>
+    <t>7 different generation, distribution, and storage technologies</t>
+  </si>
+  <si>
+    <t>one value for all materials together</t>
+  </si>
+  <si>
+    <t>single future year scenario values</t>
+  </si>
+  <si>
+    <t>Material content reduction potential, compared to 2020 baseline, of electricity generation, distribution, and storage technologies</t>
+  </si>
+  <si>
+    <t>material; material content; electricity generation; electricity storage; electricity distribution; lightweighting; circular economy; reduction;</t>
+  </si>
+  <si>
+    <t>The values indicate the material content reduction potential, in %, compared to 2020 baseline, of electricity generation, distribution, and storage technologies</t>
+  </si>
+  <si>
+    <t>Value(p,g,k,c,r,m,v)</t>
+  </si>
+  <si>
+    <t>Material content reduction potential, expressed as mass ratio of all materials in entire device in electricity generation - wind offshore in use phase - electricity infrastructure in Global built in 2050 for circular economy strategy lightweighting is 10 %/MWp.</t>
+  </si>
+  <si>
+    <t>Material content reduction potential, expressed as [Layer] of [Aspect 6] in [Aspect 3] in [Aspect 2] in [Aspect 1] in [Aspect 5] built in [Aspect 4] for circular economy strategy [Aspect 7] is [Value].</t>
+  </si>
+  <si>
+    <t>UNEP-IRP</t>
+  </si>
+  <si>
+    <t>https://wedocs.unep.org/20.500.11822/44902</t>
+  </si>
+  <si>
+    <t>Table in background material</t>
+  </si>
+  <si>
+    <t>Global Resources Outlook 2024: Bend the Trend – Pathways to a liveable planet as resource use spikes</t>
+  </si>
+  <si>
+    <t>May 9, 2025 update</t>
   </si>
 </sst>
 </file>
@@ -8806,7 +8956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -9141,6 +9291,21 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9207,19 +9372,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9562,7 +9715,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="208" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -9594,7 +9747,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B5" s="203"/>
+      <c r="B5" s="208"/>
       <c r="C5" s="26" t="s">
         <v>422</v>
       </c>
@@ -9624,7 +9777,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="204" t="s">
+      <c r="B6" s="209" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -9640,7 +9793,7 @@
       <c r="K6" s="121"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B7" s="204"/>
+      <c r="B7" s="209"/>
       <c r="C7" s="26" t="s">
         <v>424</v>
       </c>
@@ -9654,7 +9807,7 @@
       <c r="K7" s="121"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B8" s="204"/>
+      <c r="B8" s="209"/>
       <c r="C8" s="26" t="s">
         <v>425</v>
       </c>
@@ -9668,7 +9821,7 @@
       <c r="K8" s="121"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B9" s="204"/>
+      <c r="B9" s="209"/>
       <c r="C9" s="28" t="s">
         <v>426</v>
       </c>
@@ -9682,7 +9835,7 @@
       <c r="K9" s="121"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B10" s="204"/>
+      <c r="B10" s="209"/>
       <c r="C10" s="27" t="s">
         <v>427</v>
       </c>
@@ -9696,7 +9849,7 @@
       <c r="K10" s="121"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B11" s="204"/>
+      <c r="B11" s="209"/>
       <c r="C11" s="27" t="s">
         <v>428</v>
       </c>
@@ -9710,7 +9863,7 @@
       <c r="K11" s="121"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B12" s="204"/>
+      <c r="B12" s="209"/>
       <c r="C12" s="27" t="s">
         <v>429</v>
       </c>
@@ -9724,7 +9877,7 @@
       <c r="K12" s="121"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B13" s="204"/>
+      <c r="B13" s="209"/>
       <c r="C13" s="27" t="s">
         <v>430</v>
       </c>
@@ -9738,7 +9891,7 @@
       <c r="K13" s="121"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B14" s="204"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="27" t="s">
         <v>431</v>
       </c>
@@ -9752,7 +9905,7 @@
       <c r="K14" s="121"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B15" s="204"/>
+      <c r="B15" s="209"/>
       <c r="C15" s="27" t="s">
         <v>432</v>
       </c>
@@ -9766,7 +9919,7 @@
       <c r="K15" s="121"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B16" s="204"/>
+      <c r="B16" s="209"/>
       <c r="C16" s="27" t="s">
         <v>433</v>
       </c>
@@ -9780,7 +9933,7 @@
       <c r="K16" s="121"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B17" s="204"/>
+      <c r="B17" s="209"/>
       <c r="C17" s="27" t="s">
         <v>434</v>
       </c>
@@ -9794,7 +9947,7 @@
       <c r="K17" s="121"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B18" s="204"/>
+      <c r="B18" s="209"/>
       <c r="C18" s="27" t="s">
         <v>435</v>
       </c>
@@ -9808,7 +9961,7 @@
       <c r="K18" s="121"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B19" s="205" t="s">
+      <c r="B19" s="210" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -9836,7 +9989,7 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B20" s="205"/>
+      <c r="B20" s="210"/>
       <c r="C20" s="27" t="s">
         <v>437</v>
       </c>
@@ -9866,7 +10019,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B21" s="205"/>
+      <c r="B21" s="210"/>
       <c r="C21" s="27" t="s">
         <v>438</v>
       </c>
@@ -9892,7 +10045,7 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="206" t="s">
+      <c r="B22" s="211" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -9922,7 +10075,7 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B23" s="206"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="26" t="s">
         <v>440</v>
       </c>
@@ -9936,7 +10089,7 @@
       <c r="K23" s="121"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B24" s="206"/>
+      <c r="B24" s="211"/>
       <c r="C24" s="25" t="s">
         <v>441</v>
       </c>
@@ -9950,7 +10103,7 @@
       <c r="K24" s="121"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B25" s="206"/>
+      <c r="B25" s="211"/>
       <c r="C25" s="25" t="s">
         <v>443</v>
       </c>
@@ -9976,7 +10129,7 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B26" s="206"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="25" t="s">
         <v>444</v>
       </c>
@@ -9992,7 +10145,7 @@
       <c r="K26" s="121"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B27" s="206"/>
+      <c r="B27" s="211"/>
       <c r="C27" s="25" t="s">
         <v>445</v>
       </c>
@@ -10006,7 +10159,7 @@
       <c r="K27" s="121"/>
     </row>
     <row r="28" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="207" t="s">
+      <c r="B28" s="212" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -10038,7 +10191,7 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B29" s="207"/>
+      <c r="B29" s="212"/>
       <c r="C29" s="25" t="s">
         <v>447</v>
       </c>
@@ -10068,7 +10221,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B30" s="200" t="s">
+      <c r="B30" s="205" t="s">
         <v>185</v>
       </c>
       <c r="C30" s="107" t="s">
@@ -10084,7 +10237,7 @@
       <c r="K30" s="181"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B31" s="201"/>
+      <c r="B31" s="206"/>
       <c r="C31" s="108" t="s">
         <v>449</v>
       </c>
@@ -10098,7 +10251,7 @@
       <c r="K31" s="164"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B32" s="202"/>
+      <c r="B32" s="207"/>
       <c r="C32" s="109" t="s">
         <v>450</v>
       </c>
@@ -10264,7 +10417,7 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B4" s="208" t="s">
+      <c r="B4" s="213" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -10356,7 +10509,7 @@
       </c>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B5" s="209"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
       </c>
@@ -10624,7 +10777,7 @@
       </c>
     </row>
     <row r="8" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="204" t="s">
+      <c r="B8" s="209" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="54" t="s">
@@ -10714,7 +10867,7 @@
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B9" s="204"/>
+      <c r="B9" s="209"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
       </c>
@@ -10802,7 +10955,7 @@
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B10" s="204"/>
+      <c r="B10" s="209"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
       </c>
@@ -10890,7 +11043,7 @@
       </c>
     </row>
     <row r="11" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="204"/>
+      <c r="B11" s="209"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
       </c>
@@ -10978,7 +11131,7 @@
       </c>
     </row>
     <row r="12" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="204"/>
+      <c r="B12" s="209"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -11066,7 +11219,7 @@
       </c>
     </row>
     <row r="13" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="204"/>
+      <c r="B13" s="209"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -11154,7 +11307,7 @@
       </c>
     </row>
     <row r="14" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="204"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -11242,7 +11395,7 @@
       </c>
     </row>
     <row r="15" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="204"/>
+      <c r="B15" s="209"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -11330,7 +11483,7 @@
       </c>
     </row>
     <row r="16" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="204"/>
+      <c r="B16" s="209"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -11418,7 +11571,7 @@
       </c>
     </row>
     <row r="17" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="204"/>
+      <c r="B17" s="209"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -11506,7 +11659,7 @@
       </c>
     </row>
     <row r="18" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="204"/>
+      <c r="B18" s="209"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -11594,7 +11747,7 @@
       </c>
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B19" s="204"/>
+      <c r="B19" s="209"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -11682,7 +11835,7 @@
       </c>
     </row>
     <row r="20" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="204"/>
+      <c r="B20" s="209"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -11770,7 +11923,7 @@
       </c>
     </row>
     <row r="21" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="205" t="s">
+      <c r="B21" s="210" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -11860,7 +12013,7 @@
       </c>
     </row>
     <row r="22" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="205"/>
+      <c r="B22" s="210"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -11950,7 +12103,7 @@
       </c>
     </row>
     <row r="23" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B23" s="205"/>
+      <c r="B23" s="210"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
       </c>
@@ -12038,7 +12191,7 @@
       </c>
     </row>
     <row r="24" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="205"/>
+      <c r="B24" s="210"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
       </c>
@@ -12120,7 +12273,7 @@
       <c r="AE24" s="164"/>
     </row>
     <row r="25" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="206" t="s">
+      <c r="B25" s="211" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -12210,7 +12363,7 @@
       </c>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B26" s="206"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
       </c>
@@ -12298,7 +12451,7 @@
       </c>
     </row>
     <row r="27" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B27" s="206"/>
+      <c r="B27" s="211"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
       </c>
@@ -12386,7 +12539,7 @@
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B28" s="206"/>
+      <c r="B28" s="211"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
       </c>
@@ -12474,7 +12627,7 @@
       </c>
     </row>
     <row r="29" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="206"/>
+      <c r="B29" s="211"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
       </c>
@@ -12562,7 +12715,7 @@
       </c>
     </row>
     <row r="30" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="206"/>
+      <c r="B30" s="211"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
       </c>
@@ -12650,7 +12803,7 @@
       </c>
     </row>
     <row r="31" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="207" t="s">
+      <c r="B31" s="212" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -12742,7 +12895,7 @@
       </c>
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B32" s="210"/>
+      <c r="B32" s="215"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
       </c>
@@ -12832,7 +12985,7 @@
       </c>
     </row>
     <row r="33" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B33" s="200" t="s">
+      <c r="B33" s="205" t="s">
         <v>185</v>
       </c>
       <c r="C33" s="83" t="s">
@@ -12868,7 +13021,7 @@
       <c r="AE33" s="164"/>
     </row>
     <row r="34" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B34" s="201"/>
+      <c r="B34" s="206"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
       </c>
@@ -12902,7 +13055,7 @@
       <c r="AE34" s="164"/>
     </row>
     <row r="35" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B35" s="202"/>
+      <c r="B35" s="207"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
       </c>
@@ -12960,10 +13113,10 @@
   <dimension ref="A1:GW74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="FA24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="FH15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="FQ1" sqref="FQ1:FQ2"/>
+      <selection pane="bottomRight" activeCell="FS1" sqref="FS1:FS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -13024,7 +13177,7 @@
     <col min="70" max="16384" width="11.5546875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:173" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:177" x14ac:dyDescent="0.4">
       <c r="C1" s="73" t="s">
         <v>269</v>
       </c>
@@ -13501,8 +13654,12 @@
       <c r="FO1" s="174"/>
       <c r="FP1" s="174"/>
       <c r="FQ1" s="174"/>
+      <c r="FR1" s="174"/>
+      <c r="FS1" s="174"/>
+      <c r="FT1" s="174"/>
+      <c r="FU1" s="174"/>
     </row>
-    <row r="2" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:177" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B2" s="34" t="s">
         <v>183</v>
       </c>
@@ -13837,8 +13994,20 @@
       <c r="FQ2" s="154" t="s">
         <v>2796</v>
       </c>
+      <c r="FR2" s="154" t="s">
+        <v>2810</v>
+      </c>
+      <c r="FS2" s="154" t="s">
+        <v>2846</v>
+      </c>
+      <c r="FT2" s="154" t="s">
+        <v>2846</v>
+      </c>
+      <c r="FU2" s="154" t="s">
+        <v>2846</v>
+      </c>
     </row>
-    <row r="3" spans="1:173" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:177" x14ac:dyDescent="0.4">
       <c r="B3" s="58"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -14091,11 +14260,11 @@
       <c r="DS3" s="105"/>
       <c r="DT3" s="105"/>
     </row>
-    <row r="4" spans="1:173" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:177" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>1</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="218" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -14349,11 +14518,11 @@
       <c r="DS4" s="105"/>
       <c r="DT4" s="105"/>
     </row>
-    <row r="5" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="214"/>
+      <c r="B5" s="219"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -14852,7 +15021,7 @@
       <c r="FL5" s="41" t="s">
         <v>2722</v>
       </c>
-      <c r="FM5" s="222" t="s">
+      <c r="FM5" s="200" t="s">
         <v>2731</v>
       </c>
       <c r="FN5" s="187" t="s">
@@ -14867,8 +15036,20 @@
       <c r="FQ5" s="187" t="s">
         <v>2784</v>
       </c>
+      <c r="FR5" s="115" t="s">
+        <v>2797</v>
+      </c>
+      <c r="FS5" s="187" t="s">
+        <v>2811</v>
+      </c>
+      <c r="FT5" s="187" t="s">
+        <v>2821</v>
+      </c>
+      <c r="FU5" s="187" t="s">
+        <v>2832</v>
+      </c>
     </row>
-    <row r="6" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="92">
         <v>3</v>
       </c>
@@ -15369,7 +15550,7 @@
       <c r="FL6" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="FM6" s="222" t="s">
+      <c r="FM6" s="200" t="s">
         <v>1150</v>
       </c>
       <c r="FN6" s="187" t="s">
@@ -15384,12 +15565,24 @@
       <c r="FQ6" s="187" t="s">
         <v>1150</v>
       </c>
+      <c r="FR6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FS6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FT6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="FU6" s="187" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="7" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="92">
         <v>4</v>
       </c>
-      <c r="B7" s="215" t="s">
+      <c r="B7" s="220" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -15888,7 +16081,7 @@
       <c r="FL7" s="41">
         <v>27</v>
       </c>
-      <c r="FM7" s="222">
+      <c r="FM7" s="200">
         <v>21</v>
       </c>
       <c r="FN7" s="187">
@@ -15903,12 +16096,24 @@
       <c r="FQ7" s="187">
         <v>20</v>
       </c>
+      <c r="FR7" s="187">
+        <v>20</v>
+      </c>
+      <c r="FS7" s="187">
+        <v>20</v>
+      </c>
+      <c r="FT7" s="187">
+        <v>20</v>
+      </c>
+      <c r="FU7" s="187">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="92">
         <v>5</v>
       </c>
-      <c r="B8" s="215"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -16407,7 +16612,7 @@
       <c r="FL8" s="41">
         <v>6</v>
       </c>
-      <c r="FM8" s="222">
+      <c r="FM8" s="200">
         <v>2</v>
       </c>
       <c r="FN8" s="187">
@@ -16422,12 +16627,24 @@
       <c r="FQ8" s="187">
         <v>4</v>
       </c>
+      <c r="FR8" s="115">
+        <v>3</v>
+      </c>
+      <c r="FS8" s="187">
+        <v>3</v>
+      </c>
+      <c r="FT8" s="187">
+        <v>3</v>
+      </c>
+      <c r="FU8" s="187">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="92">
         <v>6</v>
       </c>
-      <c r="B9" s="215"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -16926,7 +17143,7 @@
       <c r="FL9" s="41" t="s">
         <v>2708</v>
       </c>
-      <c r="FM9" s="222" t="s">
+      <c r="FM9" s="200" t="s">
         <v>31</v>
       </c>
       <c r="FN9" s="187" t="s">
@@ -16941,12 +17158,24 @@
       <c r="FQ9" s="187" t="s">
         <v>94</v>
       </c>
+      <c r="FR9" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="FS9" s="187" t="s">
+        <v>846</v>
+      </c>
+      <c r="FT9" s="187" t="s">
+        <v>846</v>
+      </c>
+      <c r="FU9" s="187" t="s">
+        <v>846</v>
+      </c>
     </row>
-    <row r="10" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="92">
         <v>7</v>
       </c>
-      <c r="B10" s="215"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -17445,7 +17674,7 @@
       <c r="FL10" s="41" t="s">
         <v>1091</v>
       </c>
-      <c r="FM10" s="222" t="s">
+      <c r="FM10" s="200" t="s">
         <v>1025</v>
       </c>
       <c r="FN10" s="187" t="s">
@@ -17460,12 +17689,24 @@
       <c r="FQ10" s="187" t="s">
         <v>5</v>
       </c>
+      <c r="FR10" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="FS10" s="187" t="s">
+        <v>1025</v>
+      </c>
+      <c r="FT10" s="187" t="s">
+        <v>824</v>
+      </c>
+      <c r="FU10" s="187" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:173" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:177" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="92">
         <v>8</v>
       </c>
-      <c r="B11" s="216" t="s">
+      <c r="B11" s="221" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -17964,7 +18205,7 @@
       <c r="FL11" s="41" t="s">
         <v>779</v>
       </c>
-      <c r="FM11" s="222" t="s">
+      <c r="FM11" s="200" t="s">
         <v>782</v>
       </c>
       <c r="FN11" s="188" t="s">
@@ -17979,12 +18220,24 @@
       <c r="FQ11" s="188" t="s">
         <v>2785</v>
       </c>
+      <c r="FR11" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="FS11" s="188" t="s">
+        <v>782</v>
+      </c>
+      <c r="FT11" s="188" t="s">
+        <v>782</v>
+      </c>
+      <c r="FU11" s="188" t="s">
+        <v>782</v>
+      </c>
     </row>
-    <row r="12" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="92">
         <v>9</v>
       </c>
-      <c r="B12" s="217"/>
+      <c r="B12" s="222"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -18481,7 +18734,7 @@
       <c r="FL12" s="41" t="s">
         <v>868</v>
       </c>
-      <c r="FM12" s="222" t="s">
+      <c r="FM12" s="200" t="s">
         <v>152</v>
       </c>
       <c r="FN12" s="187" t="s">
@@ -18496,12 +18749,24 @@
       <c r="FQ12" s="187" t="s">
         <v>2274</v>
       </c>
+      <c r="FR12" s="115" t="s">
+        <v>152</v>
+      </c>
+      <c r="FS12" s="187" t="s">
+        <v>2274</v>
+      </c>
+      <c r="FT12" s="187" t="s">
+        <v>152</v>
+      </c>
+      <c r="FU12" s="187" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="13" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="92">
         <v>10</v>
       </c>
-      <c r="B13" s="217"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -18998,7 +19263,7 @@
       <c r="FL13" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="FM13" s="222" t="s">
+      <c r="FM13" s="200" t="s">
         <v>2641</v>
       </c>
       <c r="FN13" s="187" t="s">
@@ -19013,12 +19278,24 @@
       <c r="FQ13" s="188" t="s">
         <v>2743</v>
       </c>
+      <c r="FR13" s="115" t="s">
+        <v>2798</v>
+      </c>
+      <c r="FS13" s="187" t="s">
+        <v>2798</v>
+      </c>
+      <c r="FT13" s="187" t="s">
+        <v>2641</v>
+      </c>
+      <c r="FU13" s="187" t="s">
+        <v>2641</v>
+      </c>
     </row>
-    <row r="14" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="92">
         <v>11</v>
       </c>
-      <c r="B14" s="217"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -19515,7 +19792,7 @@
       <c r="FL14" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="FM14" s="222" t="s">
+      <c r="FM14" s="200" t="s">
         <v>2732</v>
       </c>
       <c r="FN14" s="187" t="s">
@@ -19530,12 +19807,24 @@
       <c r="FQ14" s="187" t="s">
         <v>2786</v>
       </c>
+      <c r="FR14" s="115" t="s">
+        <v>2799</v>
+      </c>
+      <c r="FS14" s="187" t="s">
+        <v>2799</v>
+      </c>
+      <c r="FT14" s="187" t="s">
+        <v>2822</v>
+      </c>
+      <c r="FU14" s="187" t="s">
+        <v>2833</v>
+      </c>
     </row>
-    <row r="15" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="92">
         <v>12</v>
       </c>
-      <c r="B15" s="217"/>
+      <c r="B15" s="222"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -20032,7 +20321,7 @@
       <c r="FL15" s="41" t="s">
         <v>2723</v>
       </c>
-      <c r="FM15" s="222" t="s">
+      <c r="FM15" s="200" t="s">
         <v>11</v>
       </c>
       <c r="FN15" s="187" t="s">
@@ -20047,12 +20336,24 @@
       <c r="FQ15" s="187" t="s">
         <v>565</v>
       </c>
+      <c r="FR15" s="115" t="s">
+        <v>2800</v>
+      </c>
+      <c r="FS15" s="187" t="s">
+        <v>2345</v>
+      </c>
+      <c r="FT15" s="187" t="s">
+        <v>2345</v>
+      </c>
+      <c r="FU15" s="187" t="s">
+        <v>2345</v>
+      </c>
     </row>
-    <row r="16" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="92">
         <v>13</v>
       </c>
-      <c r="B16" s="217"/>
+      <c r="B16" s="222"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -20549,7 +20850,7 @@
       <c r="FL16" s="41" t="s">
         <v>2724</v>
       </c>
-      <c r="FM16" s="222" t="s">
+      <c r="FM16" s="200" t="s">
         <v>11</v>
       </c>
       <c r="FN16" s="187" t="s">
@@ -20564,12 +20865,24 @@
       <c r="FQ16" s="187" t="s">
         <v>1680</v>
       </c>
+      <c r="FR16" s="115" t="s">
+        <v>2801</v>
+      </c>
+      <c r="FS16" s="187" t="s">
+        <v>2812</v>
+      </c>
+      <c r="FT16" s="187" t="s">
+        <v>2823</v>
+      </c>
+      <c r="FU16" s="187" t="s">
+        <v>2834</v>
+      </c>
     </row>
-    <row r="17" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="92">
         <v>14</v>
       </c>
-      <c r="B17" s="217"/>
+      <c r="B17" s="222"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -21066,7 +21379,7 @@
       <c r="FL17" s="41" t="s">
         <v>1422</v>
       </c>
-      <c r="FM17" s="222" t="s">
+      <c r="FM17" s="200" t="s">
         <v>819</v>
       </c>
       <c r="FN17" s="187" t="s">
@@ -21081,12 +21394,24 @@
       <c r="FQ17" s="187" t="s">
         <v>527</v>
       </c>
+      <c r="FR17" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="FS17" s="187" t="s">
+        <v>19</v>
+      </c>
+      <c r="FT17" s="187" t="s">
+        <v>819</v>
+      </c>
+      <c r="FU17" s="187" t="s">
+        <v>819</v>
+      </c>
     </row>
-    <row r="18" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="92">
         <v>15</v>
       </c>
-      <c r="B18" s="217"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -21583,7 +21908,7 @@
       <c r="FL18" s="41" t="s">
         <v>2711</v>
       </c>
-      <c r="FM18" s="222" t="s">
+      <c r="FM18" s="200" t="s">
         <v>2733</v>
       </c>
       <c r="FN18" s="187" t="s">
@@ -21598,12 +21923,24 @@
       <c r="FQ18" s="187" t="s">
         <v>2762</v>
       </c>
+      <c r="FR18" s="115" t="s">
+        <v>2802</v>
+      </c>
+      <c r="FS18" s="187" t="s">
+        <v>2813</v>
+      </c>
+      <c r="FT18" s="187" t="s">
+        <v>2824</v>
+      </c>
+      <c r="FU18" s="187" t="s">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="19" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="92">
         <v>16</v>
       </c>
-      <c r="B19" s="217"/>
+      <c r="B19" s="222"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -22100,7 +22437,7 @@
       <c r="FL19" s="41">
         <v>2020</v>
       </c>
-      <c r="FM19" s="222" t="s">
+      <c r="FM19" s="200" t="s">
         <v>2734</v>
       </c>
       <c r="FN19" s="187" t="s">
@@ -22115,12 +22452,24 @@
       <c r="FQ19" s="187">
         <v>2015</v>
       </c>
+      <c r="FR19" s="115" t="s">
+        <v>2225</v>
+      </c>
+      <c r="FS19" s="187" t="s">
+        <v>2814</v>
+      </c>
+      <c r="FT19" s="187" t="s">
+        <v>1891</v>
+      </c>
+      <c r="FU19" s="187">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="20" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="92">
         <v>17</v>
       </c>
-      <c r="B20" s="217"/>
+      <c r="B20" s="222"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -22617,7 +22966,7 @@
       <c r="FL20" s="41" t="s">
         <v>2712</v>
       </c>
-      <c r="FM20" s="222" t="s">
+      <c r="FM20" s="200" t="s">
         <v>2735</v>
       </c>
       <c r="FN20" s="187" t="s">
@@ -22632,12 +22981,24 @@
       <c r="FQ20" s="187" t="s">
         <v>2050</v>
       </c>
+      <c r="FR20" s="115" t="s">
+        <v>2803</v>
+      </c>
+      <c r="FS20" s="187" t="s">
+        <v>2815</v>
+      </c>
+      <c r="FT20" s="187" t="s">
+        <v>2825</v>
+      </c>
+      <c r="FU20" s="187" t="s">
+        <v>2835</v>
+      </c>
     </row>
-    <row r="21" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="92">
         <v>18</v>
       </c>
-      <c r="B21" s="218" t="s">
+      <c r="B21" s="223" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -23130,7 +23491,7 @@
       <c r="FL21" s="41" t="s">
         <v>2725</v>
       </c>
-      <c r="FM21" s="222" t="s">
+      <c r="FM21" s="200" t="s">
         <v>2736</v>
       </c>
       <c r="FN21" s="187" t="s">
@@ -23145,12 +23506,24 @@
       <c r="FQ21" s="187" t="s">
         <v>2787</v>
       </c>
+      <c r="FR21" s="115" t="s">
+        <v>2804</v>
+      </c>
+      <c r="FS21" s="187" t="s">
+        <v>2816</v>
+      </c>
+      <c r="FT21" s="187" t="s">
+        <v>2826</v>
+      </c>
+      <c r="FU21" s="187" t="s">
+        <v>2836</v>
+      </c>
     </row>
-    <row r="22" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="92">
         <v>19</v>
       </c>
-      <c r="B22" s="218"/>
+      <c r="B22" s="223"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -23649,7 +24022,7 @@
       <c r="FL22" s="41" t="s">
         <v>2714</v>
       </c>
-      <c r="FM22" s="222" t="s">
+      <c r="FM22" s="200" t="s">
         <v>2737</v>
       </c>
       <c r="FN22" s="187" t="s">
@@ -23664,12 +24037,24 @@
       <c r="FQ22" s="187" t="s">
         <v>2788</v>
       </c>
+      <c r="FR22" s="115" t="s">
+        <v>2805</v>
+      </c>
+      <c r="FS22" s="187" t="s">
+        <v>2817</v>
+      </c>
+      <c r="FT22" s="187" t="s">
+        <v>2827</v>
+      </c>
+      <c r="FU22" s="187" t="s">
+        <v>2837</v>
+      </c>
     </row>
-    <row r="23" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="92">
         <v>20</v>
       </c>
-      <c r="B23" s="218"/>
+      <c r="B23" s="223"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -24168,7 +24553,7 @@
       <c r="FL23" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="FM23" s="222" t="s">
+      <c r="FM23" s="200" t="s">
         <v>169</v>
       </c>
       <c r="FN23" s="187" t="s">
@@ -24183,12 +24568,24 @@
       <c r="FQ23" s="187" t="s">
         <v>634</v>
       </c>
+      <c r="FR23" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="FS23" s="187" t="s">
+        <v>24</v>
+      </c>
+      <c r="FT23" s="187" t="s">
+        <v>24</v>
+      </c>
+      <c r="FU23" s="187" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="92">
         <v>21</v>
       </c>
-      <c r="B24" s="218"/>
+      <c r="B24" s="223"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -24687,7 +25084,7 @@
       <c r="FL24" s="41">
         <v>137</v>
       </c>
-      <c r="FM24" s="222">
+      <c r="FM24" s="200">
         <v>1111</v>
       </c>
       <c r="FN24" s="155">
@@ -24702,12 +25099,24 @@
       <c r="FQ24" s="187">
         <v>18</v>
       </c>
+      <c r="FR24" s="115">
+        <v>121</v>
+      </c>
+      <c r="FS24" s="187">
+        <v>1607</v>
+      </c>
+      <c r="FT24" s="155">
+        <v>2964</v>
+      </c>
+      <c r="FU24" s="69">
+        <v>7</v>
+      </c>
     </row>
-    <row r="25" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="92">
         <v>22</v>
       </c>
-      <c r="B25" s="218"/>
+      <c r="B25" s="223"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -25201,7 +25610,7 @@
       <c r="FL25" s="41" t="s">
         <v>2726</v>
       </c>
-      <c r="FM25" s="223" t="s">
+      <c r="FM25" s="201" t="s">
         <v>11</v>
       </c>
       <c r="FN25" s="155" t="s">
@@ -25216,12 +25625,24 @@
       <c r="FQ25" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR25" s="185" t="s">
+        <v>2806</v>
+      </c>
+      <c r="FS25" s="155" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT25" s="155" t="s">
+        <v>2828</v>
+      </c>
+      <c r="FU25" s="69" t="s">
+        <v>2838</v>
+      </c>
     </row>
-    <row r="26" spans="1:173" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:177" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="92">
         <v>23</v>
       </c>
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="224" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="64" t="s">
@@ -25722,7 +26143,7 @@
       <c r="FL26" s="68" t="s">
         <v>1033</v>
       </c>
-      <c r="FM26" s="222" t="s">
+      <c r="FM26" s="200" t="s">
         <v>1440</v>
       </c>
       <c r="FN26" s="156" t="s">
@@ -25737,12 +26158,24 @@
       <c r="FQ26" s="156" t="s">
         <v>852</v>
       </c>
+      <c r="FR26" s="115" t="s">
+        <v>849</v>
+      </c>
+      <c r="FS26" s="187" t="s">
+        <v>849</v>
+      </c>
+      <c r="FT26" s="187" t="s">
+        <v>1440</v>
+      </c>
+      <c r="FU26" s="187" t="s">
+        <v>1440</v>
+      </c>
     </row>
-    <row r="27" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="92">
         <v>24</v>
       </c>
-      <c r="B27" s="219"/>
+      <c r="B27" s="224"/>
       <c r="C27" s="64" t="s">
         <v>464</v>
       </c>
@@ -26241,7 +26674,7 @@
       <c r="FL27" s="68">
         <v>4</v>
       </c>
-      <c r="FM27" s="223">
+      <c r="FM27" s="201">
         <v>6</v>
       </c>
       <c r="FN27" s="155">
@@ -26256,12 +26689,24 @@
       <c r="FQ27" s="155">
         <v>4</v>
       </c>
+      <c r="FR27" s="115">
+        <v>4</v>
+      </c>
+      <c r="FS27" s="155">
+        <v>4</v>
+      </c>
+      <c r="FT27" s="155">
+        <v>6</v>
+      </c>
+      <c r="FU27" s="69">
+        <v>6</v>
+      </c>
     </row>
-    <row r="28" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="92">
         <v>25</v>
       </c>
-      <c r="B28" s="219"/>
+      <c r="B28" s="224"/>
       <c r="C28" s="64" t="s">
         <v>465</v>
       </c>
@@ -26758,7 +27203,7 @@
       <c r="FL28" s="68" t="s">
         <v>1087</v>
       </c>
-      <c r="FM28" s="222" t="s">
+      <c r="FM28" s="200" t="s">
         <v>696</v>
       </c>
       <c r="FN28" s="187" t="s">
@@ -26773,12 +27218,24 @@
       <c r="FQ28" s="187" t="s">
         <v>1640</v>
       </c>
+      <c r="FR28" s="115" t="s">
+        <v>696</v>
+      </c>
+      <c r="FS28" s="187" t="s">
+        <v>696</v>
+      </c>
+      <c r="FT28" s="187" t="s">
+        <v>696</v>
+      </c>
+      <c r="FU28" s="187" t="s">
+        <v>696</v>
+      </c>
     </row>
-    <row r="29" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="92">
         <v>26</v>
       </c>
-      <c r="B29" s="219"/>
+      <c r="B29" s="224"/>
       <c r="C29" s="64" t="s">
         <v>466</v>
       </c>
@@ -27275,7 +27732,7 @@
       <c r="FL29" s="68">
         <v>18</v>
       </c>
-      <c r="FM29" s="222">
+      <c r="FM29" s="200">
         <v>7</v>
       </c>
       <c r="FN29" s="187">
@@ -27290,12 +27747,24 @@
       <c r="FQ29" s="155">
         <v>90</v>
       </c>
+      <c r="FR29" s="115">
+        <v>7</v>
+      </c>
+      <c r="FS29" s="155">
+        <v>7</v>
+      </c>
+      <c r="FT29" s="187">
+        <v>7</v>
+      </c>
+      <c r="FU29" s="187">
+        <v>7</v>
+      </c>
     </row>
-    <row r="30" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="92">
         <v>27</v>
       </c>
-      <c r="B30" s="219"/>
+      <c r="B30" s="224"/>
       <c r="C30" s="64" t="s">
         <v>467</v>
       </c>
@@ -27792,7 +28261,7 @@
       <c r="FL30" s="68" t="s">
         <v>1657</v>
       </c>
-      <c r="FM30" s="222" t="s">
+      <c r="FM30" s="200" t="s">
         <v>702</v>
       </c>
       <c r="FN30" s="156" t="s">
@@ -27807,12 +28276,24 @@
       <c r="FQ30" s="187" t="s">
         <v>799</v>
       </c>
+      <c r="FR30" s="115" t="s">
+        <v>697</v>
+      </c>
+      <c r="FS30" s="156" t="s">
+        <v>1440</v>
+      </c>
+      <c r="FT30" s="187" t="s">
+        <v>1640</v>
+      </c>
+      <c r="FU30" s="187" t="s">
+        <v>1640</v>
+      </c>
     </row>
-    <row r="31" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="92">
         <v>28</v>
       </c>
-      <c r="B31" s="219"/>
+      <c r="B31" s="224"/>
       <c r="C31" s="64" t="s">
         <v>468</v>
       </c>
@@ -28309,7 +28790,7 @@
       <c r="FL31" s="68">
         <v>93</v>
       </c>
-      <c r="FM31" s="222">
+      <c r="FM31" s="200">
         <v>3</v>
       </c>
       <c r="FN31" s="155">
@@ -28324,12 +28805,24 @@
       <c r="FQ31" s="155">
         <v>7</v>
       </c>
+      <c r="FR31" s="115">
+        <v>6</v>
+      </c>
+      <c r="FS31" s="155">
+        <v>6</v>
+      </c>
+      <c r="FT31" s="187">
+        <v>90</v>
+      </c>
+      <c r="FU31" s="187">
+        <v>90</v>
+      </c>
     </row>
-    <row r="32" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="92">
         <v>29</v>
       </c>
-      <c r="B32" s="219"/>
+      <c r="B32" s="224"/>
       <c r="C32" s="64" t="s">
         <v>469</v>
       </c>
@@ -28826,7 +29319,7 @@
       <c r="FL32" s="68" t="s">
         <v>698</v>
       </c>
-      <c r="FM32" s="222" t="s">
+      <c r="FM32" s="200" t="s">
         <v>698</v>
       </c>
       <c r="FN32" s="188" t="s">
@@ -28841,12 +29334,24 @@
       <c r="FQ32" s="187" t="s">
         <v>697</v>
       </c>
+      <c r="FR32" s="115" t="s">
+        <v>698</v>
+      </c>
+      <c r="FS32" s="188" t="s">
+        <v>704</v>
+      </c>
+      <c r="FT32" s="187" t="s">
+        <v>704</v>
+      </c>
+      <c r="FU32" s="187" t="s">
+        <v>704</v>
+      </c>
     </row>
-    <row r="33" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="92">
         <v>30</v>
       </c>
-      <c r="B33" s="219"/>
+      <c r="B33" s="224"/>
       <c r="C33" s="64" t="s">
         <v>470</v>
       </c>
@@ -29343,7 +29848,7 @@
       <c r="FL33" s="68">
         <v>2</v>
       </c>
-      <c r="FM33" s="222">
+      <c r="FM33" s="200">
         <v>89</v>
       </c>
       <c r="FN33" s="188">
@@ -29358,12 +29863,24 @@
       <c r="FQ33" s="155">
         <v>6</v>
       </c>
+      <c r="FR33" s="115">
+        <v>2</v>
+      </c>
+      <c r="FS33" s="155">
+        <v>14</v>
+      </c>
+      <c r="FT33" s="187">
+        <v>14</v>
+      </c>
+      <c r="FU33" s="187">
+        <v>14</v>
+      </c>
     </row>
-    <row r="34" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="92">
         <v>31</v>
       </c>
-      <c r="B34" s="219"/>
+      <c r="B34" s="224"/>
       <c r="C34" s="64" t="s">
         <v>471</v>
       </c>
@@ -29860,7 +30377,7 @@
       <c r="FL34" s="68" t="s">
         <v>702</v>
       </c>
-      <c r="FM34" s="224" t="s">
+      <c r="FM34" s="202" t="s">
         <v>1034</v>
       </c>
       <c r="FN34" s="188" t="s">
@@ -29875,12 +30392,24 @@
       <c r="FQ34" s="187" t="s">
         <v>702</v>
       </c>
+      <c r="FR34" s="115" t="s">
+        <v>704</v>
+      </c>
+      <c r="FS34" s="188" t="s">
+        <v>698</v>
+      </c>
+      <c r="FT34" s="187" t="s">
+        <v>698</v>
+      </c>
+      <c r="FU34" s="187" t="s">
+        <v>698</v>
+      </c>
     </row>
-    <row r="35" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="92">
         <v>32</v>
       </c>
-      <c r="B35" s="219"/>
+      <c r="B35" s="224"/>
       <c r="C35" s="64" t="s">
         <v>472</v>
       </c>
@@ -30377,7 +30906,7 @@
       <c r="FL35" s="68">
         <v>3</v>
       </c>
-      <c r="FM35" s="224">
+      <c r="FM35" s="202">
         <v>20</v>
       </c>
       <c r="FN35" s="188">
@@ -30392,12 +30921,24 @@
       <c r="FQ35" s="155">
         <v>3</v>
       </c>
+      <c r="FR35" s="115">
+        <v>14</v>
+      </c>
+      <c r="FS35" s="155">
+        <v>2</v>
+      </c>
+      <c r="FT35" s="187">
+        <v>2</v>
+      </c>
+      <c r="FU35" s="187">
+        <v>2</v>
+      </c>
     </row>
-    <row r="36" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="92">
         <v>33</v>
       </c>
-      <c r="B36" s="219"/>
+      <c r="B36" s="224"/>
       <c r="C36" s="64" t="s">
         <v>473</v>
       </c>
@@ -30909,12 +31450,24 @@
       <c r="FQ36" s="187" t="s">
         <v>698</v>
       </c>
+      <c r="FR36" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS36" s="187" t="s">
+        <v>1441</v>
+      </c>
+      <c r="FT36" s="156" t="s">
+        <v>849</v>
+      </c>
+      <c r="FU36" s="191" t="s">
+        <v>849</v>
+      </c>
     </row>
-    <row r="37" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="92">
         <v>34</v>
       </c>
-      <c r="B37" s="219"/>
+      <c r="B37" s="224"/>
       <c r="C37" s="64" t="s">
         <v>474</v>
       </c>
@@ -31426,12 +31979,24 @@
       <c r="FQ37" s="155">
         <v>2</v>
       </c>
+      <c r="FR37" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS37" s="155">
+        <v>86</v>
+      </c>
+      <c r="FT37" s="155">
+        <v>4</v>
+      </c>
+      <c r="FU37" s="69">
+        <v>4</v>
+      </c>
     </row>
-    <row r="38" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="92">
         <v>35</v>
       </c>
-      <c r="B38" s="219"/>
+      <c r="B38" s="224"/>
       <c r="C38" s="64" t="s">
         <v>475</v>
       </c>
@@ -31943,12 +32508,24 @@
       <c r="FQ38" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR38" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS38" s="187" t="s">
+        <v>1034</v>
+      </c>
+      <c r="FT38" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU38" s="188" t="s">
+        <v>1441</v>
+      </c>
     </row>
-    <row r="39" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="92">
         <v>36</v>
       </c>
-      <c r="B39" s="219"/>
+      <c r="B39" s="224"/>
       <c r="C39" s="64" t="s">
         <v>476</v>
       </c>
@@ -32460,12 +33037,24 @@
       <c r="FQ39" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR39" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS39" s="155">
+        <v>20</v>
+      </c>
+      <c r="FT39" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU39" s="188">
+        <v>86</v>
+      </c>
     </row>
-    <row r="40" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="92">
         <v>37</v>
       </c>
-      <c r="B40" s="219"/>
+      <c r="B40" s="224"/>
       <c r="C40" s="64" t="s">
         <v>477</v>
       </c>
@@ -32977,12 +33566,24 @@
       <c r="FQ40" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR40" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS40" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT40" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU40" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="92">
         <v>38</v>
       </c>
-      <c r="B41" s="219"/>
+      <c r="B41" s="224"/>
       <c r="C41" s="64" t="s">
         <v>478</v>
       </c>
@@ -33494,12 +34095,24 @@
       <c r="FQ41" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR41" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS41" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT41" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU41" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="42" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="92">
         <v>39</v>
       </c>
-      <c r="B42" s="219"/>
+      <c r="B42" s="224"/>
       <c r="C42" s="64" t="s">
         <v>479</v>
       </c>
@@ -34011,12 +34624,24 @@
       <c r="FQ42" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR42" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS42" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT42" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU42" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="92">
         <v>40</v>
       </c>
-      <c r="B43" s="219"/>
+      <c r="B43" s="224"/>
       <c r="C43" s="64" t="s">
         <v>480</v>
       </c>
@@ -34528,12 +35153,24 @@
       <c r="FQ43" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR43" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS43" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT43" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU43" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="44" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="92">
         <v>41</v>
       </c>
-      <c r="B44" s="219"/>
+      <c r="B44" s="224"/>
       <c r="C44" s="64" t="s">
         <v>481</v>
       </c>
@@ -35045,12 +35682,24 @@
       <c r="FQ44" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR44" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS44" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT44" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU44" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="45" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="92">
         <v>42</v>
       </c>
-      <c r="B45" s="219"/>
+      <c r="B45" s="224"/>
       <c r="C45" s="64" t="s">
         <v>482</v>
       </c>
@@ -35562,12 +36211,24 @@
       <c r="FQ45" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR45" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS45" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT45" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU45" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="46" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="92">
         <v>43</v>
       </c>
-      <c r="B46" s="219"/>
+      <c r="B46" s="224"/>
       <c r="C46" s="64" t="s">
         <v>483</v>
       </c>
@@ -36079,12 +36740,24 @@
       <c r="FQ46" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR46" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS46" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT46" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU46" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="47" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="92">
         <v>44</v>
       </c>
-      <c r="B47" s="219"/>
+      <c r="B47" s="224"/>
       <c r="C47" s="64" t="s">
         <v>484</v>
       </c>
@@ -36596,12 +37269,24 @@
       <c r="FQ47" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR47" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS47" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT47" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU47" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="48" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="92">
         <v>45</v>
       </c>
-      <c r="B48" s="219"/>
+      <c r="B48" s="224"/>
       <c r="C48" s="64" t="s">
         <v>485</v>
       </c>
@@ -37113,12 +37798,24 @@
       <c r="FQ48" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR48" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS48" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT48" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU48" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="49" spans="1:173" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:177" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="92">
         <v>46</v>
       </c>
-      <c r="B49" s="219"/>
+      <c r="B49" s="224"/>
       <c r="C49" s="64" t="s">
         <v>486</v>
       </c>
@@ -37630,12 +38327,24 @@
       <c r="FQ49" s="187" t="s">
         <v>11</v>
       </c>
+      <c r="FR49" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="FS49" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT49" s="187" t="s">
+        <v>11</v>
+      </c>
+      <c r="FU49" s="187" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="50" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="92">
         <v>47</v>
       </c>
-      <c r="B50" s="219"/>
+      <c r="B50" s="224"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -38149,12 +38858,24 @@
       <c r="FQ50" s="187" t="s">
         <v>2789</v>
       </c>
+      <c r="FR50" s="115" t="s">
+        <v>2807</v>
+      </c>
+      <c r="FS50" s="155" t="s">
+        <v>2818</v>
+      </c>
+      <c r="FT50" s="155" t="s">
+        <v>2829</v>
+      </c>
+      <c r="FU50" s="155" t="s">
+        <v>2839</v>
+      </c>
     </row>
-    <row r="51" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="92">
         <v>48</v>
       </c>
-      <c r="B51" s="219"/>
+      <c r="B51" s="224"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -38668,12 +39389,24 @@
       <c r="FQ51" s="155" t="s">
         <v>2790</v>
       </c>
+      <c r="FR51" s="115" t="s">
+        <v>2808</v>
+      </c>
+      <c r="FS51" s="155" t="s">
+        <v>2819</v>
+      </c>
+      <c r="FT51" s="155" t="s">
+        <v>2830</v>
+      </c>
+      <c r="FU51" s="155" t="s">
+        <v>2840</v>
+      </c>
     </row>
-    <row r="52" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="92">
         <v>49</v>
       </c>
-      <c r="B52" s="219"/>
+      <c r="B52" s="224"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -39187,12 +39920,24 @@
       <c r="FQ52" s="155" t="s">
         <v>2791</v>
       </c>
+      <c r="FR52" s="115" t="s">
+        <v>2809</v>
+      </c>
+      <c r="FS52" s="155" t="s">
+        <v>2820</v>
+      </c>
+      <c r="FT52" s="155" t="s">
+        <v>2831</v>
+      </c>
+      <c r="FU52" s="155" t="s">
+        <v>2841</v>
+      </c>
     </row>
-    <row r="53" spans="1:173" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:177" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="92">
         <v>50</v>
       </c>
-      <c r="B53" s="220" t="s">
+      <c r="B53" s="225" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -39693,7 +40438,7 @@
       <c r="FL53" s="41" t="s">
         <v>860</v>
       </c>
-      <c r="FM53" s="223" t="s">
+      <c r="FM53" s="201" t="s">
         <v>207</v>
       </c>
       <c r="FN53" s="155" t="s">
@@ -39708,12 +40453,24 @@
       <c r="FQ53" s="155" t="s">
         <v>206</v>
       </c>
+      <c r="FR53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="FS53" s="155" t="s">
+        <v>206</v>
+      </c>
+      <c r="FT53" s="155" t="s">
+        <v>206</v>
+      </c>
+      <c r="FU53" s="69" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="54" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:177" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A54" s="92">
         <v>51</v>
       </c>
-      <c r="B54" s="220"/>
+      <c r="B54" s="225"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -40212,7 +40969,7 @@
       <c r="FL54" s="41" t="s">
         <v>858</v>
       </c>
-      <c r="FM54" s="223" t="s">
+      <c r="FM54" s="201" t="s">
         <v>858</v>
       </c>
       <c r="FN54" s="155" t="s">
@@ -40227,12 +40984,24 @@
       <c r="FQ54" s="155" t="s">
         <v>858</v>
       </c>
+      <c r="FR54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="FS54" s="155" t="s">
+        <v>858</v>
+      </c>
+      <c r="FT54" s="155" t="s">
+        <v>2651</v>
+      </c>
+      <c r="FU54" s="69" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="55" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:177" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A55" s="92">
         <v>52</v>
       </c>
-      <c r="B55" s="220"/>
+      <c r="B55" s="225"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -40731,7 +41500,7 @@
       <c r="FL55" s="41" t="s">
         <v>2606</v>
       </c>
-      <c r="FM55" s="223" t="s">
+      <c r="FM55" s="201" t="s">
         <v>2330</v>
       </c>
       <c r="FN55" s="155" t="s">
@@ -40746,12 +41515,24 @@
       <c r="FQ55" s="155" t="s">
         <v>2792</v>
       </c>
+      <c r="FR55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FS55" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FT55" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FU55" s="69" t="s">
+        <v>2842</v>
+      </c>
     </row>
-    <row r="56" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="92">
         <v>53</v>
       </c>
-      <c r="B56" s="220"/>
+      <c r="B56" s="225"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -41248,7 +42029,7 @@
       <c r="FL56" s="41" t="s">
         <v>2728</v>
       </c>
-      <c r="FM56" s="223" t="s">
+      <c r="FM56" s="201" t="s">
         <v>2330</v>
       </c>
       <c r="FN56" s="155" t="s">
@@ -41263,12 +42044,24 @@
       <c r="FQ56" s="155" t="s">
         <v>2793</v>
       </c>
+      <c r="FR56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FS56" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FT56" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FU56" s="69" t="s">
+        <v>2843</v>
+      </c>
     </row>
-    <row r="57" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:177" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A57" s="92">
         <v>54</v>
       </c>
-      <c r="B57" s="220"/>
+      <c r="B57" s="225"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -41767,7 +42560,7 @@
       <c r="FL57" s="41" t="s">
         <v>2720</v>
       </c>
-      <c r="FM57" s="223" t="s">
+      <c r="FM57" s="201" t="s">
         <v>2330</v>
       </c>
       <c r="FN57" s="155" t="s">
@@ -41782,12 +42575,24 @@
       <c r="FQ57" s="155" t="s">
         <v>2794</v>
       </c>
+      <c r="FR57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FS57" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FT57" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FU57" s="69" t="s">
+        <v>2844</v>
+      </c>
     </row>
-    <row r="58" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="92">
         <v>55</v>
       </c>
-      <c r="B58" s="220"/>
+      <c r="B58" s="225"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -42257,7 +43062,7 @@
       <c r="FL58" s="41" t="s">
         <v>2728</v>
       </c>
-      <c r="FM58" s="223" t="s">
+      <c r="FM58" s="201" t="s">
         <v>2330</v>
       </c>
       <c r="FN58" s="155" t="s">
@@ -42272,12 +43077,24 @@
       <c r="FQ58" s="155" t="s">
         <v>2795</v>
       </c>
+      <c r="FR58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FS58" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FT58" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FU58" s="69" t="s">
+        <v>2843</v>
+      </c>
     </row>
-    <row r="59" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="92">
         <v>56</v>
       </c>
-      <c r="B59" s="220"/>
+      <c r="B59" s="225"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -42776,7 +43593,7 @@
       <c r="FL59" s="41" t="s">
         <v>2728</v>
       </c>
-      <c r="FM59" s="223" t="s">
+      <c r="FM59" s="201" t="s">
         <v>2330</v>
       </c>
       <c r="FN59" s="155" t="s">
@@ -42791,12 +43608,24 @@
       <c r="FQ59" s="155" t="s">
         <v>2795</v>
       </c>
+      <c r="FR59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FS59" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FT59" s="155" t="s">
+        <v>2330</v>
+      </c>
+      <c r="FU59" s="156" t="s">
+        <v>2845</v>
+      </c>
     </row>
-    <row r="60" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="92">
         <v>57</v>
       </c>
-      <c r="B60" s="220"/>
+      <c r="B60" s="225"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -43295,7 +44124,7 @@
       <c r="FL60" s="41">
         <v>1</v>
       </c>
-      <c r="FM60" s="224">
+      <c r="FM60" s="202">
         <v>1</v>
       </c>
       <c r="FN60" s="188">
@@ -43310,12 +44139,24 @@
       <c r="FQ60" s="188">
         <v>1</v>
       </c>
+      <c r="FR60" s="184">
+        <v>1</v>
+      </c>
+      <c r="FS60" s="188">
+        <v>1</v>
+      </c>
+      <c r="FT60" s="188">
+        <v>1</v>
+      </c>
+      <c r="FU60" s="188">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:173" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:177" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="92">
         <v>58</v>
       </c>
-      <c r="B61" s="221" t="s">
+      <c r="B61" s="226" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -43814,7 +44655,7 @@
       <c r="FL61" s="157">
         <v>45727</v>
       </c>
-      <c r="FM61" s="225">
+      <c r="FM61" s="203">
         <v>45413</v>
       </c>
       <c r="FN61" s="189">
@@ -43829,12 +44670,24 @@
       <c r="FQ61" s="189">
         <v>45413</v>
       </c>
+      <c r="FR61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="FS61" s="189">
+        <v>45413</v>
+      </c>
+      <c r="FT61" s="189">
+        <v>45413</v>
+      </c>
+      <c r="FU61" s="227">
+        <v>45413</v>
+      </c>
     </row>
-    <row r="62" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="92">
         <v>59</v>
       </c>
-      <c r="B62" s="221"/>
+      <c r="B62" s="226"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -44333,7 +45186,7 @@
       <c r="FL62" s="157">
         <v>45769</v>
       </c>
-      <c r="FM62" s="226">
+      <c r="FM62" s="204">
         <v>45709</v>
       </c>
       <c r="FN62" s="190">
@@ -44348,12 +45201,24 @@
       <c r="FQ62" s="190">
         <v>45709</v>
       </c>
+      <c r="FR62" s="192">
+        <v>45736</v>
+      </c>
+      <c r="FS62" s="190">
+        <v>45709</v>
+      </c>
+      <c r="FT62" s="190">
+        <v>45709</v>
+      </c>
+      <c r="FU62" s="190">
+        <v>45709</v>
+      </c>
     </row>
-    <row r="63" spans="1:173" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:177" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="92">
         <v>60</v>
       </c>
-      <c r="B63" s="221"/>
+      <c r="B63" s="226"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -44867,12 +45732,24 @@
       <c r="FQ63" s="155" t="s">
         <v>2386</v>
       </c>
+      <c r="FR63" s="115" t="s">
+        <v>2331</v>
+      </c>
+      <c r="FS63" s="155" t="s">
+        <v>2331</v>
+      </c>
+      <c r="FT63" s="155" t="s">
+        <v>2653</v>
+      </c>
+      <c r="FU63" s="69" t="s">
+        <v>2331</v>
+      </c>
     </row>
-    <row r="64" spans="1:173" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:177" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A64" s="92">
         <v>61</v>
       </c>
-      <c r="B64" s="221"/>
+      <c r="B64" s="226"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -45384,6 +46261,18 @@
         <v>2332</v>
       </c>
       <c r="FQ64" s="155" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FR64" s="115" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FS64" s="155" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FT64" s="155" t="s">
+        <v>2332</v>
+      </c>
+      <c r="FU64" s="69" t="s">
         <v>2332</v>
       </c>
     </row>
@@ -45391,7 +46280,7 @@
       <c r="A65" s="92">
         <v>62</v>
       </c>
-      <c r="B65" s="221"/>
+      <c r="B65" s="226"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -45593,7 +46482,7 @@
       <c r="FL65" s="157">
         <v>45772</v>
       </c>
-      <c r="FM65" s="226">
+      <c r="FM65" s="204">
         <v>45784</v>
       </c>
       <c r="FN65" s="190">
@@ -45607,13 +46496,25 @@
       </c>
       <c r="FQ65" s="190">
         <v>45782</v>
+      </c>
+      <c r="FR65" s="192">
+        <v>45785</v>
+      </c>
+      <c r="FS65" s="190">
+        <v>45786</v>
+      </c>
+      <c r="FT65" s="190">
+        <v>45736</v>
+      </c>
+      <c r="FU65" s="190">
+        <v>45786</v>
       </c>
     </row>
     <row r="66" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A66" s="92">
         <v>63</v>
       </c>
-      <c r="B66" s="221"/>
+      <c r="B66" s="226"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -45828,12 +46729,24 @@
       <c r="FQ66" s="156" t="s">
         <v>30</v>
       </c>
+      <c r="FR66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="FS66" s="156" t="s">
+        <v>30</v>
+      </c>
+      <c r="FT66" s="156" t="s">
+        <v>2741</v>
+      </c>
+      <c r="FU66" s="191" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="67" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A67" s="92">
         <v>64</v>
       </c>
-      <c r="B67" s="221"/>
+      <c r="B67" s="226"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -45927,12 +46840,16 @@
       <c r="EV67" s="196"/>
       <c r="EW67" s="169"/>
       <c r="EZ67" s="156"/>
+      <c r="FR67" s="156"/>
+      <c r="FS67" s="156"/>
+      <c r="FT67" s="156"/>
+      <c r="FU67" s="191"/>
     </row>
     <row r="68" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A68" s="92">
         <v>65</v>
       </c>
-      <c r="B68" s="211" t="s">
+      <c r="B68" s="216" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -45989,12 +46906,13 @@
       <c r="EU68" s="196"/>
       <c r="EV68" s="196"/>
       <c r="EW68" s="169"/>
+      <c r="FS68" s="156"/>
     </row>
     <row r="69" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A69" s="92">
         <v>66</v>
       </c>
-      <c r="B69" s="211"/>
+      <c r="B69" s="216"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -46041,7 +46959,7 @@
       <c r="A70" s="92">
         <v>67</v>
       </c>
-      <c r="B70" s="211"/>
+      <c r="B70" s="216"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -46079,7 +46997,7 @@
       <c r="A71" s="92">
         <v>68</v>
       </c>
-      <c r="B71" s="211"/>
+      <c r="B71" s="216"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -46114,7 +47032,7 @@
       <c r="A72" s="92">
         <v>69</v>
       </c>
-      <c r="B72" s="212"/>
+      <c r="B72" s="217"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -47018,7 +47936,7 @@
       <c r="BT3" s="36"/>
     </row>
     <row r="4" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="218" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -47187,7 +48105,7 @@
       <c r="BT4" s="12"/>
     </row>
     <row r="5" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="214"/>
+      <c r="B5" s="219"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -47519,7 +48437,7 @@
       <c r="BT6" s="2"/>
     </row>
     <row r="7" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B7" s="215" t="s">
+      <c r="B7" s="220" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -47686,7 +48604,7 @@
       <c r="BT7" s="37"/>
     </row>
     <row r="8" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="215"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -47853,7 +48771,7 @@
       <c r="BT8" s="1"/>
     </row>
     <row r="9" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="215"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -48020,7 +48938,7 @@
       <c r="BT9" s="1"/>
     </row>
     <row r="10" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="215"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -48187,7 +49105,7 @@
       <c r="BT10" s="1"/>
     </row>
     <row r="11" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="216" t="s">
+      <c r="B11" s="221" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -48354,7 +49272,7 @@
       <c r="BT11" s="106"/>
     </row>
     <row r="12" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="217"/>
+      <c r="B12" s="222"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -48519,7 +49437,7 @@
       <c r="BT12" s="2"/>
     </row>
     <row r="13" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="217"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -48684,7 +49602,7 @@
       <c r="BT13" s="106"/>
     </row>
     <row r="14" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="217"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -48849,7 +49767,7 @@
       <c r="BT14" s="2"/>
     </row>
     <row r="15" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="217"/>
+      <c r="B15" s="222"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -49014,7 +49932,7 @@
       <c r="BT15" s="2"/>
     </row>
     <row r="16" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="217"/>
+      <c r="B16" s="222"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -49179,7 +50097,7 @@
       <c r="BT16" s="2"/>
     </row>
     <row r="17" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="217"/>
+      <c r="B17" s="222"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -49344,7 +50262,7 @@
       <c r="BT17" s="2"/>
     </row>
     <row r="18" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="217"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -49509,7 +50427,7 @@
       <c r="BT18" s="2"/>
     </row>
     <row r="19" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="217"/>
+      <c r="B19" s="222"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -49674,7 +50592,7 @@
       <c r="BT19" s="2"/>
     </row>
     <row r="20" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="217"/>
+      <c r="B20" s="222"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -49839,7 +50757,7 @@
       <c r="BT20" s="2"/>
     </row>
     <row r="21" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="218" t="s">
+      <c r="B21" s="223" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -50047,7 +50965,7 @@
       <c r="BT21" s="106"/>
     </row>
     <row r="22" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="218"/>
+      <c r="B22" s="223"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -50255,7 +51173,7 @@
       <c r="BT22" s="106"/>
     </row>
     <row r="23" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="218"/>
+      <c r="B23" s="223"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -50422,7 +51340,7 @@
       <c r="BT23" s="2"/>
     </row>
     <row r="24" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="218"/>
+      <c r="B24" s="223"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -50589,7 +51507,7 @@
       <c r="BT24" s="105"/>
     </row>
     <row r="25" spans="2:72" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="218"/>
+      <c r="B25" s="223"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -50754,7 +51672,7 @@
       <c r="BT25" s="6"/>
     </row>
     <row r="26" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="224" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -50923,7 +51841,7 @@
       <c r="BT26" s="38"/>
     </row>
     <row r="27" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="219"/>
+      <c r="B27" s="224"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -51090,7 +52008,7 @@
       <c r="BT27" s="42"/>
     </row>
     <row r="28" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="219"/>
+      <c r="B28" s="224"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -51255,7 +52173,7 @@
       <c r="BT28" s="66"/>
     </row>
     <row r="29" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="219"/>
+      <c r="B29" s="224"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -51420,7 +52338,7 @@
       <c r="BT29" s="42"/>
     </row>
     <row r="30" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="219"/>
+      <c r="B30" s="224"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -51585,7 +52503,7 @@
       <c r="BT30" s="38"/>
     </row>
     <row r="31" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="219"/>
+      <c r="B31" s="224"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -51750,7 +52668,7 @@
       <c r="BT31" s="42"/>
     </row>
     <row r="32" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="219"/>
+      <c r="B32" s="224"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -51915,7 +52833,7 @@
       <c r="BT32" s="88"/>
     </row>
     <row r="33" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="219"/>
+      <c r="B33" s="224"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -52080,7 +52998,7 @@
       <c r="BT33" s="28"/>
     </row>
     <row r="34" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="219"/>
+      <c r="B34" s="224"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -52245,7 +53163,7 @@
       <c r="BT34" s="38"/>
     </row>
     <row r="35" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="219"/>
+      <c r="B35" s="224"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -52410,7 +53328,7 @@
       <c r="BT35" s="42"/>
     </row>
     <row r="36" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="219"/>
+      <c r="B36" s="224"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -52575,7 +53493,7 @@
       <c r="BT36" s="38"/>
     </row>
     <row r="37" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="219"/>
+      <c r="B37" s="224"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -52740,7 +53658,7 @@
       <c r="BT37" s="42"/>
     </row>
     <row r="38" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="219"/>
+      <c r="B38" s="224"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -52905,7 +53823,7 @@
       <c r="BT38" s="38"/>
     </row>
     <row r="39" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="219"/>
+      <c r="B39" s="224"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -53070,7 +53988,7 @@
       <c r="BT39" s="38"/>
     </row>
     <row r="40" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="219"/>
+      <c r="B40" s="224"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -53235,7 +54153,7 @@
       <c r="BT40" s="38"/>
     </row>
     <row r="41" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="219"/>
+      <c r="B41" s="224"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -53400,7 +54318,7 @@
       <c r="BT41" s="38"/>
     </row>
     <row r="42" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="219"/>
+      <c r="B42" s="224"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -53565,7 +54483,7 @@
       <c r="BT42" s="38"/>
     </row>
     <row r="43" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="219"/>
+      <c r="B43" s="224"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -53730,7 +54648,7 @@
       <c r="BT43" s="38"/>
     </row>
     <row r="44" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="219"/>
+      <c r="B44" s="224"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -53895,7 +54813,7 @@
       <c r="BT44" s="38"/>
     </row>
     <row r="45" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="219"/>
+      <c r="B45" s="224"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -54060,7 +54978,7 @@
       <c r="BT45" s="38"/>
     </row>
     <row r="46" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="219"/>
+      <c r="B46" s="224"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -54225,7 +55143,7 @@
       <c r="BT46" s="38"/>
     </row>
     <row r="47" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="219"/>
+      <c r="B47" s="224"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -54390,7 +55308,7 @@
       <c r="BT47" s="38"/>
     </row>
     <row r="48" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="219"/>
+      <c r="B48" s="224"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -54555,7 +55473,7 @@
       <c r="BT48" s="38"/>
     </row>
     <row r="49" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="219"/>
+      <c r="B49" s="224"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -54720,7 +55638,7 @@
       <c r="BT49" s="38"/>
     </row>
     <row r="50" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="219"/>
+      <c r="B50" s="224"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -54887,7 +55805,7 @@
       <c r="BT50" s="2"/>
     </row>
     <row r="51" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="219"/>
+      <c r="B51" s="224"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -55054,7 +55972,7 @@
       <c r="BT51" s="2"/>
     </row>
     <row r="52" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="219"/>
+      <c r="B52" s="224"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -55221,7 +56139,7 @@
       <c r="BT52" s="2"/>
     </row>
     <row r="53" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="220" t="s">
+      <c r="B53" s="225" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -55390,7 +56308,7 @@
       <c r="BT53" s="105"/>
     </row>
     <row r="54" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="220"/>
+      <c r="B54" s="225"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -55557,7 +56475,7 @@
       <c r="BT54" s="5"/>
     </row>
     <row r="55" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="220"/>
+      <c r="B55" s="225"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -55724,7 +56642,7 @@
       <c r="BT55" s="5"/>
     </row>
     <row r="56" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="220"/>
+      <c r="B56" s="225"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -55889,7 +56807,7 @@
       <c r="BT56" s="3"/>
     </row>
     <row r="57" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="220"/>
+      <c r="B57" s="225"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -56056,7 +56974,7 @@
       <c r="BT57" s="2"/>
     </row>
     <row r="58" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B58" s="220"/>
+      <c r="B58" s="225"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -56221,7 +57139,7 @@
       <c r="BT58" s="7"/>
     </row>
     <row r="59" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="220"/>
+      <c r="B59" s="225"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -56388,7 +57306,7 @@
       <c r="BT59" s="5"/>
     </row>
     <row r="60" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B60" s="220"/>
+      <c r="B60" s="225"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -56555,7 +57473,7 @@
       <c r="BT60" s="12"/>
     </row>
     <row r="61" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="221" t="s">
+      <c r="B61" s="226" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -56722,7 +57640,7 @@
       <c r="BT61" s="9"/>
     </row>
     <row r="62" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="221"/>
+      <c r="B62" s="226"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -56889,7 +57807,7 @@
       <c r="BT62" s="9"/>
     </row>
     <row r="63" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="221"/>
+      <c r="B63" s="226"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -57056,7 +57974,7 @@
       <c r="BT63" s="5"/>
     </row>
     <row r="64" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="221"/>
+      <c r="B64" s="226"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -57223,7 +58141,7 @@
       <c r="BT64" s="2"/>
     </row>
     <row r="65" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="221"/>
+      <c r="B65" s="226"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -57240,7 +58158,7 @@
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="221"/>
+      <c r="B66" s="226"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -57259,7 +58177,7 @@
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="221"/>
+      <c r="B67" s="226"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -57278,7 +58196,7 @@
       <c r="P67" s="1"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B68" s="211" t="s">
+      <c r="B68" s="216" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -57288,7 +58206,7 @@
       <c r="L68" s="105"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B69" s="211"/>
+      <c r="B69" s="216"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -57296,7 +58214,7 @@
       <c r="K69" s="12"/>
     </row>
     <row r="70" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B70" s="211"/>
+      <c r="B70" s="216"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -57304,7 +58222,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B71" s="211"/>
+      <c r="B71" s="216"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -57316,7 +58234,7 @@
       <c r="L71" s="105"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B72" s="212"/>
+      <c r="B72" s="217"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -57896,7 +58814,7 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="218" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -57976,7 +58894,7 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="214"/>
+      <c r="B5" s="219"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -58130,7 +59048,7 @@
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B7" s="215" t="s">
+      <c r="B7" s="220" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -58208,7 +59126,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="215"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -58286,7 +59204,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="215"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -58364,7 +59282,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="215"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -58442,7 +59360,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="216" t="s">
+      <c r="B11" s="221" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -58520,7 +59438,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="217"/>
+      <c r="B12" s="222"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -58596,7 +59514,7 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="217"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -58672,7 +59590,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="217"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -58748,7 +59666,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="217"/>
+      <c r="B15" s="222"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -58824,7 +59742,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="217"/>
+      <c r="B16" s="222"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -58900,7 +59818,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="217"/>
+      <c r="B17" s="222"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -58976,7 +59894,7 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="217"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -59052,7 +59970,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="217"/>
+      <c r="B19" s="222"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -59128,7 +60046,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="217"/>
+      <c r="B20" s="222"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -59204,7 +60122,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="218" t="s">
+      <c r="B21" s="223" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -59282,7 +60200,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="218"/>
+      <c r="B22" s="223"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -59360,7 +60278,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="218"/>
+      <c r="B23" s="223"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -59438,7 +60356,7 @@
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B24" s="218"/>
+      <c r="B24" s="223"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -59516,7 +60434,7 @@
       </c>
     </row>
     <row r="25" spans="2:27" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="218"/>
+      <c r="B25" s="223"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -59592,7 +60510,7 @@
       </c>
     </row>
     <row r="26" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="224" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -59672,7 +60590,7 @@
       </c>
     </row>
     <row r="27" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="219"/>
+      <c r="B27" s="224"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -59750,7 +60668,7 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="219"/>
+      <c r="B28" s="224"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -59826,7 +60744,7 @@
       </c>
     </row>
     <row r="29" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="219"/>
+      <c r="B29" s="224"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -59902,7 +60820,7 @@
       </c>
     </row>
     <row r="30" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="219"/>
+      <c r="B30" s="224"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -59978,7 +60896,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="219"/>
+      <c r="B31" s="224"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -60054,7 +60972,7 @@
       </c>
     </row>
     <row r="32" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="219"/>
+      <c r="B32" s="224"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -60130,7 +61048,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="219"/>
+      <c r="B33" s="224"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -60206,7 +61124,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="219"/>
+      <c r="B34" s="224"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -60282,7 +61200,7 @@
       </c>
     </row>
     <row r="35" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="219"/>
+      <c r="B35" s="224"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -60358,7 +61276,7 @@
       </c>
     </row>
     <row r="36" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="219"/>
+      <c r="B36" s="224"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -60434,7 +61352,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="219"/>
+      <c r="B37" s="224"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -60510,7 +61428,7 @@
       </c>
     </row>
     <row r="38" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="219"/>
+      <c r="B38" s="224"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -60586,7 +61504,7 @@
       </c>
     </row>
     <row r="39" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="219"/>
+      <c r="B39" s="224"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -60662,7 +61580,7 @@
       </c>
     </row>
     <row r="40" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="219"/>
+      <c r="B40" s="224"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -60738,7 +61656,7 @@
       </c>
     </row>
     <row r="41" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="219"/>
+      <c r="B41" s="224"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -60814,7 +61732,7 @@
       </c>
     </row>
     <row r="42" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="219"/>
+      <c r="B42" s="224"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -60890,7 +61808,7 @@
       </c>
     </row>
     <row r="43" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="219"/>
+      <c r="B43" s="224"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -60966,7 +61884,7 @@
       </c>
     </row>
     <row r="44" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="219"/>
+      <c r="B44" s="224"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -61042,7 +61960,7 @@
       </c>
     </row>
     <row r="45" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="219"/>
+      <c r="B45" s="224"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -61118,7 +62036,7 @@
       </c>
     </row>
     <row r="46" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="219"/>
+      <c r="B46" s="224"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -61194,7 +62112,7 @@
       </c>
     </row>
     <row r="47" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="219"/>
+      <c r="B47" s="224"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -61270,7 +62188,7 @@
       </c>
     </row>
     <row r="48" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="219"/>
+      <c r="B48" s="224"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -61346,7 +62264,7 @@
       </c>
     </row>
     <row r="49" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="219"/>
+      <c r="B49" s="224"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -61422,7 +62340,7 @@
       </c>
     </row>
     <row r="50" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="219"/>
+      <c r="B50" s="224"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -61500,7 +62418,7 @@
       </c>
     </row>
     <row r="51" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="219"/>
+      <c r="B51" s="224"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -61578,7 +62496,7 @@
       </c>
     </row>
     <row r="52" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="219"/>
+      <c r="B52" s="224"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -61656,7 +62574,7 @@
       </c>
     </row>
     <row r="53" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B53" s="220" t="s">
+      <c r="B53" s="225" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -61736,7 +62654,7 @@
       </c>
     </row>
     <row r="54" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="220"/>
+      <c r="B54" s="225"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -61814,7 +62732,7 @@
       </c>
     </row>
     <row r="55" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="220"/>
+      <c r="B55" s="225"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -61892,7 +62810,7 @@
       </c>
     </row>
     <row r="56" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="220"/>
+      <c r="B56" s="225"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -61968,7 +62886,7 @@
       </c>
     </row>
     <row r="57" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="220"/>
+      <c r="B57" s="225"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -62046,7 +62964,7 @@
       </c>
     </row>
     <row r="58" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B58" s="220"/>
+      <c r="B58" s="225"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -62122,7 +63040,7 @@
       </c>
     </row>
     <row r="59" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="220"/>
+      <c r="B59" s="225"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -62200,7 +63118,7 @@
       </c>
     </row>
     <row r="60" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B60" s="220"/>
+      <c r="B60" s="225"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -62278,7 +63196,7 @@
       </c>
     </row>
     <row r="61" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B61" s="221" t="s">
+      <c r="B61" s="226" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -62356,7 +63274,7 @@
       </c>
     </row>
     <row r="62" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="221"/>
+      <c r="B62" s="226"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -62434,7 +63352,7 @@
       </c>
     </row>
     <row r="63" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="221"/>
+      <c r="B63" s="226"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -62512,7 +63430,7 @@
       </c>
     </row>
     <row r="64" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="221"/>
+      <c r="B64" s="226"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -62590,7 +63508,7 @@
       </c>
     </row>
     <row r="65" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="221"/>
+      <c r="B65" s="226"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -62620,7 +63538,7 @@
       <c r="AA65" s="5"/>
     </row>
     <row r="66" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="221"/>
+      <c r="B66" s="226"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -62650,7 +63568,7 @@
       <c r="AA66" s="5"/>
     </row>
     <row r="67" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="221"/>
+      <c r="B67" s="226"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -62680,7 +63598,7 @@
       <c r="AA67" s="1"/>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B68" s="211" t="s">
+      <c r="B68" s="216" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -62701,7 +63619,7 @@
       <c r="Q68" s="105"/>
     </row>
     <row r="69" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B69" s="211"/>
+      <c r="B69" s="216"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -62720,7 +63638,7 @@
       <c r="Q69" s="105"/>
     </row>
     <row r="70" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B70" s="211"/>
+      <c r="B70" s="216"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -62739,7 +63657,7 @@
       <c r="Q70" s="105"/>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B71" s="211"/>
+      <c r="B71" s="216"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -62758,7 +63676,7 @@
       <c r="Q71" s="105"/>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B72" s="212"/>
+      <c r="B72" s="217"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>

</xml_diff>

<commit_message>
late May 2026 labels update.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1B0172-17F4-4B73-87E2-9B48B7F44244}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4D7B6-8174-47F2-A6EE-269A73402F15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23836" uniqueCount="2961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14577" uniqueCount="3080">
   <si>
     <t>Description</t>
   </si>
@@ -8907,6 +8907,370 @@
   </si>
   <si>
     <t>May 23, 2025 update</t>
+  </si>
+  <si>
+    <t>3_LT_Vehicles_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>1 end use sector</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vehicle</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 vehicle types</t>
+  </si>
+  <si>
+    <t>EU and EFTA countries, China, global</t>
+  </si>
+  <si>
+    <t>ca. 2021</t>
+  </si>
+  <si>
+    <t>singly year value</t>
+  </si>
+  <si>
+    <t>Lifetimes of vehicles in the use phase. Region-specific estimates compiled from different sources.</t>
+  </si>
+  <si>
+    <t>lifetime; vehicle; use phase; useful product lifetime;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value(g,r,c,p)</t>
+  </si>
+  <si>
+    <t>Lifetime of bus in use phase - vehicles registered in Hungary in 2021 is 12 yr.</t>
+  </si>
+  <si>
+    <t>[Data type] of [Aspect 1] in [Aspect 4] registered in [Aspect 3] in [Aspect 2] is [value].</t>
+  </si>
+  <si>
+    <t>Numbers manually copied from original sources to Excel spreadsheet. Additional quality check by Stefan Pauliuk</t>
+  </si>
+  <si>
+    <t>4_PY_FabricationYield_Machinery_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>product manufacturing processes, also repair, refurbishmment, and remanufacturing</t>
+  </si>
+  <si>
+    <t>aggregate manufacturing step</t>
+  </si>
+  <si>
+    <t>different types</t>
+  </si>
+  <si>
+    <t>all materials, steel, aluminium</t>
+  </si>
+  <si>
+    <t>aggregate material groups</t>
+  </si>
+  <si>
+    <t>China, United States</t>
+  </si>
+  <si>
+    <t>country specific_average</t>
+  </si>
+  <si>
+    <t>Manufacturing yield factors for various commodity production and remanufacturing processes studied by the CIRCOMOD models</t>
+  </si>
+  <si>
+    <t>machinery; manufacturing; process yield; manufacturing yield; yield loss; remanufacturing</t>
+  </si>
+  <si>
+    <t>Value(m,g,v,t,r,p)</t>
+  </si>
+  <si>
+    <t>Yield coefficient measured as mass ratio of all materials into traditional vehicle engine in manufacturing of machinery and equipment n.e.c. in year n.a. in United States for CE strategy OEM new is 85%.</t>
+  </si>
+  <si>
+    <t>[Data type] measured as [Layer] of [Aspect 1] into [Aspect 2] in [Aspect 6] in [Aspect 4] in [Aspect 5] for CE strategy [Aspect 3] is [value].</t>
+  </si>
+  <si>
+    <t>May 24, 2025 update</t>
+  </si>
+  <si>
+    <t>4_PY_Vehicle_Manufacturing_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>vehicle manufacturing</t>
+  </si>
+  <si>
+    <t>1 end use sector</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vehicle</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 passenger vehicle types</t>
+  </si>
+  <si>
+    <t>steel, sheet metal</t>
+  </si>
+  <si>
+    <t>two material groups</t>
+  </si>
+  <si>
+    <t>Global, China, Europe, USA</t>
+  </si>
+  <si>
+    <t>Single-country and region value</t>
+  </si>
+  <si>
+    <t>2009-2060</t>
+  </si>
+  <si>
+    <t>annual values for selected years</t>
+  </si>
+  <si>
+    <t>Manufacturing yield factors for vehicles in different regions, compiled for CIRCOMOD EU project</t>
+  </si>
+  <si>
+    <t>manufacturing; yield loss; manufacturing yield; vehicles; process yield; new scrap; fabrication scrap</t>
+  </si>
+  <si>
+    <t>Yield loss (new scrap rate) = 1 - manufacturing yield.</t>
+  </si>
+  <si>
+    <t>Value(m,g,p,c,r,v,U)</t>
+  </si>
+  <si>
+    <t>Yield coefficient measured as mass ratio of sheet metal into passenger vehicles, segment B in manufacturing of passenger vehicles in Global in 2009-2015 for CE strategy 'none' is 61%.</t>
+  </si>
+  <si>
+    <t>[Data type] measured as [Layer] of [Aspect 1] into [Aspect 2] in [Aspect 3] in [Aspect 5] in [Aspect 4] for CE strategy [Aspect 6] is [value].</t>
+  </si>
+  <si>
+    <t>Numbers manually copied from original sources to Excel spreadsheet. Dataset reformatted and validated by Huimei Li.</t>
+  </si>
+  <si>
+    <t>4_PY_Vehicle_EoL_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>EoL vehicle scrap revovery (dismantling, shredding, sorting)</t>
+  </si>
+  <si>
+    <t>one aggregate process step</t>
+  </si>
+  <si>
+    <t>ca. 10 different materials</t>
+  </si>
+  <si>
+    <t>Sweden, Global</t>
+  </si>
+  <si>
+    <t>ca. 2010-2050</t>
+  </si>
+  <si>
+    <t>single values for selected years</t>
+  </si>
+  <si>
+    <t>Recycling, reuse, and energy recovery potentials for EoL vehicle materials</t>
+  </si>
+  <si>
+    <t>EoL vehicles; end-of-life vehicles; reuse; recycling; waste management; dismantling; sorting; shredding; EoL-RR; end-of-life recovery rate;</t>
+  </si>
+  <si>
+    <t>Value(m,g,p,t,r,v)</t>
+  </si>
+  <si>
+    <t>Yield coefficient measured as mass ratio of aluminium recovered as scrap from end-of-life passenger car, ICEV in treatment of end-of-life vehicle hulk, shredding in Sweden in ca. 2010 for CE strategy recycling is 95%.</t>
+  </si>
+  <si>
+    <t>[Data type] measured as [Layer] of [Aspect 1] recovered as scrap from [Aspect 2] in [Aspect 3] in [Aspect 5] in [Aspect 4] for CE strategy [Aspect 6] is [value].</t>
+  </si>
+  <si>
+    <t>3_EI_Other_Vehicles_CIRCOMOD_D4.2_2025</t>
+  </si>
+  <si>
+    <t>final energy</t>
+  </si>
+  <si>
+    <t>1 end use sector</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vehicle</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>14 vehicle types other than land vehicles</t>
+  </si>
+  <si>
+    <t>2000-2050</t>
+  </si>
+  <si>
+    <t>values for specific age-cohorts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific energy consumption per unit of use of products for land vehicles other than passenger vehicles, MJ/km of vehicle driven </t>
+  </si>
+  <si>
+    <t>specific energy consumption of products; use phase; energy intensity; other vehicles; driving</t>
+  </si>
+  <si>
+    <t>Value(n,g,p,V,r,c)</t>
+  </si>
+  <si>
+    <t>Specific energy consumption of products measured as final energy of diesel consumed by bus built in 2010 to generate kilometers driven in use phase - vehicles in OECD North America is 17.3 MJ/km.</t>
+  </si>
+  <si>
+    <t>[Data type] measured as [Layer] of [Aspect 1] consumed by [Aspect 2] built in [Aspect 6] to generate [Aspect 4] in [Aspect 3] in [Aspect 5] is [Value].</t>
+  </si>
+  <si>
+    <t>May 25, 2025 update</t>
+  </si>
+  <si>
+    <t>3_LT_Machinery_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>Use phase - machinery</t>
+  </si>
+  <si>
+    <t>one aggregate use phase / service lifetime</t>
+  </si>
+  <si>
+    <t>ca. 180 different types of machinery</t>
+  </si>
+  <si>
+    <t>values for Europe and Japan</t>
+  </si>
+  <si>
+    <t>ca. 2008-2018</t>
+  </si>
+  <si>
+    <t>single values</t>
+  </si>
+  <si>
+    <t>Life time of machinery in the use phase, by type of machinery</t>
+  </si>
+  <si>
+    <t>lifetime; machinery; service life; use phase</t>
+  </si>
+  <si>
+    <t>Data compiled from different sources - see the comment for each data point for its reference.</t>
+  </si>
+  <si>
+    <t>Lifetime of shovel excavators in use phase - machinery in Japan built in ca. 2018 is 12.5 yr.</t>
+  </si>
+  <si>
+    <t>[Data type] of [Aspect 1] in [Aspect 2] in [Aspect 3] built in [Aspect 4] is [Value].</t>
+  </si>
+  <si>
+    <t>Numbers manually copied from original sources to Excel spreadsheet, Johan Vélez helped with the reformatting</t>
+  </si>
+  <si>
+    <t>3_LT_Buildings_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>Buildings and building parts</t>
+  </si>
+  <si>
+    <t>11 building types and 15 building parts</t>
+  </si>
+  <si>
+    <t>all years</t>
+  </si>
+  <si>
+    <t>Lifetime of buildings, building parts and lifetime distributions</t>
+  </si>
+  <si>
+    <t>lifetime; buildings; lifetime distribution; useful life; lifespan; use phase</t>
+  </si>
+  <si>
+    <t>Lifetime of urban detached building in use phase - buildings in IMAGE 3.0|Central Asia built in all years is 60 yr.</t>
+  </si>
+  <si>
+    <t>[Data type] of [Aspect 1] in [Aspect 4] in [Aspect 2] built in [Aspect 3] is [Value].</t>
+  </si>
+  <si>
+    <t>Christian Hauenstein</t>
+  </si>
+  <si>
+    <t>May 26, 2025 update</t>
+  </si>
+  <si>
+    <t>6_CR_EU_criticality_RMIS_2023</t>
+  </si>
+  <si>
+    <t>aggregated across all products, economy-wide</t>
+  </si>
+  <si>
+    <t>selected materials from RMIS that are not covered in the critial materials of the EU (2020 list)</t>
+  </si>
+  <si>
+    <t>20 metals and minerals</t>
+  </si>
+  <si>
+    <t>2015-2022</t>
+  </si>
+  <si>
+    <t>EU import dependencies and recycling rates as proxy for material criticality. Extracted from RMIS 3.0, released in March 2023.</t>
+  </si>
+  <si>
+    <t>EU; import; recycling rate; critical materials; material criticality; criticality indicator; RMIS</t>
+  </si>
+  <si>
+    <t>Data extracted from Raw Materials Profiles (https://rmis.jrc.ec.europa.eu/rmp/) of the European Commission. RMIS 3.0, released in March 2023. If information on extraction and processing stage were available, the processing stage (refined metals) was preferred. "Import share EU" shows the main EU sourcing countries</t>
+  </si>
+  <si>
+    <t>Criticality measured as end-of-life recycling input rate for antimony in form of refined metal for European Union in 2012 is 28%.</t>
+  </si>
+  <si>
+    <t>[Data type] measured as [Aspect 3] for [Aspect 1] in form of [Aspect 2] for [Aspect 4] in [Aspect 5] is [Value].</t>
+  </si>
+  <si>
+    <t>European Commission, JRC</t>
+  </si>
+  <si>
+    <t>https://rmis.jrc.ec.europa.eu/uploads/rmp/info-dashboard.pdf</t>
+  </si>
+  <si>
+    <t>https://rmis.jrc.ec.europa.eu/about</t>
+  </si>
+  <si>
+    <t>EU-JRC RMIS 3.0, released in March 2023.</t>
+  </si>
+  <si>
+    <t>Numbers copied from original source (website) to Excel spreadsheet</t>
+  </si>
+  <si>
+    <t>1_F_Lumber_Cement_Plastics_Production_byCountry_2020</t>
+  </si>
+  <si>
+    <t>cement, plastics, lumber</t>
+  </si>
+  <si>
+    <t>3 aggregate material groups; lumber is additionally differentiated into 3 categories</t>
+  </si>
+  <si>
+    <t>2019-2023</t>
+  </si>
+  <si>
+    <t>Production of cement, plastics, lumber, by country</t>
+  </si>
+  <si>
+    <t>cement; plastics; lumber; production; timber; wood; production statistics; production flow</t>
+  </si>
+  <si>
+    <t>For lumber, the data considered all countries and was further filtered by production quantity for the years 2019-2023 with a focus on "Sawnwood, coniferous", "Sawnwood, non-coniferous", "Veneer sheets", "Plywood and LVL", "Particle board", "Oriented strand board (OSB)", "Hardboard", "Medium/high density fibreboard (MDF/HDF)", "Other fibreboard", "Glue-laminated timber (glulam)", "Cross-laminated timber (CLT or X-lam)", "I-beams (I-joists)", "Wooden furniture (export/import)", "Prefabricated buildings of wood (export/import)" and "Other manufactured wood products (export/import)". The mass of I-beams was converted to a volume to match the other units using an estimated density of 570 kg/m³.</t>
+  </si>
+  <si>
+    <t>Mass of flow of cement from material production to market for refined materials in South Africa in 2019 was 12400000 t/yr.</t>
+  </si>
+  <si>
+    <t>[Layer] of [Data type] of [Aspect 3] flowing from [Aspect 1] to [Aspect 2] in [Aspect 4] in [Aspect 5] has [Value].</t>
+  </si>
+  <si>
+    <t>website with table</t>
+  </si>
+  <si>
+    <t>Marina Haug</t>
   </si>
 </sst>
 </file>
@@ -8916,7 +9280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -9046,6 +9410,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -9298,7 +9668,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -9665,6 +10035,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9731,6 +10112,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -10071,7 +10453,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B4" s="215" t="s">
+      <c r="B4" s="220" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -10103,7 +10485,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B5" s="215"/>
+      <c r="B5" s="220"/>
       <c r="C5" s="26" t="s">
         <v>422</v>
       </c>
@@ -10133,7 +10515,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="216" t="s">
+      <c r="B6" s="221" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -10149,7 +10531,7 @@
       <c r="K6" s="121"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B7" s="216"/>
+      <c r="B7" s="221"/>
       <c r="C7" s="26" t="s">
         <v>424</v>
       </c>
@@ -10163,7 +10545,7 @@
       <c r="K7" s="121"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B8" s="216"/>
+      <c r="B8" s="221"/>
       <c r="C8" s="26" t="s">
         <v>425</v>
       </c>
@@ -10177,7 +10559,7 @@
       <c r="K8" s="121"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B9" s="216"/>
+      <c r="B9" s="221"/>
       <c r="C9" s="28" t="s">
         <v>426</v>
       </c>
@@ -10191,7 +10573,7 @@
       <c r="K9" s="121"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B10" s="216"/>
+      <c r="B10" s="221"/>
       <c r="C10" s="27" t="s">
         <v>427</v>
       </c>
@@ -10205,7 +10587,7 @@
       <c r="K10" s="121"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B11" s="216"/>
+      <c r="B11" s="221"/>
       <c r="C11" s="27" t="s">
         <v>428</v>
       </c>
@@ -10219,7 +10601,7 @@
       <c r="K11" s="121"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B12" s="216"/>
+      <c r="B12" s="221"/>
       <c r="C12" s="27" t="s">
         <v>429</v>
       </c>
@@ -10233,7 +10615,7 @@
       <c r="K12" s="121"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B13" s="216"/>
+      <c r="B13" s="221"/>
       <c r="C13" s="27" t="s">
         <v>430</v>
       </c>
@@ -10247,7 +10629,7 @@
       <c r="K13" s="121"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B14" s="216"/>
+      <c r="B14" s="221"/>
       <c r="C14" s="27" t="s">
         <v>431</v>
       </c>
@@ -10261,7 +10643,7 @@
       <c r="K14" s="121"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B15" s="216"/>
+      <c r="B15" s="221"/>
       <c r="C15" s="27" t="s">
         <v>432</v>
       </c>
@@ -10275,7 +10657,7 @@
       <c r="K15" s="121"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B16" s="216"/>
+      <c r="B16" s="221"/>
       <c r="C16" s="27" t="s">
         <v>433</v>
       </c>
@@ -10289,7 +10671,7 @@
       <c r="K16" s="121"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B17" s="216"/>
+      <c r="B17" s="221"/>
       <c r="C17" s="27" t="s">
         <v>434</v>
       </c>
@@ -10303,7 +10685,7 @@
       <c r="K17" s="121"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B18" s="216"/>
+      <c r="B18" s="221"/>
       <c r="C18" s="27" t="s">
         <v>435</v>
       </c>
@@ -10317,7 +10699,7 @@
       <c r="K18" s="121"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B19" s="217" t="s">
+      <c r="B19" s="222" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -10345,7 +10727,7 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B20" s="217"/>
+      <c r="B20" s="222"/>
       <c r="C20" s="27" t="s">
         <v>437</v>
       </c>
@@ -10375,7 +10757,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B21" s="217"/>
+      <c r="B21" s="222"/>
       <c r="C21" s="27" t="s">
         <v>438</v>
       </c>
@@ -10401,7 +10783,7 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="218" t="s">
+      <c r="B22" s="223" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -10431,7 +10813,7 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B23" s="218"/>
+      <c r="B23" s="223"/>
       <c r="C23" s="26" t="s">
         <v>440</v>
       </c>
@@ -10445,7 +10827,7 @@
       <c r="K23" s="121"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B24" s="218"/>
+      <c r="B24" s="223"/>
       <c r="C24" s="25" t="s">
         <v>441</v>
       </c>
@@ -10459,7 +10841,7 @@
       <c r="K24" s="121"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B25" s="218"/>
+      <c r="B25" s="223"/>
       <c r="C25" s="25" t="s">
         <v>443</v>
       </c>
@@ -10485,7 +10867,7 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B26" s="218"/>
+      <c r="B26" s="223"/>
       <c r="C26" s="25" t="s">
         <v>444</v>
       </c>
@@ -10501,7 +10883,7 @@
       <c r="K26" s="121"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B27" s="218"/>
+      <c r="B27" s="223"/>
       <c r="C27" s="25" t="s">
         <v>445</v>
       </c>
@@ -10515,7 +10897,7 @@
       <c r="K27" s="121"/>
     </row>
     <row r="28" spans="2:11" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="219" t="s">
+      <c r="B28" s="224" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -10547,7 +10929,7 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B29" s="219"/>
+      <c r="B29" s="224"/>
       <c r="C29" s="25" t="s">
         <v>447</v>
       </c>
@@ -10577,7 +10959,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B30" s="212" t="s">
+      <c r="B30" s="217" t="s">
         <v>185</v>
       </c>
       <c r="C30" s="107" t="s">
@@ -10593,7 +10975,7 @@
       <c r="K30" s="181"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B31" s="213"/>
+      <c r="B31" s="218"/>
       <c r="C31" s="108" t="s">
         <v>449</v>
       </c>
@@ -10607,7 +10989,7 @@
       <c r="K31" s="164"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B32" s="214"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="109" t="s">
         <v>450</v>
       </c>
@@ -10773,7 +11155,7 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B4" s="220" t="s">
+      <c r="B4" s="225" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -10865,7 +11247,7 @@
       </c>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B5" s="221"/>
+      <c r="B5" s="226"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
       </c>
@@ -11133,7 +11515,7 @@
       </c>
     </row>
     <row r="8" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="216" t="s">
+      <c r="B8" s="221" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="54" t="s">
@@ -11223,7 +11605,7 @@
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B9" s="216"/>
+      <c r="B9" s="221"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
       </c>
@@ -11311,7 +11693,7 @@
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B10" s="216"/>
+      <c r="B10" s="221"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
       </c>
@@ -11399,7 +11781,7 @@
       </c>
     </row>
     <row r="11" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="216"/>
+      <c r="B11" s="221"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
       </c>
@@ -11487,7 +11869,7 @@
       </c>
     </row>
     <row r="12" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="216"/>
+      <c r="B12" s="221"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -11575,7 +11957,7 @@
       </c>
     </row>
     <row r="13" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="216"/>
+      <c r="B13" s="221"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -11663,7 +12045,7 @@
       </c>
     </row>
     <row r="14" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="216"/>
+      <c r="B14" s="221"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -11751,7 +12133,7 @@
       </c>
     </row>
     <row r="15" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="216"/>
+      <c r="B15" s="221"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -11839,7 +12221,7 @@
       </c>
     </row>
     <row r="16" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="216"/>
+      <c r="B16" s="221"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -11927,7 +12309,7 @@
       </c>
     </row>
     <row r="17" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="216"/>
+      <c r="B17" s="221"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -12015,7 +12397,7 @@
       </c>
     </row>
     <row r="18" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="216"/>
+      <c r="B18" s="221"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -12103,7 +12485,7 @@
       </c>
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B19" s="216"/>
+      <c r="B19" s="221"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -12191,7 +12573,7 @@
       </c>
     </row>
     <row r="20" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="216"/>
+      <c r="B20" s="221"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -12279,7 +12661,7 @@
       </c>
     </row>
     <row r="21" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="217" t="s">
+      <c r="B21" s="222" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -12369,7 +12751,7 @@
       </c>
     </row>
     <row r="22" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="217"/>
+      <c r="B22" s="222"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -12459,7 +12841,7 @@
       </c>
     </row>
     <row r="23" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B23" s="217"/>
+      <c r="B23" s="222"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
       </c>
@@ -12547,7 +12929,7 @@
       </c>
     </row>
     <row r="24" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="217"/>
+      <c r="B24" s="222"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
       </c>
@@ -12629,7 +13011,7 @@
       <c r="AE24" s="164"/>
     </row>
     <row r="25" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="218" t="s">
+      <c r="B25" s="223" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -12719,7 +13101,7 @@
       </c>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B26" s="218"/>
+      <c r="B26" s="223"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
       </c>
@@ -12807,7 +13189,7 @@
       </c>
     </row>
     <row r="27" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B27" s="218"/>
+      <c r="B27" s="223"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
       </c>
@@ -12895,7 +13277,7 @@
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B28" s="218"/>
+      <c r="B28" s="223"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
       </c>
@@ -12983,7 +13365,7 @@
       </c>
     </row>
     <row r="29" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="218"/>
+      <c r="B29" s="223"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
       </c>
@@ -13071,7 +13453,7 @@
       </c>
     </row>
     <row r="30" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="218"/>
+      <c r="B30" s="223"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
       </c>
@@ -13159,7 +13541,7 @@
       </c>
     </row>
     <row r="31" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="219" t="s">
+      <c r="B31" s="224" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -13251,7 +13633,7 @@
       </c>
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B32" s="222"/>
+      <c r="B32" s="227"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
       </c>
@@ -13341,7 +13723,7 @@
       </c>
     </row>
     <row r="33" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B33" s="212" t="s">
+      <c r="B33" s="217" t="s">
         <v>185</v>
       </c>
       <c r="C33" s="83" t="s">
@@ -13377,7 +13759,7 @@
       <c r="AE33" s="164"/>
     </row>
     <row r="34" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B34" s="213"/>
+      <c r="B34" s="218"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
       </c>
@@ -13411,7 +13793,7 @@
       <c r="AE34" s="164"/>
     </row>
     <row r="35" spans="2:31" x14ac:dyDescent="0.4">
-      <c r="B35" s="214"/>
+      <c r="B35" s="219"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
       </c>
@@ -13469,10 +13851,10 @@
   <dimension ref="A1:GW74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="FP24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="DK24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="GE3" sqref="GE3"/>
+      <selection pane="bottomRight" activeCell="DV5" sqref="DV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -13533,7 +13915,7 @@
     <col min="70" max="16384" width="11.5546875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:187" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:196" x14ac:dyDescent="0.4">
       <c r="C1" s="73" t="s">
         <v>269</v>
       </c>
@@ -14024,8 +14406,17 @@
       <c r="GC1" s="174"/>
       <c r="GD1" s="174"/>
       <c r="GE1" s="174"/>
+      <c r="GF1" s="174"/>
+      <c r="GG1" s="174"/>
+      <c r="GH1" s="174"/>
+      <c r="GI1" s="174"/>
+      <c r="GJ1" s="174"/>
+      <c r="GK1" s="174"/>
+      <c r="GL1" s="174"/>
+      <c r="GM1" s="174"/>
+      <c r="GN1" s="174"/>
     </row>
-    <row r="2" spans="1:187" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:196" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B2" s="34" t="s">
         <v>183</v>
       </c>
@@ -14402,8 +14793,35 @@
       <c r="GE2" s="154" t="s">
         <v>2960</v>
       </c>
+      <c r="GF2" s="154" t="s">
+        <v>2987</v>
+      </c>
+      <c r="GG2" s="154" t="s">
+        <v>2987</v>
+      </c>
+      <c r="GH2" s="154" t="s">
+        <v>2987</v>
+      </c>
+      <c r="GI2" s="154" t="s">
+        <v>2987</v>
+      </c>
+      <c r="GJ2" s="154" t="s">
+        <v>3030</v>
+      </c>
+      <c r="GK2" s="154" t="s">
+        <v>3053</v>
+      </c>
+      <c r="GL2" s="154" t="s">
+        <v>3053</v>
+      </c>
+      <c r="GM2" s="154" t="s">
+        <v>3053</v>
+      </c>
+      <c r="GN2" s="154" t="s">
+        <v>3053</v>
+      </c>
     </row>
-    <row r="3" spans="1:187" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:196" x14ac:dyDescent="0.4">
       <c r="B3" s="58"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -14656,11 +15074,11 @@
       <c r="DS3" s="105"/>
       <c r="DT3" s="105"/>
     </row>
-    <row r="4" spans="1:187" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:196" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>1</v>
       </c>
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="230" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -14914,11 +15332,11 @@
       <c r="DS4" s="105"/>
       <c r="DT4" s="105"/>
     </row>
-    <row r="5" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="226"/>
+      <c r="B5" s="231"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -15474,8 +15892,35 @@
       <c r="GE5" s="115" t="s">
         <v>2945</v>
       </c>
+      <c r="GF5" s="159" t="s">
+        <v>2961</v>
+      </c>
+      <c r="GG5" s="208" t="s">
+        <v>2974</v>
+      </c>
+      <c r="GH5" s="159" t="s">
+        <v>2988</v>
+      </c>
+      <c r="GI5" s="159" t="s">
+        <v>3006</v>
+      </c>
+      <c r="GJ5" s="159" t="s">
+        <v>3018</v>
+      </c>
+      <c r="GK5" s="159" t="s">
+        <v>3031</v>
+      </c>
+      <c r="GL5" s="115" t="s">
+        <v>3044</v>
+      </c>
+      <c r="GM5" s="115" t="s">
+        <v>3054</v>
+      </c>
+      <c r="GN5" s="115" t="s">
+        <v>3069</v>
+      </c>
     </row>
-    <row r="6" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="92">
         <v>3</v>
       </c>
@@ -16033,12 +16478,39 @@
       <c r="GE6" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GF6" s="159" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GG6" s="208" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GH6" s="159" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GI6" s="159" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GJ6" s="159" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GK6" s="187" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GL6" s="115" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GM6" s="115" t="s">
+        <v>1150</v>
+      </c>
+      <c r="GN6" s="115" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="7" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="92">
         <v>4</v>
       </c>
-      <c r="B7" s="227" t="s">
+      <c r="B7" s="232" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -16594,12 +17066,39 @@
       <c r="GE7" s="115" t="s">
         <v>845</v>
       </c>
+      <c r="GF7" s="159" t="s">
+        <v>845</v>
+      </c>
+      <c r="GG7" s="208">
+        <v>20</v>
+      </c>
+      <c r="GH7" s="208">
+        <v>20</v>
+      </c>
+      <c r="GI7" s="208">
+        <v>20</v>
+      </c>
+      <c r="GJ7" s="159" t="s">
+        <v>845</v>
+      </c>
+      <c r="GK7" s="187">
+        <v>20</v>
+      </c>
+      <c r="GL7" s="115">
+        <v>20</v>
+      </c>
+      <c r="GM7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GN7" s="115">
+        <v>24</v>
+      </c>
     </row>
-    <row r="8" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="92">
         <v>5</v>
       </c>
-      <c r="B8" s="227"/>
+      <c r="B8" s="232"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -17155,12 +17654,39 @@
       <c r="GE8" s="115">
         <v>3</v>
       </c>
+      <c r="GF8" s="159">
+        <v>3</v>
+      </c>
+      <c r="GG8" s="208">
+        <v>4</v>
+      </c>
+      <c r="GH8" s="159">
+        <v>4</v>
+      </c>
+      <c r="GI8" s="159">
+        <v>4</v>
+      </c>
+      <c r="GJ8" s="159">
+        <v>3</v>
+      </c>
+      <c r="GK8" s="115">
+        <v>3</v>
+      </c>
+      <c r="GL8" s="115">
+        <v>3</v>
+      </c>
+      <c r="GM8" s="115">
+        <v>6</v>
+      </c>
+      <c r="GN8" s="115">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="92">
         <v>6</v>
       </c>
-      <c r="B9" s="227"/>
+      <c r="B9" s="232"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -17716,12 +18242,39 @@
       <c r="GE9" s="115" t="s">
         <v>190</v>
       </c>
+      <c r="GF9" s="159" t="s">
+        <v>57</v>
+      </c>
+      <c r="GG9" s="208" t="s">
+        <v>94</v>
+      </c>
+      <c r="GH9" s="159" t="s">
+        <v>94</v>
+      </c>
+      <c r="GI9" s="159" t="s">
+        <v>94</v>
+      </c>
+      <c r="GJ9" s="159" t="s">
+        <v>2061</v>
+      </c>
+      <c r="GK9" s="159" t="s">
+        <v>57</v>
+      </c>
+      <c r="GL9" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="GM9" s="115" t="s">
+        <v>2708</v>
+      </c>
+      <c r="GN9" s="115" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="92">
         <v>7</v>
       </c>
-      <c r="B10" s="227"/>
+      <c r="B10" s="232"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -18277,12 +18830,39 @@
       <c r="GE10" s="115" t="s">
         <v>2873</v>
       </c>
+      <c r="GF10" s="159" t="s">
+        <v>57</v>
+      </c>
+      <c r="GG10" s="208" t="s">
+        <v>5</v>
+      </c>
+      <c r="GH10" s="159" t="s">
+        <v>5</v>
+      </c>
+      <c r="GI10" s="159" t="s">
+        <v>5</v>
+      </c>
+      <c r="GJ10" s="159" t="s">
+        <v>3019</v>
+      </c>
+      <c r="GK10" s="159" t="s">
+        <v>57</v>
+      </c>
+      <c r="GL10" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="GM10" s="115" t="s">
+        <v>1091</v>
+      </c>
+      <c r="GN10" s="115" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="11" spans="1:187" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:196" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="92">
         <v>8</v>
       </c>
-      <c r="B11" s="228" t="s">
+      <c r="B11" s="233" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -18838,12 +19418,39 @@
       <c r="GE11" s="115" t="s">
         <v>32</v>
       </c>
+      <c r="GF11" s="159" t="s">
+        <v>32</v>
+      </c>
+      <c r="GG11" s="209" t="s">
+        <v>2975</v>
+      </c>
+      <c r="GH11" s="159" t="s">
+        <v>2989</v>
+      </c>
+      <c r="GI11" s="159" t="s">
+        <v>3007</v>
+      </c>
+      <c r="GJ11" s="159" t="s">
+        <v>32</v>
+      </c>
+      <c r="GK11" s="159" t="s">
+        <v>3032</v>
+      </c>
+      <c r="GL11" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="GM11" s="115" t="s">
+        <v>779</v>
+      </c>
+      <c r="GN11" s="115" t="s">
+        <v>1474</v>
+      </c>
     </row>
-    <row r="12" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="92">
         <v>9</v>
       </c>
-      <c r="B12" s="229"/>
+      <c r="B12" s="234"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -19397,12 +20004,39 @@
       <c r="GE12" s="115" t="s">
         <v>2008</v>
       </c>
+      <c r="GF12" s="159" t="s">
+        <v>2962</v>
+      </c>
+      <c r="GG12" s="208" t="s">
+        <v>2976</v>
+      </c>
+      <c r="GH12" s="159" t="s">
+        <v>2990</v>
+      </c>
+      <c r="GI12" s="159" t="s">
+        <v>3008</v>
+      </c>
+      <c r="GJ12" s="159" t="s">
+        <v>3020</v>
+      </c>
+      <c r="GK12" s="159" t="s">
+        <v>3033</v>
+      </c>
+      <c r="GL12" s="115" t="s">
+        <v>152</v>
+      </c>
+      <c r="GM12" s="115" t="s">
+        <v>868</v>
+      </c>
+      <c r="GN12" s="115" t="s">
+        <v>2274</v>
+      </c>
     </row>
-    <row r="13" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="92">
         <v>10</v>
       </c>
-      <c r="B13" s="229"/>
+      <c r="B13" s="234"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -19956,12 +20590,39 @@
       <c r="GE13" s="115" t="s">
         <v>1561</v>
       </c>
+      <c r="GF13" s="159" t="s">
+        <v>2963</v>
+      </c>
+      <c r="GG13" s="208" t="s">
+        <v>2935</v>
+      </c>
+      <c r="GH13" s="159" t="s">
+        <v>2991</v>
+      </c>
+      <c r="GI13" s="159" t="s">
+        <v>597</v>
+      </c>
+      <c r="GJ13" s="159" t="s">
+        <v>3021</v>
+      </c>
+      <c r="GK13" s="159" t="s">
+        <v>2935</v>
+      </c>
+      <c r="GL13" s="115" t="s">
+        <v>3045</v>
+      </c>
+      <c r="GM13" s="115" t="s">
+        <v>1561</v>
+      </c>
+      <c r="GN13" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="14" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="92">
         <v>11</v>
       </c>
-      <c r="B14" s="229"/>
+      <c r="B14" s="234"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -20515,12 +21176,39 @@
       <c r="GE14" s="115" t="s">
         <v>2946</v>
       </c>
+      <c r="GF14" s="159" t="s">
+        <v>2964</v>
+      </c>
+      <c r="GG14" s="208" t="s">
+        <v>2977</v>
+      </c>
+      <c r="GH14" s="159" t="s">
+        <v>2992</v>
+      </c>
+      <c r="GI14" s="159" t="s">
+        <v>816</v>
+      </c>
+      <c r="GJ14" s="159" t="s">
+        <v>3022</v>
+      </c>
+      <c r="GK14" s="159" t="s">
+        <v>3034</v>
+      </c>
+      <c r="GL14" s="115" t="s">
+        <v>3046</v>
+      </c>
+      <c r="GM14" s="115" t="s">
+        <v>3055</v>
+      </c>
+      <c r="GN14" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="15" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="92">
         <v>12</v>
       </c>
-      <c r="B15" s="229"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -21074,12 +21762,39 @@
       <c r="GE15" s="115" t="s">
         <v>1679</v>
       </c>
+      <c r="GF15" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG15" s="208" t="s">
+        <v>2978</v>
+      </c>
+      <c r="GH15" s="159" t="s">
+        <v>2993</v>
+      </c>
+      <c r="GI15" s="159" t="s">
+        <v>2345</v>
+      </c>
+      <c r="GJ15" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK15" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL15" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM15" s="115" t="s">
+        <v>3056</v>
+      </c>
+      <c r="GN15" s="115" t="s">
+        <v>3070</v>
+      </c>
     </row>
-    <row r="16" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="92">
         <v>13</v>
       </c>
-      <c r="B16" s="229"/>
+      <c r="B16" s="234"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -21633,12 +22348,39 @@
       <c r="GE16" s="115" t="s">
         <v>2947</v>
       </c>
+      <c r="GF16" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG16" s="208" t="s">
+        <v>2979</v>
+      </c>
+      <c r="GH16" s="159" t="s">
+        <v>2994</v>
+      </c>
+      <c r="GI16" s="159" t="s">
+        <v>3009</v>
+      </c>
+      <c r="GJ16" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK16" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL16" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM16" s="115" t="s">
+        <v>3057</v>
+      </c>
+      <c r="GN16" s="115" t="s">
+        <v>3071</v>
+      </c>
     </row>
-    <row r="17" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="92">
         <v>14</v>
       </c>
-      <c r="B17" s="229"/>
+      <c r="B17" s="234"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -22192,12 +22934,39 @@
       <c r="GE17" s="115" t="s">
         <v>189</v>
       </c>
+      <c r="GF17" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="GG17" s="208" t="s">
+        <v>2980</v>
+      </c>
+      <c r="GH17" s="159" t="s">
+        <v>2995</v>
+      </c>
+      <c r="GI17" s="159" t="s">
+        <v>3010</v>
+      </c>
+      <c r="GJ17" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="GK17" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="GL17" s="115" t="s">
+        <v>819</v>
+      </c>
+      <c r="GM17" s="115" t="s">
+        <v>1422</v>
+      </c>
+      <c r="GN17" s="115" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="92">
         <v>15</v>
       </c>
-      <c r="B18" s="229"/>
+      <c r="B18" s="234"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -22751,12 +23520,39 @@
       <c r="GE18" s="115" t="s">
         <v>2688</v>
       </c>
+      <c r="GF18" s="159" t="s">
+        <v>2965</v>
+      </c>
+      <c r="GG18" s="208" t="s">
+        <v>2981</v>
+      </c>
+      <c r="GH18" s="159" t="s">
+        <v>2996</v>
+      </c>
+      <c r="GI18" s="159" t="s">
+        <v>2762</v>
+      </c>
+      <c r="GJ18" s="159" t="s">
+        <v>2996</v>
+      </c>
+      <c r="GK18" s="159" t="s">
+        <v>3035</v>
+      </c>
+      <c r="GL18" s="115" t="s">
+        <v>2762</v>
+      </c>
+      <c r="GM18" s="115" t="s">
+        <v>2711</v>
+      </c>
+      <c r="GN18" s="115" t="s">
+        <v>2658</v>
+      </c>
     </row>
-    <row r="19" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="92">
         <v>16</v>
       </c>
-      <c r="B19" s="229"/>
+      <c r="B19" s="234"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -23310,12 +24106,39 @@
       <c r="GE19" s="115" t="s">
         <v>2948</v>
       </c>
+      <c r="GF19" s="159" t="s">
+        <v>2966</v>
+      </c>
+      <c r="GG19" s="208" t="s">
+        <v>2165</v>
+      </c>
+      <c r="GH19" s="159" t="s">
+        <v>2997</v>
+      </c>
+      <c r="GI19" s="159" t="s">
+        <v>3011</v>
+      </c>
+      <c r="GJ19" s="159" t="s">
+        <v>3023</v>
+      </c>
+      <c r="GK19" s="159" t="s">
+        <v>3036</v>
+      </c>
+      <c r="GL19" s="115" t="s">
+        <v>3047</v>
+      </c>
+      <c r="GM19" s="115" t="s">
+        <v>3058</v>
+      </c>
+      <c r="GN19" s="115" t="s">
+        <v>3072</v>
+      </c>
     </row>
-    <row r="20" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="92">
         <v>17</v>
       </c>
-      <c r="B20" s="229"/>
+      <c r="B20" s="234"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -23869,12 +24692,39 @@
       <c r="GE20" s="115" t="s">
         <v>2949</v>
       </c>
+      <c r="GF20" s="159" t="s">
+        <v>2967</v>
+      </c>
+      <c r="GG20" s="208" t="s">
+        <v>2349</v>
+      </c>
+      <c r="GH20" s="159" t="s">
+        <v>2998</v>
+      </c>
+      <c r="GI20" s="159" t="s">
+        <v>3012</v>
+      </c>
+      <c r="GJ20" s="159" t="s">
+        <v>3024</v>
+      </c>
+      <c r="GK20" s="159" t="s">
+        <v>3037</v>
+      </c>
+      <c r="GL20" s="115" t="s">
+        <v>2349</v>
+      </c>
+      <c r="GM20" s="115" t="s">
+        <v>2712</v>
+      </c>
+      <c r="GN20" s="115" t="s">
+        <v>1145</v>
+      </c>
     </row>
-    <row r="21" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="92">
         <v>18</v>
       </c>
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="235" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -24424,12 +25274,39 @@
       <c r="GE21" s="115" t="s">
         <v>2950</v>
       </c>
+      <c r="GF21" s="159" t="s">
+        <v>2968</v>
+      </c>
+      <c r="GG21" s="208" t="s">
+        <v>2982</v>
+      </c>
+      <c r="GH21" s="159" t="s">
+        <v>2999</v>
+      </c>
+      <c r="GI21" s="159" t="s">
+        <v>3013</v>
+      </c>
+      <c r="GJ21" s="159" t="s">
+        <v>3025</v>
+      </c>
+      <c r="GK21" s="159" t="s">
+        <v>3038</v>
+      </c>
+      <c r="GL21" s="115" t="s">
+        <v>3048</v>
+      </c>
+      <c r="GM21" s="115" t="s">
+        <v>3059</v>
+      </c>
+      <c r="GN21" s="115" t="s">
+        <v>3073</v>
+      </c>
     </row>
-    <row r="22" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="92">
         <v>19</v>
       </c>
-      <c r="B22" s="230"/>
+      <c r="B22" s="235"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -24985,12 +25862,39 @@
       <c r="GE22" s="115" t="s">
         <v>2951</v>
       </c>
+      <c r="GF22" s="159" t="s">
+        <v>2969</v>
+      </c>
+      <c r="GG22" s="208" t="s">
+        <v>2983</v>
+      </c>
+      <c r="GH22" s="159" t="s">
+        <v>3000</v>
+      </c>
+      <c r="GI22" s="159" t="s">
+        <v>3014</v>
+      </c>
+      <c r="GJ22" s="159" t="s">
+        <v>3026</v>
+      </c>
+      <c r="GK22" s="159" t="s">
+        <v>3039</v>
+      </c>
+      <c r="GL22" s="115" t="s">
+        <v>3049</v>
+      </c>
+      <c r="GM22" s="115" t="s">
+        <v>3060</v>
+      </c>
+      <c r="GN22" s="115" t="s">
+        <v>3074</v>
+      </c>
     </row>
-    <row r="23" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="92">
         <v>20</v>
       </c>
-      <c r="B23" s="230"/>
+      <c r="B23" s="235"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -25546,12 +26450,39 @@
       <c r="GE23" s="115" t="s">
         <v>1586</v>
       </c>
+      <c r="GF23" s="159" t="s">
+        <v>2546</v>
+      </c>
+      <c r="GG23" s="208" t="s">
+        <v>24</v>
+      </c>
+      <c r="GH23" s="159" t="s">
+        <v>105</v>
+      </c>
+      <c r="GI23" s="159" t="s">
+        <v>105</v>
+      </c>
+      <c r="GJ23" s="159" t="s">
+        <v>77</v>
+      </c>
+      <c r="GK23" s="159" t="s">
+        <v>634</v>
+      </c>
+      <c r="GL23" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="GM23" s="115" t="s">
+        <v>141</v>
+      </c>
+      <c r="GN23" s="115" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="24" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="92">
         <v>21</v>
       </c>
-      <c r="B24" s="230"/>
+      <c r="B24" s="235"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -26107,12 +27038,39 @@
       <c r="GE24" s="115">
         <v>3960</v>
       </c>
+      <c r="GF24" s="183">
+        <v>128</v>
+      </c>
+      <c r="GG24" s="208">
+        <v>15</v>
+      </c>
+      <c r="GH24" s="212">
+        <v>14</v>
+      </c>
+      <c r="GI24" s="213">
+        <v>60</v>
+      </c>
+      <c r="GJ24" s="183">
+        <v>194</v>
+      </c>
+      <c r="GK24" s="159">
+        <v>180</v>
+      </c>
+      <c r="GL24" s="183">
+        <v>232</v>
+      </c>
+      <c r="GM24" s="185">
+        <v>79</v>
+      </c>
+      <c r="GN24" s="115">
+        <v>371</v>
+      </c>
     </row>
-    <row r="25" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="92">
         <v>22</v>
       </c>
-      <c r="B25" s="230"/>
+      <c r="B25" s="235"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -26663,12 +27621,37 @@
       <c r="GE25" s="115" t="s">
         <v>2952</v>
       </c>
+      <c r="GF25" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG25" s="208"/>
+      <c r="GH25" s="159" t="s">
+        <v>3001</v>
+      </c>
+      <c r="GI25" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ25" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK25" s="159" t="s">
+        <v>3040</v>
+      </c>
+      <c r="GL25" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM25" s="115" t="s">
+        <v>3061</v>
+      </c>
+      <c r="GN25" s="239" t="s">
+        <v>3075</v>
+      </c>
     </row>
-    <row r="26" spans="1:187" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:196" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="92">
         <v>23</v>
       </c>
-      <c r="B26" s="231" t="s">
+      <c r="B26" s="236" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="64" t="s">
@@ -27226,12 +28209,39 @@
       <c r="GE26" s="184" t="s">
         <v>849</v>
       </c>
+      <c r="GF26" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GG26" s="208" t="s">
+        <v>849</v>
+      </c>
+      <c r="GH26" s="159" t="s">
+        <v>849</v>
+      </c>
+      <c r="GI26" s="159" t="s">
+        <v>849</v>
+      </c>
+      <c r="GJ26" s="159" t="s">
+        <v>713</v>
+      </c>
+      <c r="GK26" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GL26" s="115" t="s">
+        <v>696</v>
+      </c>
+      <c r="GM26" s="169" t="s">
+        <v>1033</v>
+      </c>
+      <c r="GN26" s="159" t="s">
+        <v>699</v>
+      </c>
     </row>
-    <row r="27" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="92">
         <v>24</v>
       </c>
-      <c r="B27" s="231"/>
+      <c r="B27" s="236"/>
       <c r="C27" s="64" t="s">
         <v>464</v>
       </c>
@@ -27787,12 +28797,39 @@
       <c r="GE27" s="159">
         <v>4</v>
       </c>
+      <c r="GF27" s="159">
+        <v>7</v>
+      </c>
+      <c r="GG27" s="210">
+        <v>4</v>
+      </c>
+      <c r="GH27" s="159">
+        <v>4</v>
+      </c>
+      <c r="GI27" s="159">
+        <v>4</v>
+      </c>
+      <c r="GJ27" s="159">
+        <v>10</v>
+      </c>
+      <c r="GK27" s="159">
+        <v>7</v>
+      </c>
+      <c r="GL27" s="115">
+        <v>7</v>
+      </c>
+      <c r="GM27" s="115">
+        <v>4</v>
+      </c>
+      <c r="GN27" s="159">
+        <v>6</v>
+      </c>
     </row>
-    <row r="28" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="92">
         <v>25</v>
       </c>
-      <c r="B28" s="231"/>
+      <c r="B28" s="236"/>
       <c r="C28" s="64" t="s">
         <v>465</v>
       </c>
@@ -28346,12 +29383,39 @@
       <c r="GE28" s="159" t="s">
         <v>699</v>
       </c>
+      <c r="GF28" s="159" t="s">
+        <v>698</v>
+      </c>
+      <c r="GG28" s="208" t="s">
+        <v>696</v>
+      </c>
+      <c r="GH28" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GI28" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GJ28" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GK28" s="159" t="s">
+        <v>697</v>
+      </c>
+      <c r="GL28" s="115" t="s">
+        <v>698</v>
+      </c>
+      <c r="GM28" s="115" t="s">
+        <v>1087</v>
+      </c>
+      <c r="GN28" s="159" t="s">
+        <v>700</v>
+      </c>
     </row>
-    <row r="29" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="92">
         <v>26</v>
       </c>
-      <c r="B29" s="231"/>
+      <c r="B29" s="236"/>
       <c r="C29" s="64" t="s">
         <v>466</v>
       </c>
@@ -28905,12 +29969,39 @@
       <c r="GE29" s="159">
         <v>6</v>
       </c>
+      <c r="GF29" s="182">
+        <v>2</v>
+      </c>
+      <c r="GG29" s="208">
+        <v>7</v>
+      </c>
+      <c r="GH29" s="182">
+        <v>7</v>
+      </c>
+      <c r="GI29" s="182">
+        <v>7</v>
+      </c>
+      <c r="GJ29" s="182">
+        <v>7</v>
+      </c>
+      <c r="GK29" s="159">
+        <v>6</v>
+      </c>
+      <c r="GL29" s="115">
+        <v>89</v>
+      </c>
+      <c r="GM29" s="184">
+        <v>18</v>
+      </c>
+      <c r="GN29" s="184">
+        <v>6</v>
+      </c>
     </row>
-    <row r="30" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="92">
         <v>27</v>
       </c>
-      <c r="B30" s="231"/>
+      <c r="B30" s="236"/>
       <c r="C30" s="64" t="s">
         <v>467</v>
       </c>
@@ -29464,12 +30555,39 @@
       <c r="GE30" s="159" t="s">
         <v>700</v>
       </c>
+      <c r="GF30" s="159" t="s">
+        <v>704</v>
+      </c>
+      <c r="GG30" s="208" t="s">
+        <v>1441</v>
+      </c>
+      <c r="GH30" s="159" t="s">
+        <v>697</v>
+      </c>
+      <c r="GI30" s="159" t="s">
+        <v>697</v>
+      </c>
+      <c r="GJ30" s="159" t="s">
+        <v>697</v>
+      </c>
+      <c r="GK30" s="159" t="s">
+        <v>698</v>
+      </c>
+      <c r="GL30" s="115" t="s">
+        <v>704</v>
+      </c>
+      <c r="GM30" s="115" t="s">
+        <v>1657</v>
+      </c>
+      <c r="GN30" s="159" t="s">
+        <v>849</v>
+      </c>
     </row>
-    <row r="31" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="92">
         <v>28</v>
       </c>
-      <c r="B31" s="231"/>
+      <c r="B31" s="236"/>
       <c r="C31" s="64" t="s">
         <v>468</v>
       </c>
@@ -30023,12 +31141,39 @@
       <c r="GE31" s="159">
         <v>6</v>
       </c>
+      <c r="GF31" s="159">
+        <v>14</v>
+      </c>
+      <c r="GG31" s="209">
+        <v>86</v>
+      </c>
+      <c r="GH31" s="159">
+        <v>6</v>
+      </c>
+      <c r="GI31" s="159">
+        <v>6</v>
+      </c>
+      <c r="GJ31" s="159">
+        <v>6</v>
+      </c>
+      <c r="GK31" s="159">
+        <v>2</v>
+      </c>
+      <c r="GL31" s="115">
+        <v>14</v>
+      </c>
+      <c r="GM31" s="185">
+        <v>93</v>
+      </c>
+      <c r="GN31" s="159">
+        <v>4</v>
+      </c>
     </row>
-    <row r="32" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="92">
         <v>29</v>
       </c>
-      <c r="B32" s="231"/>
+      <c r="B32" s="236"/>
       <c r="C32" s="64" t="s">
         <v>469</v>
       </c>
@@ -30582,12 +31727,39 @@
       <c r="GE32" s="184" t="s">
         <v>698</v>
       </c>
+      <c r="GF32" s="182" t="s">
+        <v>1440</v>
+      </c>
+      <c r="GG32" s="211" t="s">
+        <v>702</v>
+      </c>
+      <c r="GH32" s="182" t="s">
+        <v>704</v>
+      </c>
+      <c r="GI32" s="182" t="s">
+        <v>702</v>
+      </c>
+      <c r="GJ32" s="159" t="s">
+        <v>853</v>
+      </c>
+      <c r="GK32" s="159" t="s">
+        <v>704</v>
+      </c>
+      <c r="GL32" s="197" t="s">
+        <v>697</v>
+      </c>
+      <c r="GM32" s="184" t="s">
+        <v>698</v>
+      </c>
+      <c r="GN32" s="184" t="s">
+        <v>698</v>
+      </c>
     </row>
-    <row r="33" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="92">
         <v>30</v>
       </c>
-      <c r="B33" s="231"/>
+      <c r="B33" s="236"/>
       <c r="C33" s="64" t="s">
         <v>470</v>
       </c>
@@ -31141,12 +32313,39 @@
       <c r="GE33" s="184">
         <v>2</v>
       </c>
+      <c r="GF33" s="159">
+        <v>6</v>
+      </c>
+      <c r="GG33" s="210">
+        <v>14</v>
+      </c>
+      <c r="GH33" s="159">
+        <v>14</v>
+      </c>
+      <c r="GI33" s="182">
+        <v>14</v>
+      </c>
+      <c r="GJ33" s="159">
+        <v>12</v>
+      </c>
+      <c r="GK33" s="159">
+        <v>9</v>
+      </c>
+      <c r="GL33" s="184">
+        <v>6</v>
+      </c>
+      <c r="GM33" s="115">
+        <v>2</v>
+      </c>
+      <c r="GN33" s="184">
+        <v>2</v>
+      </c>
     </row>
-    <row r="34" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="92">
         <v>31</v>
       </c>
-      <c r="B34" s="231"/>
+      <c r="B34" s="236"/>
       <c r="C34" s="64" t="s">
         <v>471</v>
       </c>
@@ -31700,12 +32899,39 @@
       <c r="GE34" s="159" t="s">
         <v>704</v>
       </c>
+      <c r="GF34" s="182" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG34" s="211" t="s">
+        <v>698</v>
+      </c>
+      <c r="GH34" s="182" t="s">
+        <v>698</v>
+      </c>
+      <c r="GI34" s="159" t="s">
+        <v>698</v>
+      </c>
+      <c r="GJ34" s="159" t="s">
+        <v>698</v>
+      </c>
+      <c r="GK34" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL34" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM34" s="115" t="s">
+        <v>702</v>
+      </c>
+      <c r="GN34" s="159" t="s">
+        <v>702</v>
+      </c>
     </row>
-    <row r="35" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="92">
         <v>32</v>
       </c>
-      <c r="B35" s="231"/>
+      <c r="B35" s="236"/>
       <c r="C35" s="64" t="s">
         <v>472</v>
       </c>
@@ -32259,12 +33485,39 @@
       <c r="GE35" s="159">
         <v>3</v>
       </c>
+      <c r="GF35" s="182" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG35" s="210">
+        <v>2</v>
+      </c>
+      <c r="GH35" s="182">
+        <v>2</v>
+      </c>
+      <c r="GI35" s="159">
+        <v>2</v>
+      </c>
+      <c r="GJ35" s="159">
+        <v>2</v>
+      </c>
+      <c r="GK35" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL35" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM35" s="115">
+        <v>3</v>
+      </c>
+      <c r="GN35" s="159">
+        <v>3</v>
+      </c>
     </row>
-    <row r="36" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="92">
         <v>33</v>
       </c>
-      <c r="B36" s="231"/>
+      <c r="B36" s="236"/>
       <c r="C36" s="64" t="s">
         <v>473</v>
       </c>
@@ -32818,12 +34071,39 @@
       <c r="GE36" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF36" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG36" s="208" t="s">
+        <v>697</v>
+      </c>
+      <c r="GH36" s="159" t="s">
+        <v>1441</v>
+      </c>
+      <c r="GI36" s="159" t="s">
+        <v>1441</v>
+      </c>
+      <c r="GJ36" s="182" t="s">
+        <v>704</v>
+      </c>
+      <c r="GK36" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL36" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM36" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN36" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="37" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="92">
         <v>34</v>
       </c>
-      <c r="B37" s="231"/>
+      <c r="B37" s="236"/>
       <c r="C37" s="64" t="s">
         <v>474</v>
       </c>
@@ -33377,12 +34657,39 @@
       <c r="GE37" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF37" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG37" s="210">
+        <v>6</v>
+      </c>
+      <c r="GH37" s="159">
+        <v>86</v>
+      </c>
+      <c r="GI37" s="159">
+        <v>86</v>
+      </c>
+      <c r="GJ37" s="159">
+        <v>3</v>
+      </c>
+      <c r="GK37" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL37" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM37" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN37" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="38" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="92">
         <v>35</v>
       </c>
-      <c r="B38" s="231"/>
+      <c r="B38" s="236"/>
       <c r="C38" s="64" t="s">
         <v>475</v>
       </c>
@@ -33936,12 +35243,39 @@
       <c r="GE38" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG38" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL38" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM38" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN38" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="39" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="92">
         <v>36</v>
       </c>
-      <c r="B39" s="231"/>
+      <c r="B39" s="236"/>
       <c r="C39" s="64" t="s">
         <v>476</v>
       </c>
@@ -34495,12 +35829,39 @@
       <c r="GE39" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG39" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL39" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM39" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN39" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="40" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="92">
         <v>37</v>
       </c>
-      <c r="B40" s="231"/>
+      <c r="B40" s="236"/>
       <c r="C40" s="64" t="s">
         <v>477</v>
       </c>
@@ -35054,12 +36415,39 @@
       <c r="GE40" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG40" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL40" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM40" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN40" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="92">
         <v>38</v>
       </c>
-      <c r="B41" s="231"/>
+      <c r="B41" s="236"/>
       <c r="C41" s="64" t="s">
         <v>478</v>
       </c>
@@ -35613,12 +37001,39 @@
       <c r="GE41" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG41" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL41" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM41" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN41" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="42" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="92">
         <v>39</v>
       </c>
-      <c r="B42" s="231"/>
+      <c r="B42" s="236"/>
       <c r="C42" s="64" t="s">
         <v>479</v>
       </c>
@@ -36172,12 +37587,39 @@
       <c r="GE42" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG42" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL42" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM42" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN42" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="92">
         <v>40</v>
       </c>
-      <c r="B43" s="231"/>
+      <c r="B43" s="236"/>
       <c r="C43" s="64" t="s">
         <v>480</v>
       </c>
@@ -36731,12 +38173,39 @@
       <c r="GE43" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG43" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL43" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM43" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN43" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="44" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="92">
         <v>41</v>
       </c>
-      <c r="B44" s="231"/>
+      <c r="B44" s="236"/>
       <c r="C44" s="64" t="s">
         <v>481</v>
       </c>
@@ -37290,12 +38759,39 @@
       <c r="GE44" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG44" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL44" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM44" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN44" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="45" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="92">
         <v>42</v>
       </c>
-      <c r="B45" s="231"/>
+      <c r="B45" s="236"/>
       <c r="C45" s="64" t="s">
         <v>482</v>
       </c>
@@ -37849,12 +39345,39 @@
       <c r="GE45" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG45" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL45" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM45" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN45" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="46" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="92">
         <v>43</v>
       </c>
-      <c r="B46" s="231"/>
+      <c r="B46" s="236"/>
       <c r="C46" s="64" t="s">
         <v>483</v>
       </c>
@@ -38408,12 +39931,39 @@
       <c r="GE46" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG46" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL46" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM46" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN46" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="47" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="92">
         <v>44</v>
       </c>
-      <c r="B47" s="231"/>
+      <c r="B47" s="236"/>
       <c r="C47" s="64" t="s">
         <v>484</v>
       </c>
@@ -38967,12 +40517,39 @@
       <c r="GE47" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG47" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL47" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM47" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN47" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="48" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="92">
         <v>45</v>
       </c>
-      <c r="B48" s="231"/>
+      <c r="B48" s="236"/>
       <c r="C48" s="64" t="s">
         <v>485</v>
       </c>
@@ -39526,12 +41103,39 @@
       <c r="GE48" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG48" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL48" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM48" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN48" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="49" spans="1:187" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:196" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="92">
         <v>46</v>
       </c>
-      <c r="B49" s="231"/>
+      <c r="B49" s="236"/>
       <c r="C49" s="64" t="s">
         <v>486</v>
       </c>
@@ -40085,12 +41689,39 @@
       <c r="GE49" s="159" t="s">
         <v>11</v>
       </c>
+      <c r="GF49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG49" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GH49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GJ49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GL49" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM49" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GN49" s="159" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="50" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="92">
         <v>47</v>
       </c>
-      <c r="B50" s="231"/>
+      <c r="B50" s="236"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -40646,12 +42277,39 @@
       <c r="GE50" s="115" t="s">
         <v>2953</v>
       </c>
+      <c r="GF50" s="159" t="s">
+        <v>2970</v>
+      </c>
+      <c r="GG50" s="208" t="s">
+        <v>2984</v>
+      </c>
+      <c r="GH50" s="159" t="s">
+        <v>3002</v>
+      </c>
+      <c r="GI50" s="159" t="s">
+        <v>3015</v>
+      </c>
+      <c r="GJ50" s="159" t="s">
+        <v>3027</v>
+      </c>
+      <c r="GK50" s="159" t="s">
+        <v>1978</v>
+      </c>
+      <c r="GL50" s="115" t="s">
+        <v>2970</v>
+      </c>
+      <c r="GM50" s="115" t="s">
+        <v>2716</v>
+      </c>
+      <c r="GN50" s="115" t="s">
+        <v>2663</v>
+      </c>
     </row>
-    <row r="51" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="92">
         <v>48</v>
       </c>
-      <c r="B51" s="231"/>
+      <c r="B51" s="236"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -41207,12 +42865,39 @@
       <c r="GE51" s="115" t="s">
         <v>2954</v>
       </c>
+      <c r="GF51" s="159" t="s">
+        <v>2971</v>
+      </c>
+      <c r="GG51" s="208" t="s">
+        <v>2985</v>
+      </c>
+      <c r="GH51" s="159" t="s">
+        <v>3003</v>
+      </c>
+      <c r="GI51" s="159" t="s">
+        <v>3016</v>
+      </c>
+      <c r="GJ51" s="159" t="s">
+        <v>3028</v>
+      </c>
+      <c r="GK51" s="159" t="s">
+        <v>3041</v>
+      </c>
+      <c r="GL51" s="216" t="s">
+        <v>3050</v>
+      </c>
+      <c r="GM51" s="115" t="s">
+        <v>3062</v>
+      </c>
+      <c r="GN51" s="115" t="s">
+        <v>3076</v>
+      </c>
     </row>
-    <row r="52" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="92">
         <v>49</v>
       </c>
-      <c r="B52" s="231"/>
+      <c r="B52" s="236"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -41768,12 +43453,39 @@
       <c r="GE52" s="115" t="s">
         <v>2955</v>
       </c>
+      <c r="GF52" s="159" t="s">
+        <v>2972</v>
+      </c>
+      <c r="GG52" s="208" t="s">
+        <v>2986</v>
+      </c>
+      <c r="GH52" s="159" t="s">
+        <v>3004</v>
+      </c>
+      <c r="GI52" s="159" t="s">
+        <v>3017</v>
+      </c>
+      <c r="GJ52" s="159" t="s">
+        <v>3029</v>
+      </c>
+      <c r="GK52" s="159" t="s">
+        <v>3042</v>
+      </c>
+      <c r="GL52" s="115" t="s">
+        <v>3051</v>
+      </c>
+      <c r="GM52" s="115" t="s">
+        <v>3063</v>
+      </c>
+      <c r="GN52" s="115" t="s">
+        <v>3077</v>
+      </c>
     </row>
-    <row r="53" spans="1:187" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:196" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="92">
         <v>50</v>
       </c>
-      <c r="B53" s="232" t="s">
+      <c r="B53" s="237" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -42331,12 +44043,39 @@
       <c r="GE53" s="185" t="s">
         <v>860</v>
       </c>
+      <c r="GF53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GG53" s="210" t="s">
+        <v>207</v>
+      </c>
+      <c r="GH53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GI53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GJ53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GK53" s="185" t="s">
+        <v>207</v>
+      </c>
+      <c r="GL53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GM53" s="185" t="s">
+        <v>860</v>
+      </c>
+      <c r="GN53" s="185" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="54" spans="1:187" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:196" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A54" s="92">
         <v>51</v>
       </c>
-      <c r="B54" s="232"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -42892,12 +44631,39 @@
       <c r="GE54" s="115" t="s">
         <v>61</v>
       </c>
+      <c r="GF54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="GG54" s="210" t="s">
+        <v>858</v>
+      </c>
+      <c r="GH54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="GI54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="GJ54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="GK54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="GL54" s="185" t="s">
+        <v>858</v>
+      </c>
+      <c r="GM54" s="206" t="s">
+        <v>61</v>
+      </c>
+      <c r="GN54" s="185" t="s">
+        <v>858</v>
+      </c>
     </row>
-    <row r="55" spans="1:187" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:196" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A55" s="92">
         <v>52</v>
       </c>
-      <c r="B55" s="232"/>
+      <c r="B55" s="237"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -43453,12 +45219,39 @@
       <c r="GE55" s="115" t="s">
         <v>2956</v>
       </c>
+      <c r="GF55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GG55" s="210" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GH55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GI55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GJ55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GK55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GL55" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GM55" s="115" t="s">
+        <v>3064</v>
+      </c>
+      <c r="GN55" s="185" t="s">
+        <v>2330</v>
+      </c>
     </row>
-    <row r="56" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="92">
         <v>53</v>
       </c>
-      <c r="B56" s="232"/>
+      <c r="B56" s="237"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -44012,12 +45805,39 @@
       <c r="GE56" s="115" t="s">
         <v>2957</v>
       </c>
+      <c r="GF56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GG56" s="69" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GH56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GI56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GJ56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GK56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GL56" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GM56" s="115" t="s">
+        <v>3065</v>
+      </c>
+      <c r="GN56" s="185" t="s">
+        <v>2330</v>
+      </c>
     </row>
-    <row r="57" spans="1:187" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:196" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A57" s="92">
         <v>54</v>
       </c>
-      <c r="B57" s="232"/>
+      <c r="B57" s="237"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -44573,12 +46393,39 @@
       <c r="GE57" s="115" t="s">
         <v>2315</v>
       </c>
+      <c r="GF57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GG57" s="69" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GH57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GI57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GJ57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GK57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GL57" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GM57" s="115" t="s">
+        <v>2083</v>
+      </c>
+      <c r="GN57" s="115" t="s">
+        <v>3078</v>
+      </c>
     </row>
-    <row r="58" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="92">
         <v>55</v>
       </c>
-      <c r="B58" s="232"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -45105,12 +46952,39 @@
       <c r="GE58" s="115" t="s">
         <v>2957</v>
       </c>
+      <c r="GF58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GG58" s="69" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GH58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GI58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GJ58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GK58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GL58" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GM58" s="206" t="s">
+        <v>3066</v>
+      </c>
+      <c r="GN58" s="185" t="s">
+        <v>2330</v>
+      </c>
     </row>
-    <row r="59" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="92">
         <v>56</v>
       </c>
-      <c r="B59" s="232"/>
+      <c r="B59" s="237"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -45666,12 +47540,39 @@
       <c r="GE59" s="115" t="s">
         <v>2957</v>
       </c>
+      <c r="GF59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GG59" s="69" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GH59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GI59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GJ59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GK59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GL59" s="185" t="s">
+        <v>2330</v>
+      </c>
+      <c r="GM59" s="206" t="s">
+        <v>3067</v>
+      </c>
+      <c r="GN59" s="185" t="s">
+        <v>2330</v>
+      </c>
     </row>
-    <row r="60" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="92">
         <v>57</v>
       </c>
-      <c r="B60" s="232"/>
+      <c r="B60" s="237"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -46227,12 +48128,39 @@
       <c r="GE60" s="65">
         <v>1</v>
       </c>
+      <c r="GF60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GG60" s="188">
+        <v>1</v>
+      </c>
+      <c r="GH60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GI60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GJ60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GK60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GL60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GM60" s="207">
+        <v>1</v>
+      </c>
+      <c r="GN60" s="184">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:187" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:196" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="92">
         <v>58</v>
       </c>
-      <c r="B61" s="233" t="s">
+      <c r="B61" s="238" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -46788,12 +48716,39 @@
       <c r="GE61" s="157">
         <v>45797</v>
       </c>
+      <c r="GF61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="GG61" s="205">
+        <v>45413</v>
+      </c>
+      <c r="GH61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="GI61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="GJ61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="GK61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="GL61" s="192">
+        <v>45413</v>
+      </c>
+      <c r="GM61" s="157">
+        <v>45796</v>
+      </c>
+      <c r="GN61" s="157">
+        <v>45796</v>
+      </c>
     </row>
-    <row r="62" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="92">
         <v>59</v>
       </c>
-      <c r="B62" s="233"/>
+      <c r="B62" s="238"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -47349,12 +49304,39 @@
       <c r="GE62" s="157">
         <v>45797</v>
       </c>
+      <c r="GF62" s="192">
+        <v>45736</v>
+      </c>
+      <c r="GG62" s="190">
+        <v>45709</v>
+      </c>
+      <c r="GH62" s="192">
+        <v>45736</v>
+      </c>
+      <c r="GI62" s="192">
+        <v>45736</v>
+      </c>
+      <c r="GJ62" s="193">
+        <v>45709</v>
+      </c>
+      <c r="GK62" s="193">
+        <v>45709</v>
+      </c>
+      <c r="GL62" s="193">
+        <v>45709</v>
+      </c>
+      <c r="GM62" s="157">
+        <v>45799</v>
+      </c>
+      <c r="GN62" s="157">
+        <v>45799</v>
+      </c>
     </row>
-    <row r="63" spans="1:187" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:196" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="92">
         <v>60</v>
       </c>
-      <c r="B63" s="233"/>
+      <c r="B63" s="238"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -47910,12 +49892,39 @@
       <c r="GE63" s="115" t="s">
         <v>2958</v>
       </c>
+      <c r="GF63" s="115" t="s">
+        <v>2331</v>
+      </c>
+      <c r="GG63" s="187" t="s">
+        <v>2386</v>
+      </c>
+      <c r="GH63" s="115" t="s">
+        <v>2386</v>
+      </c>
+      <c r="GI63" s="115" t="s">
+        <v>2386</v>
+      </c>
+      <c r="GJ63" s="159" t="s">
+        <v>2085</v>
+      </c>
+      <c r="GK63" s="115" t="s">
+        <v>2331</v>
+      </c>
+      <c r="GL63" s="115" t="s">
+        <v>2331</v>
+      </c>
+      <c r="GM63" s="115" t="s">
+        <v>3079</v>
+      </c>
+      <c r="GN63" s="115" t="s">
+        <v>3079</v>
+      </c>
     </row>
-    <row r="64" spans="1:187" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:196" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A64" s="92">
         <v>61</v>
       </c>
-      <c r="B64" s="233"/>
+      <c r="B64" s="238"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -48470,13 +50479,40 @@
       </c>
       <c r="GE64" s="115" t="s">
         <v>2959</v>
+      </c>
+      <c r="GF64" s="115" t="s">
+        <v>2973</v>
+      </c>
+      <c r="GG64" s="69" t="s">
+        <v>2332</v>
+      </c>
+      <c r="GH64" s="115" t="s">
+        <v>3005</v>
+      </c>
+      <c r="GI64" s="115" t="s">
+        <v>3005</v>
+      </c>
+      <c r="GJ64" s="159" t="s">
+        <v>72</v>
+      </c>
+      <c r="GK64" s="185" t="s">
+        <v>3043</v>
+      </c>
+      <c r="GL64" s="185" t="s">
+        <v>3043</v>
+      </c>
+      <c r="GM64" s="115" t="s">
+        <v>3068</v>
+      </c>
+      <c r="GN64" s="115" t="s">
+        <v>2669</v>
       </c>
     </row>
     <row r="65" spans="1:205" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="92">
         <v>62</v>
       </c>
-      <c r="B65" s="233"/>
+      <c r="B65" s="238"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -48735,12 +50771,39 @@
       <c r="GE65" s="157">
         <v>45800</v>
       </c>
+      <c r="GF65" s="192">
+        <v>45801</v>
+      </c>
+      <c r="GG65" s="190">
+        <v>45801</v>
+      </c>
+      <c r="GH65" s="192">
+        <v>45801</v>
+      </c>
+      <c r="GI65" s="192">
+        <v>45801</v>
+      </c>
+      <c r="GJ65" s="193">
+        <v>45782</v>
+      </c>
+      <c r="GK65" s="193">
+        <v>45803</v>
+      </c>
+      <c r="GL65" s="192">
+        <v>45798</v>
+      </c>
+      <c r="GM65" s="157">
+        <v>45803</v>
+      </c>
+      <c r="GN65" s="157">
+        <v>45803</v>
+      </c>
     </row>
     <row r="66" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A66" s="92">
         <v>63</v>
       </c>
-      <c r="B66" s="233"/>
+      <c r="B66" s="238"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -48997,12 +51060,39 @@
       <c r="GE66" s="169" t="s">
         <v>30</v>
       </c>
+      <c r="GF66" s="169" t="s">
+        <v>1843</v>
+      </c>
+      <c r="GG66" s="191" t="s">
+        <v>30</v>
+      </c>
+      <c r="GH66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GI66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GJ66" s="194" t="s">
+        <v>1843</v>
+      </c>
+      <c r="GK66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GL66" s="169" t="s">
+        <v>3052</v>
+      </c>
+      <c r="GM66" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GN66" s="115" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="67" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:205" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="92">
         <v>64</v>
       </c>
-      <c r="B67" s="233"/>
+      <c r="B67" s="238"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -49109,12 +51199,21 @@
       <c r="GC67" s="156"/>
       <c r="GD67" s="191"/>
       <c r="GE67" s="169"/>
+      <c r="GF67" s="156"/>
+      <c r="GG67" s="191"/>
+      <c r="GH67" s="186"/>
+      <c r="GI67" s="214"/>
+      <c r="GJ67" s="194"/>
+      <c r="GK67" s="194"/>
+      <c r="GL67" s="169"/>
+      <c r="GM67" s="169"/>
+      <c r="GN67" s="206"/>
     </row>
     <row r="68" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A68" s="92">
         <v>65</v>
       </c>
-      <c r="B68" s="223" t="s">
+      <c r="B68" s="228" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -49177,12 +51276,17 @@
       <c r="FX68" s="169"/>
       <c r="FZ68" s="169"/>
       <c r="GC68" s="156"/>
+      <c r="GF68" s="156"/>
+      <c r="GI68" s="215"/>
+      <c r="GL68" s="169"/>
+      <c r="GM68" s="169"/>
+      <c r="GN68" s="206"/>
     </row>
     <row r="69" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A69" s="92">
         <v>66</v>
       </c>
-      <c r="B69" s="223"/>
+      <c r="B69" s="228"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -49231,7 +51335,7 @@
       <c r="A70" s="92">
         <v>67</v>
       </c>
-      <c r="B70" s="223"/>
+      <c r="B70" s="228"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -49270,7 +51374,7 @@
       <c r="A71" s="92">
         <v>68</v>
       </c>
-      <c r="B71" s="223"/>
+      <c r="B71" s="228"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -49305,7 +51409,7 @@
       <c r="A72" s="92">
         <v>69</v>
       </c>
-      <c r="B72" s="224"/>
+      <c r="B72" s="229"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -50209,7 +52313,7 @@
       <c r="BT3" s="36"/>
     </row>
     <row r="4" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="230" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -50378,7 +52482,7 @@
       <c r="BT4" s="12"/>
     </row>
     <row r="5" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="226"/>
+      <c r="B5" s="231"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -50710,7 +52814,7 @@
       <c r="BT6" s="2"/>
     </row>
     <row r="7" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B7" s="227" t="s">
+      <c r="B7" s="232" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -50877,7 +52981,7 @@
       <c r="BT7" s="37"/>
     </row>
     <row r="8" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="227"/>
+      <c r="B8" s="232"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -51044,7 +53148,7 @@
       <c r="BT8" s="1"/>
     </row>
     <row r="9" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="227"/>
+      <c r="B9" s="232"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -51211,7 +53315,7 @@
       <c r="BT9" s="1"/>
     </row>
     <row r="10" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="227"/>
+      <c r="B10" s="232"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -51378,7 +53482,7 @@
       <c r="BT10" s="1"/>
     </row>
     <row r="11" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="228" t="s">
+      <c r="B11" s="233" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -51545,7 +53649,7 @@
       <c r="BT11" s="106"/>
     </row>
     <row r="12" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="229"/>
+      <c r="B12" s="234"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -51710,7 +53814,7 @@
       <c r="BT12" s="2"/>
     </row>
     <row r="13" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="229"/>
+      <c r="B13" s="234"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -51875,7 +53979,7 @@
       <c r="BT13" s="106"/>
     </row>
     <row r="14" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="229"/>
+      <c r="B14" s="234"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -52040,7 +54144,7 @@
       <c r="BT14" s="2"/>
     </row>
     <row r="15" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="229"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -52205,7 +54309,7 @@
       <c r="BT15" s="2"/>
     </row>
     <row r="16" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="229"/>
+      <c r="B16" s="234"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -52370,7 +54474,7 @@
       <c r="BT16" s="2"/>
     </row>
     <row r="17" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="229"/>
+      <c r="B17" s="234"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -52535,7 +54639,7 @@
       <c r="BT17" s="2"/>
     </row>
     <row r="18" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="229"/>
+      <c r="B18" s="234"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -52700,7 +54804,7 @@
       <c r="BT18" s="2"/>
     </row>
     <row r="19" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="229"/>
+      <c r="B19" s="234"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -52865,7 +54969,7 @@
       <c r="BT19" s="2"/>
     </row>
     <row r="20" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="229"/>
+      <c r="B20" s="234"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -53030,7 +55134,7 @@
       <c r="BT20" s="2"/>
     </row>
     <row r="21" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="235" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -53238,7 +55342,7 @@
       <c r="BT21" s="106"/>
     </row>
     <row r="22" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="230"/>
+      <c r="B22" s="235"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -53446,7 +55550,7 @@
       <c r="BT22" s="106"/>
     </row>
     <row r="23" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="230"/>
+      <c r="B23" s="235"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -53613,7 +55717,7 @@
       <c r="BT23" s="2"/>
     </row>
     <row r="24" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B24" s="230"/>
+      <c r="B24" s="235"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -53780,7 +55884,7 @@
       <c r="BT24" s="105"/>
     </row>
     <row r="25" spans="2:72" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="230"/>
+      <c r="B25" s="235"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -53945,7 +56049,7 @@
       <c r="BT25" s="6"/>
     </row>
     <row r="26" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="231" t="s">
+      <c r="B26" s="236" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -54114,7 +56218,7 @@
       <c r="BT26" s="38"/>
     </row>
     <row r="27" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="231"/>
+      <c r="B27" s="236"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -54281,7 +56385,7 @@
       <c r="BT27" s="42"/>
     </row>
     <row r="28" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="231"/>
+      <c r="B28" s="236"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -54446,7 +56550,7 @@
       <c r="BT28" s="66"/>
     </row>
     <row r="29" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="231"/>
+      <c r="B29" s="236"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -54611,7 +56715,7 @@
       <c r="BT29" s="42"/>
     </row>
     <row r="30" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="231"/>
+      <c r="B30" s="236"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -54776,7 +56880,7 @@
       <c r="BT30" s="38"/>
     </row>
     <row r="31" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="231"/>
+      <c r="B31" s="236"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -54941,7 +57045,7 @@
       <c r="BT31" s="42"/>
     </row>
     <row r="32" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="231"/>
+      <c r="B32" s="236"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -55106,7 +57210,7 @@
       <c r="BT32" s="88"/>
     </row>
     <row r="33" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="231"/>
+      <c r="B33" s="236"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -55271,7 +57375,7 @@
       <c r="BT33" s="28"/>
     </row>
     <row r="34" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="231"/>
+      <c r="B34" s="236"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -55436,7 +57540,7 @@
       <c r="BT34" s="38"/>
     </row>
     <row r="35" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="231"/>
+      <c r="B35" s="236"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -55601,7 +57705,7 @@
       <c r="BT35" s="42"/>
     </row>
     <row r="36" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="231"/>
+      <c r="B36" s="236"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -55766,7 +57870,7 @@
       <c r="BT36" s="38"/>
     </row>
     <row r="37" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="231"/>
+      <c r="B37" s="236"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -55931,7 +58035,7 @@
       <c r="BT37" s="42"/>
     </row>
     <row r="38" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="231"/>
+      <c r="B38" s="236"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -56096,7 +58200,7 @@
       <c r="BT38" s="38"/>
     </row>
     <row r="39" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="231"/>
+      <c r="B39" s="236"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -56261,7 +58365,7 @@
       <c r="BT39" s="38"/>
     </row>
     <row r="40" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="231"/>
+      <c r="B40" s="236"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -56426,7 +58530,7 @@
       <c r="BT40" s="38"/>
     </row>
     <row r="41" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="231"/>
+      <c r="B41" s="236"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -56591,7 +58695,7 @@
       <c r="BT41" s="38"/>
     </row>
     <row r="42" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="231"/>
+      <c r="B42" s="236"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -56756,7 +58860,7 @@
       <c r="BT42" s="38"/>
     </row>
     <row r="43" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="231"/>
+      <c r="B43" s="236"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -56921,7 +59025,7 @@
       <c r="BT43" s="38"/>
     </row>
     <row r="44" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="231"/>
+      <c r="B44" s="236"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -57086,7 +59190,7 @@
       <c r="BT44" s="38"/>
     </row>
     <row r="45" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="231"/>
+      <c r="B45" s="236"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -57251,7 +59355,7 @@
       <c r="BT45" s="38"/>
     </row>
     <row r="46" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="231"/>
+      <c r="B46" s="236"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -57416,7 +59520,7 @@
       <c r="BT46" s="38"/>
     </row>
     <row r="47" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="231"/>
+      <c r="B47" s="236"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -57581,7 +59685,7 @@
       <c r="BT47" s="38"/>
     </row>
     <row r="48" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="231"/>
+      <c r="B48" s="236"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -57746,7 +59850,7 @@
       <c r="BT48" s="38"/>
     </row>
     <row r="49" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="231"/>
+      <c r="B49" s="236"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -57911,7 +60015,7 @@
       <c r="BT49" s="38"/>
     </row>
     <row r="50" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="231"/>
+      <c r="B50" s="236"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -58078,7 +60182,7 @@
       <c r="BT50" s="2"/>
     </row>
     <row r="51" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="231"/>
+      <c r="B51" s="236"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -58245,7 +60349,7 @@
       <c r="BT51" s="2"/>
     </row>
     <row r="52" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="231"/>
+      <c r="B52" s="236"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -58412,7 +60516,7 @@
       <c r="BT52" s="2"/>
     </row>
     <row r="53" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="232" t="s">
+      <c r="B53" s="237" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -58581,7 +60685,7 @@
       <c r="BT53" s="105"/>
     </row>
     <row r="54" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="232"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -58748,7 +60852,7 @@
       <c r="BT54" s="5"/>
     </row>
     <row r="55" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="232"/>
+      <c r="B55" s="237"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -58915,7 +61019,7 @@
       <c r="BT55" s="5"/>
     </row>
     <row r="56" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="232"/>
+      <c r="B56" s="237"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -59080,7 +61184,7 @@
       <c r="BT56" s="3"/>
     </row>
     <row r="57" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="232"/>
+      <c r="B57" s="237"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -59247,7 +61351,7 @@
       <c r="BT57" s="2"/>
     </row>
     <row r="58" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B58" s="232"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -59412,7 +61516,7 @@
       <c r="BT58" s="7"/>
     </row>
     <row r="59" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="232"/>
+      <c r="B59" s="237"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -59579,7 +61683,7 @@
       <c r="BT59" s="5"/>
     </row>
     <row r="60" spans="2:72" x14ac:dyDescent="0.4">
-      <c r="B60" s="232"/>
+      <c r="B60" s="237"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -59746,7 +61850,7 @@
       <c r="BT60" s="12"/>
     </row>
     <row r="61" spans="2:72" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="233" t="s">
+      <c r="B61" s="238" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -59913,7 +62017,7 @@
       <c r="BT61" s="9"/>
     </row>
     <row r="62" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="233"/>
+      <c r="B62" s="238"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -60080,7 +62184,7 @@
       <c r="BT62" s="9"/>
     </row>
     <row r="63" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="233"/>
+      <c r="B63" s="238"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -60247,7 +62351,7 @@
       <c r="BT63" s="5"/>
     </row>
     <row r="64" spans="2:72" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="233"/>
+      <c r="B64" s="238"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -60414,7 +62518,7 @@
       <c r="BT64" s="2"/>
     </row>
     <row r="65" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="233"/>
+      <c r="B65" s="238"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -60431,7 +62535,7 @@
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="233"/>
+      <c r="B66" s="238"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -60450,7 +62554,7 @@
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="233"/>
+      <c r="B67" s="238"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -60469,7 +62573,7 @@
       <c r="P67" s="1"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B68" s="223" t="s">
+      <c r="B68" s="228" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -60479,7 +62583,7 @@
       <c r="L68" s="105"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B69" s="223"/>
+      <c r="B69" s="228"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -60487,7 +62591,7 @@
       <c r="K69" s="12"/>
     </row>
     <row r="70" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B70" s="223"/>
+      <c r="B70" s="228"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -60495,7 +62599,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:16" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B71" s="223"/>
+      <c r="B71" s="228"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -60507,7 +62611,7 @@
       <c r="L71" s="105"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B72" s="224"/>
+      <c r="B72" s="229"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>
@@ -61087,7 +63191,7 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="230" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -61167,7 +63271,7 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B5" s="226"/>
+      <c r="B5" s="231"/>
       <c r="C5" s="54" t="s">
         <v>456</v>
       </c>
@@ -61321,7 +63425,7 @@
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B7" s="227" t="s">
+      <c r="B7" s="232" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -61399,7 +63503,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B8" s="227"/>
+      <c r="B8" s="232"/>
       <c r="C8" s="54" t="s">
         <v>458</v>
       </c>
@@ -61477,7 +63581,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B9" s="227"/>
+      <c r="B9" s="232"/>
       <c r="C9" s="54" t="s">
         <v>459</v>
       </c>
@@ -61555,7 +63659,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B10" s="227"/>
+      <c r="B10" s="232"/>
       <c r="C10" s="54" t="s">
         <v>460</v>
       </c>
@@ -61633,7 +63737,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B11" s="228" t="s">
+      <c r="B11" s="233" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="55" t="s">
@@ -61711,7 +63815,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B12" s="229"/>
+      <c r="B12" s="234"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
       </c>
@@ -61787,7 +63891,7 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B13" s="229"/>
+      <c r="B13" s="234"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
       </c>
@@ -61863,7 +63967,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B14" s="229"/>
+      <c r="B14" s="234"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
       </c>
@@ -61939,7 +64043,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B15" s="229"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
       </c>
@@ -62015,7 +64119,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B16" s="229"/>
+      <c r="B16" s="234"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
       </c>
@@ -62091,7 +64195,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B17" s="229"/>
+      <c r="B17" s="234"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
       </c>
@@ -62167,7 +64271,7 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B18" s="229"/>
+      <c r="B18" s="234"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
       </c>
@@ -62243,7 +64347,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B19" s="229"/>
+      <c r="B19" s="234"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
       </c>
@@ -62319,7 +64423,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B20" s="229"/>
+      <c r="B20" s="234"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
       </c>
@@ -62395,7 +64499,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="235" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="56" t="s">
@@ -62473,7 +64577,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B22" s="230"/>
+      <c r="B22" s="235"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
       </c>
@@ -62551,7 +64655,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B23" s="230"/>
+      <c r="B23" s="235"/>
       <c r="C23" s="55" t="s">
         <v>461</v>
       </c>
@@ -62629,7 +64733,7 @@
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B24" s="230"/>
+      <c r="B24" s="235"/>
       <c r="C24" s="55" t="s">
         <v>462</v>
       </c>
@@ -62707,7 +64811,7 @@
       </c>
     </row>
     <row r="25" spans="2:27" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="B25" s="230"/>
+      <c r="B25" s="235"/>
       <c r="C25" s="56" t="s">
         <v>438</v>
       </c>
@@ -62783,7 +64887,7 @@
       </c>
     </row>
     <row r="26" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B26" s="231" t="s">
+      <c r="B26" s="236" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="55" t="s">
@@ -62863,7 +64967,7 @@
       </c>
     </row>
     <row r="27" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B27" s="231"/>
+      <c r="B27" s="236"/>
       <c r="C27" s="55" t="s">
         <v>464</v>
       </c>
@@ -62941,7 +65045,7 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B28" s="231"/>
+      <c r="B28" s="236"/>
       <c r="C28" s="55" t="s">
         <v>465</v>
       </c>
@@ -63017,7 +65121,7 @@
       </c>
     </row>
     <row r="29" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B29" s="231"/>
+      <c r="B29" s="236"/>
       <c r="C29" s="55" t="s">
         <v>466</v>
       </c>
@@ -63093,7 +65197,7 @@
       </c>
     </row>
     <row r="30" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B30" s="231"/>
+      <c r="B30" s="236"/>
       <c r="C30" s="55" t="s">
         <v>467</v>
       </c>
@@ -63169,7 +65273,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B31" s="231"/>
+      <c r="B31" s="236"/>
       <c r="C31" s="55" t="s">
         <v>468</v>
       </c>
@@ -63245,7 +65349,7 @@
       </c>
     </row>
     <row r="32" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B32" s="231"/>
+      <c r="B32" s="236"/>
       <c r="C32" s="55" t="s">
         <v>469</v>
       </c>
@@ -63321,7 +65425,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B33" s="231"/>
+      <c r="B33" s="236"/>
       <c r="C33" s="55" t="s">
         <v>470</v>
       </c>
@@ -63397,7 +65501,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B34" s="231"/>
+      <c r="B34" s="236"/>
       <c r="C34" s="55" t="s">
         <v>471</v>
       </c>
@@ -63473,7 +65577,7 @@
       </c>
     </row>
     <row r="35" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B35" s="231"/>
+      <c r="B35" s="236"/>
       <c r="C35" s="55" t="s">
         <v>472</v>
       </c>
@@ -63549,7 +65653,7 @@
       </c>
     </row>
     <row r="36" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B36" s="231"/>
+      <c r="B36" s="236"/>
       <c r="C36" s="55" t="s">
         <v>473</v>
       </c>
@@ -63625,7 +65729,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B37" s="231"/>
+      <c r="B37" s="236"/>
       <c r="C37" s="55" t="s">
         <v>474</v>
       </c>
@@ -63701,7 +65805,7 @@
       </c>
     </row>
     <row r="38" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B38" s="231"/>
+      <c r="B38" s="236"/>
       <c r="C38" s="55" t="s">
         <v>475</v>
       </c>
@@ -63777,7 +65881,7 @@
       </c>
     </row>
     <row r="39" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B39" s="231"/>
+      <c r="B39" s="236"/>
       <c r="C39" s="55" t="s">
         <v>476</v>
       </c>
@@ -63853,7 +65957,7 @@
       </c>
     </row>
     <row r="40" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B40" s="231"/>
+      <c r="B40" s="236"/>
       <c r="C40" s="55" t="s">
         <v>477</v>
       </c>
@@ -63929,7 +66033,7 @@
       </c>
     </row>
     <row r="41" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B41" s="231"/>
+      <c r="B41" s="236"/>
       <c r="C41" s="55" t="s">
         <v>478</v>
       </c>
@@ -64005,7 +66109,7 @@
       </c>
     </row>
     <row r="42" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B42" s="231"/>
+      <c r="B42" s="236"/>
       <c r="C42" s="55" t="s">
         <v>479</v>
       </c>
@@ -64081,7 +66185,7 @@
       </c>
     </row>
     <row r="43" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B43" s="231"/>
+      <c r="B43" s="236"/>
       <c r="C43" s="55" t="s">
         <v>480</v>
       </c>
@@ -64157,7 +66261,7 @@
       </c>
     </row>
     <row r="44" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B44" s="231"/>
+      <c r="B44" s="236"/>
       <c r="C44" s="55" t="s">
         <v>481</v>
       </c>
@@ -64233,7 +66337,7 @@
       </c>
     </row>
     <row r="45" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B45" s="231"/>
+      <c r="B45" s="236"/>
       <c r="C45" s="55" t="s">
         <v>482</v>
       </c>
@@ -64309,7 +66413,7 @@
       </c>
     </row>
     <row r="46" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B46" s="231"/>
+      <c r="B46" s="236"/>
       <c r="C46" s="55" t="s">
         <v>483</v>
       </c>
@@ -64385,7 +66489,7 @@
       </c>
     </row>
     <row r="47" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B47" s="231"/>
+      <c r="B47" s="236"/>
       <c r="C47" s="55" t="s">
         <v>484</v>
       </c>
@@ -64461,7 +66565,7 @@
       </c>
     </row>
     <row r="48" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B48" s="231"/>
+      <c r="B48" s="236"/>
       <c r="C48" s="55" t="s">
         <v>485</v>
       </c>
@@ -64537,7 +66641,7 @@
       </c>
     </row>
     <row r="49" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B49" s="231"/>
+      <c r="B49" s="236"/>
       <c r="C49" s="55" t="s">
         <v>486</v>
       </c>
@@ -64613,7 +66717,7 @@
       </c>
     </row>
     <row r="50" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B50" s="231"/>
+      <c r="B50" s="236"/>
       <c r="C50" s="55" t="s">
         <v>487</v>
       </c>
@@ -64691,7 +66795,7 @@
       </c>
     </row>
     <row r="51" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B51" s="231"/>
+      <c r="B51" s="236"/>
       <c r="C51" s="55" t="s">
         <v>488</v>
       </c>
@@ -64769,7 +66873,7 @@
       </c>
     </row>
     <row r="52" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B52" s="231"/>
+      <c r="B52" s="236"/>
       <c r="C52" s="55" t="s">
         <v>489</v>
       </c>
@@ -64847,7 +66951,7 @@
       </c>
     </row>
     <row r="53" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B53" s="232" t="s">
+      <c r="B53" s="237" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -64927,7 +67031,7 @@
       </c>
     </row>
     <row r="54" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B54" s="232"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="54" t="s">
         <v>440</v>
       </c>
@@ -65005,7 +67109,7 @@
       </c>
     </row>
     <row r="55" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B55" s="232"/>
+      <c r="B55" s="237"/>
       <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
@@ -65083,7 +67187,7 @@
       </c>
     </row>
     <row r="56" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B56" s="232"/>
+      <c r="B56" s="237"/>
       <c r="C56" s="13" t="s">
         <v>490</v>
       </c>
@@ -65159,7 +67263,7 @@
       </c>
     </row>
     <row r="57" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B57" s="232"/>
+      <c r="B57" s="237"/>
       <c r="C57" s="56" t="s">
         <v>491</v>
       </c>
@@ -65237,7 +67341,7 @@
       </c>
     </row>
     <row r="58" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B58" s="232"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="13" t="s">
         <v>444</v>
       </c>
@@ -65313,7 +67417,7 @@
       </c>
     </row>
     <row r="59" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B59" s="232"/>
+      <c r="B59" s="237"/>
       <c r="C59" s="13" t="s">
         <v>445</v>
       </c>
@@ -65391,7 +67495,7 @@
       </c>
     </row>
     <row r="60" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B60" s="232"/>
+      <c r="B60" s="237"/>
       <c r="C60" s="54" t="s">
         <v>492</v>
       </c>
@@ -65469,7 +67573,7 @@
       </c>
     </row>
     <row r="61" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B61" s="233" t="s">
+      <c r="B61" s="238" t="s">
         <v>342</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -65547,7 +67651,7 @@
       </c>
     </row>
     <row r="62" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B62" s="233"/>
+      <c r="B62" s="238"/>
       <c r="C62" s="13" t="s">
         <v>446</v>
       </c>
@@ -65625,7 +67729,7 @@
       </c>
     </row>
     <row r="63" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B63" s="233"/>
+      <c r="B63" s="238"/>
       <c r="C63" s="13" t="s">
         <v>447</v>
       </c>
@@ -65703,7 +67807,7 @@
       </c>
     </row>
     <row r="64" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B64" s="233"/>
+      <c r="B64" s="238"/>
       <c r="C64" s="13" t="s">
         <v>494</v>
       </c>
@@ -65781,7 +67885,7 @@
       </c>
     </row>
     <row r="65" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B65" s="233"/>
+      <c r="B65" s="238"/>
       <c r="C65" s="54" t="s">
         <v>495</v>
       </c>
@@ -65811,7 +67915,7 @@
       <c r="AA65" s="5"/>
     </row>
     <row r="66" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B66" s="233"/>
+      <c r="B66" s="238"/>
       <c r="C66" s="54" t="s">
         <v>496</v>
       </c>
@@ -65841,7 +67945,7 @@
       <c r="AA66" s="5"/>
     </row>
     <row r="67" spans="2:27" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="B67" s="233"/>
+      <c r="B67" s="238"/>
       <c r="C67" s="13" t="s">
         <v>497</v>
       </c>
@@ -65871,7 +67975,7 @@
       <c r="AA67" s="1"/>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B68" s="223" t="s">
+      <c r="B68" s="228" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -65892,7 +67996,7 @@
       <c r="Q68" s="105"/>
     </row>
     <row r="69" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B69" s="223"/>
+      <c r="B69" s="228"/>
       <c r="C69" s="15" t="s">
         <v>449</v>
       </c>
@@ -65911,7 +68015,7 @@
       <c r="Q69" s="105"/>
     </row>
     <row r="70" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B70" s="223"/>
+      <c r="B70" s="228"/>
       <c r="C70" s="15" t="s">
         <v>450</v>
       </c>
@@ -65930,7 +68034,7 @@
       <c r="Q70" s="105"/>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B71" s="223"/>
+      <c r="B71" s="228"/>
       <c r="C71" s="15" t="s">
         <v>498</v>
       </c>
@@ -65949,7 +68053,7 @@
       <c r="Q71" s="105"/>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.4">
-      <c r="B72" s="224"/>
+      <c r="B72" s="229"/>
       <c r="C72" s="16" t="s">
         <v>499</v>
       </c>

</xml_diff>

<commit_message>
August 2025 labels update.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5D6B80-1B66-47CD-A291-121CC0E464A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0B7B03-C996-4071-BBF2-CF695E677924}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9684" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14682" uniqueCount="3117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15143" uniqueCount="3256">
   <si>
     <t>Description</t>
   </si>
@@ -9085,9 +9085,6 @@
     <t>[Data type] measured as [Layer] of [Aspect 1] recovered as scrap from [Aspect 2] in [Aspect 3] in [Aspect 5] in [Aspect 4] for CE strategy [Aspect 6] is [value].</t>
   </si>
   <si>
-    <t>3_EI_Other_Vehicles_CIRCOMOD_D4.2_2025</t>
-  </si>
-  <si>
     <t>final energy</t>
   </si>
   <si>
@@ -9382,6 +9379,426 @@
   </si>
   <si>
     <t>June 5, 2025 update</t>
+  </si>
+  <si>
+    <t>4_PY_Manufacturing_Allwood_2024</t>
+  </si>
+  <si>
+    <t>steel and aluminium casting, rolling, shaping, cutting, and forging</t>
+  </si>
+  <si>
+    <t>about 10 different process steps</t>
+  </si>
+  <si>
+    <t>steel and aluminium in raw form, semi-finished, and finished metal</t>
+  </si>
+  <si>
+    <t>about 20 different product types</t>
+  </si>
+  <si>
+    <t>steel, aluminium</t>
+  </si>
+  <si>
+    <t>single representative value for global manufacturing technologies</t>
+  </si>
+  <si>
+    <t>2005-2020</t>
+  </si>
+  <si>
+    <t>single representative value</t>
+  </si>
+  <si>
+    <t>manufacturing yield ratios / yield factors for various steel and aluminium processing steps, from ore/scrap to finished metal products</t>
+  </si>
+  <si>
+    <t>manufacturing; process yield; manufacturing yield; yield loss; steel; aluminium</t>
+  </si>
+  <si>
+    <t>The process yield factors are estimated from a large number of sources, documented in the reference for this dataset. The time and geographical scope is not defined, an based on the sources cited, it was set to 2005-2020 and Global.</t>
+  </si>
+  <si>
+    <t>Value(m,B,p,F,v,t,r)</t>
+  </si>
+  <si>
+    <t>Yield coefficient measured as mass ratio of steel in slabs, blooms, billets processed into steel rods and bars in hot rolling in Global in 2005-2020 for CE strategy none is 94%.</t>
+  </si>
+  <si>
+    <t>[Data type] measured as [Layer] of [Aspect 1] in [Aspect 2] processed into [Aspect 4] in [Aspect 3] in [Aspect 6] in [Aspect 7] for CE strategy [Aspect 5] is [value].</t>
+  </si>
+  <si>
+    <t>Julian ALLWOOD</t>
+  </si>
+  <si>
+    <t>Table 1 in https://doi.org/10.1098/rsta.2023.0245</t>
+  </si>
+  <si>
+    <t>Table in pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1098/rsta.2023.0245</t>
+  </si>
+  <si>
+    <t>J.M. Allwood, O. Music. Material efficiency at the component level: how much metal can we do without? Philosophical Transactions of the Royal Society (2024) Volume 382, Issue 2284</t>
+  </si>
+  <si>
+    <t>3_LT_Electricity_System_Technologies_Victoria_et_al_2020</t>
+  </si>
+  <si>
+    <t>Electricity generation, distribution, and storage technologies</t>
+  </si>
+  <si>
+    <t>7 different technologies</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>aggregate value</t>
+  </si>
+  <si>
+    <t>Useful/operatin lifetime of electricity generation, distribution, and storage technologies, compiled from different sources and used for energy system modelling (pyPSA).</t>
+  </si>
+  <si>
+    <t>lifetime; useful life; lifespan; use phase; Europe; EU; energy; electricity; energy system; energy storage; electricity generation;</t>
+  </si>
+  <si>
+    <t>Data were compiled from different sources and used for energy system modelling. Original source indicated in comment field.</t>
+  </si>
+  <si>
+    <t>Lifetime of offshore wind power generation in use phase in EU27 built in all years is 27 yr.</t>
+  </si>
+  <si>
+    <t>Marta VICTORIA</t>
+  </si>
+  <si>
+    <t>https://static-content.springer.com/esm/art%3A10.1038%2Fs41467-020-20015-4/MediaObjects/41467_2020_20015_MOESM1_ESM.pdf</t>
+  </si>
+  <si>
+    <t>table in supplementary pdf file (supplementary table 5)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-020-20015-4</t>
+  </si>
+  <si>
+    <t>3_MC_Wooden_Multipurpose_Building_Buschbeck_2025</t>
+  </si>
+  <si>
+    <t>multipurpose building</t>
+  </si>
+  <si>
+    <t>3 different building construction and transformation types</t>
+  </si>
+  <si>
+    <t>main building materials and components</t>
+  </si>
+  <si>
+    <t>13 different materials and building components</t>
+  </si>
+  <si>
+    <t>contemporary building design derived from case study, applicable for ca. 2020-2030</t>
+  </si>
+  <si>
+    <t>Material composition of a case-study design multipurpose building (25 years of parking house, another 25 years of residential+office), for concrete reference, wood-based building with and without demolition between the two use phases.</t>
+  </si>
+  <si>
+    <t>material; material content; buildings; wooden building; circular economy; multipurpose building;</t>
+  </si>
+  <si>
+    <t>Data behind Figure 4 in the linked paper, available from the xlsx supplementary material</t>
+  </si>
+  <si>
+    <t>Value(r,Y,c,k)</t>
+  </si>
+  <si>
+    <t>Material composition of 7-storey multi-purpose building, wood-based, demolition measured as mass of laminated veneer lumber per unit of 7-storey multi-purpose building, wood-based, demolition in Germany built in ca. 2020-2030 is 212.67 kg/m².</t>
+  </si>
+  <si>
+    <t>[data type] of [Aspect 2] measured as [layer] of [Aspect 4] per area of [aspect 2] in [Aspect 1] built in [Aspect 3] is [Value].</t>
+  </si>
+  <si>
+    <t>Christian BUSCHBECK</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/uploads/15805315</t>
+  </si>
+  <si>
+    <t>table in xlsx supplement, Figure in paper</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.6094/UNIFR/268540</t>
+  </si>
+  <si>
+    <t>Numbers manually copied from original source (supplementary xlsx) to Excel spreadsheet and reformated to IEDC data model</t>
+  </si>
+  <si>
+    <t>3_SHA_EndUseShares_Steel_Aluminium_Allwood_2025</t>
+  </si>
+  <si>
+    <t>major end uses of steel and aluminium</t>
+  </si>
+  <si>
+    <t>ca. 20 end uses per metal</t>
+  </si>
+  <si>
+    <t>steel and aluminium</t>
+  </si>
+  <si>
+    <t>10 manufacturing types for steel and 8 for aluminium (extruded, forged, cast, …)</t>
+  </si>
+  <si>
+    <t>Split ratios (%) or end-use shares or sector split of final consumption of metal of a certain type going into a certain application</t>
+  </si>
+  <si>
+    <t>Sector split; end-use shares; split ratios; final use shares; steel; aluminium</t>
+  </si>
+  <si>
+    <t>Original data source: Music and Allwood (2025): https://doi.org/10.1016/j.resconrec.2024.107949. Dataset contains sector split breakdown into material types and product groups "all forms" reports the sum over all material types. Rounding errors of up to 1% occur.</t>
+  </si>
+  <si>
+    <t>Value(m,B,p,F,r,t)</t>
+  </si>
+  <si>
+    <t>Mass ratio of total final consumption of aluminium in form of aluminium, cast going into other metal goods in use phase in Global in 202 is 2.8%.</t>
+  </si>
+  <si>
+    <t>[Layer] of total final consumption of [Aspect 1] in form of [Aspect 2] going into [Aspect 4] in [Aspect 3] in [Aspect 5] in [Aspect 6] is [Value].</t>
+  </si>
+  <si>
+    <t>Figure 10 in https://doi.org/10.1016/j.cirp.2025.04.013</t>
+  </si>
+  <si>
+    <t>Figure in pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cirp.2025.04.013</t>
+  </si>
+  <si>
+    <t>3_EI_Other_Vehicles_CIRCOMOD</t>
+  </si>
+  <si>
+    <t>July 4, 2025 update</t>
+  </si>
+  <si>
+    <t>3_MC_Buildings_UK_Variability_DAI_2025</t>
+  </si>
+  <si>
+    <t>six different building types, differentiated by main building material and by age-cohort of construction</t>
+  </si>
+  <si>
+    <t>concrete, mortar, brick, stone</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>four different age-cohort ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometry-informed material intensity of UK housing, including intra-archetype material variability </t>
+  </si>
+  <si>
+    <t>material; material content; buildings; stone building; UK; construction</t>
+  </si>
+  <si>
+    <t>Data extracted from Fig. 2 and Table 1 in the paper.</t>
+  </si>
+  <si>
+    <t>Value(r,Y,c,m)</t>
+  </si>
+  <si>
+    <t>Material composition of residential building, measured as mass of mortar per area of residential building in UK built in 1930-1949 is 123 kg/m².</t>
+  </si>
+  <si>
+    <t>[data type] of [Aspect 2] measured as [layer] of [Aspect 4] per area of [Aspect 2] in [Aspect 1] built in [Aspect 3] is [Value].</t>
+  </si>
+  <si>
+    <t>Menglin DAI</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.resconrec.2025.108392</t>
+  </si>
+  <si>
+    <t>table and Figure in paper (pdf)</t>
+  </si>
+  <si>
+    <t>4_PY_Cobalt_Manufacturing_Recycling_GODOY-LEON_2020</t>
+  </si>
+  <si>
+    <t>waste collection, pre-processing, recycling, manufacturing</t>
+  </si>
+  <si>
+    <t>4 aggregated processes</t>
+  </si>
+  <si>
+    <t>cobalt-containing commodities</t>
+  </si>
+  <si>
+    <t>8 different groups</t>
+  </si>
+  <si>
+    <t>cobalt</t>
+  </si>
+  <si>
+    <t>single material</t>
+  </si>
+  <si>
+    <t>Global and some single-country values</t>
+  </si>
+  <si>
+    <t>1980-2017</t>
+  </si>
+  <si>
+    <t>single year values for individual data points</t>
+  </si>
+  <si>
+    <t>process yield coefficients for waste collection (collection rate), recycling (recycling rate), and manufacturing yield for cobalt-containing products</t>
+  </si>
+  <si>
+    <t>cobalt; products; metals; catalysts; alloys; process yield; yield loss; manufacturing yield; collection rate; recycling rate</t>
+  </si>
+  <si>
+    <t>Data extracted from different tables in the supplement, see the comment for each value</t>
+  </si>
+  <si>
+    <t>Value(m,k,o,p,d,r,t)</t>
+  </si>
+  <si>
+    <t>Yield coefficient for process recycling measured as mass ratio of outflow to market for recycled material over inflow from market for waste products and components for cobalt in battery, portable in Germany in 2011 is 90%.</t>
+  </si>
+  <si>
+    <t>[Data type] for process [Aspect 4] measured as [Layer] of outflow to [Aspect 5] over inflow from [Aspect 3] for [Aspect 1] in [Aspect 2] in [Aspect 6] in [Aspect 7] is [Value].</t>
+  </si>
+  <si>
+    <t>María Fernanda Godoy León</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.resconrec.2019.104564</t>
+  </si>
+  <si>
+    <t>Data extracted from paper supplement 1-s2.0-S0921344919304707-mmc1.pdf, pages 7-14, Tables A2-A13</t>
+  </si>
+  <si>
+    <t>4_SHR_Cobalt_Products_End_Uses_GODOY-LEON_2020</t>
+  </si>
+  <si>
+    <t>manufacturing and market for final goods and services</t>
+  </si>
+  <si>
+    <t>two aggregate process</t>
+  </si>
+  <si>
+    <t>all major applications of cobalt</t>
+  </si>
+  <si>
+    <t>seven product groups/components</t>
+  </si>
+  <si>
+    <t>European Union (with global markets)</t>
+  </si>
+  <si>
+    <t>One aggregate region</t>
+  </si>
+  <si>
+    <t>2010-2017</t>
+  </si>
+  <si>
+    <t>Shares of cobalt flows in different components in the EU manufacturing output and the EU final consumption, as share of cobalt flows in all products</t>
+  </si>
+  <si>
+    <t>cobalt; manufacturing; product shares; final consumption; end-use shares; sector split; EU; European Union</t>
+  </si>
+  <si>
+    <t>Values describe shares in manufacturing and market shares of final uses for cobalt-containing components.</t>
+  </si>
+  <si>
+    <t>Value(m,k,g,o,O,d,D,t)</t>
+  </si>
+  <si>
+    <t>Mass ratio indicating the share of cobalt in magnets in the flow of all products flowing from manufacturing in the EU to market for manufactured goods and components in the EU in 2016 is 1.67%.</t>
+  </si>
+  <si>
+    <t>[Layer] indicating the share of [Aspect 1] in [Aspect 2] in the flow of [Aspect 3] flowing from [Aspect 4] in [Aspect 5] to [Aspect 6] in [Aspect 7] in [Aspect 8] is [value].</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.resconrec.2020.104842</t>
+  </si>
+  <si>
+    <t>Data extracted from paper supplement 1-s2.0-S0921344920301622-mmc2.xlsx, sheet "Share end uses EU", rows 79-124.</t>
+  </si>
+  <si>
+    <t>1_F_Final_Metal_Demand_Watari_2020</t>
+  </si>
+  <si>
+    <t>material demand (use phase, final consumption)</t>
+  </si>
+  <si>
+    <t>all uses</t>
+  </si>
+  <si>
+    <t>depends on the different metals</t>
+  </si>
+  <si>
+    <t>Global total</t>
+  </si>
+  <si>
+    <t>2030 and 2050</t>
+  </si>
+  <si>
+    <t>Scenarios for the final demand of technology metals, compiled by Watari et al. (2020) from more than 80 different studies.</t>
+  </si>
+  <si>
+    <t>technology metals; final demand; review; scenarios; 2030; 2050</t>
+  </si>
+  <si>
+    <t>Paper mentions "demand", which here is interpreted as final demand</t>
+  </si>
+  <si>
+    <t>Value(m,g,o,d,r,t)</t>
+  </si>
+  <si>
+    <t>Mass of flow of platinum in fuel cells from market for final goods to use phase in Global in 2050 is 0.006 kt/yr with comment Extracted from: Watari et al. (2019), … .</t>
+  </si>
+  <si>
+    <t>[Layer] of [Data type] of [aspect1] in [aspect2] flowing from [aspect3] to [aspect4] in [aspect5] in [aspect6] has [value] with comment [comment].</t>
+  </si>
+  <si>
+    <t>Takuma WATARI</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.resconrec.2019.104669</t>
+  </si>
+  <si>
+    <t>pdf journal paper with supplementary xlsx</t>
+  </si>
+  <si>
+    <t>Numbers extracted from supplementary xlsx and converted to IEDC templates</t>
+  </si>
+  <si>
+    <t>3_LT_Cobalt_Products_GODOY-LEON_2020</t>
+  </si>
+  <si>
+    <t>1970-2015</t>
+  </si>
+  <si>
+    <t>time ranges (age-cohorts) for the different commodities</t>
+  </si>
+  <si>
+    <t>lifetime estimates (useful lifetime) compiled from various literature sources for MFA study on cobalt</t>
+  </si>
+  <si>
+    <t>cobalt; lifetime; products; metals; catalysts; alloys; use phase; useful product lifetime</t>
+  </si>
+  <si>
+    <t>Value(m,k,p;r,c)</t>
+  </si>
+  <si>
+    <t>Cobalt in magnets of age-cohort 1995-2015 in the use phase in region Japan has lifetime of 16.4 years.</t>
+  </si>
+  <si>
+    <t>[aspect1] in [aspect2] of [aspect5] in [aspect3] in [aspect 4] has [Layer] of [value].</t>
+  </si>
+  <si>
+    <t>August 4, 2025 update</t>
   </si>
 </sst>
 </file>
@@ -11128,13 +11545,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:AE39"/>
+  <dimension ref="B2:AF39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W17" sqref="W17"/>
+      <selection pane="bottomRight" activeCell="AI11" sqref="AI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -11159,7 +11576,7 @@
     <col min="23" max="23" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>184</v>
       </c>
@@ -11174,8 +11591,9 @@
       <c r="AC2" s="105"/>
       <c r="AD2" s="105"/>
       <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
     </row>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B3" s="32"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -11264,8 +11682,9 @@
       <c r="AE3" s="82" t="s">
         <v>2597</v>
       </c>
+      <c r="AF3" s="105"/>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B4" s="226" t="s">
         <v>2</v>
       </c>
@@ -11356,8 +11775,9 @@
       <c r="AE4" s="140">
         <v>27</v>
       </c>
+      <c r="AF4" s="105"/>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B5" s="227"/>
       <c r="C5" s="54" t="s">
         <v>452</v>
@@ -11446,8 +11866,9 @@
       <c r="AE5" s="164" t="s">
         <v>2597</v>
       </c>
+      <c r="AF5" s="105"/>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B6" s="33"/>
       <c r="C6" s="54" t="s">
         <v>453</v>
@@ -11534,8 +11955,9 @@
       <c r="AE6" s="164" t="s">
         <v>11</v>
       </c>
+      <c r="AF6" s="105"/>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
@@ -11624,8 +12046,9 @@
       <c r="AE7" s="164" t="s">
         <v>11</v>
       </c>
+      <c r="AF7" s="105"/>
     </row>
-    <row r="8" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:32" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="222" t="s">
         <v>6</v>
       </c>
@@ -11714,8 +12137,9 @@
       <c r="AE8" s="23" t="s">
         <v>2598</v>
       </c>
+      <c r="AF8" s="105"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B9" s="222"/>
       <c r="C9" s="54" t="s">
         <v>424</v>
@@ -11802,8 +12226,9 @@
       <c r="AE9" s="23" t="s">
         <v>2598</v>
       </c>
+      <c r="AF9" s="105"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B10" s="222"/>
       <c r="C10" s="54" t="s">
         <v>425</v>
@@ -11890,8 +12315,9 @@
       <c r="AE10" s="23" t="s">
         <v>2598</v>
       </c>
+      <c r="AF10" s="105"/>
     </row>
-    <row r="11" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B11" s="222"/>
       <c r="C11" s="55" t="s">
         <v>426</v>
@@ -11978,8 +12404,9 @@
       <c r="AE11" s="23" t="s">
         <v>2599</v>
       </c>
+      <c r="AF11" s="105"/>
     </row>
-    <row r="12" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B12" s="222"/>
       <c r="C12" s="56" t="s">
         <v>427</v>
@@ -12066,8 +12493,9 @@
       <c r="AE12" s="23" t="s">
         <v>2589</v>
       </c>
+      <c r="AF12" s="105"/>
     </row>
-    <row r="13" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B13" s="222"/>
       <c r="C13" s="56" t="s">
         <v>428</v>
@@ -12154,8 +12582,9 @@
       <c r="AE13" s="23" t="s">
         <v>11</v>
       </c>
+      <c r="AF13" s="105"/>
     </row>
-    <row r="14" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B14" s="222"/>
       <c r="C14" s="56" t="s">
         <v>429</v>
@@ -12242,8 +12671,9 @@
       <c r="AE14" s="23" t="s">
         <v>11</v>
       </c>
+      <c r="AF14" s="105"/>
     </row>
-    <row r="15" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B15" s="222"/>
       <c r="C15" s="56" t="s">
         <v>430</v>
@@ -12330,8 +12760,9 @@
       <c r="AE15" s="23" t="s">
         <v>2600</v>
       </c>
+      <c r="AF15" s="105"/>
     </row>
-    <row r="16" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B16" s="222"/>
       <c r="C16" s="56" t="s">
         <v>431</v>
@@ -12418,8 +12849,9 @@
       <c r="AE16" s="23" t="s">
         <v>2600</v>
       </c>
+      <c r="AF16" s="105"/>
     </row>
-    <row r="17" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B17" s="222"/>
       <c r="C17" s="56" t="s">
         <v>432</v>
@@ -12506,8 +12938,9 @@
       <c r="AE17" s="164" t="s">
         <v>1422</v>
       </c>
+      <c r="AF17" s="105"/>
     </row>
-    <row r="18" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B18" s="222"/>
       <c r="C18" s="56" t="s">
         <v>433</v>
@@ -12594,8 +13027,9 @@
       <c r="AE18" s="164" t="s">
         <v>2601</v>
       </c>
+      <c r="AF18" s="105"/>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B19" s="222"/>
       <c r="C19" s="56" t="s">
         <v>434</v>
@@ -12682,8 +13116,9 @@
       <c r="AE19" s="23" t="s">
         <v>2602</v>
       </c>
+      <c r="AF19" s="105"/>
     </row>
-    <row r="20" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B20" s="222"/>
       <c r="C20" s="56" t="s">
         <v>435</v>
@@ -12770,8 +13205,9 @@
       <c r="AE20" s="164" t="s">
         <v>2603</v>
       </c>
+      <c r="AF20" s="105"/>
     </row>
-    <row r="21" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B21" s="223" t="s">
         <v>0</v>
       </c>
@@ -12860,8 +13296,9 @@
       <c r="AE21" s="23" t="s">
         <v>2604</v>
       </c>
+      <c r="AF21" s="105"/>
     </row>
-    <row r="22" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B22" s="223"/>
       <c r="C22" s="56" t="s">
         <v>437</v>
@@ -12950,8 +13387,9 @@
       <c r="AE22" s="164" t="s">
         <v>2605</v>
       </c>
+      <c r="AF22" s="105"/>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B23" s="223"/>
       <c r="C23" s="56" t="s">
         <v>454</v>
@@ -13038,8 +13476,9 @@
       <c r="AE23" s="164" t="s">
         <v>11</v>
       </c>
+      <c r="AF23" s="105"/>
     </row>
-    <row r="24" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B24" s="223"/>
       <c r="C24" s="56" t="s">
         <v>438</v>
@@ -13120,8 +13559,9 @@
       <c r="AC24" s="164"/>
       <c r="AD24" s="164"/>
       <c r="AE24" s="164"/>
+      <c r="AF24" s="105"/>
     </row>
-    <row r="25" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:32" ht="13.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="224" t="s">
         <v>8</v>
       </c>
@@ -13210,8 +13650,9 @@
       <c r="AE25" s="23" t="s">
         <v>206</v>
       </c>
+      <c r="AF25" s="105"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B26" s="224"/>
       <c r="C26" s="54" t="s">
         <v>440</v>
@@ -13298,8 +13739,9 @@
       <c r="AE26" s="164" t="s">
         <v>858</v>
       </c>
+      <c r="AF26" s="105"/>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B27" s="224"/>
       <c r="C27" s="13" t="s">
         <v>441</v>
@@ -13386,8 +13828,9 @@
       <c r="AE27" s="164" t="s">
         <v>2606</v>
       </c>
+      <c r="AF27" s="105"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B28" s="224"/>
       <c r="C28" s="13" t="s">
         <v>443</v>
@@ -13474,8 +13917,9 @@
       <c r="AE28" s="179" t="s">
         <v>2607</v>
       </c>
+      <c r="AF28" s="105"/>
     </row>
-    <row r="29" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B29" s="224"/>
       <c r="C29" s="13" t="s">
         <v>444</v>
@@ -13562,8 +14006,9 @@
       <c r="AE29" s="179" t="s">
         <v>2607</v>
       </c>
+      <c r="AF29" s="105"/>
     </row>
-    <row r="30" spans="2:31" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:32" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B30" s="224"/>
       <c r="C30" s="13" t="s">
         <v>445</v>
@@ -13650,8 +14095,9 @@
       <c r="AE30" s="179" t="s">
         <v>2607</v>
       </c>
+      <c r="AF30" s="105"/>
     </row>
-    <row r="31" spans="2:31" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:32" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="225" t="s">
         <v>9</v>
       </c>
@@ -13742,8 +14188,9 @@
       <c r="AE31" s="161">
         <v>45772</v>
       </c>
+      <c r="AF31" s="105"/>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B32" s="228"/>
       <c r="C32" s="86" t="s">
         <v>447</v>
@@ -13832,8 +14279,9 @@
       <c r="AE32" s="164" t="s">
         <v>30</v>
       </c>
+      <c r="AF32" s="105"/>
     </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B33" s="218" t="s">
         <v>185</v>
       </c>
@@ -13868,8 +14316,9 @@
       <c r="AC33" s="164"/>
       <c r="AD33" s="164"/>
       <c r="AE33" s="164"/>
+      <c r="AF33" s="105"/>
     </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B34" s="219"/>
       <c r="C34" s="15" t="s">
         <v>449</v>
@@ -13902,8 +14351,9 @@
       <c r="AC34" s="164"/>
       <c r="AD34" s="164"/>
       <c r="AE34" s="164"/>
+      <c r="AF34" s="105"/>
     </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:32" x14ac:dyDescent="0.4">
       <c r="B35" s="220"/>
       <c r="C35" s="16" t="s">
         <v>450</v>
@@ -13936,11 +14386,12 @@
       <c r="AC35" s="166"/>
       <c r="AD35" s="166"/>
       <c r="AE35" s="166"/>
+      <c r="AF35" s="105"/>
     </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:32" x14ac:dyDescent="0.4">
       <c r="W36" s="105"/>
     </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:32" x14ac:dyDescent="0.4">
       <c r="I39" s="12"/>
     </row>
   </sheetData>
@@ -13959,13 +14410,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:GW74"/>
+  <dimension ref="A1:IU74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="FZ33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="GE30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="GP3" sqref="GP3"/>
+      <selection pane="bottomRight" activeCell="GY2" sqref="GY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -14026,7 +14477,7 @@
     <col min="70" max="16384" width="11.5546875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:198" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:207" x14ac:dyDescent="0.4">
       <c r="C1" s="73" t="s">
         <v>269</v>
       </c>
@@ -14528,8 +14979,17 @@
       <c r="GN1" s="174"/>
       <c r="GO1" s="174"/>
       <c r="GP1" s="174"/>
+      <c r="GQ1" s="174"/>
+      <c r="GR1" s="174"/>
+      <c r="GS1" s="174"/>
+      <c r="GT1" s="174"/>
+      <c r="GU1" s="174"/>
+      <c r="GV1" s="174"/>
+      <c r="GW1" s="174"/>
+      <c r="GX1" s="174"/>
+      <c r="GY1" s="174"/>
     </row>
-    <row r="2" spans="1:198" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:207" ht="13.8" x14ac:dyDescent="0.45">
       <c r="B2" s="34" t="s">
         <v>183</v>
       </c>
@@ -14919,28 +15379,55 @@
         <v>2987</v>
       </c>
       <c r="GJ2" s="154" t="s">
-        <v>3030</v>
+        <v>3029</v>
       </c>
       <c r="GK2" s="154" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="GL2" s="154" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="GM2" s="154" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="GN2" s="154" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="GO2" s="154" t="s">
-        <v>3099</v>
+        <v>3098</v>
       </c>
       <c r="GP2" s="154" t="s">
-        <v>3116</v>
+        <v>3115</v>
+      </c>
+      <c r="GQ2" s="154" t="s">
+        <v>3181</v>
+      </c>
+      <c r="GR2" s="154" t="s">
+        <v>3181</v>
+      </c>
+      <c r="GS2" s="154" t="s">
+        <v>3181</v>
+      </c>
+      <c r="GT2" s="154" t="s">
+        <v>3181</v>
+      </c>
+      <c r="GU2" s="154" t="s">
+        <v>3255</v>
+      </c>
+      <c r="GV2" s="154" t="s">
+        <v>3255</v>
+      </c>
+      <c r="GW2" s="154" t="s">
+        <v>3255</v>
+      </c>
+      <c r="GX2" s="154" t="s">
+        <v>3255</v>
+      </c>
+      <c r="GY2" s="154" t="s">
+        <v>3255</v>
       </c>
     </row>
-    <row r="3" spans="1:198" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:207" x14ac:dyDescent="0.4">
       <c r="B3" s="58"/>
       <c r="C3" s="17" t="s">
         <v>181</v>
@@ -15193,7 +15680,7 @@
       <c r="DS3" s="105"/>
       <c r="DT3" s="105"/>
     </row>
-    <row r="4" spans="1:198" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:207" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>1</v>
       </c>
@@ -15451,7 +15938,7 @@
       <c r="DS4" s="105"/>
       <c r="DT4" s="105"/>
     </row>
-    <row r="5" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="41">
         <v>2</v>
       </c>
@@ -16024,28 +16511,55 @@
         <v>3006</v>
       </c>
       <c r="GJ5" s="159" t="s">
-        <v>3018</v>
+        <v>3180</v>
       </c>
       <c r="GK5" s="159" t="s">
-        <v>3031</v>
+        <v>3030</v>
       </c>
       <c r="GL5" s="115" t="s">
-        <v>3044</v>
+        <v>3043</v>
       </c>
       <c r="GM5" s="115" t="s">
-        <v>3054</v>
+        <v>3053</v>
       </c>
       <c r="GN5" s="115" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="GO5" s="115" t="s">
-        <v>3080</v>
+        <v>3079</v>
       </c>
       <c r="GP5" s="115" t="s">
-        <v>3100</v>
+        <v>3099</v>
+      </c>
+      <c r="GQ5" s="208" t="s">
+        <v>3116</v>
+      </c>
+      <c r="GR5" s="115" t="s">
+        <v>3136</v>
+      </c>
+      <c r="GS5" s="115" t="s">
+        <v>3149</v>
+      </c>
+      <c r="GT5" s="115" t="s">
+        <v>3166</v>
+      </c>
+      <c r="GU5" s="115" t="s">
+        <v>3182</v>
+      </c>
+      <c r="GV5" s="115" t="s">
+        <v>3196</v>
+      </c>
+      <c r="GW5" s="115" t="s">
+        <v>3215</v>
+      </c>
+      <c r="GX5" s="115" t="s">
+        <v>3231</v>
+      </c>
+      <c r="GY5" s="115" t="s">
+        <v>3247</v>
       </c>
     </row>
-    <row r="6" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="92">
         <v>3</v>
       </c>
@@ -16636,8 +17150,35 @@
       <c r="GP6" s="115" t="s">
         <v>2490</v>
       </c>
+      <c r="GQ6" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX6" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY6" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="92">
         <v>4</v>
       </c>
@@ -17230,8 +17771,35 @@
       <c r="GP7" s="115" t="s">
         <v>845</v>
       </c>
+      <c r="GQ7" s="208" t="s">
+        <v>845</v>
+      </c>
+      <c r="GR7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GS7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GT7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GU7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GV7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GW7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GX7" s="115" t="s">
+        <v>845</v>
+      </c>
+      <c r="GY7" s="115" t="s">
+        <v>845</v>
+      </c>
     </row>
-    <row r="8" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="92">
         <v>5</v>
       </c>
@@ -17824,8 +18392,35 @@
       <c r="GP8" s="115">
         <v>3</v>
       </c>
+      <c r="GQ8" s="208">
+        <v>4</v>
+      </c>
+      <c r="GR8" s="115">
+        <v>3</v>
+      </c>
+      <c r="GS8" s="115">
+        <v>3</v>
+      </c>
+      <c r="GT8" s="115">
+        <v>3</v>
+      </c>
+      <c r="GU8" s="115">
+        <v>3</v>
+      </c>
+      <c r="GV8" s="115">
+        <v>4</v>
+      </c>
+      <c r="GW8" s="115">
+        <v>4</v>
+      </c>
+      <c r="GX8" s="115">
+        <v>1</v>
+      </c>
+      <c r="GY8" s="115">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="92">
         <v>6</v>
       </c>
@@ -18413,13 +19008,40 @@
         <v>1</v>
       </c>
       <c r="GO9" s="115" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
       <c r="GP9" s="115" t="s">
         <v>57</v>
       </c>
+      <c r="GQ9" s="208" t="s">
+        <v>94</v>
+      </c>
+      <c r="GR9" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="GS9" s="115" t="s">
+        <v>846</v>
+      </c>
+      <c r="GT9" s="115" t="s">
+        <v>190</v>
+      </c>
+      <c r="GU9" s="115" t="s">
+        <v>846</v>
+      </c>
+      <c r="GV9" s="115" t="s">
+        <v>94</v>
+      </c>
+      <c r="GW9" s="115" t="s">
+        <v>2904</v>
+      </c>
+      <c r="GX9" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="GY9" s="115" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="10" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="92">
         <v>7</v>
       </c>
@@ -18992,7 +19614,7 @@
         <v>5</v>
       </c>
       <c r="GJ10" s="159" t="s">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="GK10" s="159" t="s">
         <v>57</v>
@@ -19012,8 +19634,35 @@
       <c r="GP10" s="115" t="s">
         <v>57</v>
       </c>
+      <c r="GQ10" s="208" t="s">
+        <v>5</v>
+      </c>
+      <c r="GR10" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="GS10" s="115" t="s">
+        <v>824</v>
+      </c>
+      <c r="GT10" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="GU10" s="115" t="s">
+        <v>151</v>
+      </c>
+      <c r="GV10" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="GW10" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="GX10" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="GY10" s="115" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="11" spans="1:198" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:207" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="92">
         <v>8</v>
       </c>
@@ -19589,7 +20238,7 @@
         <v>32</v>
       </c>
       <c r="GK11" s="159" t="s">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="GL11" s="115" t="s">
         <v>32</v>
@@ -19601,13 +20250,40 @@
         <v>1474</v>
       </c>
       <c r="GO11" s="115" t="s">
-        <v>3082</v>
+        <v>3081</v>
       </c>
       <c r="GP11" s="115" t="s">
         <v>32</v>
       </c>
+      <c r="GQ11" s="209" t="s">
+        <v>3117</v>
+      </c>
+      <c r="GR11" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="GS11" s="115" t="s">
+        <v>782</v>
+      </c>
+      <c r="GT11" s="115" t="s">
+        <v>782</v>
+      </c>
+      <c r="GU11" s="115" t="s">
+        <v>782</v>
+      </c>
+      <c r="GV11" s="115" t="s">
+        <v>3197</v>
+      </c>
+      <c r="GW11" s="115" t="s">
+        <v>3216</v>
+      </c>
+      <c r="GX11" s="115" t="s">
+        <v>3232</v>
+      </c>
+      <c r="GY11" s="115" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="12" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="92">
         <v>9</v>
       </c>
@@ -20178,10 +20854,10 @@
         <v>3008</v>
       </c>
       <c r="GJ12" s="159" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
       <c r="GK12" s="159" t="s">
-        <v>3033</v>
+        <v>3032</v>
       </c>
       <c r="GL12" s="115" t="s">
         <v>152</v>
@@ -20193,13 +20869,40 @@
         <v>2274</v>
       </c>
       <c r="GO12" s="115" t="s">
-        <v>3083</v>
+        <v>3082</v>
       </c>
       <c r="GP12" s="115" t="s">
         <v>152</v>
       </c>
+      <c r="GQ12" s="208" t="s">
+        <v>3118</v>
+      </c>
+      <c r="GR12" s="115" t="s">
+        <v>152</v>
+      </c>
+      <c r="GS12" s="115" t="s">
+        <v>2274</v>
+      </c>
+      <c r="GT12" s="115" t="s">
+        <v>2274</v>
+      </c>
+      <c r="GU12" s="115" t="s">
+        <v>2274</v>
+      </c>
+      <c r="GV12" s="115" t="s">
+        <v>3198</v>
+      </c>
+      <c r="GW12" s="115" t="s">
+        <v>3217</v>
+      </c>
+      <c r="GX12" s="115" t="s">
+        <v>2274</v>
+      </c>
+      <c r="GY12" s="115" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="13" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="92">
         <v>10</v>
       </c>
@@ -20770,13 +21473,13 @@
         <v>597</v>
       </c>
       <c r="GJ13" s="159" t="s">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="GK13" s="159" t="s">
         <v>2935</v>
       </c>
       <c r="GL13" s="115" t="s">
-        <v>3045</v>
+        <v>3044</v>
       </c>
       <c r="GM13" s="115" t="s">
         <v>1561</v>
@@ -20785,13 +21488,40 @@
         <v>11</v>
       </c>
       <c r="GO13" s="115" t="s">
-        <v>3084</v>
+        <v>3083</v>
       </c>
       <c r="GP13" s="115" t="s">
-        <v>3101</v>
+        <v>3100</v>
+      </c>
+      <c r="GQ13" s="208" t="s">
+        <v>3119</v>
+      </c>
+      <c r="GR13" s="115" t="s">
+        <v>3137</v>
+      </c>
+      <c r="GS13" s="115" t="s">
+        <v>3150</v>
+      </c>
+      <c r="GT13" s="115" t="s">
+        <v>3167</v>
+      </c>
+      <c r="GU13" s="115" t="s">
+        <v>756</v>
+      </c>
+      <c r="GV13" s="115" t="s">
+        <v>3199</v>
+      </c>
+      <c r="GW13" s="115" t="s">
+        <v>3218</v>
+      </c>
+      <c r="GX13" s="115" t="s">
+        <v>3233</v>
+      </c>
+      <c r="GY13" s="115" t="s">
+        <v>3199</v>
       </c>
     </row>
-    <row r="14" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="92">
         <v>11</v>
       </c>
@@ -21362,28 +22092,55 @@
         <v>816</v>
       </c>
       <c r="GJ14" s="159" t="s">
-        <v>3022</v>
+        <v>3021</v>
       </c>
       <c r="GK14" s="159" t="s">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="GL14" s="115" t="s">
-        <v>3046</v>
+        <v>3045</v>
       </c>
       <c r="GM14" s="115" t="s">
-        <v>3055</v>
+        <v>3054</v>
       </c>
       <c r="GN14" s="115" t="s">
         <v>11</v>
       </c>
       <c r="GO14" s="115" t="s">
-        <v>3085</v>
+        <v>3084</v>
       </c>
       <c r="GP14" s="115" t="s">
-        <v>3102</v>
+        <v>3101</v>
+      </c>
+      <c r="GQ14" s="208" t="s">
+        <v>3120</v>
+      </c>
+      <c r="GR14" s="115" t="s">
+        <v>3138</v>
+      </c>
+      <c r="GS14" s="115" t="s">
+        <v>3151</v>
+      </c>
+      <c r="GT14" s="115" t="s">
+        <v>3168</v>
+      </c>
+      <c r="GU14" s="115" t="s">
+        <v>3183</v>
+      </c>
+      <c r="GV14" s="115" t="s">
+        <v>3200</v>
+      </c>
+      <c r="GW14" s="115" t="s">
+        <v>3219</v>
+      </c>
+      <c r="GX14" s="115" t="s">
+        <v>3234</v>
+      </c>
+      <c r="GY14" s="115" t="s">
+        <v>3200</v>
       </c>
     </row>
-    <row r="15" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="92">
         <v>12</v>
       </c>
@@ -21963,19 +22720,46 @@
         <v>11</v>
       </c>
       <c r="GM15" s="115" t="s">
-        <v>3056</v>
+        <v>3055</v>
       </c>
       <c r="GN15" s="115" t="s">
-        <v>3070</v>
+        <v>3069</v>
       </c>
       <c r="GO15" s="115" t="s">
         <v>347</v>
       </c>
       <c r="GP15" s="115" t="s">
-        <v>3103</v>
+        <v>3102</v>
+      </c>
+      <c r="GQ15" s="208" t="s">
+        <v>3121</v>
+      </c>
+      <c r="GR15" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS15" s="115" t="s">
+        <v>3152</v>
+      </c>
+      <c r="GT15" s="115" t="s">
+        <v>3169</v>
+      </c>
+      <c r="GU15" s="115" t="s">
+        <v>3152</v>
+      </c>
+      <c r="GV15" s="115" t="s">
+        <v>3201</v>
+      </c>
+      <c r="GW15" s="115" t="s">
+        <v>3201</v>
+      </c>
+      <c r="GX15" s="115" t="s">
+        <v>2656</v>
+      </c>
+      <c r="GY15" s="115" t="s">
+        <v>3201</v>
       </c>
     </row>
-    <row r="16" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="92">
         <v>13</v>
       </c>
@@ -22555,19 +23339,46 @@
         <v>11</v>
       </c>
       <c r="GM16" s="115" t="s">
-        <v>3057</v>
+        <v>3056</v>
       </c>
       <c r="GN16" s="115" t="s">
-        <v>3071</v>
+        <v>3070</v>
       </c>
       <c r="GO16" s="115" t="s">
-        <v>3086</v>
+        <v>3085</v>
       </c>
       <c r="GP16" s="115" t="s">
-        <v>3104</v>
+        <v>3103</v>
+      </c>
+      <c r="GQ16" s="208" t="s">
+        <v>2979</v>
+      </c>
+      <c r="GR16" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS16" s="115" t="s">
+        <v>3153</v>
+      </c>
+      <c r="GT16" s="115" t="s">
+        <v>3170</v>
+      </c>
+      <c r="GU16" s="115" t="s">
+        <v>3184</v>
+      </c>
+      <c r="GV16" s="115" t="s">
+        <v>3202</v>
+      </c>
+      <c r="GW16" s="115" t="s">
+        <v>1680</v>
+      </c>
+      <c r="GX16" s="115" t="s">
+        <v>2657</v>
+      </c>
+      <c r="GY16" s="115" t="s">
+        <v>3202</v>
       </c>
     </row>
-    <row r="17" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="92">
         <v>14</v>
       </c>
@@ -23153,13 +23964,40 @@
         <v>19</v>
       </c>
       <c r="GO17" s="115" t="s">
-        <v>3087</v>
+        <v>3086</v>
       </c>
       <c r="GP17" s="115" t="s">
         <v>138</v>
       </c>
+      <c r="GQ17" s="208" t="s">
+        <v>19</v>
+      </c>
+      <c r="GR17" s="115" t="s">
+        <v>3139</v>
+      </c>
+      <c r="GS17" s="115" t="s">
+        <v>138</v>
+      </c>
+      <c r="GT17" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="GU17" s="115" t="s">
+        <v>3185</v>
+      </c>
+      <c r="GV17" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="GW17" s="115" t="s">
+        <v>3220</v>
+      </c>
+      <c r="GX17" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="GY17" s="115" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="92">
         <v>15</v>
       </c>
@@ -23733,7 +24571,7 @@
         <v>2996</v>
       </c>
       <c r="GK18" s="159" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="GL18" s="115" t="s">
         <v>2762</v>
@@ -23745,13 +24583,40 @@
         <v>2658</v>
       </c>
       <c r="GO18" s="115" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="GP18" s="115" t="s">
         <v>2762</v>
       </c>
+      <c r="GQ18" s="208" t="s">
+        <v>3122</v>
+      </c>
+      <c r="GR18" s="115" t="s">
+        <v>3140</v>
+      </c>
+      <c r="GS18" s="115" t="s">
+        <v>2050</v>
+      </c>
+      <c r="GT18" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="GU18" s="115" t="s">
+        <v>2050</v>
+      </c>
+      <c r="GV18" s="115" t="s">
+        <v>3203</v>
+      </c>
+      <c r="GW18" s="115" t="s">
+        <v>3221</v>
+      </c>
+      <c r="GX18" s="115" t="s">
+        <v>3235</v>
+      </c>
+      <c r="GY18" s="115" t="s">
+        <v>3203</v>
+      </c>
     </row>
-    <row r="19" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="92">
         <v>16</v>
       </c>
@@ -24322,28 +25187,55 @@
         <v>3011</v>
       </c>
       <c r="GJ19" s="159" t="s">
-        <v>3023</v>
+        <v>3022</v>
       </c>
       <c r="GK19" s="159" t="s">
-        <v>3036</v>
+        <v>3035</v>
       </c>
       <c r="GL19" s="115" t="s">
-        <v>3047</v>
+        <v>3046</v>
       </c>
       <c r="GM19" s="115" t="s">
-        <v>3058</v>
+        <v>3057</v>
       </c>
       <c r="GN19" s="115" t="s">
-        <v>3072</v>
+        <v>3071</v>
       </c>
       <c r="GO19" s="115" t="s">
-        <v>3089</v>
+        <v>3088</v>
       </c>
       <c r="GP19" s="115" t="s">
-        <v>3047</v>
+        <v>3046</v>
+      </c>
+      <c r="GQ19" s="208" t="s">
+        <v>3123</v>
+      </c>
+      <c r="GR19" s="115" t="s">
+        <v>3046</v>
+      </c>
+      <c r="GS19" s="115" t="s">
+        <v>3154</v>
+      </c>
+      <c r="GT19" s="115">
+        <v>2023</v>
+      </c>
+      <c r="GU19" s="115" t="s">
+        <v>1811</v>
+      </c>
+      <c r="GV19" s="115" t="s">
+        <v>3204</v>
+      </c>
+      <c r="GW19" s="115" t="s">
+        <v>3222</v>
+      </c>
+      <c r="GX19" s="115" t="s">
+        <v>3236</v>
+      </c>
+      <c r="GY19" s="115" t="s">
+        <v>3248</v>
       </c>
     </row>
-    <row r="20" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="92">
         <v>17</v>
       </c>
@@ -24914,10 +25806,10 @@
         <v>3012</v>
       </c>
       <c r="GJ20" s="159" t="s">
-        <v>3024</v>
+        <v>3023</v>
       </c>
       <c r="GK20" s="159" t="s">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="GL20" s="115" t="s">
         <v>2349</v>
@@ -24932,10 +25824,37 @@
         <v>1145</v>
       </c>
       <c r="GP20" s="115" t="s">
-        <v>3105</v>
+        <v>3104</v>
+      </c>
+      <c r="GQ20" s="208" t="s">
+        <v>3124</v>
+      </c>
+      <c r="GR20" s="115" t="s">
+        <v>3104</v>
+      </c>
+      <c r="GS20" s="115" t="s">
+        <v>2050</v>
+      </c>
+      <c r="GT20" s="115" t="s">
+        <v>311</v>
+      </c>
+      <c r="GU20" s="115" t="s">
+        <v>3186</v>
+      </c>
+      <c r="GV20" s="115" t="s">
+        <v>3205</v>
+      </c>
+      <c r="GW20" s="115" t="s">
+        <v>1145</v>
+      </c>
+      <c r="GX20" s="115" t="s">
+        <v>1145</v>
+      </c>
+      <c r="GY20" s="115" t="s">
+        <v>3249</v>
       </c>
     </row>
-    <row r="21" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="92">
         <v>18</v>
       </c>
@@ -25502,28 +26421,55 @@
         <v>3013</v>
       </c>
       <c r="GJ21" s="159" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="GK21" s="159" t="s">
-        <v>3038</v>
+        <v>3037</v>
       </c>
       <c r="GL21" s="115" t="s">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="GM21" s="115" t="s">
-        <v>3059</v>
+        <v>3058</v>
       </c>
       <c r="GN21" s="115" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="GO21" s="115" t="s">
-        <v>3090</v>
+        <v>3089</v>
       </c>
       <c r="GP21" s="115" t="s">
-        <v>3106</v>
+        <v>3105</v>
+      </c>
+      <c r="GQ21" s="208" t="s">
+        <v>3125</v>
+      </c>
+      <c r="GR21" s="115" t="s">
+        <v>3141</v>
+      </c>
+      <c r="GS21" s="115" t="s">
+        <v>3155</v>
+      </c>
+      <c r="GT21" s="115" t="s">
+        <v>3171</v>
+      </c>
+      <c r="GU21" s="115" t="s">
+        <v>3187</v>
+      </c>
+      <c r="GV21" s="115" t="s">
+        <v>3206</v>
+      </c>
+      <c r="GW21" s="115" t="s">
+        <v>3223</v>
+      </c>
+      <c r="GX21" s="115" t="s">
+        <v>3237</v>
+      </c>
+      <c r="GY21" s="115" t="s">
+        <v>3250</v>
       </c>
     </row>
-    <row r="22" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="92">
         <v>19</v>
       </c>
@@ -26096,28 +27042,55 @@
         <v>3014</v>
       </c>
       <c r="GJ22" s="159" t="s">
-        <v>3026</v>
+        <v>3025</v>
       </c>
       <c r="GK22" s="159" t="s">
-        <v>3039</v>
+        <v>3038</v>
       </c>
       <c r="GL22" s="115" t="s">
-        <v>3049</v>
+        <v>3048</v>
       </c>
       <c r="GM22" s="115" t="s">
-        <v>3060</v>
+        <v>3059</v>
       </c>
       <c r="GN22" s="115" t="s">
-        <v>3074</v>
+        <v>3073</v>
       </c>
       <c r="GO22" s="115" t="s">
-        <v>3091</v>
+        <v>3090</v>
       </c>
       <c r="GP22" s="115" t="s">
-        <v>3107</v>
+        <v>3106</v>
+      </c>
+      <c r="GQ22" s="208" t="s">
+        <v>3126</v>
+      </c>
+      <c r="GR22" s="115" t="s">
+        <v>3142</v>
+      </c>
+      <c r="GS22" s="115" t="s">
+        <v>3156</v>
+      </c>
+      <c r="GT22" s="115" t="s">
+        <v>3172</v>
+      </c>
+      <c r="GU22" s="115" t="s">
+        <v>3188</v>
+      </c>
+      <c r="GV22" s="115" t="s">
+        <v>3207</v>
+      </c>
+      <c r="GW22" s="115" t="s">
+        <v>3224</v>
+      </c>
+      <c r="GX22" s="115" t="s">
+        <v>3238</v>
+      </c>
+      <c r="GY22" s="115" t="s">
+        <v>3251</v>
       </c>
     </row>
-    <row r="23" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="92">
         <v>20</v>
       </c>
@@ -26710,8 +27683,35 @@
       <c r="GP23" s="115" t="s">
         <v>77</v>
       </c>
+      <c r="GQ23" s="208" t="s">
+        <v>24</v>
+      </c>
+      <c r="GR23" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="GS23" s="115" t="s">
+        <v>1054</v>
+      </c>
+      <c r="GT23" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="GU23" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="GV23" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="GW23" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="GX23" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="GY23" s="115" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="92">
         <v>21</v>
       </c>
@@ -27304,8 +28304,35 @@
       <c r="GP24" s="183">
         <v>32</v>
       </c>
+      <c r="GQ24" s="208">
+        <v>25</v>
+      </c>
+      <c r="GR24" s="183">
+        <v>36</v>
+      </c>
+      <c r="GS24" s="115">
+        <v>45</v>
+      </c>
+      <c r="GT24" s="69">
+        <v>419</v>
+      </c>
+      <c r="GU24" s="115">
+        <v>94</v>
+      </c>
+      <c r="GV24" s="115">
+        <v>134</v>
+      </c>
+      <c r="GW24" s="115">
+        <v>105</v>
+      </c>
+      <c r="GX24" s="115">
+        <v>549</v>
+      </c>
+      <c r="GY24" s="115">
+        <v>59</v>
+      </c>
     </row>
-    <row r="25" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="92">
         <v>22</v>
       </c>
@@ -27874,16 +28901,16 @@
         <v>11</v>
       </c>
       <c r="GK25" s="159" t="s">
-        <v>3040</v>
+        <v>3039</v>
       </c>
       <c r="GL25" s="115" t="s">
         <v>11</v>
       </c>
       <c r="GM25" s="115" t="s">
-        <v>3061</v>
+        <v>3060</v>
       </c>
       <c r="GN25" s="217" t="s">
-        <v>3075</v>
+        <v>3074</v>
       </c>
       <c r="GO25" s="115" t="s">
         <v>11</v>
@@ -27891,8 +28918,35 @@
       <c r="GP25" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ25" s="208" t="s">
+        <v>3127</v>
+      </c>
+      <c r="GR25" s="115" t="s">
+        <v>3143</v>
+      </c>
+      <c r="GS25" s="115" t="s">
+        <v>3157</v>
+      </c>
+      <c r="GT25" s="115" t="s">
+        <v>3173</v>
+      </c>
+      <c r="GU25" s="115" t="s">
+        <v>3189</v>
+      </c>
+      <c r="GV25" s="115" t="s">
+        <v>3208</v>
+      </c>
+      <c r="GW25" s="115" t="s">
+        <v>3225</v>
+      </c>
+      <c r="GX25" s="115" t="s">
+        <v>3239</v>
+      </c>
+      <c r="GY25" s="115" t="s">
+        <v>3208</v>
+      </c>
     </row>
-    <row r="26" spans="1:198" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:207" s="68" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="92">
         <v>23</v>
       </c>
@@ -28487,8 +29541,35 @@
       <c r="GP26" s="115" t="s">
         <v>849</v>
       </c>
+      <c r="GQ26" s="208" t="s">
+        <v>849</v>
+      </c>
+      <c r="GR26" s="115" t="s">
+        <v>696</v>
+      </c>
+      <c r="GS26" s="159" t="s">
+        <v>698</v>
+      </c>
+      <c r="GT26" s="159" t="s">
+        <v>849</v>
+      </c>
+      <c r="GU26" s="159" t="s">
+        <v>698</v>
+      </c>
+      <c r="GV26" s="159" t="s">
+        <v>849</v>
+      </c>
+      <c r="GW26" s="159" t="s">
+        <v>849</v>
+      </c>
+      <c r="GX26" s="159" t="s">
+        <v>849</v>
+      </c>
+      <c r="GY26" s="115" t="s">
+        <v>849</v>
+      </c>
     </row>
-    <row r="27" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="92">
         <v>24</v>
       </c>
@@ -29081,8 +30162,35 @@
       <c r="GP27" s="115">
         <v>4</v>
       </c>
+      <c r="GQ27" s="210">
+        <v>4</v>
+      </c>
+      <c r="GR27" s="115">
+        <v>7</v>
+      </c>
+      <c r="GS27" s="159">
+        <v>2</v>
+      </c>
+      <c r="GT27" s="159">
+        <v>4</v>
+      </c>
+      <c r="GU27" s="159">
+        <v>2</v>
+      </c>
+      <c r="GV27" s="159">
+        <v>4</v>
+      </c>
+      <c r="GW27" s="159">
+        <v>4</v>
+      </c>
+      <c r="GX27" s="159">
+        <v>4</v>
+      </c>
+      <c r="GY27" s="115">
+        <v>4</v>
+      </c>
     </row>
-    <row r="28" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="92">
         <v>25</v>
       </c>
@@ -29673,8 +30781,35 @@
       <c r="GP28" s="115" t="s">
         <v>696</v>
       </c>
+      <c r="GQ28" s="208" t="s">
+        <v>707</v>
+      </c>
+      <c r="GR28" s="169" t="s">
+        <v>697</v>
+      </c>
+      <c r="GS28" s="159" t="s">
+        <v>851</v>
+      </c>
+      <c r="GT28" s="159" t="s">
+        <v>707</v>
+      </c>
+      <c r="GU28" s="159" t="s">
+        <v>851</v>
+      </c>
+      <c r="GV28" s="159" t="s">
+        <v>1640</v>
+      </c>
+      <c r="GW28" s="159" t="s">
+        <v>1640</v>
+      </c>
+      <c r="GX28" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GY28" s="115" t="s">
+        <v>1640</v>
+      </c>
     </row>
-    <row r="29" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="92">
         <v>26</v>
       </c>
@@ -30265,8 +31400,35 @@
       <c r="GP29" s="115">
         <v>7</v>
       </c>
+      <c r="GQ29" s="208">
+        <v>7</v>
+      </c>
+      <c r="GR29" s="184">
+        <v>6</v>
+      </c>
+      <c r="GS29" s="182">
+        <v>13</v>
+      </c>
+      <c r="GT29" s="159">
+        <v>7</v>
+      </c>
+      <c r="GU29" s="182">
+        <v>13</v>
+      </c>
+      <c r="GV29" s="184">
+        <v>90</v>
+      </c>
+      <c r="GW29" s="184">
+        <v>90</v>
+      </c>
+      <c r="GX29" s="184">
+        <v>7</v>
+      </c>
+      <c r="GY29" s="115">
+        <v>90</v>
+      </c>
     </row>
-    <row r="30" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="92">
         <v>27</v>
       </c>
@@ -30857,8 +32019,35 @@
       <c r="GP30" s="169" t="s">
         <v>697</v>
       </c>
+      <c r="GQ30" s="208" t="s">
+        <v>697</v>
+      </c>
+      <c r="GR30" s="115" t="s">
+        <v>698</v>
+      </c>
+      <c r="GS30" s="159" t="s">
+        <v>704</v>
+      </c>
+      <c r="GT30" s="159" t="s">
+        <v>697</v>
+      </c>
+      <c r="GU30" s="159" t="s">
+        <v>704</v>
+      </c>
+      <c r="GV30" s="159" t="s">
+        <v>699</v>
+      </c>
+      <c r="GW30" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="GX30" s="159" t="s">
+        <v>699</v>
+      </c>
+      <c r="GY30" s="115" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="31" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="92">
         <v>28</v>
       </c>
@@ -31449,8 +32638,35 @@
       <c r="GP31" s="184">
         <v>6</v>
       </c>
+      <c r="GQ31" s="209">
+        <v>6</v>
+      </c>
+      <c r="GR31" s="115">
+        <v>2</v>
+      </c>
+      <c r="GS31" s="159">
+        <v>14</v>
+      </c>
+      <c r="GT31" s="159">
+        <v>6</v>
+      </c>
+      <c r="GU31" s="159">
+        <v>14</v>
+      </c>
+      <c r="GV31" s="159">
+        <v>6</v>
+      </c>
+      <c r="GW31" s="159">
+        <v>7</v>
+      </c>
+      <c r="GX31" s="159">
+        <v>6</v>
+      </c>
+      <c r="GY31" s="184">
+        <v>6</v>
+      </c>
     </row>
-    <row r="32" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="92">
         <v>29</v>
       </c>
@@ -32041,8 +33257,35 @@
       <c r="GP32" s="115" t="s">
         <v>698</v>
       </c>
+      <c r="GQ32" s="208" t="s">
+        <v>799</v>
+      </c>
+      <c r="GR32" s="115" t="s">
+        <v>704</v>
+      </c>
+      <c r="GS32" s="184" t="s">
+        <v>1640</v>
+      </c>
+      <c r="GT32" s="159" t="s">
+        <v>799</v>
+      </c>
+      <c r="GU32" s="184" t="s">
+        <v>849</v>
+      </c>
+      <c r="GV32" s="159" t="s">
+        <v>697</v>
+      </c>
+      <c r="GW32" s="159" t="s">
+        <v>699</v>
+      </c>
+      <c r="GX32" s="159" t="s">
+        <v>700</v>
+      </c>
+      <c r="GY32" s="115" t="s">
+        <v>698</v>
+      </c>
     </row>
-    <row r="33" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="92">
         <v>30</v>
       </c>
@@ -32633,8 +33876,35 @@
       <c r="GP33" s="115">
         <v>2</v>
       </c>
+      <c r="GQ33" s="208">
+        <v>7</v>
+      </c>
+      <c r="GR33" s="115">
+        <v>14</v>
+      </c>
+      <c r="GS33" s="159">
+        <v>81</v>
+      </c>
+      <c r="GT33" s="159">
+        <v>7</v>
+      </c>
+      <c r="GU33" s="159">
+        <v>4</v>
+      </c>
+      <c r="GV33" s="159">
+        <v>6</v>
+      </c>
+      <c r="GW33" s="159">
+        <v>6</v>
+      </c>
+      <c r="GX33" s="184">
+        <v>6</v>
+      </c>
+      <c r="GY33" s="115">
+        <v>2</v>
+      </c>
     </row>
-    <row r="34" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="92">
         <v>31</v>
       </c>
@@ -33225,8 +34495,35 @@
       <c r="GP34" s="115" t="s">
         <v>704</v>
       </c>
+      <c r="GQ34" s="208" t="s">
+        <v>1441</v>
+      </c>
+      <c r="GR34" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS34" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT34" s="184" t="s">
+        <v>698</v>
+      </c>
+      <c r="GU34" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV34" s="159" t="s">
+        <v>700</v>
+      </c>
+      <c r="GW34" s="184" t="s">
+        <v>804</v>
+      </c>
+      <c r="GX34" s="184" t="s">
+        <v>698</v>
+      </c>
+      <c r="GY34" s="184" t="s">
+        <v>704</v>
+      </c>
     </row>
-    <row r="35" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="92">
         <v>32</v>
       </c>
@@ -33817,8 +35114,35 @@
       <c r="GP35" s="115">
         <v>14</v>
       </c>
+      <c r="GQ35" s="209">
+        <v>86</v>
+      </c>
+      <c r="GR35" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS35" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT35" s="159">
+        <v>2</v>
+      </c>
+      <c r="GU35" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV35" s="184">
+        <v>6</v>
+      </c>
+      <c r="GW35" s="184">
+        <v>2</v>
+      </c>
+      <c r="GX35" s="184">
+        <v>2</v>
+      </c>
+      <c r="GY35" s="115">
+        <v>14</v>
+      </c>
     </row>
-    <row r="36" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="92">
         <v>33</v>
       </c>
@@ -34409,8 +35733,35 @@
       <c r="GP36" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ36" s="211" t="s">
+        <v>702</v>
+      </c>
+      <c r="GR36" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS36" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT36" s="184" t="s">
+        <v>702</v>
+      </c>
+      <c r="GU36" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV36" s="184" t="s">
+        <v>698</v>
+      </c>
+      <c r="GW36" s="159" t="s">
+        <v>700</v>
+      </c>
+      <c r="GX36" s="159" t="s">
+        <v>702</v>
+      </c>
+      <c r="GY36" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="37" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="92">
         <v>34</v>
       </c>
@@ -35001,8 +36352,35 @@
       <c r="GP37" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ37" s="210">
+        <v>14</v>
+      </c>
+      <c r="GR37" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS37" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT37" s="184">
+        <v>3</v>
+      </c>
+      <c r="GU37" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV37" s="184">
+        <v>2</v>
+      </c>
+      <c r="GW37" s="184">
+        <v>6</v>
+      </c>
+      <c r="GX37" s="159">
+        <v>3</v>
+      </c>
+      <c r="GY37" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="38" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="92">
         <v>35</v>
       </c>
@@ -35593,8 +36971,35 @@
       <c r="GP38" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ38" s="211" t="s">
+        <v>698</v>
+      </c>
+      <c r="GR38" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV38" s="159" t="s">
+        <v>702</v>
+      </c>
+      <c r="GW38" s="184" t="s">
+        <v>805</v>
+      </c>
+      <c r="GX38" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY38" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="39" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="92">
         <v>36</v>
       </c>
@@ -36185,8 +37590,35 @@
       <c r="GP39" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ39" s="210">
+        <v>2</v>
+      </c>
+      <c r="GR39" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV39" s="159">
+        <v>3</v>
+      </c>
+      <c r="GW39" s="184">
+        <v>2</v>
+      </c>
+      <c r="GX39" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY39" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="40" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="92">
         <v>37</v>
       </c>
@@ -36777,8 +38209,35 @@
       <c r="GP40" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ40" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR40" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW40" s="159" t="s">
+        <v>702</v>
+      </c>
+      <c r="GX40" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY40" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="92">
         <v>38</v>
       </c>
@@ -37369,8 +38828,35 @@
       <c r="GP41" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ41" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR41" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW41" s="159">
+        <v>3</v>
+      </c>
+      <c r="GX41" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY41" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="42" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="92">
         <v>39</v>
       </c>
@@ -37961,8 +39447,35 @@
       <c r="GP42" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ42" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR42" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX42" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY42" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="92">
         <v>40</v>
       </c>
@@ -38553,8 +40066,35 @@
       <c r="GP43" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ43" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR43" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX43" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY43" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="44" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="92">
         <v>41</v>
       </c>
@@ -39145,8 +40685,35 @@
       <c r="GP44" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ44" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR44" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX44" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY44" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="45" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="92">
         <v>42</v>
       </c>
@@ -39737,8 +41304,35 @@
       <c r="GP45" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ45" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR45" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX45" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY45" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="46" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="92">
         <v>43</v>
       </c>
@@ -40329,8 +41923,35 @@
       <c r="GP46" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ46" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR46" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX46" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY46" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="47" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="92">
         <v>44</v>
       </c>
@@ -40921,8 +42542,35 @@
       <c r="GP47" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ47" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR47" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX47" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY47" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="48" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="92">
         <v>45</v>
       </c>
@@ -41513,8 +43161,35 @@
       <c r="GP48" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ48" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR48" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX48" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY48" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="49" spans="1:198" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:207" s="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="92">
         <v>46</v>
       </c>
@@ -42105,8 +43780,35 @@
       <c r="GP49" s="115" t="s">
         <v>11</v>
       </c>
+      <c r="GQ49" s="208" t="s">
+        <v>11</v>
+      </c>
+      <c r="GR49" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX49" s="159" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY49" s="115" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="50" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="92">
         <v>47</v>
       </c>
@@ -42679,7 +44381,7 @@
         <v>3015</v>
       </c>
       <c r="GJ50" s="159" t="s">
-        <v>3027</v>
+        <v>3026</v>
       </c>
       <c r="GK50" s="159" t="s">
         <v>1978</v>
@@ -42694,13 +44396,40 @@
         <v>2663</v>
       </c>
       <c r="GO50" s="115" t="s">
-        <v>3092</v>
+        <v>3091</v>
       </c>
       <c r="GP50" s="115" t="s">
         <v>2807</v>
       </c>
+      <c r="GQ50" s="208" t="s">
+        <v>3128</v>
+      </c>
+      <c r="GR50" s="115" t="s">
+        <v>1978</v>
+      </c>
+      <c r="GS50" s="115" t="s">
+        <v>3158</v>
+      </c>
+      <c r="GT50" s="115" t="s">
+        <v>3174</v>
+      </c>
+      <c r="GU50" s="115" t="s">
+        <v>3190</v>
+      </c>
+      <c r="GV50" s="115" t="s">
+        <v>3209</v>
+      </c>
+      <c r="GW50" s="115" t="s">
+        <v>3226</v>
+      </c>
+      <c r="GX50" s="115" t="s">
+        <v>3240</v>
+      </c>
+      <c r="GY50" s="115" t="s">
+        <v>3252</v>
+      </c>
     </row>
-    <row r="51" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="92">
         <v>48</v>
       </c>
@@ -43273,28 +45002,55 @@
         <v>3016</v>
       </c>
       <c r="GJ51" s="159" t="s">
-        <v>3028</v>
+        <v>3027</v>
       </c>
       <c r="GK51" s="159" t="s">
-        <v>3041</v>
+        <v>3040</v>
       </c>
       <c r="GL51" s="216" t="s">
-        <v>3050</v>
+        <v>3049</v>
       </c>
       <c r="GM51" s="115" t="s">
-        <v>3062</v>
+        <v>3061</v>
       </c>
       <c r="GN51" s="115" t="s">
-        <v>3076</v>
+        <v>3075</v>
       </c>
       <c r="GO51" s="115" t="s">
-        <v>3093</v>
+        <v>3092</v>
       </c>
       <c r="GP51" s="216" t="s">
-        <v>3108</v>
+        <v>3107</v>
+      </c>
+      <c r="GQ51" s="208" t="s">
+        <v>3129</v>
+      </c>
+      <c r="GR51" s="216" t="s">
+        <v>3144</v>
+      </c>
+      <c r="GS51" s="115" t="s">
+        <v>3159</v>
+      </c>
+      <c r="GT51" s="115" t="s">
+        <v>3175</v>
+      </c>
+      <c r="GU51" s="115" t="s">
+        <v>3191</v>
+      </c>
+      <c r="GV51" s="159" t="s">
+        <v>3210</v>
+      </c>
+      <c r="GW51" s="159" t="s">
+        <v>3227</v>
+      </c>
+      <c r="GX51" s="115" t="s">
+        <v>3241</v>
+      </c>
+      <c r="GY51" s="115" t="s">
+        <v>3253</v>
       </c>
     </row>
-    <row r="52" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="92">
         <v>49</v>
       </c>
@@ -43867,28 +45623,55 @@
         <v>3017</v>
       </c>
       <c r="GJ52" s="159" t="s">
-        <v>3029</v>
+        <v>3028</v>
       </c>
       <c r="GK52" s="159" t="s">
-        <v>3042</v>
+        <v>3041</v>
       </c>
       <c r="GL52" s="115" t="s">
-        <v>3051</v>
+        <v>3050</v>
       </c>
       <c r="GM52" s="115" t="s">
-        <v>3063</v>
+        <v>3062</v>
       </c>
       <c r="GN52" s="115" t="s">
-        <v>3077</v>
+        <v>3076</v>
       </c>
       <c r="GO52" s="115" t="s">
-        <v>3094</v>
+        <v>3093</v>
       </c>
       <c r="GP52" s="115" t="s">
-        <v>3109</v>
+        <v>3108</v>
+      </c>
+      <c r="GQ52" s="208" t="s">
+        <v>3130</v>
+      </c>
+      <c r="GR52" s="115" t="s">
+        <v>3041</v>
+      </c>
+      <c r="GS52" s="115" t="s">
+        <v>3160</v>
+      </c>
+      <c r="GT52" s="115" t="s">
+        <v>3176</v>
+      </c>
+      <c r="GU52" s="115" t="s">
+        <v>3192</v>
+      </c>
+      <c r="GV52" s="159" t="s">
+        <v>3211</v>
+      </c>
+      <c r="GW52" s="159" t="s">
+        <v>3228</v>
+      </c>
+      <c r="GX52" s="115" t="s">
+        <v>3242</v>
+      </c>
+      <c r="GY52" s="115" t="s">
+        <v>3254</v>
       </c>
     </row>
-    <row r="53" spans="1:198" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:207" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="92">
         <v>50</v>
       </c>
@@ -44483,8 +46266,35 @@
       <c r="GP53" s="185" t="s">
         <v>206</v>
       </c>
+      <c r="GQ53" s="210" t="s">
+        <v>206</v>
+      </c>
+      <c r="GR53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GS53" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="GT53" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="GU53" s="183" t="s">
+        <v>207</v>
+      </c>
+      <c r="GV53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GW53" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="GX53" s="206" t="s">
+        <v>206</v>
+      </c>
+      <c r="GY53" s="185" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="54" spans="1:198" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:207" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A54" s="92">
         <v>51</v>
       </c>
@@ -45075,10 +46885,37 @@
         <v>61</v>
       </c>
       <c r="GP54" s="185" t="s">
-        <v>3110</v>
+        <v>3109</v>
+      </c>
+      <c r="GQ54" s="210" t="s">
+        <v>61</v>
+      </c>
+      <c r="GR54" s="185" t="s">
+        <v>61</v>
+      </c>
+      <c r="GS54" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="GT54" s="183" t="s">
+        <v>61</v>
+      </c>
+      <c r="GU54" s="115" t="s">
+        <v>728</v>
+      </c>
+      <c r="GV54" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="GW54" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="GX54" s="185" t="s">
+        <v>61</v>
+      </c>
+      <c r="GY54" s="115" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:198" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:207" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A55" s="92">
         <v>52</v>
       </c>
@@ -45660,19 +47497,46 @@
         <v>2330</v>
       </c>
       <c r="GM55" s="115" t="s">
-        <v>3064</v>
+        <v>3063</v>
       </c>
       <c r="GN55" s="185" t="s">
         <v>2330</v>
       </c>
       <c r="GO55" s="115" t="s">
-        <v>3095</v>
+        <v>3094</v>
       </c>
       <c r="GP55" s="185" t="s">
-        <v>3111</v>
+        <v>3110</v>
+      </c>
+      <c r="GQ55" s="210" t="s">
+        <v>3131</v>
+      </c>
+      <c r="GR55" s="185" t="s">
+        <v>3145</v>
+      </c>
+      <c r="GS55" s="159" t="s">
+        <v>3161</v>
+      </c>
+      <c r="GT55" s="183" t="s">
+        <v>3131</v>
+      </c>
+      <c r="GU55" s="159" t="s">
+        <v>3193</v>
+      </c>
+      <c r="GV55" s="115" t="s">
+        <v>3212</v>
+      </c>
+      <c r="GW55" s="115" t="s">
+        <v>3212</v>
+      </c>
+      <c r="GX55" s="185" t="s">
+        <v>3243</v>
+      </c>
+      <c r="GY55" s="115" t="s">
+        <v>3212</v>
       </c>
     </row>
-    <row r="56" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="92">
         <v>53</v>
       </c>
@@ -46252,19 +48116,46 @@
         <v>2330</v>
       </c>
       <c r="GM56" s="115" t="s">
-        <v>3065</v>
+        <v>3064</v>
       </c>
       <c r="GN56" s="185" t="s">
         <v>2330</v>
       </c>
       <c r="GO56" s="186" t="s">
-        <v>3096</v>
+        <v>3095</v>
       </c>
       <c r="GP56" s="185" t="s">
-        <v>3112</v>
+        <v>3111</v>
+      </c>
+      <c r="GQ56" s="69" t="s">
+        <v>3132</v>
+      </c>
+      <c r="GR56" s="185" t="s">
+        <v>3146</v>
+      </c>
+      <c r="GS56" s="159" t="s">
+        <v>3162</v>
+      </c>
+      <c r="GT56" s="185" t="s">
+        <v>3177</v>
+      </c>
+      <c r="GU56" s="159" t="s">
+        <v>3194</v>
+      </c>
+      <c r="GV56" s="115" t="s">
+        <v>3213</v>
+      </c>
+      <c r="GW56" s="115" t="s">
+        <v>3229</v>
+      </c>
+      <c r="GX56" s="169" t="s">
+        <v>3244</v>
+      </c>
+      <c r="GY56" s="115" t="s">
+        <v>3213</v>
       </c>
     </row>
-    <row r="57" spans="1:198" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:207" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A57" s="92">
         <v>54</v>
       </c>
@@ -46849,16 +48740,43 @@
         <v>2083</v>
       </c>
       <c r="GN57" s="115" t="s">
-        <v>3078</v>
+        <v>3077</v>
       </c>
       <c r="GO57" s="115" t="s">
-        <v>3097</v>
+        <v>3096</v>
       </c>
       <c r="GP57" s="185" t="s">
-        <v>3113</v>
+        <v>3112</v>
+      </c>
+      <c r="GQ57" s="69" t="s">
+        <v>3133</v>
+      </c>
+      <c r="GR57" s="185" t="s">
+        <v>3147</v>
+      </c>
+      <c r="GS57" s="159" t="s">
+        <v>3163</v>
+      </c>
+      <c r="GT57" s="185" t="s">
+        <v>3178</v>
+      </c>
+      <c r="GU57" s="159" t="s">
+        <v>3195</v>
+      </c>
+      <c r="GV57" s="115" t="s">
+        <v>3214</v>
+      </c>
+      <c r="GW57" s="115" t="s">
+        <v>3230</v>
+      </c>
+      <c r="GX57" s="115" t="s">
+        <v>3245</v>
+      </c>
+      <c r="GY57" s="115" t="s">
+        <v>3214</v>
       </c>
     </row>
-    <row r="58" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="92">
         <v>55</v>
       </c>
@@ -47411,19 +49329,46 @@
         <v>2330</v>
       </c>
       <c r="GM58" s="206" t="s">
-        <v>3066</v>
+        <v>3065</v>
       </c>
       <c r="GN58" s="185" t="s">
         <v>2330</v>
       </c>
       <c r="GO58" s="186" t="s">
-        <v>3096</v>
+        <v>3095</v>
       </c>
       <c r="GP58" s="185" t="s">
-        <v>3114</v>
+        <v>3113</v>
+      </c>
+      <c r="GQ58" s="186" t="s">
+        <v>3134</v>
+      </c>
+      <c r="GR58" s="185" t="s">
+        <v>3148</v>
+      </c>
+      <c r="GS58" s="159" t="s">
+        <v>3164</v>
+      </c>
+      <c r="GT58" s="194" t="s">
+        <v>3179</v>
+      </c>
+      <c r="GU58" s="159" t="s">
+        <v>3194</v>
+      </c>
+      <c r="GV58" s="115" t="s">
+        <v>3213</v>
+      </c>
+      <c r="GW58" s="115" t="s">
+        <v>3229</v>
+      </c>
+      <c r="GX58" s="169" t="s">
+        <v>3244</v>
+      </c>
+      <c r="GY58" s="115" t="s">
+        <v>3213</v>
       </c>
     </row>
-    <row r="59" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="92">
         <v>56</v>
       </c>
@@ -48005,19 +49950,46 @@
         <v>2330</v>
       </c>
       <c r="GM59" s="206" t="s">
-        <v>3067</v>
+        <v>3066</v>
       </c>
       <c r="GN59" s="185" t="s">
         <v>2330</v>
       </c>
       <c r="GO59" s="186" t="s">
-        <v>3096</v>
+        <v>3095</v>
       </c>
       <c r="GP59" s="185" t="s">
-        <v>3114</v>
+        <v>3113</v>
+      </c>
+      <c r="GQ59" s="69" t="s">
+        <v>3135</v>
+      </c>
+      <c r="GR59" s="185" t="s">
+        <v>3148</v>
+      </c>
+      <c r="GS59" s="159" t="s">
+        <v>3164</v>
+      </c>
+      <c r="GT59" s="194" t="s">
+        <v>3179</v>
+      </c>
+      <c r="GU59" s="159" t="s">
+        <v>3194</v>
+      </c>
+      <c r="GV59" s="115" t="s">
+        <v>3213</v>
+      </c>
+      <c r="GW59" s="115" t="s">
+        <v>3229</v>
+      </c>
+      <c r="GX59" s="169" t="s">
+        <v>3244</v>
+      </c>
+      <c r="GY59" s="115" t="s">
+        <v>3213</v>
       </c>
     </row>
-    <row r="60" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="92">
         <v>57</v>
       </c>
@@ -48610,8 +50582,35 @@
       <c r="GP60" s="184">
         <v>1</v>
       </c>
+      <c r="GQ60" s="188">
+        <v>1</v>
+      </c>
+      <c r="GR60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GS60" s="182">
+        <v>1</v>
+      </c>
+      <c r="GT60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GU60" s="182">
+        <v>1</v>
+      </c>
+      <c r="GV60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GW60" s="184">
+        <v>1</v>
+      </c>
+      <c r="GX60" s="65">
+        <v>1</v>
+      </c>
+      <c r="GY60" s="184">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:198" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:207" ht="14.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="92">
         <v>58</v>
       </c>
@@ -49204,8 +51203,35 @@
       <c r="GP61" s="192">
         <v>45813</v>
       </c>
+      <c r="GQ61" s="205">
+        <v>45840</v>
+      </c>
+      <c r="GR61" s="192">
+        <v>45841</v>
+      </c>
+      <c r="GS61" s="157">
+        <v>45835</v>
+      </c>
+      <c r="GT61" s="192">
+        <v>45840</v>
+      </c>
+      <c r="GU61" s="157">
+        <v>45841</v>
+      </c>
+      <c r="GV61" s="157">
+        <v>45870</v>
+      </c>
+      <c r="GW61" s="157">
+        <v>45870</v>
+      </c>
+      <c r="GX61" s="193">
+        <v>45839</v>
+      </c>
+      <c r="GY61" s="157">
+        <v>45870</v>
+      </c>
     </row>
-    <row r="62" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="92">
         <v>59</v>
       </c>
@@ -49798,8 +51824,35 @@
       <c r="GP62" s="192">
         <v>45813</v>
       </c>
+      <c r="GQ62" s="205">
+        <v>45840</v>
+      </c>
+      <c r="GR62" s="192">
+        <v>45841</v>
+      </c>
+      <c r="GS62" s="157">
+        <v>45835</v>
+      </c>
+      <c r="GT62" s="192">
+        <v>45840</v>
+      </c>
+      <c r="GU62" s="157">
+        <v>45866</v>
+      </c>
+      <c r="GV62" s="157">
+        <v>45872</v>
+      </c>
+      <c r="GW62" s="157">
+        <v>45871</v>
+      </c>
+      <c r="GX62" s="193">
+        <v>45867</v>
+      </c>
+      <c r="GY62" s="157">
+        <v>45871</v>
+      </c>
     </row>
-    <row r="63" spans="1:198" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:207" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="92">
         <v>60</v>
       </c>
@@ -50381,10 +52434,10 @@
         <v>2331</v>
       </c>
       <c r="GM63" s="115" t="s">
-        <v>3079</v>
+        <v>3078</v>
       </c>
       <c r="GN63" s="115" t="s">
-        <v>3079</v>
+        <v>3078</v>
       </c>
       <c r="GO63" s="115" t="s">
         <v>2462</v>
@@ -50392,8 +52445,35 @@
       <c r="GP63" s="115" t="s">
         <v>30</v>
       </c>
+      <c r="GQ63" s="191" t="s">
+        <v>30</v>
+      </c>
+      <c r="GR63" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GS63" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GT63" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GU63" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GV63" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GW63" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GX63" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GY63" s="115" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="64" spans="1:198" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:207" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A64" s="92">
         <v>61</v>
       </c>
@@ -50969,25 +53049,52 @@
         <v>72</v>
       </c>
       <c r="GK64" s="185" t="s">
-        <v>3043</v>
+        <v>3042</v>
       </c>
       <c r="GL64" s="185" t="s">
-        <v>3043</v>
+        <v>3042</v>
       </c>
       <c r="GM64" s="115" t="s">
-        <v>3068</v>
+        <v>3067</v>
       </c>
       <c r="GN64" s="115" t="s">
         <v>2669</v>
       </c>
       <c r="GO64" s="115" t="s">
-        <v>3098</v>
+        <v>3097</v>
       </c>
       <c r="GP64" s="185" t="s">
-        <v>3115</v>
+        <v>3114</v>
+      </c>
+      <c r="GQ64" s="69" t="s">
+        <v>2332</v>
+      </c>
+      <c r="GR64" s="185" t="s">
+        <v>3114</v>
+      </c>
+      <c r="GS64" s="115" t="s">
+        <v>3165</v>
+      </c>
+      <c r="GT64" s="185" t="s">
+        <v>2332</v>
+      </c>
+      <c r="GU64" s="115" t="s">
+        <v>3165</v>
+      </c>
+      <c r="GV64" s="115" t="s">
+        <v>2698</v>
+      </c>
+      <c r="GW64" s="115" t="s">
+        <v>2698</v>
+      </c>
+      <c r="GX64" s="115" t="s">
+        <v>3246</v>
+      </c>
+      <c r="GY64" s="115" t="s">
+        <v>2698</v>
       </c>
     </row>
-    <row r="65" spans="1:205" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:255" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="92">
         <v>62</v>
       </c>
@@ -51283,8 +53390,35 @@
       <c r="GP65" s="192">
         <v>45813</v>
       </c>
+      <c r="GQ65" s="205">
+        <v>45840</v>
+      </c>
+      <c r="GR65" s="192">
+        <v>45841</v>
+      </c>
+      <c r="GS65" s="157">
+        <v>45842</v>
+      </c>
+      <c r="GT65" s="192">
+        <v>45840</v>
+      </c>
+      <c r="GU65" s="157">
+        <v>45866</v>
+      </c>
+      <c r="GV65" s="157">
+        <v>45872</v>
+      </c>
+      <c r="GW65" s="157">
+        <v>45871</v>
+      </c>
+      <c r="GX65" s="193">
+        <v>45867</v>
+      </c>
+      <c r="GY65" s="157">
+        <v>45871</v>
+      </c>
     </row>
-    <row r="66" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:255" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A66" s="92">
         <v>63</v>
       </c>
@@ -51564,7 +53698,7 @@
         <v>30</v>
       </c>
       <c r="GL66" s="169" t="s">
-        <v>3052</v>
+        <v>3051</v>
       </c>
       <c r="GM66" s="115" t="s">
         <v>30</v>
@@ -51578,8 +53712,35 @@
       <c r="GP66" s="115" t="s">
         <v>30</v>
       </c>
+      <c r="GQ66" s="191" t="s">
+        <v>30</v>
+      </c>
+      <c r="GR66" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GS66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GT66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GU66" s="169" t="s">
+        <v>30</v>
+      </c>
+      <c r="GV66" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GW66" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GX66" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="GY66" s="115" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="67" spans="1:205" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:255" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="92">
         <v>64</v>
       </c>
@@ -51701,8 +53862,17 @@
       <c r="GN67" s="206"/>
       <c r="GO67" s="169"/>
       <c r="GP67" s="169"/>
+      <c r="GQ67" s="191"/>
+      <c r="GR67" s="169"/>
+      <c r="GS67" s="169"/>
+      <c r="GT67" s="169"/>
+      <c r="GU67" s="169"/>
+      <c r="GV67" s="206"/>
+      <c r="GW67" s="206"/>
+      <c r="GX67" s="156"/>
+      <c r="GY67" s="156"/>
     </row>
-    <row r="68" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:255" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A68" s="92">
         <v>65</v>
       </c>
@@ -51774,8 +53944,12 @@
       <c r="GL68" s="169"/>
       <c r="GM68" s="169"/>
       <c r="GN68" s="206"/>
+      <c r="GU68" s="169"/>
+      <c r="GW68" s="206"/>
+      <c r="GX68" s="156"/>
+      <c r="GY68" s="156"/>
     </row>
-    <row r="69" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:255" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A69" s="92">
         <v>66</v>
       </c>
@@ -51823,8 +53997,9 @@
       <c r="EV69" s="196"/>
       <c r="FV69" s="196"/>
       <c r="GC69" s="156"/>
+      <c r="GW69" s="206"/>
     </row>
-    <row r="70" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:255" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A70" s="92">
         <v>67</v>
       </c>
@@ -51862,8 +54037,9 @@
       <c r="EN70" s="169"/>
       <c r="ER70" s="169"/>
       <c r="GC70" s="156"/>
+      <c r="GW70" s="206"/>
     </row>
-    <row r="71" spans="1:205" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:255" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A71" s="92">
         <v>68</v>
       </c>
@@ -51898,7 +54074,7 @@
       <c r="EG71" s="156"/>
       <c r="ER71" s="169"/>
     </row>
-    <row r="72" spans="1:205" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:255" x14ac:dyDescent="0.4">
       <c r="A72" s="92">
         <v>69</v>
       </c>
@@ -51930,7 +54106,7 @@
       <c r="BY72" s="158"/>
       <c r="BZ72" s="158"/>
     </row>
-    <row r="73" spans="1:205" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:255" x14ac:dyDescent="0.4">
       <c r="U73" s="12"/>
       <c r="AF73" s="48"/>
       <c r="AG73" s="49"/>
@@ -51952,7 +54128,7 @@
       <c r="BY73" s="90"/>
       <c r="BZ73" s="90"/>
     </row>
-    <row r="74" spans="1:205" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:255" x14ac:dyDescent="0.4">
       <c r="A74" s="37"/>
       <c r="D74" s="37"/>
       <c r="E74" s="105"/>
@@ -52429,6 +54605,156 @@
       </c>
       <c r="GW74" s="167">
         <v>200</v>
+      </c>
+      <c r="GX74" s="167">
+        <v>201</v>
+      </c>
+      <c r="GY74" s="168">
+        <v>202</v>
+      </c>
+      <c r="GZ74" s="167">
+        <v>203</v>
+      </c>
+      <c r="HA74" s="167">
+        <v>204</v>
+      </c>
+      <c r="HB74" s="168">
+        <v>205</v>
+      </c>
+      <c r="HC74" s="167">
+        <v>206</v>
+      </c>
+      <c r="HD74" s="167">
+        <v>207</v>
+      </c>
+      <c r="HE74" s="168">
+        <v>208</v>
+      </c>
+      <c r="HF74" s="167">
+        <v>209</v>
+      </c>
+      <c r="HG74" s="167">
+        <v>210</v>
+      </c>
+      <c r="HH74" s="168">
+        <v>211</v>
+      </c>
+      <c r="HI74" s="167">
+        <v>212</v>
+      </c>
+      <c r="HJ74" s="167">
+        <v>213</v>
+      </c>
+      <c r="HK74" s="168">
+        <v>214</v>
+      </c>
+      <c r="HL74" s="167">
+        <v>215</v>
+      </c>
+      <c r="HM74" s="167">
+        <v>216</v>
+      </c>
+      <c r="HN74" s="168">
+        <v>217</v>
+      </c>
+      <c r="HO74" s="167">
+        <v>218</v>
+      </c>
+      <c r="HP74" s="167">
+        <v>219</v>
+      </c>
+      <c r="HQ74" s="168">
+        <v>220</v>
+      </c>
+      <c r="HR74" s="167">
+        <v>221</v>
+      </c>
+      <c r="HS74" s="167">
+        <v>222</v>
+      </c>
+      <c r="HT74" s="168">
+        <v>223</v>
+      </c>
+      <c r="HU74" s="167">
+        <v>224</v>
+      </c>
+      <c r="HV74" s="167">
+        <v>225</v>
+      </c>
+      <c r="HW74" s="168">
+        <v>226</v>
+      </c>
+      <c r="HX74" s="167">
+        <v>227</v>
+      </c>
+      <c r="HY74" s="167">
+        <v>228</v>
+      </c>
+      <c r="HZ74" s="168">
+        <v>229</v>
+      </c>
+      <c r="IA74" s="167">
+        <v>230</v>
+      </c>
+      <c r="IB74" s="167">
+        <v>231</v>
+      </c>
+      <c r="IC74" s="168">
+        <v>232</v>
+      </c>
+      <c r="ID74" s="167">
+        <v>233</v>
+      </c>
+      <c r="IE74" s="168">
+        <v>234</v>
+      </c>
+      <c r="IF74" s="167">
+        <v>235</v>
+      </c>
+      <c r="IG74" s="168">
+        <v>236</v>
+      </c>
+      <c r="IH74" s="167">
+        <v>237</v>
+      </c>
+      <c r="II74" s="168">
+        <v>238</v>
+      </c>
+      <c r="IJ74" s="167">
+        <v>239</v>
+      </c>
+      <c r="IK74" s="168">
+        <v>240</v>
+      </c>
+      <c r="IL74" s="167">
+        <v>241</v>
+      </c>
+      <c r="IM74" s="168">
+        <v>242</v>
+      </c>
+      <c r="IN74" s="167">
+        <v>243</v>
+      </c>
+      <c r="IO74" s="168">
+        <v>244</v>
+      </c>
+      <c r="IP74" s="167">
+        <v>245</v>
+      </c>
+      <c r="IQ74" s="168">
+        <v>246</v>
+      </c>
+      <c r="IR74" s="167">
+        <v>247</v>
+      </c>
+      <c r="IS74" s="167">
+        <v>248</v>
+      </c>
+      <c r="IT74" s="168">
+        <v>249</v>
+      </c>
+      <c r="IU74" s="167">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>